<commit_message>
update results: confirmed pattern from excel_results
</commit_message>
<xml_diff>
--- a/swertres/excel_results.xlsx
+++ b/swertres/excel_results.xlsx
@@ -43,11 +43,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="00ff6699"/>
       </patternFill>
     </fill>
@@ -89,6 +84,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="0066cc33"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -220,6 +220,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -244,16 +247,13 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1306,7 +1306,7 @@
           <t>871</t>
         </is>
       </c>
-      <c r="T5" s="17" t="inlineStr">
+      <c r="T5" s="11" t="inlineStr">
         <is>
           <t>362</t>
         </is>
@@ -1735,7 +1735,7 @@
           <t>303</t>
         </is>
       </c>
-      <c r="AE7" s="14" t="inlineStr">
+      <c r="AE7" s="17" t="inlineStr">
         <is>
           <t>566</t>
         </is>
@@ -2555,7 +2555,7 @@
           <t>678</t>
         </is>
       </c>
-      <c r="H12" s="17" t="inlineStr">
+      <c r="H12" s="7" t="inlineStr">
         <is>
           <t>623</t>
         </is>
@@ -2904,7 +2904,7 @@
           <t>052</t>
         </is>
       </c>
-      <c r="C14" s="17" t="inlineStr">
+      <c r="C14" s="5" t="inlineStr">
         <is>
           <t>632</t>
         </is>
@@ -3019,7 +3019,7 @@
           <t>280</t>
         </is>
       </c>
-      <c r="Z14" s="17" t="inlineStr">
+      <c r="Z14" s="13" t="inlineStr">
         <is>
           <t>623</t>
         </is>
@@ -5522,7 +5522,7 @@
           <t>339</t>
         </is>
       </c>
-      <c r="C28" s="17" t="inlineStr">
+      <c r="C28" s="5" t="inlineStr">
         <is>
           <t>263</t>
         </is>
@@ -8701,7 +8701,7 @@
           <t>832</t>
         </is>
       </c>
-      <c r="W47" s="17" t="inlineStr">
+      <c r="W47" s="12" t="inlineStr">
         <is>
           <t>263</t>
         </is>
@@ -9399,7 +9399,7 @@
           <t>039</t>
         </is>
       </c>
-      <c r="M51" s="8" t="inlineStr">
+      <c r="M51" s="17" t="inlineStr">
         <is>
           <t>418</t>
         </is>
@@ -11112,7 +11112,7 @@
           <t>971</t>
         </is>
       </c>
-      <c r="S60" s="17" t="inlineStr">
+      <c r="S60" s="10" t="inlineStr">
         <is>
           <t>623</t>
         </is>
@@ -11379,7 +11379,7 @@
           <t>230</t>
         </is>
       </c>
-      <c r="AI61" s="17" t="inlineStr">
+      <c r="AI61" s="16" t="inlineStr">
         <is>
           <t>362</t>
         </is>
@@ -11598,7 +11598,7 @@
           <t>582</t>
         </is>
       </c>
-      <c r="D63" s="5" t="inlineStr">
+      <c r="D63" s="17" t="inlineStr">
         <is>
           <t>418</t>
         </is>
@@ -12032,7 +12032,7 @@
           <t>791</t>
         </is>
       </c>
-      <c r="P65" s="9" t="inlineStr">
+      <c r="P65" s="17" t="inlineStr">
         <is>
           <t>418</t>
         </is>
@@ -12194,7 +12194,7 @@
           <t>429</t>
         </is>
       </c>
-      <c r="K66" s="17" t="inlineStr">
+      <c r="K66" s="8" t="inlineStr">
         <is>
           <t>326</t>
         </is>
@@ -12411,7 +12411,7 @@
           <t>269</t>
         </is>
       </c>
-      <c r="Q67" s="17" t="inlineStr">
+      <c r="Q67" s="10" t="inlineStr">
         <is>
           <t>623</t>
         </is>
@@ -13443,7 +13443,7 @@
           <t>008</t>
         </is>
       </c>
-      <c r="S75" s="17" t="inlineStr">
+      <c r="S75" s="10" t="inlineStr">
         <is>
           <t>326</t>
         </is>
@@ -13752,7 +13752,7 @@
           <t>248</t>
         </is>
       </c>
-      <c r="F77" s="17" t="inlineStr">
+      <c r="F77" s="6" t="inlineStr">
         <is>
           <t>326</t>
         </is>
@@ -13984,7 +13984,7 @@
           <t>994</t>
         </is>
       </c>
-      <c r="O78" s="17" t="inlineStr">
+      <c r="O78" s="9" t="inlineStr">
         <is>
           <t>362</t>
         </is>
@@ -14251,7 +14251,7 @@
           <t>819</t>
         </is>
       </c>
-      <c r="AE79" s="17" t="inlineStr">
+      <c r="AE79" s="14" t="inlineStr">
         <is>
           <t>362</t>
         </is>
@@ -15480,7 +15480,7 @@
           <t>216</t>
         </is>
       </c>
-      <c r="O86" s="17" t="inlineStr">
+      <c r="O86" s="9" t="inlineStr">
         <is>
           <t>632</t>
         </is>
@@ -16627,7 +16627,7 @@
           <t>118</t>
         </is>
       </c>
-      <c r="T92" s="17" t="inlineStr">
+      <c r="T92" s="11" t="inlineStr">
         <is>
           <t>623</t>
         </is>
@@ -16921,7 +16921,7 @@
           <t>831</t>
         </is>
       </c>
-      <c r="D94" s="17" t="inlineStr">
+      <c r="D94" s="5" t="inlineStr">
         <is>
           <t>623</t>
         </is>
@@ -17158,7 +17158,7 @@
           <t>772</t>
         </is>
       </c>
-      <c r="N95" s="17" t="inlineStr">
+      <c r="N95" s="9" t="inlineStr">
         <is>
           <t>362</t>
         </is>
@@ -18198,7 +18198,7 @@
           <t>536</t>
         </is>
       </c>
-      <c r="AI100" s="16" t="inlineStr">
+      <c r="AI100" s="17" t="inlineStr">
         <is>
           <t>566</t>
         </is>
@@ -20374,7 +20374,7 @@
           <t>631</t>
         </is>
       </c>
-      <c r="D115" s="17" t="inlineStr">
+      <c r="D115" s="5" t="inlineStr">
         <is>
           <t>623</t>
         </is>
@@ -20514,7 +20514,7 @@
           <t>767</t>
         </is>
       </c>
-      <c r="AF115" s="17" t="inlineStr">
+      <c r="AF115" s="15" t="inlineStr">
         <is>
           <t>623</t>
         </is>
@@ -21010,7 +21010,7 @@
           <t>846</t>
         </is>
       </c>
-      <c r="S118" s="10" t="inlineStr">
+      <c r="S118" s="17" t="inlineStr">
         <is>
           <t>418</t>
         </is>
@@ -21055,7 +21055,7 @@
           <t>283</t>
         </is>
       </c>
-      <c r="AB118" s="17" t="inlineStr">
+      <c r="AB118" s="13" t="inlineStr">
         <is>
           <t>632</t>
         </is>
@@ -23249,7 +23249,7 @@
           <t>887</t>
         </is>
       </c>
-      <c r="R130" s="17" t="inlineStr">
+      <c r="R130" s="10" t="inlineStr">
         <is>
           <t>263</t>
         </is>
@@ -24274,7 +24274,7 @@
           <t>824</t>
         </is>
       </c>
-      <c r="AJ135" s="17" t="inlineStr">
+      <c r="AJ135" s="16" t="inlineStr">
         <is>
           <t>236</t>
         </is>
@@ -24548,7 +24548,7 @@
           <t>610</t>
         </is>
       </c>
-      <c r="P137" s="17" t="inlineStr">
+      <c r="P137" s="9" t="inlineStr">
         <is>
           <t>326</t>
         </is>
@@ -25186,7 +25186,7 @@
           <t>682</t>
         </is>
       </c>
-      <c r="N143" s="17" t="inlineStr">
+      <c r="N143" s="9" t="inlineStr">
         <is>
           <t>632</t>
         </is>
@@ -27213,7 +27213,7 @@
           <t>023</t>
         </is>
       </c>
-      <c r="H154" s="7" t="inlineStr">
+      <c r="H154" s="17" t="inlineStr">
         <is>
           <t>418</t>
         </is>
@@ -28769,7 +28769,7 @@
           <t>088</t>
         </is>
       </c>
-      <c r="T162" s="17" t="inlineStr">
+      <c r="T162" s="11" t="inlineStr">
         <is>
           <t>623</t>
         </is>
@@ -28871,7 +28871,7 @@
           <t>036</t>
         </is>
       </c>
-      <c r="C163" s="5" t="inlineStr">
+      <c r="C163" s="17" t="inlineStr">
         <is>
           <t>566</t>
         </is>
@@ -29315,7 +29315,7 @@
           <t>053</t>
         </is>
       </c>
-      <c r="Q165" s="17" t="inlineStr">
+      <c r="Q165" s="10" t="inlineStr">
         <is>
           <t>623</t>
         </is>
@@ -29644,7 +29644,7 @@
           <t>850</t>
         </is>
       </c>
-      <c r="H167" s="17" t="inlineStr">
+      <c r="H167" s="7" t="inlineStr">
         <is>
           <t>632</t>
         </is>
@@ -31424,7 +31424,7 @@
           <t>053</t>
         </is>
       </c>
-      <c r="J179" s="17" t="inlineStr">
+      <c r="J179" s="7" t="inlineStr">
         <is>
           <t>236</t>
         </is>
@@ -33975,7 +33975,7 @@
           <t>493</t>
         </is>
       </c>
-      <c r="AH192" s="15" t="inlineStr">
+      <c r="AH192" s="17" t="inlineStr">
         <is>
           <t>418</t>
         </is>
@@ -34314,7 +34314,7 @@
           <t>622</t>
         </is>
       </c>
-      <c r="AA194" s="17" t="inlineStr">
+      <c r="AA194" s="13" t="inlineStr">
         <is>
           <t>236</t>
         </is>
@@ -34568,7 +34568,7 @@
           <t>531</t>
         </is>
       </c>
-      <c r="C196" s="5" t="inlineStr">
+      <c r="C196" s="17" t="inlineStr">
         <is>
           <t>418</t>
         </is>
@@ -36670,7 +36670,7 @@
           <t>638</t>
         </is>
       </c>
-      <c r="L207" s="17" t="inlineStr">
+      <c r="L207" s="8" t="inlineStr">
         <is>
           <t>362</t>
         </is>
@@ -36715,7 +36715,7 @@
           <t>222</t>
         </is>
       </c>
-      <c r="U207" s="17" t="inlineStr">
+      <c r="U207" s="11" t="inlineStr">
         <is>
           <t>236</t>
         </is>
@@ -38435,7 +38435,7 @@
           <t>507</t>
         </is>
       </c>
-      <c r="K219" s="17" t="inlineStr">
+      <c r="K219" s="8" t="inlineStr">
         <is>
           <t>623</t>
         </is>
@@ -41305,7 +41305,7 @@
           <t>465</t>
         </is>
       </c>
-      <c r="X234" s="12" t="inlineStr">
+      <c r="X234" s="17" t="inlineStr">
         <is>
           <t>566</t>
         </is>
@@ -41609,7 +41609,7 @@
           <t>905</t>
         </is>
       </c>
-      <c r="J236" s="17" t="inlineStr">
+      <c r="J236" s="7" t="inlineStr">
         <is>
           <t>236</t>
         </is>
@@ -42165,7 +42165,7 @@
           <t>627</t>
         </is>
       </c>
-      <c r="I239" s="17" t="inlineStr">
+      <c r="I239" s="7" t="inlineStr">
         <is>
           <t>263</t>
         </is>
@@ -42594,7 +42594,7 @@
           <t>482</t>
         </is>
       </c>
-      <c r="T241" s="17" t="inlineStr">
+      <c r="T241" s="11" t="inlineStr">
         <is>
           <t>623</t>
         </is>
@@ -43275,17 +43275,17 @@
       </c>
       <c r="B256" s="5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>523</t>
         </is>
       </c>
       <c r="C256" s="5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>520</t>
         </is>
       </c>
       <c r="D256" s="5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>869</t>
         </is>
       </c>
     </row>
@@ -43297,17 +43297,17 @@
       </c>
       <c r="B257" s="5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>302</t>
         </is>
       </c>
       <c r="C257" s="5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>220</t>
         </is>
       </c>
       <c r="D257" s="5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>469</t>
         </is>
       </c>
     </row>
@@ -43319,17 +43319,17 @@
       </c>
       <c r="B258" s="5" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C258" s="5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D258" s="5" t="inlineStr">
-        <is>
-          <t>-</t>
+          <t>991</t>
+        </is>
+      </c>
+      <c r="C258" s="17" t="inlineStr">
+        <is>
+          <t>566</t>
+        </is>
+      </c>
+      <c r="D258" s="17" t="inlineStr">
+        <is>
+          <t>418</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
switch color scheme for columns
</commit_message>
<xml_diff>
--- a/swertres/excel_results.xlsx
+++ b/swertres/excel_results.xlsx
@@ -38,12 +38,27 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="00ff6699"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="00ff6666"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00ff6699"/>
+        <fgColor rgb="00ff6633"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00ccff33"/>
       </patternFill>
     </fill>
     <fill>
@@ -53,7 +68,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="0066cc33"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="006699ff"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="006666ff"/>
       </patternFill>
     </fill>
     <fill>
@@ -63,32 +88,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00ccff33"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00ff6633"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="00339933"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00009966"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0066cc33"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FFFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -98,7 +98,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="006666ff"/>
+        <fgColor rgb="00009966"/>
       </patternFill>
     </fill>
   </fills>
@@ -220,9 +220,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -247,13 +244,16 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1735,7 +1735,7 @@
           <t>303</t>
         </is>
       </c>
-      <c r="AE7" s="17" t="inlineStr">
+      <c r="AE7" s="14" t="inlineStr">
         <is>
           <t>566</t>
         </is>
@@ -1969,7 +1969,7 @@
           <t>170</t>
         </is>
       </c>
-      <c r="C9" s="5" t="inlineStr">
+      <c r="C9" s="17" t="inlineStr">
         <is>
           <t>869</t>
         </is>
@@ -4026,7 +4026,7 @@
           <t>001</t>
         </is>
       </c>
-      <c r="C20" s="5" t="inlineStr">
+      <c r="C20" s="17" t="inlineStr">
         <is>
           <t>811</t>
         </is>
@@ -4041,7 +4041,7 @@
           <t>478</t>
         </is>
       </c>
-      <c r="F20" s="6" t="inlineStr">
+      <c r="F20" s="17" t="inlineStr">
         <is>
           <t>869</t>
         </is>
@@ -5709,7 +5709,7 @@
           <t>232</t>
         </is>
       </c>
-      <c r="C29" s="5" t="inlineStr">
+      <c r="C29" s="17" t="inlineStr">
         <is>
           <t>811</t>
         </is>
@@ -9399,7 +9399,7 @@
           <t>039</t>
         </is>
       </c>
-      <c r="M51" s="17" t="inlineStr">
+      <c r="M51" s="8" t="inlineStr">
         <is>
           <t>418</t>
         </is>
@@ -10055,7 +10055,7 @@
           <t>075</t>
         </is>
       </c>
-      <c r="AF54" s="15" t="inlineStr">
+      <c r="AF54" s="17" t="inlineStr">
         <is>
           <t>811</t>
         </is>
@@ -11598,7 +11598,7 @@
           <t>582</t>
         </is>
       </c>
-      <c r="D63" s="17" t="inlineStr">
+      <c r="D63" s="5" t="inlineStr">
         <is>
           <t>418</t>
         </is>
@@ -12032,7 +12032,7 @@
           <t>791</t>
         </is>
       </c>
-      <c r="P65" s="17" t="inlineStr">
+      <c r="P65" s="9" t="inlineStr">
         <is>
           <t>418</t>
         </is>
@@ -13034,7 +13034,7 @@
           <t>250</t>
         </is>
       </c>
-      <c r="L73" s="8" t="inlineStr">
+      <c r="L73" s="17" t="inlineStr">
         <is>
           <t>869</t>
         </is>
@@ -13261,7 +13261,7 @@
           <t>255</t>
         </is>
       </c>
-      <c r="T74" s="11" t="inlineStr">
+      <c r="T74" s="17" t="inlineStr">
         <is>
           <t>869</t>
         </is>
@@ -14044,7 +14044,7 @@
           <t>618</t>
         </is>
       </c>
-      <c r="AA78" s="13" t="inlineStr">
+      <c r="AA78" s="17" t="inlineStr">
         <is>
           <t>811</t>
         </is>
@@ -14697,7 +14697,7 @@
           <t>342</t>
         </is>
       </c>
-      <c r="H82" s="7" t="inlineStr">
+      <c r="H82" s="17" t="inlineStr">
         <is>
           <t>869</t>
         </is>
@@ -18078,7 +18078,7 @@
           <t>332</t>
         </is>
       </c>
-      <c r="K100" s="8" t="inlineStr">
+      <c r="K100" s="17" t="inlineStr">
         <is>
           <t>869</t>
         </is>
@@ -18198,7 +18198,7 @@
           <t>536</t>
         </is>
       </c>
-      <c r="AI100" s="17" t="inlineStr">
+      <c r="AI100" s="16" t="inlineStr">
         <is>
           <t>566</t>
         </is>
@@ -21010,7 +21010,7 @@
           <t>846</t>
         </is>
       </c>
-      <c r="S118" s="17" t="inlineStr">
+      <c r="S118" s="10" t="inlineStr">
         <is>
           <t>418</t>
         </is>
@@ -27213,7 +27213,7 @@
           <t>023</t>
         </is>
       </c>
-      <c r="H154" s="17" t="inlineStr">
+      <c r="H154" s="7" t="inlineStr">
         <is>
           <t>418</t>
         </is>
@@ -28268,7 +28268,7 @@
           <t>588</t>
         </is>
       </c>
-      <c r="AF159" s="15" t="inlineStr">
+      <c r="AF159" s="17" t="inlineStr">
         <is>
           <t>811</t>
         </is>
@@ -28871,7 +28871,7 @@
           <t>036</t>
         </is>
       </c>
-      <c r="C163" s="17" t="inlineStr">
+      <c r="C163" s="5" t="inlineStr">
         <is>
           <t>566</t>
         </is>
@@ -33975,7 +33975,7 @@
           <t>493</t>
         </is>
       </c>
-      <c r="AH192" s="17" t="inlineStr">
+      <c r="AH192" s="15" t="inlineStr">
         <is>
           <t>418</t>
         </is>
@@ -34568,7 +34568,7 @@
           <t>531</t>
         </is>
       </c>
-      <c r="C196" s="17" t="inlineStr">
+      <c r="C196" s="5" t="inlineStr">
         <is>
           <t>418</t>
         </is>
@@ -39445,7 +39445,7 @@
           <t>222</t>
         </is>
       </c>
-      <c r="Z224" s="13" t="inlineStr">
+      <c r="Z224" s="17" t="inlineStr">
         <is>
           <t>811</t>
         </is>
@@ -41305,7 +41305,7 @@
           <t>465</t>
         </is>
       </c>
-      <c r="X234" s="17" t="inlineStr">
+      <c r="X234" s="12" t="inlineStr">
         <is>
           <t>566</t>
         </is>
@@ -43283,7 +43283,7 @@
           <t>520</t>
         </is>
       </c>
-      <c r="D256" s="5" t="inlineStr">
+      <c r="D256" s="17" t="inlineStr">
         <is>
           <t>869</t>
         </is>
@@ -43322,12 +43322,12 @@
           <t>991</t>
         </is>
       </c>
-      <c r="C258" s="17" t="inlineStr">
+      <c r="C258" s="5" t="inlineStr">
         <is>
           <t>566</t>
         </is>
       </c>
-      <c r="D258" s="17" t="inlineStr">
+      <c r="D258" s="5" t="inlineStr">
         <is>
           <t>418</t>
         </is>
@@ -43341,17 +43341,17 @@
       </c>
       <c r="B259" s="5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>945</t>
         </is>
       </c>
       <c r="C259" s="5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>642</t>
         </is>
       </c>
       <c r="D259" s="5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>831</t>
         </is>
       </c>
     </row>
@@ -43361,19 +43361,19 @@
           <t>13</t>
         </is>
       </c>
-      <c r="B260" s="5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C260" s="5" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="B260" s="17" t="inlineStr">
+        <is>
+          <t>869</t>
+        </is>
+      </c>
+      <c r="C260" s="17" t="inlineStr">
+        <is>
+          <t>811</t>
         </is>
       </c>
       <c r="D260" s="5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>592</t>
         </is>
       </c>
     </row>
@@ -43385,17 +43385,17 @@
       </c>
       <c r="B261" s="5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>717</t>
         </is>
       </c>
       <c r="C261" s="5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>809</t>
         </is>
       </c>
       <c r="D261" s="5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>891</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
add function to print found matches
</commit_message>
<xml_diff>
--- a/swertres/excel_results.xlsx
+++ b/swertres/excel_results.xlsx
@@ -43,12 +43,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FFFFFF"/>
+        <fgColor rgb="00ff6666"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00ff6666"/>
+        <fgColor rgb="00FFFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -220,7 +220,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
@@ -253,7 +253,7 @@
     <xf numFmtId="0" fontId="1" fillId="14" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1488,7 +1488,7 @@
           <t>612</t>
         </is>
       </c>
-      <c r="S6" s="10" t="inlineStr">
+      <c r="S6" s="17" t="inlineStr">
         <is>
           <t>741</t>
         </is>
@@ -1595,7 +1595,7 @@
           <t>752</t>
         </is>
       </c>
-      <c r="C7" s="17" t="inlineStr">
+      <c r="C7" s="5" t="inlineStr">
         <is>
           <t>027</t>
         </is>
@@ -2545,7 +2545,7 @@
           <t>237</t>
         </is>
       </c>
-      <c r="F12" s="6" t="inlineStr">
+      <c r="F12" s="17" t="inlineStr">
         <is>
           <t>864</t>
         </is>
@@ -3433,7 +3433,7 @@
           <t>969</t>
         </is>
       </c>
-      <c r="AH16" s="17" t="inlineStr">
+      <c r="AH16" s="15" t="inlineStr">
         <is>
           <t>373</t>
         </is>
@@ -6592,7 +6592,7 @@
           <t>474</t>
         </is>
       </c>
-      <c r="AD33" s="17" t="inlineStr">
+      <c r="AD33" s="14" t="inlineStr">
         <is>
           <t>373</t>
         </is>
@@ -7629,7 +7629,7 @@
           <t>971</t>
         </is>
       </c>
-      <c r="AG41" s="17" t="inlineStr">
+      <c r="AG41" s="15" t="inlineStr">
         <is>
           <t>027</t>
         </is>
@@ -8756,7 +8756,7 @@
           <t>511</t>
         </is>
       </c>
-      <c r="AH47" s="15" t="inlineStr">
+      <c r="AH47" s="17" t="inlineStr">
         <is>
           <t>741</t>
         </is>
@@ -10930,7 +10930,7 @@
           <t>039</t>
         </is>
       </c>
-      <c r="T59" s="11" t="inlineStr">
+      <c r="T59" s="17" t="inlineStr">
         <is>
           <t>864</t>
         </is>
@@ -11052,7 +11052,7 @@
           <t>657</t>
         </is>
       </c>
-      <c r="G60" s="6" t="inlineStr">
+      <c r="G60" s="17" t="inlineStr">
         <is>
           <t>864</t>
         </is>
@@ -17138,7 +17138,7 @@
           <t>863</t>
         </is>
       </c>
-      <c r="J95" s="17" t="inlineStr">
+      <c r="J95" s="7" t="inlineStr">
         <is>
           <t>373</t>
         </is>
@@ -22486,7 +22486,7 @@
           <t>602</t>
         </is>
       </c>
-      <c r="O126" s="9" t="inlineStr">
+      <c r="O126" s="17" t="inlineStr">
         <is>
           <t>741</t>
         </is>
@@ -22678,7 +22678,7 @@
           <t>577</t>
         </is>
       </c>
-      <c r="P127" s="9" t="inlineStr">
+      <c r="P127" s="17" t="inlineStr">
         <is>
           <t>864</t>
         </is>
@@ -23775,7 +23775,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="K133" s="17" t="inlineStr">
+      <c r="K133" s="8" t="inlineStr">
         <is>
           <t>027</t>
         </is>
@@ -24805,7 +24805,7 @@
           <t>774</t>
         </is>
       </c>
-      <c r="AD138" s="17" t="inlineStr">
+      <c r="AD138" s="14" t="inlineStr">
         <is>
           <t>373</t>
         </is>
@@ -27562,7 +27562,7 @@
           <t>603</t>
         </is>
       </c>
-      <c r="C156" s="17" t="inlineStr">
+      <c r="C156" s="5" t="inlineStr">
         <is>
           <t>373</t>
         </is>
@@ -28218,7 +28218,7 @@
           <t>210</t>
         </is>
       </c>
-      <c r="V159" s="17" t="inlineStr">
+      <c r="V159" s="11" t="inlineStr">
         <is>
           <t>027</t>
         </is>
@@ -29582,7 +29582,7 @@
           <t>202</t>
         </is>
       </c>
-      <c r="AG166" s="17" t="inlineStr">
+      <c r="AG166" s="15" t="inlineStr">
         <is>
           <t>373</t>
         </is>
@@ -29961,7 +29961,7 @@
           <t>270</t>
         </is>
       </c>
-      <c r="AH168" s="15" t="inlineStr">
+      <c r="AH168" s="17" t="inlineStr">
         <is>
           <t>741</t>
         </is>
@@ -30133,7 +30133,7 @@
           <t>907</t>
         </is>
       </c>
-      <c r="AE169" s="14" t="inlineStr">
+      <c r="AE169" s="17" t="inlineStr">
         <is>
           <t>864</t>
         </is>
@@ -35441,7 +35441,7 @@
           <t>258</t>
         </is>
       </c>
-      <c r="AB200" s="17" t="inlineStr">
+      <c r="AB200" s="13" t="inlineStr">
         <is>
           <t>027</t>
         </is>
@@ -39370,7 +39370,7 @@
           <t>926</t>
         </is>
       </c>
-      <c r="K224" s="8" t="inlineStr">
+      <c r="K224" s="17" t="inlineStr">
         <is>
           <t>741</t>
         </is>
@@ -39699,7 +39699,7 @@
           <t>14</t>
         </is>
       </c>
-      <c r="B226" s="5" t="inlineStr">
+      <c r="B226" s="17" t="inlineStr">
         <is>
           <t>864</t>
         </is>
@@ -41148,12 +41148,12 @@
           <t>941</t>
         </is>
       </c>
-      <c r="AD233" s="14" t="inlineStr">
+      <c r="AD233" s="17" t="inlineStr">
         <is>
           <t>741</t>
         </is>
       </c>
-      <c r="AE233" s="17" t="inlineStr">
+      <c r="AE233" s="14" t="inlineStr">
         <is>
           <t>027</t>
         </is>
@@ -41856,7 +41856,7 @@
           <t>184</t>
         </is>
       </c>
-      <c r="V237" s="11" t="inlineStr">
+      <c r="V237" s="17" t="inlineStr">
         <is>
           <t>864</t>
         </is>
@@ -43583,12 +43583,12 @@
           <t>037</t>
         </is>
       </c>
-      <c r="F260" s="17" t="inlineStr">
+      <c r="F260" s="6" t="inlineStr">
         <is>
           <t>027</t>
         </is>
       </c>
-      <c r="G260" s="17" t="inlineStr">
+      <c r="G260" s="6" t="inlineStr">
         <is>
           <t>373</t>
         </is>
@@ -43691,17 +43691,17 @@
       </c>
       <c r="E263" s="6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>167</t>
         </is>
       </c>
       <c r="F263" s="6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>827</t>
         </is>
       </c>
       <c r="G263" s="6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>058</t>
         </is>
       </c>
     </row>
@@ -43728,17 +43728,17 @@
       </c>
       <c r="E264" s="6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>725</t>
         </is>
       </c>
       <c r="F264" s="6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>419</t>
         </is>
       </c>
       <c r="G264" s="6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>840</t>
         </is>
       </c>
     </row>
@@ -43765,17 +43765,17 @@
       </c>
       <c r="E265" s="6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>292</t>
         </is>
       </c>
       <c r="F265" s="6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>407</t>
         </is>
       </c>
       <c r="G265" s="6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>227</t>
         </is>
       </c>
     </row>
@@ -43802,17 +43802,17 @@
       </c>
       <c r="E266" s="6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>904</t>
         </is>
       </c>
       <c r="F266" s="6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>827</t>
         </is>
       </c>
       <c r="G266" s="6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>886</t>
         </is>
       </c>
     </row>
@@ -43839,17 +43839,17 @@
       </c>
       <c r="E267" s="6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>602</t>
         </is>
       </c>
       <c r="F267" s="6" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G267" s="6" t="inlineStr">
-        <is>
-          <t>-</t>
+          <t>439</t>
+        </is>
+      </c>
+      <c r="G267" s="17" t="inlineStr">
+        <is>
+          <t>741</t>
         </is>
       </c>
     </row>
@@ -43874,19 +43874,19 @@
           <t>757</t>
         </is>
       </c>
-      <c r="E268" s="6" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="E268" s="17" t="inlineStr">
+        <is>
+          <t>864</t>
         </is>
       </c>
       <c r="F268" s="6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>175</t>
         </is>
       </c>
       <c r="G268" s="6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>002</t>
         </is>
       </c>
     </row>
@@ -43913,17 +43913,17 @@
       </c>
       <c r="E269" s="6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>906</t>
         </is>
       </c>
       <c r="F269" s="6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>957</t>
         </is>
       </c>
       <c r="G269" s="6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>308</t>
         </is>
       </c>
     </row>
@@ -43950,17 +43950,17 @@
       </c>
       <c r="E270" s="6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>422</t>
         </is>
       </c>
       <c r="F270" s="6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>937</t>
         </is>
       </c>
       <c r="G270" s="6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>177</t>
         </is>
       </c>
     </row>
@@ -43987,17 +43987,17 @@
       </c>
       <c r="E271" s="6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>665</t>
         </is>
       </c>
       <c r="F271" s="6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>128</t>
         </is>
       </c>
       <c r="G271" s="6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>310</t>
         </is>
       </c>
     </row>
@@ -44024,17 +44024,17 @@
       </c>
       <c r="E272" s="6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>717</t>
         </is>
       </c>
       <c r="F272" s="6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>157</t>
         </is>
       </c>
       <c r="G272" s="6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>854</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
update results; fix misreplaced script
</commit_message>
<xml_diff>
--- a/swertres/excel_results.xlsx
+++ b/swertres/excel_results.xlsx
@@ -48,12 +48,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FFFFFF"/>
+        <fgColor rgb="00ff6633"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00ff6633"/>
+        <fgColor rgb="00FFFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -223,7 +223,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
@@ -253,7 +253,7 @@
     <xf numFmtId="0" fontId="1" fillId="14" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1079,7 +1079,7 @@
           <t>657</t>
         </is>
       </c>
-      <c r="L4" s="8" t="inlineStr">
+      <c r="L4" s="17" t="inlineStr">
         <is>
           <t>163</t>
         </is>
@@ -1488,7 +1488,7 @@
           <t>612</t>
         </is>
       </c>
-      <c r="S6" s="17" t="inlineStr">
+      <c r="S6" s="10" t="inlineStr">
         <is>
           <t>741</t>
         </is>
@@ -2545,7 +2545,7 @@
           <t>237</t>
         </is>
       </c>
-      <c r="F12" s="17" t="inlineStr">
+      <c r="F12" s="6" t="inlineStr">
         <is>
           <t>864</t>
         </is>
@@ -3682,7 +3682,7 @@
           <t>336</t>
         </is>
       </c>
-      <c r="I18" s="7" t="inlineStr">
+      <c r="I18" s="17" t="inlineStr">
         <is>
           <t>163</t>
         </is>
@@ -4742,7 +4742,7 @@
           <t>372</t>
         </is>
       </c>
-      <c r="AH23" s="15" t="inlineStr">
+      <c r="AH23" s="17" t="inlineStr">
         <is>
           <t>163</t>
         </is>
@@ -4854,7 +4854,7 @@
           <t>367</t>
         </is>
       </c>
-      <c r="S24" s="10" t="inlineStr">
+      <c r="S24" s="17" t="inlineStr">
         <is>
           <t>163</t>
         </is>
@@ -8756,7 +8756,7 @@
           <t>511</t>
         </is>
       </c>
-      <c r="AH47" s="17" t="inlineStr">
+      <c r="AH47" s="15" t="inlineStr">
         <is>
           <t>741</t>
         </is>
@@ -10930,7 +10930,7 @@
           <t>039</t>
         </is>
       </c>
-      <c r="T59" s="17" t="inlineStr">
+      <c r="T59" s="11" t="inlineStr">
         <is>
           <t>864</t>
         </is>
@@ -11052,7 +11052,7 @@
           <t>657</t>
         </is>
       </c>
-      <c r="G60" s="17" t="inlineStr">
+      <c r="G60" s="6" t="inlineStr">
         <is>
           <t>864</t>
         </is>
@@ -11319,7 +11319,7 @@
           <t>714</t>
         </is>
       </c>
-      <c r="W61" s="12" t="inlineStr">
+      <c r="W61" s="17" t="inlineStr">
         <is>
           <t>701</t>
         </is>
@@ -14515,7 +14515,7 @@
           <t>823</t>
         </is>
       </c>
-      <c r="I81" s="7" t="inlineStr">
+      <c r="I81" s="17" t="inlineStr">
         <is>
           <t>163</t>
         </is>
@@ -15934,7 +15934,7 @@
           <t>786</t>
         </is>
       </c>
-      <c r="AE88" s="14" t="inlineStr">
+      <c r="AE88" s="17" t="inlineStr">
         <is>
           <t>163</t>
         </is>
@@ -22486,7 +22486,7 @@
           <t>602</t>
         </is>
       </c>
-      <c r="O126" s="17" t="inlineStr">
+      <c r="O126" s="9" t="inlineStr">
         <is>
           <t>741</t>
         </is>
@@ -22678,7 +22678,7 @@
           <t>577</t>
         </is>
       </c>
-      <c r="P127" s="17" t="inlineStr">
+      <c r="P127" s="9" t="inlineStr">
         <is>
           <t>864</t>
         </is>
@@ -23905,7 +23905,7 @@
           <t>631</t>
         </is>
       </c>
-      <c r="AK133" s="16" t="inlineStr">
+      <c r="AK133" s="17" t="inlineStr">
         <is>
           <t>701</t>
         </is>
@@ -23932,7 +23932,7 @@
           <t>587</t>
         </is>
       </c>
-      <c r="E134" s="6" t="inlineStr">
+      <c r="E134" s="17" t="inlineStr">
         <is>
           <t>163</t>
         </is>
@@ -27273,7 +27273,7 @@
           <t>402</t>
         </is>
       </c>
-      <c r="T154" s="11" t="inlineStr">
+      <c r="T154" s="17" t="inlineStr">
         <is>
           <t>163</t>
         </is>
@@ -27567,7 +27567,7 @@
           <t>373</t>
         </is>
       </c>
-      <c r="D156" s="5" t="inlineStr">
+      <c r="D156" s="17" t="inlineStr">
         <is>
           <t>163</t>
         </is>
@@ -29961,7 +29961,7 @@
           <t>270</t>
         </is>
       </c>
-      <c r="AH168" s="17" t="inlineStr">
+      <c r="AH168" s="15" t="inlineStr">
         <is>
           <t>741</t>
         </is>
@@ -30133,7 +30133,7 @@
           <t>907</t>
         </is>
       </c>
-      <c r="AE169" s="17" t="inlineStr">
+      <c r="AE169" s="14" t="inlineStr">
         <is>
           <t>864</t>
         </is>
@@ -32045,7 +32045,7 @@
           <t>780</t>
         </is>
       </c>
-      <c r="V182" s="11" t="inlineStr">
+      <c r="V182" s="17" t="inlineStr">
         <is>
           <t>163</t>
         </is>
@@ -32207,7 +32207,7 @@
           <t>983</t>
         </is>
       </c>
-      <c r="Q183" s="10" t="inlineStr">
+      <c r="Q183" s="17" t="inlineStr">
         <is>
           <t>701</t>
         </is>
@@ -33359,7 +33359,7 @@
           <t>255</t>
         </is>
       </c>
-      <c r="W189" s="12" t="inlineStr">
+      <c r="W189" s="17" t="inlineStr">
         <is>
           <t>701</t>
         </is>
@@ -36261,7 +36261,7 @@
           <t>164</t>
         </is>
       </c>
-      <c r="E205" s="6" t="inlineStr">
+      <c r="E205" s="17" t="inlineStr">
         <is>
           <t>163</t>
         </is>
@@ -38233,7 +38233,7 @@
           <t>695</t>
         </is>
       </c>
-      <c r="H218" s="7" t="inlineStr">
+      <c r="H218" s="17" t="inlineStr">
         <is>
           <t>163</t>
         </is>
@@ -38779,7 +38779,7 @@
           <t>419</t>
         </is>
       </c>
-      <c r="E221" s="6" t="inlineStr">
+      <c r="E221" s="17" t="inlineStr">
         <is>
           <t>163</t>
         </is>
@@ -39056,7 +39056,7 @@
           <t>951</t>
         </is>
       </c>
-      <c r="W222" s="12" t="inlineStr">
+      <c r="W222" s="17" t="inlineStr">
         <is>
           <t>701</t>
         </is>
@@ -39370,7 +39370,7 @@
           <t>926</t>
         </is>
       </c>
-      <c r="K224" s="17" t="inlineStr">
+      <c r="K224" s="8" t="inlineStr">
         <is>
           <t>741</t>
         </is>
@@ -39699,7 +39699,7 @@
           <t>14</t>
         </is>
       </c>
-      <c r="B226" s="17" t="inlineStr">
+      <c r="B226" s="5" t="inlineStr">
         <is>
           <t>864</t>
         </is>
@@ -41148,7 +41148,7 @@
           <t>941</t>
         </is>
       </c>
-      <c r="AD233" s="17" t="inlineStr">
+      <c r="AD233" s="14" t="inlineStr">
         <is>
           <t>741</t>
         </is>
@@ -41856,7 +41856,7 @@
           <t>184</t>
         </is>
       </c>
-      <c r="V237" s="17" t="inlineStr">
+      <c r="V237" s="11" t="inlineStr">
         <is>
           <t>864</t>
         </is>
@@ -43847,7 +43847,7 @@
           <t>439</t>
         </is>
       </c>
-      <c r="G267" s="17" t="inlineStr">
+      <c r="G267" s="6" t="inlineStr">
         <is>
           <t>741</t>
         </is>
@@ -43874,7 +43874,7 @@
           <t>757</t>
         </is>
       </c>
-      <c r="E268" s="17" t="inlineStr">
+      <c r="E268" s="6" t="inlineStr">
         <is>
           <t>864</t>
         </is>

</xml_diff>

<commit_message>
fix index out of range on after_match results
</commit_message>
<xml_diff>
--- a/swertres/excel_results.xlsx
+++ b/swertres/excel_results.xlsx
@@ -43,6 +43,11 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="00FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="00ff6666"/>
       </patternFill>
     </fill>
@@ -54,11 +59,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="00ccff33"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FFFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -220,13 +220,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
@@ -253,7 +253,7 @@
     <xf numFmtId="0" fontId="1" fillId="14" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1655,7 +1655,7 @@
           <t>217</t>
         </is>
       </c>
-      <c r="O7" s="17" t="inlineStr">
+      <c r="O7" s="9" t="inlineStr">
         <is>
           <t>426</t>
         </is>
@@ -2074,7 +2074,7 @@
           <t>154</t>
         </is>
       </c>
-      <c r="X9" s="17" t="inlineStr">
+      <c r="X9" s="12" t="inlineStr">
         <is>
           <t>426</t>
         </is>
@@ -2535,7 +2535,7 @@
           <t>453</t>
         </is>
       </c>
-      <c r="D12" s="5" t="inlineStr">
+      <c r="D12" s="17" t="inlineStr">
         <is>
           <t>134</t>
         </is>
@@ -2580,7 +2580,7 @@
           <t>176</t>
         </is>
       </c>
-      <c r="M12" s="17" t="inlineStr">
+      <c r="M12" s="8" t="inlineStr">
         <is>
           <t>426</t>
         </is>
@@ -6133,7 +6133,7 @@
           <t>153</t>
         </is>
       </c>
-      <c r="M31" s="17" t="inlineStr">
+      <c r="M31" s="8" t="inlineStr">
         <is>
           <t>426</t>
         </is>
@@ -7671,7 +7671,7 @@
           <t>936</t>
         </is>
       </c>
-      <c r="D42" s="17" t="inlineStr">
+      <c r="D42" s="5" t="inlineStr">
         <is>
           <t>426</t>
         </is>
@@ -8803,7 +8803,7 @@
           <t>709</t>
         </is>
       </c>
-      <c r="F48" s="17" t="inlineStr">
+      <c r="F48" s="6" t="inlineStr">
         <is>
           <t>426</t>
         </is>
@@ -9509,7 +9509,7 @@
           <t>720</t>
         </is>
       </c>
-      <c r="AI51" s="17" t="inlineStr">
+      <c r="AI51" s="16" t="inlineStr">
         <is>
           <t>426</t>
         </is>
@@ -9828,7 +9828,7 @@
           <t>429</t>
         </is>
       </c>
-      <c r="X53" s="12" t="inlineStr">
+      <c r="X53" s="17" t="inlineStr">
         <is>
           <t>489</t>
         </is>
@@ -10818,7 +10818,7 @@
           <t>608</t>
         </is>
       </c>
-      <c r="AI58" s="17" t="inlineStr">
+      <c r="AI58" s="16" t="inlineStr">
         <is>
           <t>581</t>
         </is>
@@ -10900,7 +10900,7 @@
           <t>818</t>
         </is>
       </c>
-      <c r="N59" s="9" t="inlineStr">
+      <c r="N59" s="17" t="inlineStr">
         <is>
           <t>134</t>
         </is>
@@ -11279,7 +11279,7 @@
           <t>923</t>
         </is>
       </c>
-      <c r="O61" s="9" t="inlineStr">
+      <c r="O61" s="17" t="inlineStr">
         <is>
           <t>489</t>
         </is>
@@ -12062,7 +12062,7 @@
           <t>742</t>
         </is>
       </c>
-      <c r="V65" s="11" t="inlineStr">
+      <c r="V65" s="17" t="inlineStr">
         <is>
           <t>134</t>
         </is>
@@ -12289,7 +12289,7 @@
           <t>556</t>
         </is>
       </c>
-      <c r="AD66" s="17" t="inlineStr">
+      <c r="AD66" s="14" t="inlineStr">
         <is>
           <t>581</t>
         </is>
@@ -13358,7 +13358,7 @@
           <t>03</t>
         </is>
       </c>
-      <c r="B75" s="17" t="inlineStr">
+      <c r="B75" s="5" t="inlineStr">
         <is>
           <t>581</t>
         </is>
@@ -13817,7 +13817,7 @@
           <t>886</t>
         </is>
       </c>
-      <c r="S77" s="17" t="inlineStr">
+      <c r="S77" s="10" t="inlineStr">
         <is>
           <t>581</t>
         </is>
@@ -14752,7 +14752,7 @@
           <t>086</t>
         </is>
       </c>
-      <c r="S82" s="17" t="inlineStr">
+      <c r="S82" s="10" t="inlineStr">
         <is>
           <t>426</t>
         </is>
@@ -14989,7 +14989,7 @@
           <t>815</t>
         </is>
       </c>
-      <c r="AC83" s="14" t="inlineStr">
+      <c r="AC83" s="17" t="inlineStr">
         <is>
           <t>489</t>
         </is>
@@ -15166,7 +15166,7 @@
           <t>910</t>
         </is>
       </c>
-      <c r="AA84" s="13" t="inlineStr">
+      <c r="AA84" s="17" t="inlineStr">
         <is>
           <t>134</t>
         </is>
@@ -16587,7 +16587,7 @@
           <t>349</t>
         </is>
       </c>
-      <c r="L92" s="8" t="inlineStr">
+      <c r="L92" s="17" t="inlineStr">
         <is>
           <t>134</t>
         </is>
@@ -16657,7 +16657,7 @@
           <t>018</t>
         </is>
       </c>
-      <c r="Z92" s="13" t="inlineStr">
+      <c r="Z92" s="17" t="inlineStr">
         <is>
           <t>134</t>
         </is>
@@ -20748,7 +20748,7 @@
           <t>082</t>
         </is>
       </c>
-      <c r="D117" s="17" t="inlineStr">
+      <c r="D117" s="5" t="inlineStr">
         <is>
           <t>581</t>
         </is>
@@ -30472,7 +30472,7 @@
           <t>946</t>
         </is>
       </c>
-      <c r="X171" s="12" t="inlineStr">
+      <c r="X171" s="17" t="inlineStr">
         <is>
           <t>134</t>
         </is>
@@ -31621,7 +31621,7 @@
           <t>325</t>
         </is>
       </c>
-      <c r="L180" s="8" t="inlineStr">
+      <c r="L180" s="17" t="inlineStr">
         <is>
           <t>489</t>
         </is>
@@ -34997,7 +34997,7 @@
           <t>414</t>
         </is>
       </c>
-      <c r="N198" s="17" t="inlineStr">
+      <c r="N198" s="9" t="inlineStr">
         <is>
           <t>426</t>
         </is>
@@ -35289,7 +35289,7 @@
           <t>364</t>
         </is>
       </c>
-      <c r="AI199" s="16" t="inlineStr">
+      <c r="AI199" s="17" t="inlineStr">
         <is>
           <t>489</t>
         </is>
@@ -38328,7 +38328,7 @@
           <t>401</t>
         </is>
       </c>
-      <c r="AA218" s="17" t="inlineStr">
+      <c r="AA218" s="13" t="inlineStr">
         <is>
           <t>426</t>
         </is>
@@ -39587,7 +39587,7 @@
           <t>774</t>
         </is>
       </c>
-      <c r="Q225" s="10" t="inlineStr">
+      <c r="Q225" s="17" t="inlineStr">
         <is>
           <t>134</t>
         </is>
@@ -40901,7 +40901,7 @@
           <t>188</t>
         </is>
       </c>
-      <c r="R232" s="10" t="inlineStr">
+      <c r="R232" s="17" t="inlineStr">
         <is>
           <t>489</t>
         </is>
@@ -41225,7 +41225,7 @@
           <t>705</t>
         </is>
       </c>
-      <c r="H234" s="17" t="inlineStr">
+      <c r="H234" s="7" t="inlineStr">
         <is>
           <t>581</t>
         </is>
@@ -42609,7 +42609,7 @@
           <t>949</t>
         </is>
       </c>
-      <c r="W241" s="12" t="inlineStr">
+      <c r="W241" s="17" t="inlineStr">
         <is>
           <t>134</t>
         </is>
@@ -42948,7 +42948,7 @@
           <t>986</t>
         </is>
       </c>
-      <c r="P243" s="17" t="inlineStr">
+      <c r="P243" s="9" t="inlineStr">
         <is>
           <t>426</t>
         </is>
@@ -43079,6 +43079,13 @@
       </c>
       <c r="F246" s="2" t="n"/>
       <c r="G246" s="3" t="n"/>
+      <c r="H246" s="1" t="inlineStr">
+        <is>
+          <t>March 2020</t>
+        </is>
+      </c>
+      <c r="I246" s="2" t="n"/>
+      <c r="J246" s="3" t="n"/>
     </row>
     <row r="247">
       <c r="A247" s="4" t="n"/>
@@ -43112,6 +43119,21 @@
           <t>9PM</t>
         </is>
       </c>
+      <c r="H247" s="1" t="inlineStr">
+        <is>
+          <t>11AM</t>
+        </is>
+      </c>
+      <c r="I247" s="1" t="inlineStr">
+        <is>
+          <t>4PM</t>
+        </is>
+      </c>
+      <c r="J247" s="1" t="inlineStr">
+        <is>
+          <t>9PM</t>
+        </is>
+      </c>
     </row>
     <row r="248">
       <c r="A248" s="1" t="inlineStr">
@@ -43149,6 +43171,21 @@
           <t>034</t>
         </is>
       </c>
+      <c r="H248" s="7" t="inlineStr">
+        <is>
+          <t>565</t>
+        </is>
+      </c>
+      <c r="I248" s="7" t="inlineStr">
+        <is>
+          <t>151</t>
+        </is>
+      </c>
+      <c r="J248" s="7" t="inlineStr">
+        <is>
+          <t>708</t>
+        </is>
+      </c>
     </row>
     <row r="249">
       <c r="A249" s="1" t="inlineStr">
@@ -43186,6 +43223,21 @@
           <t>605</t>
         </is>
       </c>
+      <c r="H249" s="7" t="inlineStr">
+        <is>
+          <t>059</t>
+        </is>
+      </c>
+      <c r="I249" s="7" t="inlineStr">
+        <is>
+          <t>208</t>
+        </is>
+      </c>
+      <c r="J249" s="7" t="inlineStr">
+        <is>
+          <t>310</t>
+        </is>
+      </c>
     </row>
     <row r="250">
       <c r="A250" s="1" t="inlineStr">
@@ -43223,6 +43275,21 @@
           <t>130</t>
         </is>
       </c>
+      <c r="H250" s="7" t="inlineStr">
+        <is>
+          <t>440</t>
+        </is>
+      </c>
+      <c r="I250" s="7" t="inlineStr">
+        <is>
+          <t>109</t>
+        </is>
+      </c>
+      <c r="J250" s="7" t="inlineStr">
+        <is>
+          <t>795</t>
+        </is>
+      </c>
     </row>
     <row r="251">
       <c r="A251" s="1" t="inlineStr">
@@ -43260,6 +43327,21 @@
           <t>242</t>
         </is>
       </c>
+      <c r="H251" s="7" t="inlineStr">
+        <is>
+          <t>464</t>
+        </is>
+      </c>
+      <c r="I251" s="7" t="inlineStr">
+        <is>
+          <t>197</t>
+        </is>
+      </c>
+      <c r="J251" s="7" t="inlineStr">
+        <is>
+          <t>886</t>
+        </is>
+      </c>
     </row>
     <row r="252">
       <c r="A252" s="1" t="inlineStr">
@@ -43297,6 +43379,21 @@
           <t>580</t>
         </is>
       </c>
+      <c r="H252" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I252" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J252" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="253">
       <c r="A253" s="1" t="inlineStr">
@@ -43334,6 +43431,21 @@
           <t>368</t>
         </is>
       </c>
+      <c r="H253" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I253" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J253" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="254">
       <c r="A254" s="1" t="inlineStr">
@@ -43371,6 +43483,21 @@
           <t>965</t>
         </is>
       </c>
+      <c r="H254" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I254" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J254" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="255">
       <c r="A255" s="1" t="inlineStr">
@@ -43408,6 +43535,21 @@
           <t>015</t>
         </is>
       </c>
+      <c r="H255" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I255" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J255" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="256">
       <c r="A256" s="1" t="inlineStr">
@@ -43445,6 +43587,21 @@
           <t>028</t>
         </is>
       </c>
+      <c r="H256" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I256" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J256" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="257">
       <c r="A257" s="1" t="inlineStr">
@@ -43482,6 +43639,21 @@
           <t>162</t>
         </is>
       </c>
+      <c r="H257" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I257" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J257" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="258">
       <c r="A258" s="1" t="inlineStr">
@@ -43519,6 +43691,21 @@
           <t>212</t>
         </is>
       </c>
+      <c r="H258" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I258" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J258" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="259">
       <c r="A259" s="1" t="inlineStr">
@@ -43556,6 +43743,21 @@
           <t>211</t>
         </is>
       </c>
+      <c r="H259" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I259" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J259" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="260">
       <c r="A260" s="1" t="inlineStr">
@@ -43593,6 +43795,21 @@
           <t>373</t>
         </is>
       </c>
+      <c r="H260" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I260" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J260" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="261">
       <c r="A261" s="1" t="inlineStr">
@@ -43630,6 +43847,21 @@
           <t>952</t>
         </is>
       </c>
+      <c r="H261" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I261" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J261" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="262">
       <c r="A262" s="1" t="inlineStr">
@@ -43667,6 +43899,21 @@
           <t>206</t>
         </is>
       </c>
+      <c r="H262" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I262" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J262" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="263">
       <c r="A263" s="1" t="inlineStr">
@@ -43704,6 +43951,21 @@
           <t>058</t>
         </is>
       </c>
+      <c r="H263" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I263" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J263" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="264">
       <c r="A264" s="1" t="inlineStr">
@@ -43741,6 +44003,21 @@
           <t>840</t>
         </is>
       </c>
+      <c r="H264" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I264" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J264" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="265">
       <c r="A265" s="1" t="inlineStr">
@@ -43778,6 +44055,21 @@
           <t>227</t>
         </is>
       </c>
+      <c r="H265" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I265" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J265" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="266">
       <c r="A266" s="1" t="inlineStr">
@@ -43815,6 +44107,21 @@
           <t>886</t>
         </is>
       </c>
+      <c r="H266" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I266" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J266" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="267">
       <c r="A267" s="1" t="inlineStr">
@@ -43852,6 +44159,21 @@
           <t>741</t>
         </is>
       </c>
+      <c r="H267" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I267" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J267" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="268">
       <c r="A268" s="1" t="inlineStr">
@@ -43889,6 +44211,21 @@
           <t>002</t>
         </is>
       </c>
+      <c r="H268" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I268" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J268" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="269">
       <c r="A269" s="1" t="inlineStr">
@@ -43926,6 +44263,21 @@
           <t>308</t>
         </is>
       </c>
+      <c r="H269" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I269" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J269" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="270">
       <c r="A270" s="1" t="inlineStr">
@@ -43963,6 +44315,21 @@
           <t>177</t>
         </is>
       </c>
+      <c r="H270" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I270" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J270" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="271">
       <c r="A271" s="1" t="inlineStr">
@@ -44000,6 +44367,21 @@
           <t>310</t>
         </is>
       </c>
+      <c r="H271" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I271" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J271" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="272">
       <c r="A272" s="1" t="inlineStr">
@@ -44037,6 +44419,21 @@
           <t>854</t>
         </is>
       </c>
+      <c r="H272" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I272" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J272" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="inlineStr">
@@ -44074,6 +44471,21 @@
           <t>230</t>
         </is>
       </c>
+      <c r="H273" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I273" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J273" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="inlineStr">
@@ -44111,6 +44523,21 @@
           <t>484</t>
         </is>
       </c>
+      <c r="H274" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I274" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J274" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="inlineStr">
@@ -44138,14 +44565,29 @@
           <t>628</t>
         </is>
       </c>
-      <c r="F275" s="17" t="inlineStr">
+      <c r="F275" s="6" t="inlineStr">
         <is>
           <t>581</t>
         </is>
       </c>
-      <c r="G275" s="17" t="inlineStr">
+      <c r="G275" s="6" t="inlineStr">
         <is>
           <t>426</t>
+        </is>
+      </c>
+      <c r="H275" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I275" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J275" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
     </row>
@@ -44170,17 +44612,32 @@
           <t>639</t>
         </is>
       </c>
-      <c r="E276" s="6" t="inlineStr">
+      <c r="E276" s="17" t="inlineStr">
+        <is>
+          <t>489</t>
+        </is>
+      </c>
+      <c r="F276" s="17" t="inlineStr">
+        <is>
+          <t>134</t>
+        </is>
+      </c>
+      <c r="G276" s="6" t="inlineStr">
+        <is>
+          <t>824</t>
+        </is>
+      </c>
+      <c r="H276" s="7" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="F276" s="6" t="inlineStr">
+      <c r="I276" s="7" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="G276" s="6" t="inlineStr">
+      <c r="J276" s="7" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -44222,6 +44679,21 @@
           <t>-</t>
         </is>
       </c>
+      <c r="H277" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I277" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J277" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="inlineStr">
@@ -44259,9 +44731,24 @@
           <t>-</t>
         </is>
       </c>
+      <c r="H278" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I278" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J278" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="94">
+  <mergeCells count="95">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
@@ -44356,6 +44843,7 @@
     <mergeCell ref="A246:A247"/>
     <mergeCell ref="B246:D246"/>
     <mergeCell ref="E246:G246"/>
+    <mergeCell ref="H246:J246"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
fix plus minus script
</commit_message>
<xml_diff>
--- a/swertres/excel_results.xlsx
+++ b/swertres/excel_results.xlsx
@@ -29,7 +29,7 @@
       <sz val="15"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="14">
     <fill>
       <patternFill/>
     </fill>
@@ -39,11 +39,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="00ff6699"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FFFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -209,7 +204,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
@@ -218,6 +213,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
@@ -248,12 +246,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2535,7 +2527,7 @@
           <t>453</t>
         </is>
       </c>
-      <c r="D12" s="17" t="inlineStr">
+      <c r="D12" s="5" t="inlineStr">
         <is>
           <t>134</t>
         </is>
@@ -9828,7 +9820,7 @@
           <t>429</t>
         </is>
       </c>
-      <c r="X53" s="17" t="inlineStr">
+      <c r="X53" s="12" t="inlineStr">
         <is>
           <t>489</t>
         </is>
@@ -10900,7 +10892,7 @@
           <t>818</t>
         </is>
       </c>
-      <c r="N59" s="17" t="inlineStr">
+      <c r="N59" s="9" t="inlineStr">
         <is>
           <t>134</t>
         </is>
@@ -11279,7 +11271,7 @@
           <t>923</t>
         </is>
       </c>
-      <c r="O61" s="17" t="inlineStr">
+      <c r="O61" s="9" t="inlineStr">
         <is>
           <t>489</t>
         </is>
@@ -12062,7 +12054,7 @@
           <t>742</t>
         </is>
       </c>
-      <c r="V65" s="17" t="inlineStr">
+      <c r="V65" s="11" t="inlineStr">
         <is>
           <t>134</t>
         </is>
@@ -14989,7 +14981,7 @@
           <t>815</t>
         </is>
       </c>
-      <c r="AC83" s="17" t="inlineStr">
+      <c r="AC83" s="14" t="inlineStr">
         <is>
           <t>489</t>
         </is>
@@ -15166,7 +15158,7 @@
           <t>910</t>
         </is>
       </c>
-      <c r="AA84" s="17" t="inlineStr">
+      <c r="AA84" s="13" t="inlineStr">
         <is>
           <t>134</t>
         </is>
@@ -16587,7 +16579,7 @@
           <t>349</t>
         </is>
       </c>
-      <c r="L92" s="17" t="inlineStr">
+      <c r="L92" s="8" t="inlineStr">
         <is>
           <t>134</t>
         </is>
@@ -16657,7 +16649,7 @@
           <t>018</t>
         </is>
       </c>
-      <c r="Z92" s="17" t="inlineStr">
+      <c r="Z92" s="13" t="inlineStr">
         <is>
           <t>134</t>
         </is>
@@ -30472,7 +30464,7 @@
           <t>946</t>
         </is>
       </c>
-      <c r="X171" s="17" t="inlineStr">
+      <c r="X171" s="12" t="inlineStr">
         <is>
           <t>134</t>
         </is>
@@ -31621,7 +31613,7 @@
           <t>325</t>
         </is>
       </c>
-      <c r="L180" s="17" t="inlineStr">
+      <c r="L180" s="8" t="inlineStr">
         <is>
           <t>489</t>
         </is>
@@ -35289,7 +35281,7 @@
           <t>364</t>
         </is>
       </c>
-      <c r="AI199" s="17" t="inlineStr">
+      <c r="AI199" s="16" t="inlineStr">
         <is>
           <t>489</t>
         </is>
@@ -39587,7 +39579,7 @@
           <t>774</t>
         </is>
       </c>
-      <c r="Q225" s="17" t="inlineStr">
+      <c r="Q225" s="10" t="inlineStr">
         <is>
           <t>134</t>
         </is>
@@ -40901,7 +40893,7 @@
           <t>188</t>
         </is>
       </c>
-      <c r="R232" s="17" t="inlineStr">
+      <c r="R232" s="10" t="inlineStr">
         <is>
           <t>489</t>
         </is>
@@ -42609,7 +42601,7 @@
           <t>949</t>
         </is>
       </c>
-      <c r="W241" s="17" t="inlineStr">
+      <c r="W241" s="12" t="inlineStr">
         <is>
           <t>134</t>
         </is>
@@ -43381,17 +43373,17 @@
       </c>
       <c r="H252" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>513</t>
         </is>
       </c>
       <c r="I252" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>274</t>
         </is>
       </c>
       <c r="J252" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>221</t>
         </is>
       </c>
     </row>
@@ -44612,12 +44604,12 @@
           <t>639</t>
         </is>
       </c>
-      <c r="E276" s="17" t="inlineStr">
+      <c r="E276" s="6" t="inlineStr">
         <is>
           <t>489</t>
         </is>
       </c>
-      <c r="F276" s="17" t="inlineStr">
+      <c r="F276" s="6" t="inlineStr">
         <is>
           <t>134</t>
         </is>

</xml_diff>

<commit_message>
new pattern found for excel_results
</commit_message>
<xml_diff>
--- a/swertres/excel_results.xlsx
+++ b/swertres/excel_results.xlsx
@@ -39,11 +39,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="00ff6699"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FFFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -99,6 +94,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="00009966"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -220,6 +220,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -251,9 +254,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1413,7 +1413,7 @@
           <t>047</t>
         </is>
       </c>
-      <c r="D6" s="17" t="inlineStr">
+      <c r="D6" s="5" t="inlineStr">
         <is>
           <t>886</t>
         </is>
@@ -3146,7 +3146,7 @@
           <t>356</t>
         </is>
       </c>
-      <c r="N15" s="17" t="inlineStr">
+      <c r="N15" s="9" t="inlineStr">
         <is>
           <t>886</t>
         </is>
@@ -3460,7 +3460,7 @@
           <t>15</t>
         </is>
       </c>
-      <c r="B17" s="17" t="inlineStr">
+      <c r="B17" s="5" t="inlineStr">
         <is>
           <t>513</t>
         </is>
@@ -4156,7 +4156,7 @@
           <t>208</t>
         </is>
       </c>
-      <c r="AC20" s="17" t="inlineStr">
+      <c r="AC20" s="14" t="inlineStr">
         <is>
           <t>513</t>
         </is>
@@ -4607,7 +4607,7 @@
           <t>520</t>
         </is>
       </c>
-      <c r="G23" s="17" t="inlineStr">
+      <c r="G23" s="6" t="inlineStr">
         <is>
           <t>886</t>
         </is>
@@ -4859,7 +4859,7 @@
           <t>163</t>
         </is>
       </c>
-      <c r="T24" s="17" t="inlineStr">
+      <c r="T24" s="11" t="inlineStr">
         <is>
           <t>886</t>
         </is>
@@ -7524,7 +7524,7 @@
           <t>785</t>
         </is>
       </c>
-      <c r="L41" s="17" t="inlineStr">
+      <c r="L41" s="8" t="inlineStr">
         <is>
           <t>886</t>
         </is>
@@ -7661,7 +7661,7 @@
           <t>05</t>
         </is>
       </c>
-      <c r="B42" s="17" t="inlineStr">
+      <c r="B42" s="5" t="inlineStr">
         <is>
           <t>886</t>
         </is>
@@ -7741,7 +7741,7 @@
           <t>720</t>
         </is>
       </c>
-      <c r="R42" s="17" t="inlineStr">
+      <c r="R42" s="10" t="inlineStr">
         <is>
           <t>513</t>
         </is>
@@ -8928,7 +8928,7 @@
           <t>655</t>
         </is>
       </c>
-      <c r="AE48" s="14" t="inlineStr">
+      <c r="AE48" s="17" t="inlineStr">
         <is>
           <t>197</t>
         </is>
@@ -9222,7 +9222,7 @@
           <t>322</t>
         </is>
       </c>
-      <c r="O50" s="9" t="inlineStr">
+      <c r="O50" s="17" t="inlineStr">
         <is>
           <t>464</t>
         </is>
@@ -9302,7 +9302,7 @@
           <t>634</t>
         </is>
       </c>
-      <c r="AE50" s="14" t="inlineStr">
+      <c r="AE50" s="17" t="inlineStr">
         <is>
           <t>197</t>
         </is>
@@ -11588,7 +11588,7 @@
           <t>26</t>
         </is>
       </c>
-      <c r="B63" s="5" t="inlineStr">
+      <c r="B63" s="17" t="inlineStr">
         <is>
           <t>197</t>
         </is>
@@ -13812,7 +13812,7 @@
           <t>984</t>
         </is>
       </c>
-      <c r="R77" s="17" t="inlineStr">
+      <c r="R77" s="10" t="inlineStr">
         <is>
           <t>886</t>
         </is>
@@ -13929,7 +13929,7 @@
           <t>750</t>
         </is>
       </c>
-      <c r="D78" s="5" t="inlineStr">
+      <c r="D78" s="17" t="inlineStr">
         <is>
           <t>197</t>
         </is>
@@ -14363,7 +14363,7 @@
           <t>706</t>
         </is>
       </c>
-      <c r="P80" s="9" t="inlineStr">
+      <c r="P80" s="17" t="inlineStr">
         <is>
           <t>197</t>
         </is>
@@ -15338,7 +15338,7 @@
           <t>304</t>
         </is>
       </c>
-      <c r="X85" s="17" t="inlineStr">
+      <c r="X85" s="12" t="inlineStr">
         <is>
           <t>886</t>
         </is>
@@ -17345,7 +17345,7 @@
           <t>636</t>
         </is>
       </c>
-      <c r="N96" s="9" t="inlineStr">
+      <c r="N96" s="17" t="inlineStr">
         <is>
           <t>464</t>
         </is>
@@ -18138,7 +18138,7 @@
           <t>971</t>
         </is>
       </c>
-      <c r="W100" s="12" t="inlineStr">
+      <c r="W100" s="17" t="inlineStr">
         <is>
           <t>197</t>
         </is>
@@ -18729,7 +18729,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="AC103" s="14" t="inlineStr">
+      <c r="AC103" s="17" t="inlineStr">
         <is>
           <t>197</t>
         </is>
@@ -24411,7 +24411,7 @@
           <t>186</t>
         </is>
       </c>
-      <c r="Z136" s="17" t="inlineStr">
+      <c r="Z136" s="13" t="inlineStr">
         <is>
           <t>886</t>
         </is>
@@ -26560,7 +26560,7 @@
           <t>544</t>
         </is>
       </c>
-      <c r="AA150" s="13" t="inlineStr">
+      <c r="AA150" s="17" t="inlineStr">
         <is>
           <t>464</t>
         </is>
@@ -26909,7 +26909,7 @@
           <t>223</t>
         </is>
       </c>
-      <c r="V152" s="17" t="inlineStr">
+      <c r="V152" s="11" t="inlineStr">
         <is>
           <t>513</t>
         </is>
@@ -26996,7 +26996,7 @@
           <t>11</t>
         </is>
       </c>
-      <c r="B153" s="5" t="inlineStr">
+      <c r="B153" s="17" t="inlineStr">
         <is>
           <t>464</t>
         </is>
@@ -27011,7 +27011,7 @@
           <t>748</t>
         </is>
       </c>
-      <c r="E153" s="17" t="inlineStr">
+      <c r="E153" s="6" t="inlineStr">
         <is>
           <t>886</t>
         </is>
@@ -30220,7 +30220,7 @@
           <t>321</t>
         </is>
       </c>
-      <c r="K170" s="8" t="inlineStr">
+      <c r="K170" s="17" t="inlineStr">
         <is>
           <t>197</t>
         </is>
@@ -31843,7 +31843,7 @@
           <t>631</t>
         </is>
       </c>
-      <c r="S181" s="10" t="inlineStr">
+      <c r="S181" s="17" t="inlineStr">
         <is>
           <t>464</t>
         </is>
@@ -32177,7 +32177,7 @@
           <t>515</t>
         </is>
       </c>
-      <c r="K183" s="8" t="inlineStr">
+      <c r="K183" s="17" t="inlineStr">
         <is>
           <t>197</t>
         </is>
@@ -32591,7 +32591,7 @@
           <t>552</t>
         </is>
       </c>
-      <c r="S185" s="17" t="inlineStr">
+      <c r="S185" s="10" t="inlineStr">
         <is>
           <t>513</t>
         </is>
@@ -32738,7 +32738,7 @@
           <t>665</t>
         </is>
       </c>
-      <c r="K186" s="17" t="inlineStr">
+      <c r="K186" s="8" t="inlineStr">
         <is>
           <t>886</t>
         </is>
@@ -32895,7 +32895,7 @@
           <t>280</t>
         </is>
       </c>
-      <c r="E187" s="6" t="inlineStr">
+      <c r="E187" s="17" t="inlineStr">
         <is>
           <t>197</t>
         </is>
@@ -33324,7 +33324,7 @@
           <t>682</t>
         </is>
       </c>
-      <c r="P189" s="9" t="inlineStr">
+      <c r="P189" s="17" t="inlineStr">
         <is>
           <t>197</t>
         </is>
@@ -33374,7 +33374,7 @@
           <t>774</t>
         </is>
       </c>
-      <c r="Z189" s="17" t="inlineStr">
+      <c r="Z189" s="13" t="inlineStr">
         <is>
           <t>513</t>
         </is>
@@ -33541,7 +33541,7 @@
           <t>705</t>
         </is>
       </c>
-      <c r="V190" s="17" t="inlineStr">
+      <c r="V190" s="11" t="inlineStr">
         <is>
           <t>886</t>
         </is>
@@ -33855,7 +33855,7 @@
           <t>166</t>
         </is>
       </c>
-      <c r="J192" s="7" t="inlineStr">
+      <c r="J192" s="17" t="inlineStr">
         <is>
           <t>197</t>
         </is>
@@ -35042,7 +35042,7 @@
           <t>553</t>
         </is>
       </c>
-      <c r="W198" s="17" t="inlineStr">
+      <c r="W198" s="12" t="inlineStr">
         <is>
           <t>886</t>
         </is>
@@ -36027,7 +36027,7 @@
           <t>491</t>
         </is>
       </c>
-      <c r="AG203" s="17" t="inlineStr">
+      <c r="AG203" s="15" t="inlineStr">
         <is>
           <t>513</t>
         </is>
@@ -36164,7 +36164,7 @@
           <t>193</t>
         </is>
       </c>
-      <c r="W204" s="12" t="inlineStr">
+      <c r="W204" s="17" t="inlineStr">
         <is>
           <t>464</t>
         </is>
@@ -36401,7 +36401,7 @@
           <t>742</t>
         </is>
       </c>
-      <c r="AG205" s="15" t="inlineStr">
+      <c r="AG205" s="17" t="inlineStr">
         <is>
           <t>464</t>
         </is>
@@ -37313,7 +37313,7 @@
           <t>670</t>
         </is>
       </c>
-      <c r="K213" s="17" t="inlineStr">
+      <c r="K213" s="8" t="inlineStr">
         <is>
           <t>886</t>
         </is>
@@ -37540,7 +37540,7 @@
           <t>724</t>
         </is>
       </c>
-      <c r="S214" s="10" t="inlineStr">
+      <c r="S214" s="17" t="inlineStr">
         <is>
           <t>197</t>
         </is>
@@ -37727,7 +37727,7 @@
           <t>731</t>
         </is>
       </c>
-      <c r="S215" s="17" t="inlineStr">
+      <c r="S215" s="10" t="inlineStr">
         <is>
           <t>886</t>
         </is>
@@ -37904,7 +37904,7 @@
           <t>574</t>
         </is>
       </c>
-      <c r="Q216" s="17" t="inlineStr">
+      <c r="Q216" s="10" t="inlineStr">
         <is>
           <t>886</t>
         </is>
@@ -38727,7 +38727,7 @@
           <t>559</t>
         </is>
       </c>
-      <c r="AF220" s="17" t="inlineStr">
+      <c r="AF220" s="15" t="inlineStr">
         <is>
           <t>513</t>
         </is>
@@ -39121,7 +39121,7 @@
           <t>243</t>
         </is>
       </c>
-      <c r="AJ222" s="16" t="inlineStr">
+      <c r="AJ222" s="17" t="inlineStr">
         <is>
           <t>464</t>
         </is>
@@ -42836,7 +42836,7 @@
           <t>964</t>
         </is>
       </c>
-      <c r="AE242" s="14" t="inlineStr">
+      <c r="AE242" s="17" t="inlineStr">
         <is>
           <t>464</t>
         </is>
@@ -43327,17 +43327,17 @@
           <t>242</t>
         </is>
       </c>
-      <c r="H251" s="7" t="inlineStr">
+      <c r="H251" s="17" t="inlineStr">
         <is>
           <t>464</t>
         </is>
       </c>
-      <c r="I251" s="7" t="inlineStr">
+      <c r="I251" s="17" t="inlineStr">
         <is>
           <t>197</t>
         </is>
       </c>
-      <c r="J251" s="17" t="inlineStr">
+      <c r="J251" s="7" t="inlineStr">
         <is>
           <t>886</t>
         </is>
@@ -43379,7 +43379,7 @@
           <t>580</t>
         </is>
       </c>
-      <c r="H252" s="17" t="inlineStr">
+      <c r="H252" s="7" t="inlineStr">
         <is>
           <t>513</t>
         </is>
@@ -43537,17 +43537,17 @@
       </c>
       <c r="H255" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>503</t>
         </is>
       </c>
       <c r="I255" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>990</t>
         </is>
       </c>
       <c r="J255" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>105</t>
         </is>
       </c>
     </row>
@@ -44102,7 +44102,7 @@
           <t>827</t>
         </is>
       </c>
-      <c r="G266" s="17" t="inlineStr">
+      <c r="G266" s="6" t="inlineStr">
         <is>
           <t>886</t>
         </is>

</xml_diff>

<commit_message>
make spot_patterns_v1 and v1.2 to export results
</commit_message>
<xml_diff>
--- a/swertres/excel_results.xlsx
+++ b/swertres/excel_results.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -43,12 +43,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FFFFFF"/>
+        <fgColor rgb="00ff6666"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00ff6666"/>
+        <fgColor rgb="00FFFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -220,7 +220,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
@@ -253,7 +253,7 @@
     <xf numFmtId="0" fontId="1" fillId="14" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2717,7 +2717,7 @@
           <t>790</t>
         </is>
       </c>
-      <c r="C13" s="17" t="inlineStr">
+      <c r="C13" s="5" t="inlineStr">
         <is>
           <t>640</t>
         </is>
@@ -3288,7 +3288,7 @@
           <t>601</t>
         </is>
       </c>
-      <c r="E16" s="6" t="inlineStr">
+      <c r="E16" s="17" t="inlineStr">
         <is>
           <t>066</t>
         </is>
@@ -3772,7 +3772,7 @@
           <t>878</t>
         </is>
       </c>
-      <c r="AA18" s="13" t="inlineStr">
+      <c r="AA18" s="17" t="inlineStr">
         <is>
           <t>066</t>
         </is>
@@ -3894,7 +3894,7 @@
           <t>518</t>
         </is>
       </c>
-      <c r="N19" s="9" t="inlineStr">
+      <c r="N19" s="17" t="inlineStr">
         <is>
           <t>004</t>
         </is>
@@ -5906,7 +5906,7 @@
           <t>760</t>
         </is>
       </c>
-      <c r="E30" s="17" t="inlineStr">
+      <c r="E30" s="6" t="inlineStr">
         <is>
           <t>640</t>
         </is>
@@ -11436,7 +11436,7 @@
           <t>288</t>
         </is>
       </c>
-      <c r="I62" s="7" t="inlineStr">
+      <c r="I62" s="17" t="inlineStr">
         <is>
           <t>066</t>
         </is>
@@ -11628,7 +11628,7 @@
           <t>662</t>
         </is>
       </c>
-      <c r="J63" s="7" t="inlineStr">
+      <c r="J63" s="17" t="inlineStr">
         <is>
           <t>066</t>
         </is>
@@ -11703,7 +11703,7 @@
           <t>128</t>
         </is>
       </c>
-      <c r="Y63" s="12" t="inlineStr">
+      <c r="Y63" s="17" t="inlineStr">
         <is>
           <t>004</t>
         </is>
@@ -12102,7 +12102,7 @@
           <t>008</t>
         </is>
       </c>
-      <c r="AD65" s="14" t="inlineStr">
+      <c r="AD65" s="17" t="inlineStr">
         <is>
           <t>004</t>
         </is>
@@ -15358,7 +15358,7 @@
           <t>054</t>
         </is>
       </c>
-      <c r="AB85" s="17" t="inlineStr">
+      <c r="AB85" s="13" t="inlineStr">
         <is>
           <t>484</t>
         </is>
@@ -16435,7 +16435,7 @@
           <t>221</t>
         </is>
       </c>
-      <c r="S91" s="17" t="inlineStr">
+      <c r="S91" s="10" t="inlineStr">
         <is>
           <t>484</t>
         </is>
@@ -17704,7 +17704,7 @@
           <t>610</t>
         </is>
       </c>
-      <c r="K98" s="17" t="inlineStr">
+      <c r="K98" s="8" t="inlineStr">
         <is>
           <t>484</t>
         </is>
@@ -17739,7 +17739,7 @@
           <t>328</t>
         </is>
       </c>
-      <c r="R98" s="10" t="inlineStr">
+      <c r="R98" s="17" t="inlineStr">
         <is>
           <t>066</t>
         </is>
@@ -20302,7 +20302,7 @@
           <t>768</t>
         </is>
       </c>
-      <c r="AA114" s="17" t="inlineStr">
+      <c r="AA114" s="13" t="inlineStr">
         <is>
           <t>484</t>
         </is>
@@ -26515,7 +26515,7 @@
           <t>773</t>
         </is>
       </c>
-      <c r="R150" s="17" t="inlineStr">
+      <c r="R150" s="10" t="inlineStr">
         <is>
           <t>640</t>
         </is>
@@ -29290,7 +29290,7 @@
           <t>642</t>
         </is>
       </c>
-      <c r="L165" s="17" t="inlineStr">
+      <c r="L165" s="8" t="inlineStr">
         <is>
           <t>640</t>
         </is>
@@ -32753,7 +32753,7 @@
           <t>921</t>
         </is>
       </c>
-      <c r="N186" s="9" t="inlineStr">
+      <c r="N186" s="17" t="inlineStr">
         <is>
           <t>004</t>
         </is>
@@ -32773,7 +32773,7 @@
           <t>724</t>
         </is>
       </c>
-      <c r="R186" s="10" t="inlineStr">
+      <c r="R186" s="17" t="inlineStr">
         <is>
           <t>066</t>
         </is>
@@ -34344,7 +34344,7 @@
           <t>965</t>
         </is>
       </c>
-      <c r="AG194" s="17" t="inlineStr">
+      <c r="AG194" s="15" t="inlineStr">
         <is>
           <t>484</t>
         </is>
@@ -35299,7 +35299,7 @@
           <t>202</t>
         </is>
       </c>
-      <c r="AK199" s="17" t="inlineStr">
+      <c r="AK199" s="16" t="inlineStr">
         <is>
           <t>640</t>
         </is>
@@ -36770,7 +36770,7 @@
           <t>127</t>
         </is>
       </c>
-      <c r="AF207" s="17" t="inlineStr">
+      <c r="AF207" s="15" t="inlineStr">
         <is>
           <t>484</t>
         </is>
@@ -37378,7 +37378,7 @@
           <t>234</t>
         </is>
       </c>
-      <c r="X213" s="17" t="inlineStr">
+      <c r="X213" s="12" t="inlineStr">
         <is>
           <t>640</t>
         </is>
@@ -37782,7 +37782,7 @@
           <t>548</t>
         </is>
       </c>
-      <c r="AD215" s="17" t="inlineStr">
+      <c r="AD215" s="14" t="inlineStr">
         <is>
           <t>484</t>
         </is>
@@ -38213,7 +38213,7 @@
           <t>706</t>
         </is>
       </c>
-      <c r="D218" s="5" t="inlineStr">
+      <c r="D218" s="17" t="inlineStr">
         <is>
           <t>004</t>
         </is>
@@ -40041,7 +40041,7 @@
           <t>892</t>
         </is>
       </c>
-      <c r="AG227" s="17" t="inlineStr">
+      <c r="AG227" s="15" t="inlineStr">
         <is>
           <t>484</t>
         </is>
@@ -40507,7 +40507,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="N230" s="9" t="inlineStr">
+      <c r="N230" s="17" t="inlineStr">
         <is>
           <t>004</t>
         </is>
@@ -41138,7 +41138,7 @@
           <t>685</t>
         </is>
       </c>
-      <c r="AB233" s="13" t="inlineStr">
+      <c r="AB233" s="17" t="inlineStr">
         <is>
           <t>066</t>
         </is>
@@ -43043,7 +43043,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="AI243" s="17" t="inlineStr">
+      <c r="AI243" s="16" t="inlineStr">
         <is>
           <t>484</t>
         </is>
@@ -43589,17 +43589,17 @@
       </c>
       <c r="H256" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>731</t>
         </is>
       </c>
       <c r="I256" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>508</t>
         </is>
       </c>
       <c r="J256" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>999</t>
         </is>
       </c>
     </row>
@@ -43641,17 +43641,17 @@
       </c>
       <c r="H257" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>542</t>
         </is>
       </c>
       <c r="I257" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>917</t>
         </is>
       </c>
       <c r="J257" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>171</t>
         </is>
       </c>
     </row>
@@ -43693,17 +43693,17 @@
       </c>
       <c r="H258" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>565</t>
         </is>
       </c>
       <c r="I258" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>896</t>
         </is>
       </c>
       <c r="J258" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>764</t>
         </is>
       </c>
     </row>
@@ -43745,17 +43745,17 @@
       </c>
       <c r="H259" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>178</t>
         </is>
       </c>
       <c r="I259" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>806</t>
         </is>
       </c>
       <c r="J259" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>439</t>
         </is>
       </c>
     </row>
@@ -43797,17 +43797,17 @@
       </c>
       <c r="H260" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>797</t>
         </is>
       </c>
       <c r="I260" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>144</t>
         </is>
       </c>
       <c r="J260" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>759</t>
         </is>
       </c>
     </row>
@@ -43849,17 +43849,17 @@
       </c>
       <c r="H261" s="7" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I261" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J261" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
+          <t>527</t>
+        </is>
+      </c>
+      <c r="I261" s="17" t="inlineStr">
+        <is>
+          <t>066</t>
+        </is>
+      </c>
+      <c r="J261" s="17" t="inlineStr">
+        <is>
+          <t>004</t>
         </is>
       </c>
     </row>
@@ -44513,12 +44513,12 @@
           <t>525</t>
         </is>
       </c>
-      <c r="F274" s="17" t="inlineStr">
+      <c r="F274" s="6" t="inlineStr">
         <is>
           <t>640</t>
         </is>
       </c>
-      <c r="G274" s="17" t="inlineStr">
+      <c r="G274" s="6" t="inlineStr">
         <is>
           <t>484</t>
         </is>

</xml_diff>

<commit_message>
add script to filter previous month pair and digits
</commit_message>
<xml_diff>
--- a/swertres/excel_results.xlsx
+++ b/swertres/excel_results.xlsx
@@ -53,11 +53,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="00ccff33"/>
       </patternFill>
     </fill>
@@ -69,6 +64,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="0066cc33"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -226,13 +226,13 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
@@ -253,7 +253,7 @@
     <xf numFmtId="0" fontId="1" fillId="14" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1488,7 +1488,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="S6" s="10" t="inlineStr">
+      <c r="S6" s="17" t="inlineStr">
         <is>
           <t>927</t>
         </is>
@@ -4480,7 +4480,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="S22" s="17" t="inlineStr">
+      <c r="S22" s="10" t="inlineStr">
         <is>
           <t>003</t>
         </is>
@@ -5931,7 +5931,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="J30" s="17" t="inlineStr">
+      <c r="J30" s="7" t="inlineStr">
         <is>
           <t>300</t>
         </is>
@@ -7489,7 +7489,7 @@
           <t>121</t>
         </is>
       </c>
-      <c r="E41" s="6" t="inlineStr">
+      <c r="E41" s="17" t="inlineStr">
         <is>
           <t>297</t>
         </is>
@@ -7564,7 +7564,7 @@
           <t>481</t>
         </is>
       </c>
-      <c r="T41" s="11" t="inlineStr">
+      <c r="T41" s="17" t="inlineStr">
         <is>
           <t>279</t>
         </is>
@@ -8524,7 +8524,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="Y46" s="12" t="inlineStr">
+      <c r="Y46" s="17" t="inlineStr">
         <is>
           <t>792</t>
         </is>
@@ -8686,7 +8686,7 @@
           <t>160</t>
         </is>
       </c>
-      <c r="T47" s="11" t="inlineStr">
+      <c r="T47" s="17" t="inlineStr">
         <is>
           <t>297</t>
         </is>
@@ -9000,7 +9000,7 @@
           <t>238</t>
         </is>
       </c>
-      <c r="H49" s="7" t="inlineStr">
+      <c r="H49" s="17" t="inlineStr">
         <is>
           <t>297</t>
         </is>
@@ -9120,7 +9120,7 @@
           <t>318</t>
         </is>
       </c>
-      <c r="AF49" s="17" t="inlineStr">
+      <c r="AF49" s="15" t="inlineStr">
         <is>
           <t>030</t>
         </is>
@@ -9212,7 +9212,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="M50" s="8" t="inlineStr">
+      <c r="M50" s="17" t="inlineStr">
         <is>
           <t>279</t>
         </is>
@@ -9277,7 +9277,7 @@
           <t>429</t>
         </is>
       </c>
-      <c r="Z50" s="13" t="inlineStr">
+      <c r="Z50" s="17" t="inlineStr">
         <is>
           <t>792</t>
         </is>
@@ -11334,7 +11334,7 @@
           <t>104</t>
         </is>
       </c>
-      <c r="Z61" s="17" t="inlineStr">
+      <c r="Z61" s="13" t="inlineStr">
         <is>
           <t>300</t>
         </is>
@@ -11800,7 +11800,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="G64" s="6" t="inlineStr">
+      <c r="G64" s="17" t="inlineStr">
         <is>
           <t>729</t>
         </is>
@@ -12406,7 +12406,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="P67" s="17" t="inlineStr">
+      <c r="P67" s="9" t="inlineStr">
         <is>
           <t>300</t>
         </is>
@@ -12511,7 +12511,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="AK67" s="16" t="inlineStr">
+      <c r="AK67" s="17" t="inlineStr">
         <is>
           <t>927</t>
         </is>
@@ -13009,7 +13009,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="G73" s="6" t="inlineStr">
+      <c r="G73" s="17" t="inlineStr">
         <is>
           <t>729</t>
         </is>
@@ -13518,7 +13518,7 @@
           <t>046</t>
         </is>
       </c>
-      <c r="AH75" s="15" t="inlineStr">
+      <c r="AH75" s="17" t="inlineStr">
         <is>
           <t>729</t>
         </is>
@@ -13872,7 +13872,7 @@
           <t>933</t>
         </is>
       </c>
-      <c r="AD77" s="14" t="inlineStr">
+      <c r="AD77" s="17" t="inlineStr">
         <is>
           <t>279</t>
         </is>
@@ -14079,7 +14079,7 @@
           <t>176</t>
         </is>
       </c>
-      <c r="AH78" s="15" t="inlineStr">
+      <c r="AH78" s="17" t="inlineStr">
         <is>
           <t>729</t>
         </is>
@@ -14338,7 +14338,7 @@
           <t>236</t>
         </is>
       </c>
-      <c r="K80" s="8" t="inlineStr">
+      <c r="K80" s="17" t="inlineStr">
         <is>
           <t>927</t>
         </is>
@@ -15066,7 +15066,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="G84" s="6" t="inlineStr">
+      <c r="G84" s="17" t="inlineStr">
         <is>
           <t>792</t>
         </is>
@@ -15141,7 +15141,7 @@
           <t>334</t>
         </is>
       </c>
-      <c r="V84" s="11" t="inlineStr">
+      <c r="V84" s="17" t="inlineStr">
         <is>
           <t>792</t>
         </is>
@@ -16961,7 +16961,7 @@
           <t>661</t>
         </is>
       </c>
-      <c r="L94" s="8" t="inlineStr">
+      <c r="L94" s="17" t="inlineStr">
         <is>
           <t>297</t>
         </is>
@@ -17390,7 +17390,7 @@
           <t>139</t>
         </is>
       </c>
-      <c r="W96" s="17" t="inlineStr">
+      <c r="W96" s="12" t="inlineStr">
         <is>
           <t>300</t>
         </is>
@@ -18502,7 +18502,7 @@
           <t>856</t>
         </is>
       </c>
-      <c r="U102" s="11" t="inlineStr">
+      <c r="U102" s="17" t="inlineStr">
         <is>
           <t>792</t>
         </is>
@@ -19180,7 +19180,7 @@
           <t>447</t>
         </is>
       </c>
-      <c r="AA108" s="17" t="inlineStr">
+      <c r="AA108" s="13" t="inlineStr">
         <is>
           <t>003</t>
         </is>
@@ -19342,7 +19342,7 @@
           <t>323</t>
         </is>
       </c>
-      <c r="V109" s="11" t="inlineStr">
+      <c r="V109" s="17" t="inlineStr">
         <is>
           <t>279</t>
         </is>
@@ -20272,7 +20272,7 @@
           <t>869</t>
         </is>
       </c>
-      <c r="U114" s="11" t="inlineStr">
+      <c r="U114" s="17" t="inlineStr">
         <is>
           <t>927</t>
         </is>
@@ -20571,7 +20571,7 @@
           <t>281</t>
         </is>
       </c>
-      <c r="F116" s="6" t="inlineStr">
+      <c r="F116" s="17" t="inlineStr">
         <is>
           <t>972</t>
         </is>
@@ -20873,7 +20873,7 @@
           <t>924</t>
         </is>
       </c>
-      <c r="AC117" s="14" t="inlineStr">
+      <c r="AC117" s="17" t="inlineStr">
         <is>
           <t>729</t>
         </is>
@@ -21025,7 +21025,7 @@
           <t>662</t>
         </is>
       </c>
-      <c r="V118" s="11" t="inlineStr">
+      <c r="V118" s="17" t="inlineStr">
         <is>
           <t>972</t>
         </is>
@@ -21459,7 +21459,7 @@
           <t>611</t>
         </is>
       </c>
-      <c r="AH120" s="15" t="inlineStr">
+      <c r="AH120" s="17" t="inlineStr">
         <is>
           <t>972</t>
         </is>
@@ -21843,7 +21843,7 @@
           <t>975</t>
         </is>
       </c>
-      <c r="AJ122" s="16" t="inlineStr">
+      <c r="AJ122" s="17" t="inlineStr">
         <is>
           <t>297</t>
         </is>
@@ -21980,7 +21980,7 @@
           <t>368</t>
         </is>
       </c>
-      <c r="Z123" s="17" t="inlineStr">
+      <c r="Z123" s="13" t="inlineStr">
         <is>
           <t>030</t>
         </is>
@@ -23052,7 +23052,7 @@
           <t>049</t>
         </is>
       </c>
-      <c r="P129" s="9" t="inlineStr">
+      <c r="P129" s="17" t="inlineStr">
         <is>
           <t>279</t>
         </is>
@@ -23244,7 +23244,7 @@
           <t>064</t>
         </is>
       </c>
-      <c r="Q130" s="10" t="inlineStr">
+      <c r="Q130" s="17" t="inlineStr">
         <is>
           <t>729</t>
         </is>
@@ -23668,7 +23668,7 @@
           <t>781</t>
         </is>
       </c>
-      <c r="AA132" s="13" t="inlineStr">
+      <c r="AA132" s="17" t="inlineStr">
         <is>
           <t>927</t>
         </is>
@@ -24159,7 +24159,7 @@
           <t>389</t>
         </is>
       </c>
-      <c r="M135" s="8" t="inlineStr">
+      <c r="M135" s="17" t="inlineStr">
         <is>
           <t>927</t>
         </is>
@@ -25453,7 +25453,7 @@
           <t>291</t>
         </is>
       </c>
-      <c r="AD144" s="14" t="inlineStr">
+      <c r="AD144" s="17" t="inlineStr">
         <is>
           <t>927</t>
         </is>
@@ -26383,7 +26383,7 @@
           <t>394</t>
         </is>
       </c>
-      <c r="AC149" s="14" t="inlineStr">
+      <c r="AC149" s="17" t="inlineStr">
         <is>
           <t>792</t>
         </is>
@@ -26717,7 +26717,7 @@
           <t>697</t>
         </is>
       </c>
-      <c r="U151" s="17" t="inlineStr">
+      <c r="U151" s="11" t="inlineStr">
         <is>
           <t>030</t>
         </is>
@@ -26809,7 +26809,7 @@
           <t>10</t>
         </is>
       </c>
-      <c r="B152" s="17" t="inlineStr">
+      <c r="B152" s="5" t="inlineStr">
         <is>
           <t>300</t>
         </is>
@@ -27026,7 +27026,7 @@
           <t>601</t>
         </is>
       </c>
-      <c r="H153" s="17" t="inlineStr">
+      <c r="H153" s="7" t="inlineStr">
         <is>
           <t>300</t>
         </is>
@@ -27146,7 +27146,7 @@
           <t>718</t>
         </is>
       </c>
-      <c r="AF153" s="15" t="inlineStr">
+      <c r="AF153" s="17" t="inlineStr">
         <is>
           <t>297</t>
         </is>
@@ -28375,7 +28375,7 @@
           <t>237</t>
         </is>
       </c>
-      <c r="P160" s="17" t="inlineStr">
+      <c r="P160" s="9" t="inlineStr">
         <is>
           <t>030</t>
         </is>
@@ -30013,7 +30013,7 @@
           <t>757</t>
         </is>
       </c>
-      <c r="G169" s="17" t="inlineStr">
+      <c r="G169" s="6" t="inlineStr">
         <is>
           <t>300</t>
         </is>
@@ -30230,7 +30230,7 @@
           <t>094</t>
         </is>
       </c>
-      <c r="M170" s="17" t="inlineStr">
+      <c r="M170" s="8" t="inlineStr">
         <is>
           <t>030</t>
         </is>
@@ -30477,7 +30477,7 @@
           <t>772</t>
         </is>
       </c>
-      <c r="Y171" s="12" t="inlineStr">
+      <c r="Y171" s="17" t="inlineStr">
         <is>
           <t>927</t>
         </is>
@@ -31686,7 +31686,7 @@
           <t>547</t>
         </is>
       </c>
-      <c r="Y180" s="12" t="inlineStr">
+      <c r="Y180" s="17" t="inlineStr">
         <is>
           <t>297</t>
         </is>
@@ -31918,7 +31918,7 @@
           <t>848</t>
         </is>
       </c>
-      <c r="AH181" s="15" t="inlineStr">
+      <c r="AH181" s="17" t="inlineStr">
         <is>
           <t>927</t>
         </is>
@@ -31965,7 +31965,7 @@
           <t>872</t>
         </is>
       </c>
-      <c r="F182" s="6" t="inlineStr">
+      <c r="F182" s="17" t="inlineStr">
         <is>
           <t>279</t>
         </is>
@@ -32287,7 +32287,7 @@
           <t>420</t>
         </is>
       </c>
-      <c r="AG183" s="15" t="inlineStr">
+      <c r="AG183" s="17" t="inlineStr">
         <is>
           <t>279</t>
         </is>
@@ -32586,7 +32586,7 @@
           <t>435</t>
         </is>
       </c>
-      <c r="R185" s="10" t="inlineStr">
+      <c r="R185" s="17" t="inlineStr">
         <is>
           <t>792</t>
         </is>
@@ -32808,7 +32808,7 @@
           <t>517</t>
         </is>
       </c>
-      <c r="Y186" s="12" t="inlineStr">
+      <c r="Y186" s="17" t="inlineStr">
         <is>
           <t>297</t>
         </is>
@@ -33825,7 +33825,7 @@
           <t>705</t>
         </is>
       </c>
-      <c r="D192" s="5" t="inlineStr">
+      <c r="D192" s="17" t="inlineStr">
         <is>
           <t>927</t>
         </is>
@@ -34142,7 +34142,7 @@
           <t>721</t>
         </is>
       </c>
-      <c r="AD193" s="17" t="inlineStr">
+      <c r="AD193" s="14" t="inlineStr">
         <is>
           <t>003</t>
         </is>
@@ -34214,7 +34214,7 @@
           <t>582</t>
         </is>
       </c>
-      <c r="G194" s="6" t="inlineStr">
+      <c r="G194" s="17" t="inlineStr">
         <is>
           <t>972</t>
         </is>
@@ -35149,7 +35149,7 @@
           <t>427</t>
         </is>
       </c>
-      <c r="G199" s="6" t="inlineStr">
+      <c r="G199" s="17" t="inlineStr">
         <is>
           <t>972</t>
         </is>
@@ -35294,7 +35294,7 @@
           <t>983</t>
         </is>
       </c>
-      <c r="AJ199" s="16" t="inlineStr">
+      <c r="AJ199" s="17" t="inlineStr">
         <is>
           <t>297</t>
         </is>
@@ -35962,7 +35962,7 @@
           <t>171</t>
         </is>
       </c>
-      <c r="T203" s="17" t="inlineStr">
+      <c r="T203" s="11" t="inlineStr">
         <is>
           <t>003</t>
         </is>
@@ -37879,7 +37879,7 @@
           <t>886</t>
         </is>
       </c>
-      <c r="L216" s="8" t="inlineStr">
+      <c r="L216" s="17" t="inlineStr">
         <is>
           <t>792</t>
         </is>
@@ -38036,7 +38036,7 @@
           <t>913</t>
         </is>
       </c>
-      <c r="F217" s="17" t="inlineStr">
+      <c r="F217" s="6" t="inlineStr">
         <is>
           <t>030</t>
         </is>
@@ -40335,7 +40335,7 @@
           <t>055</t>
         </is>
       </c>
-      <c r="Q229" s="17" t="inlineStr">
+      <c r="Q229" s="10" t="inlineStr">
         <is>
           <t>030</t>
         </is>
@@ -41240,7 +41240,7 @@
           <t>772</t>
         </is>
       </c>
-      <c r="K234" s="8" t="inlineStr">
+      <c r="K234" s="17" t="inlineStr">
         <is>
           <t>927</t>
         </is>
@@ -41507,7 +41507,7 @@
           <t>185</t>
         </is>
       </c>
-      <c r="AA235" s="13" t="inlineStr">
+      <c r="AA235" s="17" t="inlineStr">
         <is>
           <t>972</t>
         </is>
@@ -42594,7 +42594,7 @@
           <t>386</t>
         </is>
       </c>
-      <c r="T241" s="11" t="inlineStr">
+      <c r="T241" s="17" t="inlineStr">
         <is>
           <t>972</t>
         </is>
@@ -45010,7 +45010,7 @@
           <t>860</t>
         </is>
       </c>
-      <c r="AK256" s="16" t="inlineStr">
+      <c r="AK256" s="17" t="inlineStr">
         <is>
           <t>972</t>
         </is>
@@ -45733,7 +45733,7 @@
           <t>474</t>
         </is>
       </c>
-      <c r="AF260" s="17" t="inlineStr">
+      <c r="AF260" s="15" t="inlineStr">
         <is>
           <t>300</t>
         </is>
@@ -46067,7 +46067,7 @@
           <t>500</t>
         </is>
       </c>
-      <c r="X262" s="17" t="inlineStr">
+      <c r="X262" s="12" t="inlineStr">
         <is>
           <t>300</t>
         </is>
@@ -46760,7 +46760,7 @@
           <t>088</t>
         </is>
       </c>
-      <c r="M266" s="8" t="inlineStr">
+      <c r="M266" s="17" t="inlineStr">
         <is>
           <t>279</t>
         </is>
@@ -48655,7 +48655,7 @@
           <t>696</t>
         </is>
       </c>
-      <c r="R276" s="10" t="inlineStr">
+      <c r="R276" s="17" t="inlineStr">
         <is>
           <t>972</t>
         </is>
@@ -48882,7 +48882,7 @@
           <t>514</t>
         </is>
       </c>
-      <c r="Z277" s="13" t="inlineStr">
+      <c r="Z277" s="17" t="inlineStr">
         <is>
           <t>972</t>
         </is>
@@ -49727,7 +49727,7 @@
           <t>804</t>
         </is>
       </c>
-      <c r="AB284" s="13" t="inlineStr">
+      <c r="AB284" s="17" t="inlineStr">
         <is>
           <t>279</t>
         </is>
@@ -50460,7 +50460,7 @@
           <t>865</t>
         </is>
       </c>
-      <c r="Y288" s="12" t="inlineStr">
+      <c r="Y288" s="17" t="inlineStr">
         <is>
           <t>927</t>
         </is>
@@ -50874,7 +50874,7 @@
           <t>344</t>
         </is>
       </c>
-      <c r="AG290" s="15" t="inlineStr">
+      <c r="AG290" s="17" t="inlineStr">
         <is>
           <t>729</t>
         </is>
@@ -50991,7 +50991,7 @@
           <t>752</t>
         </is>
       </c>
-      <c r="S291" s="17" t="inlineStr">
+      <c r="S291" s="10" t="inlineStr">
         <is>
           <t>030</t>
         </is>
@@ -52270,7 +52270,7 @@
           <t>011</t>
         </is>
       </c>
-      <c r="M298" s="8" t="inlineStr">
+      <c r="M298" s="17" t="inlineStr">
         <is>
           <t>297</t>
         </is>
@@ -53088,7 +53088,7 @@
           <t>636</t>
         </is>
       </c>
-      <c r="AA302" s="13" t="inlineStr">
+      <c r="AA302" s="17" t="inlineStr">
         <is>
           <t>972</t>
         </is>
@@ -54766,7 +54766,7 @@
           <t>037</t>
         </is>
       </c>
-      <c r="Z311" s="13" t="inlineStr">
+      <c r="Z311" s="17" t="inlineStr">
         <is>
           <t>792</t>
         </is>
@@ -56057,7 +56057,7 @@
           <t>399</t>
         </is>
       </c>
-      <c r="E321" s="6" t="inlineStr">
+      <c r="E321" s="17" t="inlineStr">
         <is>
           <t>927</t>
         </is>
@@ -56431,7 +56431,7 @@
           <t>197</t>
         </is>
       </c>
-      <c r="E323" s="6" t="inlineStr">
+      <c r="E323" s="17" t="inlineStr">
         <is>
           <t>729</t>
         </is>
@@ -56441,7 +56441,7 @@
           <t>070</t>
         </is>
       </c>
-      <c r="G323" s="6" t="inlineStr">
+      <c r="G323" s="17" t="inlineStr">
         <is>
           <t>729</t>
         </is>
@@ -57785,7 +57785,7 @@
           <t>353</t>
         </is>
       </c>
-      <c r="N330" s="17" t="inlineStr">
+      <c r="N330" s="9" t="inlineStr">
         <is>
           <t>300</t>
         </is>
@@ -58376,7 +58376,7 @@
           <t>708</t>
         </is>
       </c>
-      <c r="T333" s="17" t="inlineStr">
+      <c r="T333" s="11" t="inlineStr">
         <is>
           <t>300</t>
         </is>
@@ -58498,7 +58498,7 @@
           <t>552</t>
         </is>
       </c>
-      <c r="G334" s="17" t="inlineStr">
+      <c r="G334" s="6" t="inlineStr">
         <is>
           <t>003</t>
         </is>
@@ -58770,7 +58770,7 @@
           <t>804</t>
         </is>
       </c>
-      <c r="X335" s="12" t="inlineStr">
+      <c r="X335" s="17" t="inlineStr">
         <is>
           <t>279</t>
         </is>
@@ -59109,7 +59109,7 @@
           <t>105</t>
         </is>
       </c>
-      <c r="Q337" s="10" t="inlineStr">
+      <c r="Q337" s="17" t="inlineStr">
         <is>
           <t>972</t>
         </is>
@@ -59852,7 +59852,7 @@
           <t>171</t>
         </is>
       </c>
-      <c r="P341" s="9" t="inlineStr">
+      <c r="P341" s="17" t="inlineStr">
         <is>
           <t>279</t>
         </is>
@@ -59979,7 +59979,7 @@
           <t>937</t>
         </is>
       </c>
-      <c r="D342" s="5" t="inlineStr">
+      <c r="D342" s="17" t="inlineStr">
         <is>
           <t>972</t>
         </is>
@@ -60944,7 +60944,7 @@
           <t>712</t>
         </is>
       </c>
-      <c r="J347" s="7" t="inlineStr">
+      <c r="J347" s="17" t="inlineStr">
         <is>
           <t>297</t>
         </is>
@@ -61156,7 +61156,7 @@
           <t>588</t>
         </is>
       </c>
-      <c r="O348" s="9" t="inlineStr">
+      <c r="O348" s="17" t="inlineStr">
         <is>
           <t>297</t>
         </is>
@@ -62071,7 +62071,7 @@
           <t>237</t>
         </is>
       </c>
-      <c r="AE355" s="14" t="inlineStr">
+      <c r="AE355" s="17" t="inlineStr">
         <is>
           <t>297</t>
         </is>
@@ -62470,7 +62470,7 @@
           <t>095</t>
         </is>
       </c>
-      <c r="AJ357" s="17" t="inlineStr">
+      <c r="AJ357" s="16" t="inlineStr">
         <is>
           <t>030</t>
         </is>
@@ -63442,7 +63442,7 @@
           <t>533</t>
         </is>
       </c>
-      <c r="F363" s="6" t="inlineStr">
+      <c r="F363" s="17" t="inlineStr">
         <is>
           <t>279</t>
         </is>
@@ -63764,7 +63764,7 @@
           <t>545</t>
         </is>
       </c>
-      <c r="AG364" s="15" t="inlineStr">
+      <c r="AG364" s="17" t="inlineStr">
         <is>
           <t>972</t>
         </is>
@@ -63926,7 +63926,7 @@
           <t>480</t>
         </is>
       </c>
-      <c r="AB365" s="13" t="inlineStr">
+      <c r="AB365" s="17" t="inlineStr">
         <is>
           <t>729</t>
         </is>
@@ -64609,7 +64609,7 @@
           <t>803</t>
         </is>
       </c>
-      <c r="O369" s="9" t="inlineStr">
+      <c r="O369" s="17" t="inlineStr">
         <is>
           <t>972</t>
         </is>
@@ -65644,7 +65644,7 @@
           <t>280</t>
         </is>
       </c>
-      <c r="AI374" s="17" t="inlineStr">
+      <c r="AI374" s="16" t="inlineStr">
         <is>
           <t>030</t>
         </is>
@@ -66008,7 +66008,7 @@
           <t>351</t>
         </is>
       </c>
-      <c r="AG376" s="17" t="inlineStr">
+      <c r="AG376" s="15" t="inlineStr">
         <is>
           <t>003</t>
         </is>
@@ -67075,7 +67075,7 @@
           <t>287</t>
         </is>
       </c>
-      <c r="V382" s="17" t="inlineStr">
+      <c r="V382" s="11" t="inlineStr">
         <is>
           <t>300</t>
         </is>
@@ -67167,7 +67167,7 @@
           <t>314</t>
         </is>
       </c>
-      <c r="C383" s="5" t="inlineStr">
+      <c r="C383" s="17" t="inlineStr">
         <is>
           <t>297</t>
         </is>
@@ -67227,7 +67227,7 @@
           <t>036</t>
         </is>
       </c>
-      <c r="O383" s="9" t="inlineStr">
+      <c r="O383" s="17" t="inlineStr">
         <is>
           <t>729</t>
         </is>
@@ -67277,7 +67277,7 @@
           <t>817</t>
         </is>
       </c>
-      <c r="Y383" s="12" t="inlineStr">
+      <c r="Y383" s="17" t="inlineStr">
         <is>
           <t>729</t>
         </is>
@@ -67748,7 +67748,7 @@
           <t>896</t>
         </is>
       </c>
-      <c r="AA388" s="13" t="inlineStr">
+      <c r="AA388" s="17" t="inlineStr">
         <is>
           <t>792</t>
         </is>
@@ -67855,7 +67855,7 @@
           <t>872</t>
         </is>
       </c>
-      <c r="K389" s="17" t="inlineStr">
+      <c r="K389" s="8" t="inlineStr">
         <is>
           <t>003</t>
         </is>
@@ -68506,7 +68506,7 @@
           <t>857</t>
         </is>
       </c>
-      <c r="AC392" s="17" t="inlineStr">
+      <c r="AC392" s="14" t="inlineStr">
         <is>
           <t>030</t>
         </is>
@@ -68900,7 +68900,7 @@
           <t>732</t>
         </is>
       </c>
-      <c r="AG394" s="15" t="inlineStr">
+      <c r="AG394" s="17" t="inlineStr">
         <is>
           <t>972</t>
         </is>
@@ -70528,7 +70528,7 @@
           <t>138</t>
         </is>
       </c>
-      <c r="V403" s="11" t="inlineStr">
+      <c r="V403" s="17" t="inlineStr">
         <is>
           <t>729</t>
         </is>
@@ -71296,7 +71296,7 @@
           <t>266</t>
         </is>
       </c>
-      <c r="Z407" s="13" t="inlineStr">
+      <c r="Z407" s="17" t="inlineStr">
         <is>
           <t>927</t>
         </is>
@@ -71999,7 +71999,7 @@
           <t>973</t>
         </is>
       </c>
-      <c r="Q411" s="10" t="inlineStr">
+      <c r="Q411" s="17" t="inlineStr">
         <is>
           <t>297</t>
         </is>
@@ -72151,7 +72151,7 @@
           <t>403</t>
         </is>
       </c>
-      <c r="J412" s="7" t="inlineStr">
+      <c r="J412" s="17" t="inlineStr">
         <is>
           <t>279</t>
         </is>
@@ -72727,7 +72727,7 @@
           <t>704</t>
         </is>
       </c>
-      <c r="M415" s="17" t="inlineStr">
+      <c r="M415" s="8" t="inlineStr">
         <is>
           <t>003</t>
         </is>
@@ -73009,7 +73009,7 @@
           <t>298</t>
         </is>
       </c>
-      <c r="AF416" s="17" t="inlineStr">
+      <c r="AF416" s="15" t="inlineStr">
         <is>
           <t>300</t>
         </is>
@@ -73051,7 +73051,7 @@
           <t>468</t>
         </is>
       </c>
-      <c r="C417" s="5" t="inlineStr">
+      <c r="C417" s="17" t="inlineStr">
         <is>
           <t>927</t>
         </is>
@@ -73136,7 +73136,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="T417" s="17" t="inlineStr">
+      <c r="T417" s="11" t="inlineStr">
         <is>
           <t>003</t>
         </is>
@@ -74395,7 +74395,7 @@
           <t>081</t>
         </is>
       </c>
-      <c r="AD426" s="14" t="inlineStr">
+      <c r="AD426" s="17" t="inlineStr">
         <is>
           <t>729</t>
         </is>
@@ -75751,7 +75751,7 @@
           <t>12</t>
         </is>
       </c>
-      <c r="B434" s="17" t="inlineStr">
+      <c r="B434" s="5" t="inlineStr">
         <is>
           <t>003</t>
         </is>
@@ -76003,7 +76003,7 @@
           <t>046</t>
         </is>
       </c>
-      <c r="O435" s="9" t="inlineStr">
+      <c r="O435" s="17" t="inlineStr">
         <is>
           <t>279</t>
         </is>
@@ -76477,7 +76477,7 @@
           <t>418</t>
         </is>
       </c>
-      <c r="AI437" s="16" t="inlineStr">
+      <c r="AI437" s="17" t="inlineStr">
         <is>
           <t>972</t>
         </is>
@@ -76669,7 +76669,7 @@
           <t>486</t>
         </is>
       </c>
-      <c r="AJ438" s="17" t="inlineStr">
+      <c r="AJ438" s="16" t="inlineStr">
         <is>
           <t>300</t>
         </is>
@@ -76908,7 +76908,7 @@
           <t>225</t>
         </is>
       </c>
-      <c r="I440" s="7" t="inlineStr">
+      <c r="I440" s="17" t="inlineStr">
         <is>
           <t>279</t>
         </is>
@@ -78571,7 +78571,7 @@
           <t>384</t>
         </is>
       </c>
-      <c r="E449" s="6" t="inlineStr">
+      <c r="E449" s="17" t="inlineStr">
         <is>
           <t>972</t>
         </is>
@@ -79000,7 +79000,7 @@
           <t>086</t>
         </is>
       </c>
-      <c r="P451" s="9" t="inlineStr">
+      <c r="P451" s="17" t="inlineStr">
         <is>
           <t>297</t>
         </is>
@@ -81902,7 +81902,7 @@
           <t>349</t>
         </is>
       </c>
-      <c r="R469" s="10" t="inlineStr">
+      <c r="R469" s="17" t="inlineStr">
         <is>
           <t>927</t>
         </is>
@@ -83019,7 +83019,7 @@
           <t>918</t>
         </is>
       </c>
-      <c r="Q475" s="10" t="inlineStr">
+      <c r="Q475" s="17" t="inlineStr">
         <is>
           <t>792</t>
         </is>
@@ -83231,7 +83231,7 @@
           <t>641</t>
         </is>
       </c>
-      <c r="V476" s="11" t="inlineStr">
+      <c r="V476" s="17" t="inlineStr">
         <is>
           <t>279</t>
         </is>
@@ -84196,7 +84196,7 @@
           <t>321</t>
         </is>
       </c>
-      <c r="AB481" s="13" t="inlineStr">
+      <c r="AB481" s="17" t="inlineStr">
         <is>
           <t>729</t>
         </is>
@@ -84288,7 +84288,7 @@
           <t>968</t>
         </is>
       </c>
-      <c r="I482" s="7" t="inlineStr">
+      <c r="I482" s="17" t="inlineStr">
         <is>
           <t>927</t>
         </is>
@@ -84500,7 +84500,7 @@
           <t>959</t>
         </is>
       </c>
-      <c r="N483" s="17" t="inlineStr">
+      <c r="N483" s="9" t="inlineStr">
         <is>
           <t>030</t>
         </is>
@@ -85303,7 +85303,7 @@
           <t>254</t>
         </is>
       </c>
-      <c r="Y487" s="12" t="inlineStr">
+      <c r="Y487" s="17" t="inlineStr">
         <is>
           <t>297</t>
         </is>
@@ -86011,7 +86011,7 @@
           <t>648</t>
         </is>
       </c>
-      <c r="AK493" s="16" t="inlineStr">
+      <c r="AK493" s="17" t="inlineStr">
         <is>
           <t>729</t>
         </is>
@@ -86038,7 +86038,7 @@
           <t>062</t>
         </is>
       </c>
-      <c r="E494" s="6" t="inlineStr">
+      <c r="E494" s="17" t="inlineStr">
         <is>
           <t>297</t>
         </is>
@@ -87320,7 +87320,7 @@
           <t>695</t>
         </is>
       </c>
-      <c r="AK500" s="17" t="inlineStr">
+      <c r="AK500" s="16" t="inlineStr">
         <is>
           <t>003</t>
         </is>
@@ -88058,7 +88058,7 @@
           <t>276</t>
         </is>
       </c>
-      <c r="AI504" s="16" t="inlineStr">
+      <c r="AI504" s="17" t="inlineStr">
         <is>
           <t>279</t>
         </is>
@@ -89888,7 +89888,7 @@
           <t>096</t>
         </is>
       </c>
-      <c r="AA514" s="17" t="inlineStr">
+      <c r="AA514" s="13" t="inlineStr">
         <is>
           <t>300</t>
         </is>
@@ -90105,7 +90105,7 @@
           <t>477</t>
         </is>
       </c>
-      <c r="AG515" s="15" t="inlineStr">
+      <c r="AG515" s="17" t="inlineStr">
         <is>
           <t>927</t>
         </is>
@@ -90125,7 +90125,7 @@
           <t>443</t>
         </is>
       </c>
-      <c r="AK515" s="17" t="inlineStr">
+      <c r="AK515" s="16" t="inlineStr">
         <is>
           <t>003</t>
         </is>
@@ -90304,17 +90304,17 @@
       </c>
       <c r="AI516" s="16" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>511</t>
         </is>
       </c>
       <c r="AJ516" s="16" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>387</t>
         </is>
       </c>
       <c r="AK516" s="16" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>808</t>
         </is>
       </c>
     </row>
@@ -90678,17 +90678,17 @@
       </c>
       <c r="AI518" s="16" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>283</t>
         </is>
       </c>
       <c r="AJ518" s="16" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>258</t>
         </is>
       </c>
       <c r="AK518" s="16" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>086</t>
         </is>
       </c>
     </row>
@@ -90865,17 +90865,17 @@
       </c>
       <c r="AI519" s="16" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>915</t>
         </is>
       </c>
       <c r="AJ519" s="16" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>750</t>
         </is>
       </c>
       <c r="AK519" s="16" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>761</t>
         </is>
       </c>
     </row>
@@ -91052,17 +91052,17 @@
       </c>
       <c r="AI520" s="16" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>639</t>
         </is>
       </c>
       <c r="AJ520" s="16" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AK520" s="16" t="inlineStr">
-        <is>
-          <t>-</t>
+          <t>247</t>
+        </is>
+      </c>
+      <c r="AK520" s="17" t="inlineStr">
+        <is>
+          <t>792</t>
         </is>
       </c>
     </row>
@@ -91202,7 +91202,7 @@
           <t>690</t>
         </is>
       </c>
-      <c r="AB521" s="13" t="inlineStr">
+      <c r="AB521" s="17" t="inlineStr">
         <is>
           <t>279</t>
         </is>

</xml_diff>

<commit_message>
add script excel results to auto run script
</commit_message>
<xml_diff>
--- a/swertres/excel_results.xlsx
+++ b/swertres/excel_results.xlsx
@@ -29,7 +29,7 @@
       <sz val="15"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="14">
     <fill>
       <patternFill/>
     </fill>
@@ -59,11 +59,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="009966ff"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FFFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -209,7 +204,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
@@ -232,6 +227,9 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -248,12 +246,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1286,7 +1278,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="P5" s="17" t="inlineStr">
+      <c r="P5" s="9" t="inlineStr">
         <is>
           <t>194</t>
         </is>
@@ -6938,7 +6930,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="G38" s="17" t="inlineStr">
+      <c r="G38" s="6" t="inlineStr">
         <is>
           <t>941</t>
         </is>
@@ -8464,7 +8456,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="M46" s="17" t="inlineStr">
+      <c r="M46" s="8" t="inlineStr">
         <is>
           <t>914</t>
         </is>
@@ -8611,7 +8603,7 @@
           <t>168</t>
         </is>
       </c>
-      <c r="E47" s="17" t="inlineStr">
+      <c r="E47" s="6" t="inlineStr">
         <is>
           <t>914</t>
         </is>
@@ -8943,7 +8935,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="AH48" s="17" t="inlineStr">
+      <c r="AH48" s="15" t="inlineStr">
         <is>
           <t>419</t>
         </is>
@@ -9045,7 +9037,7 @@
           <t>172</t>
         </is>
       </c>
-      <c r="Q49" s="17" t="inlineStr">
+      <c r="Q49" s="10" t="inlineStr">
         <is>
           <t>194</t>
         </is>
@@ -9145,7 +9137,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="AK49" s="17" t="inlineStr">
+      <c r="AK49" s="16" t="inlineStr">
         <is>
           <t>941</t>
         </is>
@@ -10137,7 +10129,7 @@
           <t>046</t>
         </is>
       </c>
-      <c r="K55" s="17" t="inlineStr">
+      <c r="K55" s="8" t="inlineStr">
         <is>
           <t>419</t>
         </is>
@@ -12107,7 +12099,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="AE65" s="17" t="inlineStr">
+      <c r="AE65" s="14" t="inlineStr">
         <is>
           <t>149</t>
         </is>
@@ -13757,7 +13749,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="G77" s="17" t="inlineStr">
+      <c r="G77" s="6" t="inlineStr">
         <is>
           <t>149</t>
         </is>
@@ -14116,7 +14108,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="D79" s="17" t="inlineStr">
+      <c r="D79" s="5" t="inlineStr">
         <is>
           <t>194</t>
         </is>
@@ -14303,7 +14295,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="D80" s="17" t="inlineStr">
+      <c r="D80" s="5" t="inlineStr">
         <is>
           <t>491</t>
         </is>
@@ -15425,7 +15417,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="D86" s="17" t="inlineStr">
+      <c r="D86" s="5" t="inlineStr">
         <is>
           <t>914</t>
         </is>
@@ -15590,7 +15582,7 @@
           <t>127</t>
         </is>
       </c>
-      <c r="AK86" s="17" t="inlineStr">
+      <c r="AK86" s="16" t="inlineStr">
         <is>
           <t>194</t>
         </is>
@@ -16193,7 +16185,7 @@
           <t>366</t>
         </is>
       </c>
-      <c r="H90" s="17" t="inlineStr">
+      <c r="H90" s="7" t="inlineStr">
         <is>
           <t>149</t>
         </is>
@@ -17061,7 +17053,7 @@
           <t>315</t>
         </is>
       </c>
-      <c r="AF94" s="17" t="inlineStr">
+      <c r="AF94" s="15" t="inlineStr">
         <is>
           <t>941</t>
         </is>
@@ -20187,7 +20179,7 @@
           <t>252</t>
         </is>
       </c>
-      <c r="D114" s="17" t="inlineStr">
+      <c r="D114" s="5" t="inlineStr">
         <is>
           <t>914</t>
         </is>
@@ -20202,7 +20194,7 @@
           <t>383</t>
         </is>
       </c>
-      <c r="G114" s="17" t="inlineStr">
+      <c r="G114" s="6" t="inlineStr">
         <is>
           <t>941</t>
         </is>
@@ -21985,7 +21977,7 @@
           <t>030</t>
         </is>
       </c>
-      <c r="AA123" s="17" t="inlineStr">
+      <c r="AA123" s="13" t="inlineStr">
         <is>
           <t>941</t>
         </is>
@@ -22546,7 +22538,7 @@
           <t>331</t>
         </is>
       </c>
-      <c r="AA126" s="17" t="inlineStr">
+      <c r="AA126" s="13" t="inlineStr">
         <is>
           <t>149</t>
         </is>
@@ -23905,7 +23897,7 @@
           <t>560</t>
         </is>
       </c>
-      <c r="AK133" s="17" t="inlineStr">
+      <c r="AK133" s="16" t="inlineStr">
         <is>
           <t>941</t>
         </is>
@@ -24361,7 +24353,7 @@
           <t>110</t>
         </is>
       </c>
-      <c r="P136" s="17" t="inlineStr">
+      <c r="P136" s="9" t="inlineStr">
         <is>
           <t>419</t>
         </is>
@@ -25408,7 +25400,7 @@
           <t>857</t>
         </is>
       </c>
-      <c r="U144" s="17" t="inlineStr">
+      <c r="U144" s="11" t="inlineStr">
         <is>
           <t>149</t>
         </is>
@@ -25762,7 +25754,7 @@
           <t>639</t>
         </is>
       </c>
-      <c r="Q146" s="17" t="inlineStr">
+      <c r="Q146" s="10" t="inlineStr">
         <is>
           <t>149</t>
         </is>
@@ -26328,7 +26320,7 @@
           <t>005</t>
         </is>
       </c>
-      <c r="R149" s="17" t="inlineStr">
+      <c r="R149" s="10" t="inlineStr">
         <is>
           <t>419</t>
         </is>
@@ -26722,7 +26714,7 @@
           <t>030</t>
         </is>
       </c>
-      <c r="V151" s="17" t="inlineStr">
+      <c r="V151" s="11" t="inlineStr">
         <is>
           <t>914</t>
         </is>
@@ -26949,7 +26941,7 @@
           <t>766</t>
         </is>
       </c>
-      <c r="AD152" s="17" t="inlineStr">
+      <c r="AD152" s="14" t="inlineStr">
         <is>
           <t>149</t>
         </is>
@@ -27056,7 +27048,7 @@
           <t>320</t>
         </is>
       </c>
-      <c r="N153" s="17" t="inlineStr">
+      <c r="N153" s="9" t="inlineStr">
         <is>
           <t>194</t>
         </is>
@@ -27293,7 +27285,7 @@
           <t>559</t>
         </is>
       </c>
-      <c r="X154" s="17" t="inlineStr">
+      <c r="X154" s="12" t="inlineStr">
         <is>
           <t>914</t>
         </is>
@@ -27430,7 +27422,7 @@
           <t>344</t>
         </is>
       </c>
-      <c r="N155" s="17" t="inlineStr">
+      <c r="N155" s="9" t="inlineStr">
         <is>
           <t>419</t>
         </is>
@@ -27540,7 +27532,7 @@
           <t>719</t>
         </is>
       </c>
-      <c r="AJ155" s="17" t="inlineStr">
+      <c r="AJ155" s="16" t="inlineStr">
         <is>
           <t>419</t>
         </is>
@@ -27727,7 +27719,7 @@
           <t>202</t>
         </is>
       </c>
-      <c r="AJ156" s="17" t="inlineStr">
+      <c r="AJ156" s="16" t="inlineStr">
         <is>
           <t>194</t>
         </is>
@@ -28502,7 +28494,7 @@
           <t>446</t>
         </is>
       </c>
-      <c r="D161" s="17" t="inlineStr">
+      <c r="D161" s="5" t="inlineStr">
         <is>
           <t>194</t>
         </is>
@@ -29442,7 +29434,7 @@
           <t>848</t>
         </is>
       </c>
-      <c r="E166" s="17" t="inlineStr">
+      <c r="E166" s="6" t="inlineStr">
         <is>
           <t>914</t>
         </is>
@@ -29679,7 +29671,7 @@
           <t>735</t>
         </is>
       </c>
-      <c r="O167" s="17" t="inlineStr">
+      <c r="O167" s="9" t="inlineStr">
         <is>
           <t>941</t>
         </is>
@@ -29806,7 +29798,7 @@
           <t>595</t>
         </is>
       </c>
-      <c r="C168" s="17" t="inlineStr">
+      <c r="C168" s="5" t="inlineStr">
         <is>
           <t>914</t>
         </is>
@@ -31641,7 +31633,7 @@
           <t>895</t>
         </is>
       </c>
-      <c r="P180" s="17" t="inlineStr">
+      <c r="P180" s="9" t="inlineStr">
         <is>
           <t>914</t>
         </is>
@@ -34189,7 +34181,7 @@
           <t>17</t>
         </is>
       </c>
-      <c r="B194" s="17" t="inlineStr">
+      <c r="B194" s="5" t="inlineStr">
         <is>
           <t>941</t>
         </is>
@@ -34254,7 +34246,7 @@
           <t>664</t>
         </is>
       </c>
-      <c r="O194" s="17" t="inlineStr">
+      <c r="O194" s="9" t="inlineStr">
         <is>
           <t>194</t>
         </is>
@@ -34476,7 +34468,7 @@
           <t>676</t>
         </is>
       </c>
-      <c r="V195" s="17" t="inlineStr">
+      <c r="V195" s="11" t="inlineStr">
         <is>
           <t>941</t>
         </is>
@@ -35154,7 +35146,7 @@
           <t>972</t>
         </is>
       </c>
-      <c r="H199" s="17" t="inlineStr">
+      <c r="H199" s="7" t="inlineStr">
         <is>
           <t>149</t>
         </is>
@@ -37525,7 +37517,7 @@
           <t>867</t>
         </is>
       </c>
-      <c r="P214" s="17" t="inlineStr">
+      <c r="P214" s="9" t="inlineStr">
         <is>
           <t>914</t>
         </is>
@@ -39193,7 +39185,7 @@
           <t>129</t>
         </is>
       </c>
-      <c r="M223" s="17" t="inlineStr">
+      <c r="M223" s="8" t="inlineStr">
         <is>
           <t>149</t>
         </is>
@@ -40203,7 +40195,7 @@
           <t>984</t>
         </is>
       </c>
-      <c r="AB228" s="17" t="inlineStr">
+      <c r="AB228" s="13" t="inlineStr">
         <is>
           <t>941</t>
         </is>
@@ -42659,7 +42651,7 @@
           <t>553</t>
         </is>
       </c>
-      <c r="AG241" s="17" t="inlineStr">
+      <c r="AG241" s="15" t="inlineStr">
         <is>
           <t>491</t>
         </is>
@@ -43439,7 +43431,7 @@
           <t>001</t>
         </is>
       </c>
-      <c r="V248" s="17" t="inlineStr">
+      <c r="V248" s="11" t="inlineStr">
         <is>
           <t>419</t>
         </is>
@@ -44117,7 +44109,7 @@
           <t>417</t>
         </is>
       </c>
-      <c r="H252" s="17" t="inlineStr">
+      <c r="H252" s="7" t="inlineStr">
         <is>
           <t>491</t>
         </is>
@@ -44945,7 +44937,7 @@
           <t>211</t>
         </is>
       </c>
-      <c r="X256" s="17" t="inlineStr">
+      <c r="X256" s="12" t="inlineStr">
         <is>
           <t>941</t>
         </is>
@@ -47316,7 +47308,7 @@
           <t>839</t>
         </is>
       </c>
-      <c r="L269" s="17" t="inlineStr">
+      <c r="L269" s="8" t="inlineStr">
         <is>
           <t>419</t>
         </is>
@@ -48690,7 +48682,7 @@
           <t>384</t>
         </is>
       </c>
-      <c r="Y276" s="17" t="inlineStr">
+      <c r="Y276" s="12" t="inlineStr">
         <is>
           <t>941</t>
         </is>
@@ -48917,7 +48909,7 @@
           <t>661</t>
         </is>
       </c>
-      <c r="AG277" s="17" t="inlineStr">
+      <c r="AG277" s="15" t="inlineStr">
         <is>
           <t>491</t>
         </is>
@@ -50532,7 +50524,7 @@
           <t>07</t>
         </is>
       </c>
-      <c r="B289" s="17" t="inlineStr">
+      <c r="B289" s="5" t="inlineStr">
         <is>
           <t>194</t>
         </is>
@@ -51001,7 +50993,7 @@
           <t>980</t>
         </is>
       </c>
-      <c r="U291" s="17" t="inlineStr">
+      <c r="U291" s="11" t="inlineStr">
         <is>
           <t>941</t>
         </is>
@@ -51435,7 +51427,7 @@
           <t>222</t>
         </is>
       </c>
-      <c r="AG293" s="17" t="inlineStr">
+      <c r="AG293" s="15" t="inlineStr">
         <is>
           <t>941</t>
         </is>
@@ -51986,7 +51978,7 @@
           <t>753</t>
         </is>
       </c>
-      <c r="AE296" s="17" t="inlineStr">
+      <c r="AE296" s="14" t="inlineStr">
         <is>
           <t>914</t>
         </is>
@@ -53058,7 +53050,7 @@
           <t>232</t>
         </is>
       </c>
-      <c r="U302" s="17" t="inlineStr">
+      <c r="U302" s="11" t="inlineStr">
         <is>
           <t>941</t>
         </is>
@@ -53452,7 +53444,7 @@
           <t>580</t>
         </is>
       </c>
-      <c r="Y304" s="17" t="inlineStr">
+      <c r="Y304" s="12" t="inlineStr">
         <is>
           <t>419</t>
         </is>
@@ -53569,7 +53561,7 @@
           <t>835</t>
         </is>
       </c>
-      <c r="K305" s="17" t="inlineStr">
+      <c r="K305" s="8" t="inlineStr">
         <is>
           <t>419</t>
         </is>
@@ -54100,7 +54092,7 @@
           <t>418</t>
         </is>
       </c>
-      <c r="E308" s="17" t="inlineStr">
+      <c r="E308" s="6" t="inlineStr">
         <is>
           <t>941</t>
         </is>
@@ -56142,7 +56134,7 @@
           <t>270</t>
         </is>
       </c>
-      <c r="V321" s="17" t="inlineStr">
+      <c r="V321" s="11" t="inlineStr">
         <is>
           <t>914</t>
         </is>
@@ -56369,7 +56361,7 @@
           <t>884</t>
         </is>
       </c>
-      <c r="AD322" s="17" t="inlineStr">
+      <c r="AD322" s="14" t="inlineStr">
         <is>
           <t>149</t>
         </is>
@@ -56404,7 +56396,7 @@
           <t>808</t>
         </is>
       </c>
-      <c r="AK322" s="17" t="inlineStr">
+      <c r="AK322" s="16" t="inlineStr">
         <is>
           <t>419</t>
         </is>
@@ -56658,7 +56650,7 @@
           <t>515</t>
         </is>
       </c>
-      <c r="M324" s="17" t="inlineStr">
+      <c r="M324" s="8" t="inlineStr">
         <is>
           <t>491</t>
         </is>
@@ -59261,7 +59253,7 @@
           <t>322</t>
         </is>
       </c>
-      <c r="J338" s="17" t="inlineStr">
+      <c r="J338" s="7" t="inlineStr">
         <is>
           <t>419</t>
         </is>
@@ -62128,7 +62120,7 @@
           <t>220</t>
         </is>
       </c>
-      <c r="E356" s="17" t="inlineStr">
+      <c r="E356" s="6" t="inlineStr">
         <is>
           <t>914</t>
         </is>
@@ -62208,7 +62200,7 @@
           <t>251</t>
         </is>
       </c>
-      <c r="U356" s="17" t="inlineStr">
+      <c r="U356" s="11" t="inlineStr">
         <is>
           <t>491</t>
         </is>
@@ -62861,7 +62853,7 @@
           <t>08</t>
         </is>
       </c>
-      <c r="B360" s="17" t="inlineStr">
+      <c r="B360" s="5" t="inlineStr">
         <is>
           <t>914</t>
         </is>
@@ -64731,7 +64723,7 @@
           <t>18</t>
         </is>
       </c>
-      <c r="B370" s="17" t="inlineStr">
+      <c r="B370" s="5" t="inlineStr">
         <is>
           <t>149</t>
         </is>
@@ -64938,7 +64930,7 @@
           <t>843</t>
         </is>
       </c>
-      <c r="F371" s="17" t="inlineStr">
+      <c r="F371" s="6" t="inlineStr">
         <is>
           <t>491</t>
         </is>
@@ -65853,7 +65845,7 @@
           <t>24</t>
         </is>
       </c>
-      <c r="B376" s="17" t="inlineStr">
+      <c r="B376" s="5" t="inlineStr">
         <is>
           <t>941</t>
         </is>
@@ -66282,7 +66274,7 @@
           <t>932</t>
         </is>
       </c>
-      <c r="M378" s="17" t="inlineStr">
+      <c r="M378" s="8" t="inlineStr">
         <is>
           <t>914</t>
         </is>
@@ -67125,7 +67117,7 @@
           <t>697</t>
         </is>
       </c>
-      <c r="AF382" s="17" t="inlineStr">
+      <c r="AF382" s="15" t="inlineStr">
         <is>
           <t>491</t>
         </is>
@@ -68047,7 +68039,7 @@
           <t>111</t>
         </is>
       </c>
-      <c r="L390" s="17" t="inlineStr">
+      <c r="L390" s="8" t="inlineStr">
         <is>
           <t>149</t>
         </is>
@@ -69124,7 +69116,7 @@
           <t>672</t>
         </is>
       </c>
-      <c r="C396" s="17" t="inlineStr">
+      <c r="C396" s="5" t="inlineStr">
         <is>
           <t>194</t>
         </is>
@@ -73338,7 +73330,7 @@
           <t>344</t>
         </is>
       </c>
-      <c r="W418" s="17" t="inlineStr">
+      <c r="W418" s="12" t="inlineStr">
         <is>
           <t>194</t>
         </is>
@@ -74385,7 +74377,7 @@
           <t>356</t>
         </is>
       </c>
-      <c r="AB426" s="17" t="inlineStr">
+      <c r="AB426" s="13" t="inlineStr">
         <is>
           <t>419</t>
         </is>
@@ -76028,7 +76020,7 @@
           <t>071</t>
         </is>
       </c>
-      <c r="T435" s="17" t="inlineStr">
+      <c r="T435" s="11" t="inlineStr">
         <is>
           <t>194</t>
         </is>
@@ -76078,7 +76070,7 @@
           <t>044</t>
         </is>
       </c>
-      <c r="AD435" s="17" t="inlineStr">
+      <c r="AD435" s="14" t="inlineStr">
         <is>
           <t>491</t>
         </is>
@@ -76150,7 +76142,7 @@
           <t>231</t>
         </is>
       </c>
-      <c r="G436" s="17" t="inlineStr">
+      <c r="G436" s="6" t="inlineStr">
         <is>
           <t>941</t>
         </is>
@@ -78519,7 +78511,7 @@
           <t>889</t>
         </is>
       </c>
-      <c r="AF448" s="17" t="inlineStr">
+      <c r="AF448" s="15" t="inlineStr">
         <is>
           <t>491</t>
         </is>
@@ -80179,7 +80171,7 @@
           <t>401</t>
         </is>
       </c>
-      <c r="J460" s="17" t="inlineStr">
+      <c r="J460" s="7" t="inlineStr">
         <is>
           <t>941</t>
         </is>
@@ -80623,7 +80615,7 @@
           <t>563</t>
         </is>
       </c>
-      <c r="X462" s="17" t="inlineStr">
+      <c r="X462" s="12" t="inlineStr">
         <is>
           <t>194</t>
         </is>
@@ -81271,7 +81263,7 @@
           <t>544</t>
         </is>
       </c>
-      <c r="D466" s="17" t="inlineStr">
+      <c r="D466" s="5" t="inlineStr">
         <is>
           <t>419</t>
         </is>
@@ -81887,7 +81879,7 @@
           <t>223</t>
         </is>
       </c>
-      <c r="O469" s="17" t="inlineStr">
+      <c r="O469" s="9" t="inlineStr">
         <is>
           <t>491</t>
         </is>
@@ -82089,7 +82081,7 @@
           <t>134</t>
         </is>
       </c>
-      <c r="R470" s="17" t="inlineStr">
+      <c r="R470" s="10" t="inlineStr">
         <is>
           <t>491</t>
         </is>
@@ -82822,7 +82814,7 @@
           <t>764</t>
         </is>
       </c>
-      <c r="O474" s="17" t="inlineStr">
+      <c r="O474" s="9" t="inlineStr">
         <is>
           <t>914</t>
         </is>
@@ -83640,7 +83632,7 @@
           <t>066</t>
         </is>
       </c>
-      <c r="AC478" s="17" t="inlineStr">
+      <c r="AC478" s="14" t="inlineStr">
         <is>
           <t>941</t>
         </is>
@@ -85076,7 +85068,7 @@
           <t>887</t>
         </is>
       </c>
-      <c r="Q486" s="17" t="inlineStr">
+      <c r="Q486" s="10" t="inlineStr">
         <is>
           <t>194</t>
         </is>
@@ -88848,7 +88840,7 @@
           <t>725</t>
         </is>
       </c>
-      <c r="F509" s="17" t="inlineStr">
+      <c r="F509" s="6" t="inlineStr">
         <is>
           <t>419</t>
         </is>
@@ -91785,7 +91777,7 @@
           <t>783</t>
         </is>
       </c>
-      <c r="D533" s="17" t="inlineStr">
+      <c r="D533" s="5" t="inlineStr">
         <is>
           <t>941</t>
         </is>
@@ -91799,17 +91791,17 @@
       </c>
       <c r="B534" s="5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>294</t>
         </is>
       </c>
       <c r="C534" s="5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>114</t>
         </is>
       </c>
       <c r="D534" s="5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>020</t>
         </is>
       </c>
     </row>
@@ -91821,17 +91813,17 @@
       </c>
       <c r="B535" s="5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>930</t>
         </is>
       </c>
       <c r="C535" s="5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>925</t>
         </is>
       </c>
       <c r="D535" s="5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>113</t>
         </is>
       </c>
     </row>
@@ -91843,17 +91835,17 @@
       </c>
       <c r="B536" s="5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>039</t>
         </is>
       </c>
       <c r="C536" s="5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>904</t>
         </is>
       </c>
       <c r="D536" s="5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>733</t>
         </is>
       </c>
     </row>
@@ -91865,17 +91857,17 @@
       </c>
       <c r="B537" s="5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>157</t>
         </is>
       </c>
       <c r="C537" s="5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>267</t>
         </is>
       </c>
       <c r="D537" s="5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>824</t>
         </is>
       </c>
     </row>
@@ -91887,17 +91879,17 @@
       </c>
       <c r="B538" s="5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>309</t>
         </is>
       </c>
       <c r="C538" s="5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>152</t>
         </is>
       </c>
       <c r="D538" s="5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>668</t>
         </is>
       </c>
     </row>
@@ -91909,17 +91901,17 @@
       </c>
       <c r="B539" s="5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>750</t>
         </is>
       </c>
       <c r="C539" s="5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>445</t>
         </is>
       </c>
       <c r="D539" s="5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>101</t>
         </is>
       </c>
     </row>
@@ -91931,17 +91923,17 @@
       </c>
       <c r="B540" s="5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>806</t>
         </is>
       </c>
       <c r="C540" s="5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>275</t>
         </is>
       </c>
       <c r="D540" s="5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>508</t>
         </is>
       </c>
     </row>
@@ -91953,17 +91945,17 @@
       </c>
       <c r="B541" s="5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>255</t>
         </is>
       </c>
       <c r="C541" s="5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>986</t>
         </is>
       </c>
       <c r="D541" s="5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>932</t>
         </is>
       </c>
     </row>
@@ -91975,17 +91967,17 @@
       </c>
       <c r="B542" s="5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>156</t>
         </is>
       </c>
       <c r="C542" s="5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>366</t>
         </is>
       </c>
       <c r="D542" s="5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>498</t>
         </is>
       </c>
     </row>
@@ -91997,7 +91989,7 @@
       </c>
       <c r="B543" s="5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>730</t>
         </is>
       </c>
       <c r="C543" s="5" t="inlineStr">

</xml_diff>

<commit_message>
update results; fix input filter for excel results
</commit_message>
<xml_diff>
--- a/swertres/excel_results.xlsx
+++ b/swertres/excel_results.xlsx
@@ -92082,12 +92082,12 @@
       </c>
       <c r="C547" s="5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>012</t>
         </is>
       </c>
       <c r="D547" s="5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>956</t>
         </is>
       </c>
     </row>
@@ -92099,17 +92099,17 @@
       </c>
       <c r="B548" s="5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>393</t>
         </is>
       </c>
       <c r="C548" s="5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>940</t>
         </is>
       </c>
       <c r="D548" s="5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>109</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
add another variation of the new giude
</commit_message>
<xml_diff>
--- a/swertres/excel_results.xlsx
+++ b/swertres/excel_results.xlsx
@@ -68,12 +68,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="006699ff"/>
+        <fgColor rgb="00FFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FFFFFF"/>
+        <fgColor rgb="006699ff"/>
       </patternFill>
     </fill>
     <fill>
@@ -235,7 +235,7 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
@@ -253,7 +253,7 @@
     <xf numFmtId="0" fontId="1" fillId="14" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1548,7 +1548,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="AE6" s="17" t="inlineStr">
+      <c r="AE6" s="14" t="inlineStr">
         <is>
           <t>618</t>
         </is>
@@ -2857,7 +2857,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="AE13" s="17" t="inlineStr">
+      <c r="AE13" s="14" t="inlineStr">
         <is>
           <t>861</t>
         </is>
@@ -3949,7 +3949,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="Y19" s="17" t="inlineStr">
+      <c r="Y19" s="12" t="inlineStr">
         <is>
           <t>681</t>
         </is>
@@ -4121,7 +4121,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="V20" s="17" t="inlineStr">
+      <c r="V20" s="11" t="inlineStr">
         <is>
           <t>168</t>
         </is>
@@ -4854,7 +4854,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="S24" s="10" t="inlineStr">
+      <c r="S24" s="17" t="inlineStr">
         <is>
           <t>377</t>
         </is>
@@ -6943,7 +6943,7 @@
           <t>941</t>
         </is>
       </c>
-      <c r="H38" s="17" t="inlineStr">
+      <c r="H38" s="7" t="inlineStr">
         <is>
           <t>861</t>
         </is>
@@ -7115,7 +7115,7 @@
           <t>367</t>
         </is>
       </c>
-      <c r="E39" s="17" t="inlineStr">
+      <c r="E39" s="6" t="inlineStr">
         <is>
           <t>816</t>
         </is>
@@ -8606,7 +8606,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="D47" s="17" t="inlineStr">
+      <c r="D47" s="5" t="inlineStr">
         <is>
           <t>168</t>
         </is>
@@ -9691,7 +9691,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="AH52" s="15" t="inlineStr">
+      <c r="AH52" s="17" t="inlineStr">
         <is>
           <t>377</t>
         </is>
@@ -10349,12 +10349,12 @@
           <t>-</t>
         </is>
       </c>
-      <c r="P56" s="9" t="inlineStr">
+      <c r="P56" s="17" t="inlineStr">
         <is>
           <t>773</t>
         </is>
       </c>
-      <c r="Q56" s="17" t="inlineStr">
+      <c r="Q56" s="10" t="inlineStr">
         <is>
           <t>618</t>
         </is>
@@ -11269,7 +11269,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="M61" s="17" t="inlineStr">
+      <c r="M61" s="8" t="inlineStr">
         <is>
           <t>186</t>
         </is>
@@ -11304,7 +11304,7 @@
           <t>090</t>
         </is>
       </c>
-      <c r="T61" s="17" t="inlineStr">
+      <c r="T61" s="11" t="inlineStr">
         <is>
           <t>618</t>
         </is>
@@ -11551,7 +11551,7 @@
           <t>225</t>
         </is>
       </c>
-      <c r="AF62" s="17" t="inlineStr">
+      <c r="AF62" s="15" t="inlineStr">
         <is>
           <t>618</t>
         </is>
@@ -12299,7 +12299,7 @@
           <t>607</t>
         </is>
       </c>
-      <c r="AF66" s="15" t="inlineStr">
+      <c r="AF66" s="17" t="inlineStr">
         <is>
           <t>773</t>
         </is>
@@ -13493,7 +13493,7 @@
           <t>119</t>
         </is>
       </c>
-      <c r="AC75" s="14" t="inlineStr">
+      <c r="AC75" s="17" t="inlineStr">
         <is>
           <t>773</t>
         </is>
@@ -13892,7 +13892,7 @@
           <t>565</t>
         </is>
       </c>
-      <c r="AH77" s="17" t="inlineStr">
+      <c r="AH77" s="15" t="inlineStr">
         <is>
           <t>168</t>
         </is>
@@ -14767,7 +14767,7 @@
           <t>598</t>
         </is>
       </c>
-      <c r="V82" s="17" t="inlineStr">
+      <c r="V82" s="11" t="inlineStr">
         <is>
           <t>618</t>
         </is>
@@ -14974,7 +14974,7 @@
           <t>274</t>
         </is>
       </c>
-      <c r="Z83" s="17" t="inlineStr">
+      <c r="Z83" s="13" t="inlineStr">
         <is>
           <t>816</t>
         </is>
@@ -15333,7 +15333,7 @@
           <t>936</t>
         </is>
       </c>
-      <c r="W85" s="17" t="inlineStr">
+      <c r="W85" s="12" t="inlineStr">
         <is>
           <t>168</t>
         </is>
@@ -17188,7 +17188,7 @@
           <t>764</t>
         </is>
       </c>
-      <c r="T95" s="17" t="inlineStr">
+      <c r="T95" s="11" t="inlineStr">
         <is>
           <t>681</t>
         </is>
@@ -17415,7 +17415,7 @@
           <t>031</t>
         </is>
       </c>
-      <c r="AB96" s="17" t="inlineStr">
+      <c r="AB96" s="13" t="inlineStr">
         <is>
           <t>168</t>
         </is>
@@ -18769,7 +18769,7 @@
           <t>107</t>
         </is>
       </c>
-      <c r="AK103" s="16" t="inlineStr">
+      <c r="AK103" s="17" t="inlineStr">
         <is>
           <t>737</t>
         </is>
@@ -19220,7 +19220,7 @@
           <t>412</t>
         </is>
       </c>
-      <c r="AI108" s="17" t="inlineStr">
+      <c r="AI108" s="16" t="inlineStr">
         <is>
           <t>168</t>
         </is>
@@ -19948,7 +19948,7 @@
           <t>105</t>
         </is>
       </c>
-      <c r="AE112" s="17" t="inlineStr">
+      <c r="AE112" s="14" t="inlineStr">
         <is>
           <t>168</t>
         </is>
@@ -20394,7 +20394,7 @@
           <t>478</t>
         </is>
       </c>
-      <c r="H115" s="7" t="inlineStr">
+      <c r="H115" s="17" t="inlineStr">
         <is>
           <t>377</t>
         </is>
@@ -21606,7 +21606,7 @@
           <t>359</t>
         </is>
       </c>
-      <c r="Z121" s="17" t="inlineStr">
+      <c r="Z121" s="13" t="inlineStr">
         <is>
           <t>186</t>
         </is>
@@ -21656,7 +21656,7 @@
           <t>856</t>
         </is>
       </c>
-      <c r="AJ121" s="17" t="inlineStr">
+      <c r="AJ121" s="16" t="inlineStr">
         <is>
           <t>681</t>
         </is>
@@ -22890,7 +22890,7 @@
           <t>565</t>
         </is>
       </c>
-      <c r="U128" s="11" t="inlineStr">
+      <c r="U128" s="17" t="inlineStr">
         <is>
           <t>377</t>
         </is>
@@ -22945,7 +22945,7 @@
           <t>814</t>
         </is>
       </c>
-      <c r="AF128" s="17" t="inlineStr">
+      <c r="AF128" s="15" t="inlineStr">
         <is>
           <t>861</t>
         </is>
@@ -23254,7 +23254,7 @@
           <t>007</t>
         </is>
       </c>
-      <c r="S130" s="17" t="inlineStr">
+      <c r="S130" s="10" t="inlineStr">
         <is>
           <t>816</t>
         </is>
@@ -25296,7 +25296,7 @@
           <t>124</t>
         </is>
       </c>
-      <c r="AJ143" s="17" t="inlineStr">
+      <c r="AJ143" s="16" t="inlineStr">
         <is>
           <t>816</t>
         </is>
@@ -25792,7 +25792,7 @@
           <t>662</t>
         </is>
       </c>
-      <c r="W146" s="17" t="inlineStr">
+      <c r="W146" s="12" t="inlineStr">
         <is>
           <t>618</t>
         </is>
@@ -26061,7 +26061,7 @@
           <t>06</t>
         </is>
       </c>
-      <c r="B148" s="17" t="inlineStr">
+      <c r="B148" s="5" t="inlineStr">
         <is>
           <t>861</t>
         </is>
@@ -26136,12 +26136,12 @@
           <t>573</t>
         </is>
       </c>
-      <c r="Q148" s="10" t="inlineStr">
+      <c r="Q148" s="17" t="inlineStr">
         <is>
           <t>377</t>
         </is>
       </c>
-      <c r="R148" s="17" t="inlineStr">
+      <c r="R148" s="10" t="inlineStr">
         <is>
           <t>618</t>
         </is>
@@ -26687,7 +26687,7 @@
           <t>490</t>
         </is>
       </c>
-      <c r="O151" s="9" t="inlineStr">
+      <c r="O151" s="17" t="inlineStr">
         <is>
           <t>773</t>
         </is>
@@ -27652,7 +27652,7 @@
           <t>395</t>
         </is>
       </c>
-      <c r="U156" s="11" t="inlineStr">
+      <c r="U156" s="17" t="inlineStr">
         <is>
           <t>377</t>
         </is>
@@ -27784,7 +27784,7 @@
           <t>985</t>
         </is>
       </c>
-      <c r="J157" s="7" t="inlineStr">
+      <c r="J157" s="17" t="inlineStr">
         <is>
           <t>773</t>
         </is>
@@ -27936,7 +27936,7 @@
           <t>932</t>
         </is>
       </c>
-      <c r="C158" s="5" t="inlineStr">
+      <c r="C158" s="17" t="inlineStr">
         <is>
           <t>737</t>
         </is>
@@ -28118,7 +28118,7 @@
           <t>17</t>
         </is>
       </c>
-      <c r="B159" s="17" t="inlineStr">
+      <c r="B159" s="5" t="inlineStr">
         <is>
           <t>186</t>
         </is>
@@ -28627,7 +28627,7 @@
           <t>179</t>
         </is>
       </c>
-      <c r="AC161" s="14" t="inlineStr">
+      <c r="AC161" s="17" t="inlineStr">
         <is>
           <t>737</t>
         </is>
@@ -29118,7 +29118,7 @@
           <t>098</t>
         </is>
       </c>
-      <c r="O164" s="17" t="inlineStr">
+      <c r="O164" s="9" t="inlineStr">
         <is>
           <t>681</t>
         </is>
@@ -30118,7 +30118,7 @@
           <t>996</t>
         </is>
       </c>
-      <c r="AB169" s="13" t="inlineStr">
+      <c r="AB169" s="17" t="inlineStr">
         <is>
           <t>773</t>
         </is>
@@ -30881,7 +30881,7 @@
           <t>094</t>
         </is>
       </c>
-      <c r="AE173" s="17" t="inlineStr">
+      <c r="AE173" s="14" t="inlineStr">
         <is>
           <t>186</t>
         </is>
@@ -32950,7 +32950,7 @@
           <t>989</t>
         </is>
       </c>
-      <c r="P187" s="17" t="inlineStr">
+      <c r="P187" s="9" t="inlineStr">
         <is>
           <t>618</t>
         </is>
@@ -33122,7 +33122,7 @@
           <t>610</t>
         </is>
       </c>
-      <c r="M188" s="8" t="inlineStr">
+      <c r="M188" s="17" t="inlineStr">
         <is>
           <t>377</t>
         </is>
@@ -33187,7 +33187,7 @@
           <t>957</t>
         </is>
       </c>
-      <c r="Z188" s="17" t="inlineStr">
+      <c r="Z188" s="13" t="inlineStr">
         <is>
           <t>681</t>
         </is>
@@ -33683,7 +33683,7 @@
           <t>232</t>
         </is>
       </c>
-      <c r="M191" s="17" t="inlineStr">
+      <c r="M191" s="8" t="inlineStr">
         <is>
           <t>186</t>
         </is>
@@ -34027,7 +34027,7 @@
           <t>027</t>
         </is>
       </c>
-      <c r="G193" s="17" t="inlineStr">
+      <c r="G193" s="6" t="inlineStr">
         <is>
           <t>168</t>
         </is>
@@ -34920,7 +34920,7 @@
           <t>502</t>
         </is>
       </c>
-      <c r="AJ197" s="16" t="inlineStr">
+      <c r="AJ197" s="17" t="inlineStr">
         <is>
           <t>773</t>
         </is>
@@ -36421,7 +36421,7 @@
           <t>749</t>
         </is>
       </c>
-      <c r="AK205" s="16" t="inlineStr">
+      <c r="AK205" s="17" t="inlineStr">
         <is>
           <t>773</t>
         </is>
@@ -36690,12 +36690,12 @@
           <t>355</t>
         </is>
       </c>
-      <c r="P207" s="17" t="inlineStr">
+      <c r="P207" s="9" t="inlineStr">
         <is>
           <t>618</t>
         </is>
       </c>
-      <c r="Q207" s="17" t="inlineStr">
+      <c r="Q207" s="10" t="inlineStr">
         <is>
           <t>816</t>
         </is>
@@ -37418,7 +37418,7 @@
           <t>197</t>
         </is>
       </c>
-      <c r="AF213" s="15" t="inlineStr">
+      <c r="AF213" s="17" t="inlineStr">
         <is>
           <t>737</t>
         </is>
@@ -37540,7 +37540,7 @@
           <t>571</t>
         </is>
       </c>
-      <c r="S214" s="17" t="inlineStr">
+      <c r="S214" s="10" t="inlineStr">
         <is>
           <t>186</t>
         </is>
@@ -38490,7 +38490,7 @@
           <t>352</t>
         </is>
       </c>
-      <c r="V219" s="11" t="inlineStr">
+      <c r="V219" s="17" t="inlineStr">
         <is>
           <t>377</t>
         </is>
@@ -39111,7 +39111,7 @@
           <t>287</t>
         </is>
       </c>
-      <c r="AH222" s="17" t="inlineStr">
+      <c r="AH222" s="15" t="inlineStr">
         <is>
           <t>186</t>
         </is>
@@ -39485,7 +39485,7 @@
           <t>921</t>
         </is>
       </c>
-      <c r="AH224" s="17" t="inlineStr">
+      <c r="AH224" s="15" t="inlineStr">
         <is>
           <t>681</t>
         </is>
@@ -39874,7 +39874,7 @@
           <t>207</t>
         </is>
       </c>
-      <c r="AK226" s="16" t="inlineStr">
+      <c r="AK226" s="17" t="inlineStr">
         <is>
           <t>377</t>
         </is>
@@ -40951,7 +40951,7 @@
           <t>414</t>
         </is>
       </c>
-      <c r="AB232" s="17" t="inlineStr">
+      <c r="AB232" s="13" t="inlineStr">
         <is>
           <t>861</t>
         </is>
@@ -41694,7 +41694,7 @@
           <t>814</t>
         </is>
       </c>
-      <c r="AA236" s="17" t="inlineStr">
+      <c r="AA236" s="13" t="inlineStr">
         <is>
           <t>681</t>
         </is>
@@ -41831,7 +41831,7 @@
           <t>040</t>
         </is>
       </c>
-      <c r="Q237" s="17" t="inlineStr">
+      <c r="Q237" s="10" t="inlineStr">
         <is>
           <t>186</t>
         </is>
@@ -41978,7 +41978,7 @@
           <t>646</t>
         </is>
       </c>
-      <c r="I238" s="17" t="inlineStr">
+      <c r="I238" s="7" t="inlineStr">
         <is>
           <t>186</t>
         </is>
@@ -43494,7 +43494,7 @@
           <t>272</t>
         </is>
       </c>
-      <c r="AG248" s="17" t="inlineStr">
+      <c r="AG248" s="15" t="inlineStr">
         <is>
           <t>186</t>
         </is>
@@ -43915,7 +43915,7 @@
           <t>886</t>
         </is>
       </c>
-      <c r="E251" s="17" t="inlineStr">
+      <c r="E251" s="6" t="inlineStr">
         <is>
           <t>681</t>
         </is>
@@ -44279,7 +44279,7 @@
           <t>620</t>
         </is>
       </c>
-      <c r="C253" s="5" t="inlineStr">
+      <c r="C253" s="17" t="inlineStr">
         <is>
           <t>737</t>
         </is>
@@ -45112,7 +45112,7 @@
           <t>361</t>
         </is>
       </c>
-      <c r="T257" s="17" t="inlineStr">
+      <c r="T257" s="11" t="inlineStr">
         <is>
           <t>681</t>
         </is>
@@ -46401,7 +46401,7 @@
           <t>940</t>
         </is>
       </c>
-      <c r="P264" s="9" t="inlineStr">
+      <c r="P264" s="17" t="inlineStr">
         <is>
           <t>773</t>
         </is>
@@ -46820,7 +46820,7 @@
           <t>143</t>
         </is>
       </c>
-      <c r="Y266" s="12" t="inlineStr">
+      <c r="Y266" s="17" t="inlineStr">
         <is>
           <t>773</t>
         </is>
@@ -46927,7 +46927,7 @@
           <t>783</t>
         </is>
       </c>
-      <c r="I267" s="17" t="inlineStr">
+      <c r="I267" s="7" t="inlineStr">
         <is>
           <t>816</t>
         </is>
@@ -47371,7 +47371,7 @@
           <t>011</t>
         </is>
       </c>
-      <c r="W269" s="17" t="inlineStr">
+      <c r="W269" s="12" t="inlineStr">
         <is>
           <t>618</t>
         </is>
@@ -47640,7 +47640,7 @@
           <t>24</t>
         </is>
       </c>
-      <c r="B271" s="5" t="inlineStr">
+      <c r="B271" s="17" t="inlineStr">
         <is>
           <t>737</t>
         </is>
@@ -48266,7 +48266,7 @@
           <t>191</t>
         </is>
       </c>
-      <c r="O274" s="17" t="inlineStr">
+      <c r="O274" s="9" t="inlineStr">
         <is>
           <t>186</t>
         </is>
@@ -48443,7 +48443,7 @@
           <t>714</t>
         </is>
       </c>
-      <c r="M275" s="8" t="inlineStr">
+      <c r="M275" s="17" t="inlineStr">
         <is>
           <t>773</t>
         </is>
@@ -50036,7 +50036,7 @@
           <t>837</t>
         </is>
       </c>
-      <c r="O286" s="17" t="inlineStr">
+      <c r="O286" s="9" t="inlineStr">
         <is>
           <t>618</t>
         </is>
@@ -50911,7 +50911,7 @@
           <t>132</t>
         </is>
       </c>
-      <c r="C291" s="17" t="inlineStr">
+      <c r="C291" s="5" t="inlineStr">
         <is>
           <t>618</t>
         </is>
@@ -51036,7 +51036,7 @@
           <t>507</t>
         </is>
       </c>
-      <c r="AB291" s="17" t="inlineStr">
+      <c r="AB291" s="13" t="inlineStr">
         <is>
           <t>168</t>
         </is>
@@ -51592,7 +51592,7 @@
           <t>957</t>
         </is>
       </c>
-      <c r="AA294" s="17" t="inlineStr">
+      <c r="AA294" s="13" t="inlineStr">
         <is>
           <t>861</t>
         </is>
@@ -52629,7 +52629,7 @@
           <t>185</t>
         </is>
       </c>
-      <c r="J300" s="17" t="inlineStr">
+      <c r="J300" s="7" t="inlineStr">
         <is>
           <t>861</t>
         </is>
@@ -53255,7 +53255,7 @@
           <t>891</t>
         </is>
       </c>
-      <c r="W303" s="17" t="inlineStr">
+      <c r="W303" s="12" t="inlineStr">
         <is>
           <t>816</t>
         </is>
@@ -54220,7 +54220,7 @@
           <t>371</t>
         </is>
       </c>
-      <c r="AC308" s="17" t="inlineStr">
+      <c r="AC308" s="14" t="inlineStr">
         <is>
           <t>816</t>
         </is>
@@ -54479,7 +54479,7 @@
           <t>525</t>
         </is>
       </c>
-      <c r="F310" s="6" t="inlineStr">
+      <c r="F310" s="17" t="inlineStr">
         <is>
           <t>737</t>
         </is>
@@ -54489,7 +54489,7 @@
           <t>563</t>
         </is>
       </c>
-      <c r="H310" s="17" t="inlineStr">
+      <c r="H310" s="7" t="inlineStr">
         <is>
           <t>816</t>
         </is>
@@ -55020,7 +55020,7 @@
           <t>31</t>
         </is>
       </c>
-      <c r="B313" s="5" t="inlineStr">
+      <c r="B313" s="17" t="inlineStr">
         <is>
           <t>737</t>
         </is>
@@ -56132,7 +56132,7 @@
           <t>691</t>
         </is>
       </c>
-      <c r="T321" s="17" t="inlineStr">
+      <c r="T321" s="11" t="inlineStr">
         <is>
           <t>816</t>
         </is>
@@ -56536,7 +56536,7 @@
           <t>704</t>
         </is>
       </c>
-      <c r="Z323" s="17" t="inlineStr">
+      <c r="Z323" s="13" t="inlineStr">
         <is>
           <t>618</t>
         </is>
@@ -56895,7 +56895,7 @@
           <t>925</t>
         </is>
       </c>
-      <c r="W325" s="12" t="inlineStr">
+      <c r="W325" s="17" t="inlineStr">
         <is>
           <t>737</t>
         </is>
@@ -57147,7 +57147,7 @@
           <t>745</t>
         </is>
       </c>
-      <c r="AJ326" s="17" t="inlineStr">
+      <c r="AJ326" s="16" t="inlineStr">
         <is>
           <t>618</t>
         </is>
@@ -57568,7 +57568,7 @@
           <t>663</t>
         </is>
       </c>
-      <c r="H329" s="17" t="inlineStr">
+      <c r="H329" s="7" t="inlineStr">
         <is>
           <t>618</t>
         </is>
@@ -58179,7 +58179,7 @@
           <t>542</t>
         </is>
       </c>
-      <c r="R332" s="10" t="inlineStr">
+      <c r="R332" s="17" t="inlineStr">
         <is>
           <t>737</t>
         </is>
@@ -58381,7 +58381,7 @@
           <t>300</t>
         </is>
       </c>
-      <c r="U333" s="11" t="inlineStr">
+      <c r="U333" s="17" t="inlineStr">
         <is>
           <t>737</t>
         </is>
@@ -58401,7 +58401,7 @@
           <t>315</t>
         </is>
       </c>
-      <c r="Y333" s="12" t="inlineStr">
+      <c r="Y333" s="17" t="inlineStr">
         <is>
           <t>773</t>
         </is>
@@ -58488,7 +58488,7 @@
           <t>458</t>
         </is>
       </c>
-      <c r="E334" s="6" t="inlineStr">
+      <c r="E334" s="17" t="inlineStr">
         <is>
           <t>773</t>
         </is>
@@ -58685,7 +58685,7 @@
           <t>910</t>
         </is>
       </c>
-      <c r="G335" s="6" t="inlineStr">
+      <c r="G335" s="17" t="inlineStr">
         <is>
           <t>773</t>
         </is>
@@ -58982,7 +58982,7 @@
           <t>311</t>
         </is>
       </c>
-      <c r="AC336" s="17" t="inlineStr">
+      <c r="AC336" s="14" t="inlineStr">
         <is>
           <t>186</t>
         </is>
@@ -59443,7 +59443,7 @@
           <t>224</t>
         </is>
       </c>
-      <c r="I339" s="7" t="inlineStr">
+      <c r="I339" s="17" t="inlineStr">
         <is>
           <t>377</t>
         </is>
@@ -60206,7 +60206,7 @@
           <t>484</t>
         </is>
       </c>
-      <c r="L343" s="8" t="inlineStr">
+      <c r="L343" s="17" t="inlineStr">
         <is>
           <t>773</t>
         </is>
@@ -60685,7 +60685,7 @@
           <t>952</t>
         </is>
       </c>
-      <c r="AG345" s="17" t="inlineStr">
+      <c r="AG345" s="15" t="inlineStr">
         <is>
           <t>816</t>
         </is>
@@ -60989,7 +60989,7 @@
           <t>569</t>
         </is>
       </c>
-      <c r="S347" s="17" t="inlineStr">
+      <c r="S347" s="10" t="inlineStr">
         <is>
           <t>168</t>
         </is>
@@ -61717,7 +61717,7 @@
           <t>288</t>
         </is>
       </c>
-      <c r="AI353" s="16" t="inlineStr">
+      <c r="AI353" s="17" t="inlineStr">
         <is>
           <t>377</t>
         </is>
@@ -61956,7 +61956,7 @@
           <t>455</t>
         </is>
       </c>
-      <c r="H355" s="7" t="inlineStr">
+      <c r="H355" s="17" t="inlineStr">
         <is>
           <t>377</t>
         </is>
@@ -62492,7 +62492,7 @@
           <t>341</t>
         </is>
       </c>
-      <c r="C358" s="5" t="inlineStr">
+      <c r="C358" s="17" t="inlineStr">
         <is>
           <t>377</t>
         </is>
@@ -63128,7 +63128,7 @@
           <t>029</t>
         </is>
       </c>
-      <c r="R361" s="17" t="inlineStr">
+      <c r="R361" s="10" t="inlineStr">
         <is>
           <t>816</t>
         </is>
@@ -63447,7 +63447,7 @@
           <t>279</t>
         </is>
       </c>
-      <c r="G363" s="6" t="inlineStr">
+      <c r="G363" s="17" t="inlineStr">
         <is>
           <t>377</t>
         </is>
@@ -64806,7 +64806,7 @@
           <t>472</t>
         </is>
       </c>
-      <c r="Q370" s="17" t="inlineStr">
+      <c r="Q370" s="10" t="inlineStr">
         <is>
           <t>618</t>
         </is>
@@ -65457,7 +65457,7 @@
           <t>470</t>
         </is>
       </c>
-      <c r="AI373" s="16" t="inlineStr">
+      <c r="AI373" s="17" t="inlineStr">
         <is>
           <t>737</t>
         </is>
@@ -65494,7 +65494,7 @@
           <t>386</t>
         </is>
       </c>
-      <c r="E374" s="17" t="inlineStr">
+      <c r="E374" s="6" t="inlineStr">
         <is>
           <t>816</t>
         </is>
@@ -66579,7 +66579,7 @@
           <t>498</t>
         </is>
       </c>
-      <c r="AI379" s="17" t="inlineStr">
+      <c r="AI379" s="16" t="inlineStr">
         <is>
           <t>861</t>
         </is>
@@ -66903,7 +66903,7 @@
           <t>176</t>
         </is>
       </c>
-      <c r="Y381" s="17" t="inlineStr">
+      <c r="Y381" s="12" t="inlineStr">
         <is>
           <t>186</t>
         </is>
@@ -67262,7 +67262,7 @@
           <t>341</t>
         </is>
       </c>
-      <c r="V383" s="17" t="inlineStr">
+      <c r="V383" s="11" t="inlineStr">
         <is>
           <t>618</t>
         </is>
@@ -67910,7 +67910,7 @@
           <t>289</t>
         </is>
       </c>
-      <c r="V389" s="17" t="inlineStr">
+      <c r="V389" s="11" t="inlineStr">
         <is>
           <t>816</t>
         </is>
@@ -68573,7 +68573,7 @@
           <t>029</t>
         </is>
       </c>
-      <c r="E393" s="17" t="inlineStr">
+      <c r="E393" s="6" t="inlineStr">
         <is>
           <t>168</t>
         </is>
@@ -68875,7 +68875,7 @@
           <t>855</t>
         </is>
       </c>
-      <c r="AB394" s="13" t="inlineStr">
+      <c r="AB394" s="17" t="inlineStr">
         <is>
           <t>377</t>
         </is>
@@ -69007,7 +69007,7 @@
           <t>250</t>
         </is>
       </c>
-      <c r="Q395" s="10" t="inlineStr">
+      <c r="Q395" s="17" t="inlineStr">
         <is>
           <t>773</t>
         </is>
@@ -69062,7 +69062,7 @@
           <t>464</t>
         </is>
       </c>
-      <c r="AB395" s="17" t="inlineStr">
+      <c r="AB395" s="13" t="inlineStr">
         <is>
           <t>168</t>
         </is>
@@ -70149,7 +70149,7 @@
           <t>543</t>
         </is>
       </c>
-      <c r="U401" s="11" t="inlineStr">
+      <c r="U401" s="17" t="inlineStr">
         <is>
           <t>773</t>
         </is>
@@ -70735,7 +70735,7 @@
           <t>754</t>
         </is>
       </c>
-      <c r="Z404" s="17" t="inlineStr">
+      <c r="Z404" s="13" t="inlineStr">
         <is>
           <t>681</t>
         </is>
@@ -70952,7 +70952,7 @@
           <t>420</t>
         </is>
       </c>
-      <c r="AF405" s="17" t="inlineStr">
+      <c r="AF405" s="15" t="inlineStr">
         <is>
           <t>168</t>
         </is>
@@ -71024,7 +71024,7 @@
           <t>733</t>
         </is>
       </c>
-      <c r="I406" s="17" t="inlineStr">
+      <c r="I406" s="7" t="inlineStr">
         <is>
           <t>681</t>
         </is>
@@ -71523,7 +71523,7 @@
           <t>525</t>
         </is>
       </c>
-      <c r="AH408" s="17" t="inlineStr">
+      <c r="AH408" s="15" t="inlineStr">
         <is>
           <t>618</t>
         </is>
@@ -71625,7 +71625,7 @@
           <t>202</t>
         </is>
       </c>
-      <c r="Q409" s="17" t="inlineStr">
+      <c r="Q409" s="10" t="inlineStr">
         <is>
           <t>618</t>
         </is>
@@ -72707,7 +72707,7 @@
           <t>976</t>
         </is>
       </c>
-      <c r="I415" s="17" t="inlineStr">
+      <c r="I415" s="7" t="inlineStr">
         <is>
           <t>861</t>
         </is>
@@ -73211,7 +73211,7 @@
           <t>193</t>
         </is>
       </c>
-      <c r="AI417" s="17" t="inlineStr">
+      <c r="AI417" s="16" t="inlineStr">
         <is>
           <t>186</t>
         </is>
@@ -75786,7 +75786,7 @@
           <t>563</t>
         </is>
       </c>
-      <c r="I434" s="7" t="inlineStr">
+      <c r="I434" s="17" t="inlineStr">
         <is>
           <t>377</t>
         </is>
@@ -77180,7 +77180,7 @@
           <t>960</t>
         </is>
       </c>
-      <c r="Z441" s="13" t="inlineStr">
+      <c r="Z441" s="17" t="inlineStr">
         <is>
           <t>773</t>
         </is>
@@ -77272,7 +77272,7 @@
           <t>328</t>
         </is>
       </c>
-      <c r="G442" s="6" t="inlineStr">
+      <c r="G442" s="17" t="inlineStr">
         <is>
           <t>377</t>
         </is>
@@ -77514,7 +77514,7 @@
           <t>877</t>
         </is>
       </c>
-      <c r="R443" s="17" t="inlineStr">
+      <c r="R443" s="10" t="inlineStr">
         <is>
           <t>186</t>
         </is>
@@ -78711,7 +78711,7 @@
           <t>985</t>
         </is>
       </c>
-      <c r="AG449" s="15" t="inlineStr">
+      <c r="AG449" s="17" t="inlineStr">
         <is>
           <t>737</t>
         </is>
@@ -80356,7 +80356,7 @@
           <t>302</t>
         </is>
       </c>
-      <c r="H461" s="17" t="inlineStr">
+      <c r="H461" s="7" t="inlineStr">
         <is>
           <t>861</t>
         </is>
@@ -82261,7 +82261,7 @@
           <t>427</t>
         </is>
       </c>
-      <c r="O471" s="9" t="inlineStr">
+      <c r="O471" s="17" t="inlineStr">
         <is>
           <t>377</t>
         </is>
@@ -82757,7 +82757,7 @@
           <t>17</t>
         </is>
       </c>
-      <c r="B474" s="5" t="inlineStr">
+      <c r="B474" s="17" t="inlineStr">
         <is>
           <t>377</t>
         </is>
@@ -82902,7 +82902,7 @@
           <t>375</t>
         </is>
       </c>
-      <c r="AE474" s="17" t="inlineStr">
+      <c r="AE474" s="14" t="inlineStr">
         <is>
           <t>681</t>
         </is>
@@ -82912,7 +82912,7 @@
           <t>846</t>
         </is>
       </c>
-      <c r="AG474" s="15" t="inlineStr">
+      <c r="AG474" s="17" t="inlineStr">
         <is>
           <t>773</t>
         </is>
@@ -83767,7 +83767,7 @@
           <t>184</t>
         </is>
       </c>
-      <c r="Q479" s="17" t="inlineStr">
+      <c r="Q479" s="10" t="inlineStr">
         <is>
           <t>861</t>
         </is>
@@ -84091,7 +84091,7 @@
           <t>112</t>
         </is>
       </c>
-      <c r="G481" s="17" t="inlineStr">
+      <c r="G481" s="6" t="inlineStr">
         <is>
           <t>186</t>
         </is>
@@ -84570,7 +84570,7 @@
           <t>333</t>
         </is>
       </c>
-      <c r="AB483" s="17" t="inlineStr">
+      <c r="AB483" s="13" t="inlineStr">
         <is>
           <t>681</t>
         </is>
@@ -85126,12 +85126,12 @@
           <t>119</t>
         </is>
       </c>
-      <c r="AA486" s="13" t="inlineStr">
+      <c r="AA486" s="17" t="inlineStr">
         <is>
           <t>377</t>
         </is>
       </c>
-      <c r="AB486" s="13" t="inlineStr">
+      <c r="AB486" s="17" t="inlineStr">
         <is>
           <t>773</t>
         </is>
@@ -85375,7 +85375,7 @@
           <t>31</t>
         </is>
       </c>
-      <c r="B488" s="17" t="inlineStr">
+      <c r="B488" s="5" t="inlineStr">
         <is>
           <t>186</t>
         </is>
@@ -88454,7 +88454,7 @@
           <t>15</t>
         </is>
       </c>
-      <c r="B507" s="5" t="inlineStr">
+      <c r="B507" s="17" t="inlineStr">
         <is>
           <t>773</t>
         </is>
@@ -89170,7 +89170,7 @@
           <t>248</t>
         </is>
       </c>
-      <c r="AG510" s="17" t="inlineStr">
+      <c r="AG510" s="15" t="inlineStr">
         <is>
           <t>168</t>
         </is>
@@ -89322,7 +89322,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="Z511" s="13" t="inlineStr">
+      <c r="Z511" s="17" t="inlineStr">
         <is>
           <t>737</t>
         </is>
@@ -91451,7 +91451,7 @@
           <t>094</t>
         </is>
       </c>
-      <c r="C523" s="5" t="inlineStr">
+      <c r="C523" s="17" t="inlineStr">
         <is>
           <t>377</t>
         </is>
@@ -92146,7 +92146,7 @@
           <t>508</t>
         </is>
       </c>
-      <c r="E540" s="17" t="inlineStr">
+      <c r="E540" s="6" t="inlineStr">
         <is>
           <t>816</t>
         </is>
@@ -92188,7 +92188,7 @@
           <t>842</t>
         </is>
       </c>
-      <c r="F541" s="6" t="inlineStr">
+      <c r="F541" s="17" t="inlineStr">
         <is>
           <t>773</t>
         </is>

</xml_diff>

<commit_message>
update results with new pattern
</commit_message>
<xml_diff>
--- a/swertres/excel_results.xlsx
+++ b/swertres/excel_results.xlsx
@@ -92097,17 +92097,17 @@
       </c>
       <c r="H535" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>342</t>
         </is>
       </c>
       <c r="I535" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>251</t>
         </is>
       </c>
       <c r="J535" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>681</t>
         </is>
       </c>
     </row>
@@ -92149,17 +92149,17 @@
       </c>
       <c r="H536" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>124</t>
         </is>
       </c>
       <c r="I536" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>918</t>
         </is>
       </c>
       <c r="J536" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>363</t>
         </is>
       </c>
     </row>
@@ -92201,17 +92201,17 @@
       </c>
       <c r="H537" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>854</t>
         </is>
       </c>
       <c r="I537" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>930</t>
         </is>
       </c>
       <c r="J537" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>607</t>
         </is>
       </c>
     </row>
@@ -92253,17 +92253,17 @@
       </c>
       <c r="H538" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>920</t>
         </is>
       </c>
       <c r="I538" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>962</t>
         </is>
       </c>
       <c r="J538" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>811</t>
         </is>
       </c>
     </row>
@@ -92305,17 +92305,17 @@
       </c>
       <c r="H539" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>085</t>
         </is>
       </c>
       <c r="I539" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>659</t>
         </is>
       </c>
       <c r="J539" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>996</t>
         </is>
       </c>
     </row>
@@ -92357,17 +92357,17 @@
       </c>
       <c r="H540" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>676</t>
         </is>
       </c>
       <c r="I540" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>496</t>
         </is>
       </c>
       <c r="J540" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>442</t>
         </is>
       </c>
     </row>
@@ -92409,17 +92409,17 @@
       </c>
       <c r="H541" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>487</t>
         </is>
       </c>
       <c r="I541" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>095</t>
         </is>
       </c>
       <c r="J541" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>126</t>
         </is>
       </c>
     </row>
@@ -92461,17 +92461,17 @@
       </c>
       <c r="H542" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>356</t>
         </is>
       </c>
       <c r="I542" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>462</t>
         </is>
       </c>
       <c r="J542" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>950</t>
         </is>
       </c>
     </row>
@@ -92513,17 +92513,17 @@
       </c>
       <c r="H543" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>261</t>
         </is>
       </c>
       <c r="I543" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>196</t>
         </is>
       </c>
       <c r="J543" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>274</t>
         </is>
       </c>
     </row>
@@ -92565,17 +92565,17 @@
       </c>
       <c r="H544" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>339</t>
         </is>
       </c>
       <c r="I544" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>693</t>
         </is>
       </c>
       <c r="J544" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>584</t>
         </is>
       </c>
     </row>
@@ -92617,12 +92617,12 @@
       </c>
       <c r="H545" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>657</t>
         </is>
       </c>
       <c r="I545" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>336</t>
         </is>
       </c>
       <c r="J545" s="7" t="inlineStr">

</xml_diff>

<commit_message>
update results and more info on solid patterns
</commit_message>
<xml_diff>
--- a/swertres/excel_results.xlsx
+++ b/swertres/excel_results.xlsx
@@ -2782,7 +2782,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="P13" s="9" t="inlineStr">
+      <c r="P13" s="17" t="inlineStr">
         <is>
           <t>234</t>
         </is>
@@ -2827,7 +2827,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="Y13" s="17" t="inlineStr">
+      <c r="Y13" s="12" t="inlineStr">
         <is>
           <t>042</t>
         </is>
@@ -3807,7 +3807,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="AH18" s="15" t="inlineStr">
+      <c r="AH18" s="17" t="inlineStr">
         <is>
           <t>702</t>
         </is>
@@ -4368,7 +4368,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="AH21" s="15" t="inlineStr">
+      <c r="AH21" s="17" t="inlineStr">
         <is>
           <t>342</t>
         </is>
@@ -5011,7 +5011,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="M25" s="17" t="inlineStr">
+      <c r="M25" s="8" t="inlineStr">
         <is>
           <t>042</t>
         </is>
@@ -5198,7 +5198,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="M26" s="8" t="inlineStr">
+      <c r="M26" s="17" t="inlineStr">
         <is>
           <t>072</t>
         </is>
@@ -6928,7 +6928,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="E38" s="6" t="inlineStr">
+      <c r="E38" s="17" t="inlineStr">
         <is>
           <t>702</t>
         </is>
@@ -7170,7 +7170,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="P39" s="9" t="inlineStr">
+      <c r="P39" s="17" t="inlineStr">
         <is>
           <t>342</t>
         </is>
@@ -7736,7 +7736,7 @@
           <t>906</t>
         </is>
       </c>
-      <c r="Q42" s="17" t="inlineStr">
+      <c r="Q42" s="10" t="inlineStr">
         <is>
           <t>402</t>
         </is>
@@ -7953,7 +7953,7 @@
           <t>817</t>
         </is>
       </c>
-      <c r="W43" s="12" t="inlineStr">
+      <c r="W43" s="17" t="inlineStr">
         <is>
           <t>432</t>
         </is>
@@ -8357,7 +8357,7 @@
           <t>346</t>
         </is>
       </c>
-      <c r="AC45" s="14" t="inlineStr">
+      <c r="AC45" s="17" t="inlineStr">
         <is>
           <t>243</t>
         </is>
@@ -8479,7 +8479,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="P46" s="17" t="inlineStr">
+      <c r="P46" s="9" t="inlineStr">
         <is>
           <t>402</t>
         </is>
@@ -8636,7 +8636,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="J47" s="7" t="inlineStr">
+      <c r="J47" s="17" t="inlineStr">
         <is>
           <t>342</t>
         </is>
@@ -9172,7 +9172,7 @@
           <t>877</t>
         </is>
       </c>
-      <c r="E50" s="17" t="inlineStr">
+      <c r="E50" s="6" t="inlineStr">
         <is>
           <t>420</t>
         </is>
@@ -9504,7 +9504,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="AH51" s="15" t="inlineStr">
+      <c r="AH51" s="17" t="inlineStr">
         <is>
           <t>072</t>
         </is>
@@ -9743,7 +9743,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="G53" s="6" t="inlineStr">
+      <c r="G53" s="17" t="inlineStr">
         <is>
           <t>270</t>
         </is>
@@ -9758,7 +9758,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="J53" s="7" t="inlineStr">
+      <c r="J53" s="17" t="inlineStr">
         <is>
           <t>072</t>
         </is>
@@ -10092,7 +10092,7 @@
           <t>18</t>
         </is>
       </c>
-      <c r="B55" s="5" t="inlineStr">
+      <c r="B55" s="17" t="inlineStr">
         <is>
           <t>423</t>
         </is>
@@ -10384,7 +10384,7 @@
           <t>672</t>
         </is>
       </c>
-      <c r="W56" s="17" t="inlineStr">
+      <c r="W56" s="12" t="inlineStr">
         <is>
           <t>204</t>
         </is>
@@ -11015,7 +11015,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="AK59" s="16" t="inlineStr">
+      <c r="AK59" s="17" t="inlineStr">
         <is>
           <t>342</t>
         </is>
@@ -11132,7 +11132,7 @@
           <t>130</t>
         </is>
       </c>
-      <c r="W60" s="12" t="inlineStr">
+      <c r="W60" s="17" t="inlineStr">
         <is>
           <t>072</t>
         </is>
@@ -11319,7 +11319,7 @@
           <t>617</t>
         </is>
       </c>
-      <c r="W61" s="12" t="inlineStr">
+      <c r="W61" s="17" t="inlineStr">
         <is>
           <t>342</t>
         </is>
@@ -11940,7 +11940,7 @@
           <t>930</t>
         </is>
       </c>
-      <c r="AI64" s="16" t="inlineStr">
+      <c r="AI64" s="17" t="inlineStr">
         <is>
           <t>432</t>
         </is>
@@ -13276,7 +13276,7 @@
           <t>995</t>
         </is>
       </c>
-      <c r="W74" s="17" t="inlineStr">
+      <c r="W74" s="12" t="inlineStr">
         <is>
           <t>204</t>
         </is>
@@ -13635,7 +13635,7 @@
           <t>510</t>
         </is>
       </c>
-      <c r="T76" s="11" t="inlineStr">
+      <c r="T76" s="17" t="inlineStr">
         <is>
           <t>027</t>
         </is>
@@ -13715,7 +13715,7 @@
           <t>145</t>
         </is>
       </c>
-      <c r="AJ76" s="17" t="inlineStr">
+      <c r="AJ76" s="16" t="inlineStr">
         <is>
           <t>204</t>
         </is>
@@ -14171,12 +14171,12 @@
           <t>213</t>
         </is>
       </c>
-      <c r="O79" s="17" t="inlineStr">
+      <c r="O79" s="9" t="inlineStr">
         <is>
           <t>240</t>
         </is>
       </c>
-      <c r="P79" s="17" t="inlineStr">
+      <c r="P79" s="9" t="inlineStr">
         <is>
           <t>204</t>
         </is>
@@ -14827,7 +14827,7 @@
           <t>858</t>
         </is>
       </c>
-      <c r="AH82" s="15" t="inlineStr">
+      <c r="AH82" s="17" t="inlineStr">
         <is>
           <t>324</t>
         </is>
@@ -15667,7 +15667,7 @@
           <t>904</t>
         </is>
       </c>
-      <c r="O87" s="9" t="inlineStr">
+      <c r="O87" s="17" t="inlineStr">
         <is>
           <t>720</t>
         </is>
@@ -16263,7 +16263,7 @@
           <t>798</t>
         </is>
       </c>
-      <c r="V90" s="11" t="inlineStr">
+      <c r="V90" s="17" t="inlineStr">
         <is>
           <t>720</t>
         </is>
@@ -17749,7 +17749,7 @@
           <t>408</t>
         </is>
       </c>
-      <c r="T98" s="11" t="inlineStr">
+      <c r="T98" s="17" t="inlineStr">
         <is>
           <t>027</t>
         </is>
@@ -17931,7 +17931,7 @@
           <t>748</t>
         </is>
       </c>
-      <c r="S99" s="10" t="inlineStr">
+      <c r="S99" s="17" t="inlineStr">
         <is>
           <t>234</t>
         </is>
@@ -18128,7 +18128,7 @@
           <t>863</t>
         </is>
       </c>
-      <c r="U100" s="11" t="inlineStr">
+      <c r="U100" s="17" t="inlineStr">
         <is>
           <t>234</t>
         </is>
@@ -18335,7 +18335,7 @@
           <t>031</t>
         </is>
       </c>
-      <c r="Y101" s="12" t="inlineStr">
+      <c r="Y101" s="17" t="inlineStr">
         <is>
           <t>342</t>
         </is>
@@ -19085,7 +19085,7 @@
           <t>846</t>
         </is>
       </c>
-      <c r="H108" s="7" t="inlineStr">
+      <c r="H108" s="17" t="inlineStr">
         <is>
           <t>324</t>
         </is>
@@ -19135,7 +19135,7 @@
           <t>796</t>
         </is>
       </c>
-      <c r="R108" s="17" t="inlineStr">
+      <c r="R108" s="10" t="inlineStr">
         <is>
           <t>042</t>
         </is>
@@ -19454,7 +19454,7 @@
           <t>227</t>
         </is>
       </c>
-      <c r="G110" s="17" t="inlineStr">
+      <c r="G110" s="6" t="inlineStr">
         <is>
           <t>204</t>
         </is>
@@ -19781,7 +19781,7 @@
           <t>883</t>
         </is>
       </c>
-      <c r="AI111" s="16" t="inlineStr">
+      <c r="AI111" s="17" t="inlineStr">
         <is>
           <t>072</t>
         </is>
@@ -19918,7 +19918,7 @@
           <t>357</t>
         </is>
       </c>
-      <c r="Y112" s="12" t="inlineStr">
+      <c r="Y112" s="17" t="inlineStr">
         <is>
           <t>243</t>
         </is>
@@ -22638,7 +22638,7 @@
           <t>739</t>
         </is>
       </c>
-      <c r="H127" s="7" t="inlineStr">
+      <c r="H127" s="17" t="inlineStr">
         <is>
           <t>423</t>
         </is>
@@ -22850,7 +22850,7 @@
           <t>267</t>
         </is>
       </c>
-      <c r="M128" s="8" t="inlineStr">
+      <c r="M128" s="17" t="inlineStr">
         <is>
           <t>720</t>
         </is>
@@ -22895,7 +22895,7 @@
           <t>377</t>
         </is>
       </c>
-      <c r="V128" s="11" t="inlineStr">
+      <c r="V128" s="17" t="inlineStr">
         <is>
           <t>720</t>
         </is>
@@ -23042,7 +23042,7 @@
           <t>610</t>
         </is>
       </c>
-      <c r="N129" s="17" t="inlineStr">
+      <c r="N129" s="9" t="inlineStr">
         <is>
           <t>420</t>
         </is>
@@ -23087,7 +23087,7 @@
           <t>906</t>
         </is>
       </c>
-      <c r="W129" s="12" t="inlineStr">
+      <c r="W129" s="17" t="inlineStr">
         <is>
           <t>243</t>
         </is>
@@ -23122,7 +23122,7 @@
           <t>450</t>
         </is>
       </c>
-      <c r="AD129" s="14" t="inlineStr">
+      <c r="AD129" s="17" t="inlineStr">
         <is>
           <t>270</t>
         </is>
@@ -23451,7 +23451,7 @@
           <t>717</t>
         </is>
       </c>
-      <c r="U131" s="11" t="inlineStr">
+      <c r="U131" s="17" t="inlineStr">
         <is>
           <t>423</t>
         </is>
@@ -23543,7 +23543,7 @@
           <t>25</t>
         </is>
       </c>
-      <c r="B132" s="5" t="inlineStr">
+      <c r="B132" s="17" t="inlineStr">
         <is>
           <t>243</t>
         </is>
@@ -23568,7 +23568,7 @@
           <t>919</t>
         </is>
       </c>
-      <c r="G132" s="17" t="inlineStr">
+      <c r="G132" s="6" t="inlineStr">
         <is>
           <t>240</t>
         </is>
@@ -23643,7 +23643,7 @@
           <t>699</t>
         </is>
       </c>
-      <c r="V132" s="17" t="inlineStr">
+      <c r="V132" s="11" t="inlineStr">
         <is>
           <t>042</t>
         </is>
@@ -24239,7 +24239,7 @@
           <t>586</t>
         </is>
       </c>
-      <c r="AC135" s="14" t="inlineStr">
+      <c r="AC135" s="17" t="inlineStr">
         <is>
           <t>702</t>
         </is>
@@ -24249,7 +24249,7 @@
           <t>195</t>
         </is>
       </c>
-      <c r="AE135" s="17" t="inlineStr">
+      <c r="AE135" s="14" t="inlineStr">
         <is>
           <t>420</t>
         </is>
@@ -24775,7 +24775,7 @@
           <t>239</t>
         </is>
       </c>
-      <c r="X138" s="12" t="inlineStr">
+      <c r="X138" s="17" t="inlineStr">
         <is>
           <t>423</t>
         </is>
@@ -25510,7 +25510,7 @@
           <t>517</t>
         </is>
       </c>
-      <c r="D145" s="5" t="inlineStr">
+      <c r="D145" s="17" t="inlineStr">
         <is>
           <t>324</t>
         </is>
@@ -25605,7 +25605,7 @@
           <t>256</t>
         </is>
       </c>
-      <c r="W145" s="17" t="inlineStr">
+      <c r="W145" s="12" t="inlineStr">
         <is>
           <t>042</t>
         </is>
@@ -26226,7 +26226,7 @@
           <t>439</t>
         </is>
       </c>
-      <c r="AI148" s="16" t="inlineStr">
+      <c r="AI148" s="17" t="inlineStr">
         <is>
           <t>342</t>
         </is>
@@ -26540,7 +26540,7 @@
           <t>880</t>
         </is>
       </c>
-      <c r="W150" s="12" t="inlineStr">
+      <c r="W150" s="17" t="inlineStr">
         <is>
           <t>720</t>
         </is>
@@ -26939,7 +26939,7 @@
           <t>470</t>
         </is>
       </c>
-      <c r="AB152" s="13" t="inlineStr">
+      <c r="AB152" s="17" t="inlineStr">
         <is>
           <t>324</t>
         </is>
@@ -27076,12 +27076,12 @@
           <t>487</t>
         </is>
       </c>
-      <c r="R153" s="10" t="inlineStr">
+      <c r="R153" s="17" t="inlineStr">
         <is>
           <t>243</t>
         </is>
       </c>
-      <c r="S153" s="10" t="inlineStr">
+      <c r="S153" s="17" t="inlineStr">
         <is>
           <t>027</t>
         </is>
@@ -27218,7 +27218,7 @@
           <t>428</t>
         </is>
       </c>
-      <c r="I154" s="7" t="inlineStr">
+      <c r="I154" s="17" t="inlineStr">
         <is>
           <t>243</t>
         </is>
@@ -27495,7 +27495,7 @@
           <t>662</t>
         </is>
       </c>
-      <c r="AA155" s="17" t="inlineStr">
+      <c r="AA155" s="13" t="inlineStr">
         <is>
           <t>420</t>
         </is>
@@ -27662,7 +27662,7 @@
           <t>538</t>
         </is>
       </c>
-      <c r="W156" s="12" t="inlineStr">
+      <c r="W156" s="17" t="inlineStr">
         <is>
           <t>432</t>
         </is>
@@ -28320,7 +28320,7 @@
           <t>531</t>
         </is>
       </c>
-      <c r="E160" s="17" t="inlineStr">
+      <c r="E160" s="6" t="inlineStr">
         <is>
           <t>420</t>
         </is>
@@ -28749,7 +28749,7 @@
           <t>351</t>
         </is>
       </c>
-      <c r="P162" s="17" t="inlineStr">
+      <c r="P162" s="9" t="inlineStr">
         <is>
           <t>402</t>
         </is>
@@ -29203,7 +29203,7 @@
           <t>076</t>
         </is>
       </c>
-      <c r="AF164" s="15" t="inlineStr">
+      <c r="AF164" s="17" t="inlineStr">
         <is>
           <t>702</t>
         </is>
@@ -30689,7 +30689,7 @@
           <t>909</t>
         </is>
       </c>
-      <c r="AD172" s="14" t="inlineStr">
+      <c r="AD172" s="17" t="inlineStr">
         <is>
           <t>342</t>
         </is>
@@ -31763,7 +31763,7 @@
           <t>462</t>
         </is>
       </c>
-      <c r="C181" s="5" t="inlineStr">
+      <c r="C181" s="17" t="inlineStr">
         <is>
           <t>324</t>
         </is>
@@ -31858,7 +31858,7 @@
           <t>803</t>
         </is>
       </c>
-      <c r="V181" s="11" t="inlineStr">
+      <c r="V181" s="17" t="inlineStr">
         <is>
           <t>270</t>
         </is>
@@ -31903,7 +31903,7 @@
           <t>474</t>
         </is>
       </c>
-      <c r="AE181" s="17" t="inlineStr">
+      <c r="AE181" s="14" t="inlineStr">
         <is>
           <t>204</t>
         </is>
@@ -32282,7 +32282,7 @@
           <t>225</t>
         </is>
       </c>
-      <c r="AF183" s="17" t="inlineStr">
+      <c r="AF183" s="15" t="inlineStr">
         <is>
           <t>420</t>
         </is>
@@ -33217,12 +33217,12 @@
           <t>898</t>
         </is>
       </c>
-      <c r="AF188" s="15" t="inlineStr">
+      <c r="AF188" s="17" t="inlineStr">
         <is>
           <t>243</t>
         </is>
       </c>
-      <c r="AG188" s="17" t="inlineStr">
+      <c r="AG188" s="15" t="inlineStr">
         <is>
           <t>024</t>
         </is>
@@ -33409,7 +33409,7 @@
           <t>565</t>
         </is>
       </c>
-      <c r="AG189" s="15" t="inlineStr">
+      <c r="AG189" s="17" t="inlineStr">
         <is>
           <t>423</t>
         </is>
@@ -33536,7 +33536,7 @@
           <t>251</t>
         </is>
       </c>
-      <c r="U190" s="11" t="inlineStr">
+      <c r="U190" s="17" t="inlineStr">
         <is>
           <t>270</t>
         </is>
@@ -34022,7 +34022,7 @@
           <t>970</t>
         </is>
       </c>
-      <c r="F193" s="6" t="inlineStr">
+      <c r="F193" s="17" t="inlineStr">
         <is>
           <t>027</t>
         </is>
@@ -34618,7 +34618,7 @@
           <t>989</t>
         </is>
       </c>
-      <c r="M196" s="8" t="inlineStr">
+      <c r="M196" s="17" t="inlineStr">
         <is>
           <t>243</t>
         </is>
@@ -34713,7 +34713,7 @@
           <t>069</t>
         </is>
       </c>
-      <c r="AF196" s="15" t="inlineStr">
+      <c r="AF196" s="17" t="inlineStr">
         <is>
           <t>423</t>
         </is>
@@ -34942,7 +34942,7 @@
           <t>087</t>
         </is>
       </c>
-      <c r="C198" s="5" t="inlineStr">
+      <c r="C198" s="17" t="inlineStr">
         <is>
           <t>720</t>
         </is>
@@ -35047,7 +35047,7 @@
           <t>124</t>
         </is>
       </c>
-      <c r="X198" s="17" t="inlineStr">
+      <c r="X198" s="12" t="inlineStr">
         <is>
           <t>042</t>
         </is>
@@ -35259,7 +35259,7 @@
           <t>059</t>
         </is>
       </c>
-      <c r="AC199" s="14" t="inlineStr">
+      <c r="AC199" s="17" t="inlineStr">
         <is>
           <t>207</t>
         </is>
@@ -35346,7 +35346,7 @@
           <t>715</t>
         </is>
       </c>
-      <c r="I200" s="7" t="inlineStr">
+      <c r="I200" s="17" t="inlineStr">
         <is>
           <t>234</t>
         </is>
@@ -35735,7 +35735,7 @@
           <t>872</t>
         </is>
       </c>
-      <c r="L202" s="17" t="inlineStr">
+      <c r="L202" s="8" t="inlineStr">
         <is>
           <t>402</t>
         </is>
@@ -35987,7 +35987,7 @@
           <t>068</t>
         </is>
       </c>
-      <c r="Y203" s="12" t="inlineStr">
+      <c r="Y203" s="17" t="inlineStr">
         <is>
           <t>243</t>
         </is>
@@ -36169,7 +36169,7 @@
           <t>987</t>
         </is>
       </c>
-      <c r="X204" s="17" t="inlineStr">
+      <c r="X204" s="12" t="inlineStr">
         <is>
           <t>042</t>
         </is>
@@ -37782,7 +37782,7 @@
           <t>119</t>
         </is>
       </c>
-      <c r="AD215" s="17" t="inlineStr">
+      <c r="AD215" s="14" t="inlineStr">
         <is>
           <t>204</t>
         </is>
@@ -38116,7 +38116,7 @@
           <t>905</t>
         </is>
       </c>
-      <c r="V217" s="11" t="inlineStr">
+      <c r="V217" s="17" t="inlineStr">
         <is>
           <t>423</t>
         </is>
@@ -38859,7 +38859,7 @@
           <t>022</t>
         </is>
       </c>
-      <c r="U221" s="17" t="inlineStr">
+      <c r="U221" s="11" t="inlineStr">
         <is>
           <t>204</t>
         </is>
@@ -38939,7 +38939,7 @@
           <t>018</t>
         </is>
       </c>
-      <c r="AK221" s="16" t="inlineStr">
+      <c r="AK221" s="17" t="inlineStr">
         <is>
           <t>342</t>
         </is>
@@ -39258,7 +39258,7 @@
           <t>528</t>
         </is>
       </c>
-      <c r="Z223" s="17" t="inlineStr">
+      <c r="Z223" s="13" t="inlineStr">
         <is>
           <t>024</t>
         </is>
@@ -39435,7 +39435,7 @@
           <t>608</t>
         </is>
       </c>
-      <c r="X224" s="17" t="inlineStr">
+      <c r="X224" s="12" t="inlineStr">
         <is>
           <t>024</t>
         </is>
@@ -39734,7 +39734,7 @@
           <t>488</t>
         </is>
       </c>
-      <c r="I226" s="7" t="inlineStr">
+      <c r="I226" s="17" t="inlineStr">
         <is>
           <t>072</t>
         </is>
@@ -39869,7 +39869,7 @@
           <t>411</t>
         </is>
       </c>
-      <c r="AJ226" s="16" t="inlineStr">
+      <c r="AJ226" s="17" t="inlineStr">
         <is>
           <t>207</t>
         </is>
@@ -40183,7 +40183,7 @@
           <t>479</t>
         </is>
       </c>
-      <c r="X228" s="12" t="inlineStr">
+      <c r="X228" s="17" t="inlineStr">
         <is>
           <t>720</t>
         </is>
@@ -40634,7 +40634,7 @@
           <t>19</t>
         </is>
       </c>
-      <c r="B231" s="5" t="inlineStr">
+      <c r="B231" s="17" t="inlineStr">
         <is>
           <t>234</t>
         </is>
@@ -40759,7 +40759,7 @@
           <t>122</t>
         </is>
       </c>
-      <c r="AA231" s="13" t="inlineStr">
+      <c r="AA231" s="17" t="inlineStr">
         <is>
           <t>432</t>
         </is>
@@ -40794,7 +40794,7 @@
           <t>658</t>
         </is>
       </c>
-      <c r="AH231" s="17" t="inlineStr">
+      <c r="AH231" s="15" t="inlineStr">
         <is>
           <t>204</t>
         </is>
@@ -40981,7 +40981,7 @@
           <t>671</t>
         </is>
       </c>
-      <c r="AH232" s="15" t="inlineStr">
+      <c r="AH232" s="17" t="inlineStr">
         <is>
           <t>720</t>
         </is>
@@ -41088,7 +41088,7 @@
           <t>615</t>
         </is>
       </c>
-      <c r="R233" s="10" t="inlineStr">
+      <c r="R233" s="17" t="inlineStr">
         <is>
           <t>234</t>
         </is>
@@ -41200,7 +41200,7 @@
           <t>852</t>
         </is>
       </c>
-      <c r="C234" s="17" t="inlineStr">
+      <c r="C234" s="5" t="inlineStr">
         <is>
           <t>204</t>
         </is>
@@ -41629,7 +41629,7 @@
           <t>372</t>
         </is>
       </c>
-      <c r="N236" s="9" t="inlineStr">
+      <c r="N236" s="17" t="inlineStr">
         <is>
           <t>027</t>
         </is>
@@ -41821,7 +41821,7 @@
           <t>786</t>
         </is>
       </c>
-      <c r="O237" s="9" t="inlineStr">
+      <c r="O237" s="17" t="inlineStr">
         <is>
           <t>027</t>
         </is>
@@ -42068,7 +42068,7 @@
           <t>935</t>
         </is>
       </c>
-      <c r="AA238" s="13" t="inlineStr">
+      <c r="AA238" s="17" t="inlineStr">
         <is>
           <t>324</t>
         </is>
@@ -42230,7 +42230,7 @@
           <t>881</t>
         </is>
       </c>
-      <c r="V239" s="11" t="inlineStr">
+      <c r="V239" s="17" t="inlineStr">
         <is>
           <t>234</t>
         </is>
@@ -42337,7 +42337,7 @@
           <t>228</t>
         </is>
       </c>
-      <c r="F240" s="6" t="inlineStr">
+      <c r="F240" s="17" t="inlineStr">
         <is>
           <t>432</t>
         </is>
@@ -43920,7 +43920,7 @@
           <t>681</t>
         </is>
       </c>
-      <c r="F251" s="6" t="inlineStr">
+      <c r="F251" s="17" t="inlineStr">
         <is>
           <t>720</t>
         </is>
@@ -44030,7 +44030,7 @@
           <t>867</t>
         </is>
       </c>
-      <c r="AB251" s="17" t="inlineStr">
+      <c r="AB251" s="13" t="inlineStr">
         <is>
           <t>402</t>
         </is>
@@ -44055,7 +44055,7 @@
           <t>594</t>
         </is>
       </c>
-      <c r="AG251" s="17" t="inlineStr">
+      <c r="AG251" s="15" t="inlineStr">
         <is>
           <t>420</t>
         </is>
@@ -44092,7 +44092,7 @@
           <t>752</t>
         </is>
       </c>
-      <c r="C252" s="5" t="inlineStr">
+      <c r="C252" s="17" t="inlineStr">
         <is>
           <t>027</t>
         </is>
@@ -44182,7 +44182,7 @@
           <t>813</t>
         </is>
       </c>
-      <c r="U252" s="11" t="inlineStr">
+      <c r="U252" s="17" t="inlineStr">
         <is>
           <t>423</t>
         </is>
@@ -44439,7 +44439,7 @@
           <t>320</t>
         </is>
       </c>
-      <c r="AI253" s="16" t="inlineStr">
+      <c r="AI253" s="17" t="inlineStr">
         <is>
           <t>324</t>
         </is>
@@ -45022,7 +45022,7 @@
           <t>10</t>
         </is>
       </c>
-      <c r="B257" s="17" t="inlineStr">
+      <c r="B257" s="5" t="inlineStr">
         <is>
           <t>402</t>
         </is>
@@ -45172,7 +45172,7 @@
           <t>258</t>
         </is>
       </c>
-      <c r="AF257" s="17" t="inlineStr">
+      <c r="AF257" s="15" t="inlineStr">
         <is>
           <t>420</t>
         </is>
@@ -45224,7 +45224,7 @@
           <t>790</t>
         </is>
       </c>
-      <c r="E258" s="17" t="inlineStr">
+      <c r="E258" s="6" t="inlineStr">
         <is>
           <t>402</t>
         </is>
@@ -45314,7 +45314,7 @@
           <t>047</t>
         </is>
       </c>
-      <c r="W258" s="12" t="inlineStr">
+      <c r="W258" s="17" t="inlineStr">
         <is>
           <t>270</t>
         </is>
@@ -45521,7 +45521,7 @@
           <t>623</t>
         </is>
       </c>
-      <c r="AA259" s="17" t="inlineStr">
+      <c r="AA259" s="13" t="inlineStr">
         <is>
           <t>204</t>
         </is>
@@ -46169,7 +46169,7 @@
           <t>288</t>
         </is>
       </c>
-      <c r="G263" s="17" t="inlineStr">
+      <c r="G263" s="6" t="inlineStr">
         <is>
           <t>204</t>
         </is>
@@ -46304,7 +46304,7 @@
           <t>756</t>
         </is>
       </c>
-      <c r="AH263" s="15" t="inlineStr">
+      <c r="AH263" s="17" t="inlineStr">
         <is>
           <t>324</t>
         </is>
@@ -46892,7 +46892,7 @@
           <t>20</t>
         </is>
       </c>
-      <c r="B267" s="17" t="inlineStr">
+      <c r="B267" s="5" t="inlineStr">
         <is>
           <t>204</t>
         </is>
@@ -47032,7 +47032,7 @@
           <t>299</t>
         </is>
       </c>
-      <c r="AD267" s="17" t="inlineStr">
+      <c r="AD267" s="14" t="inlineStr">
         <is>
           <t>402</t>
         </is>
@@ -47276,7 +47276,7 @@
           <t>054</t>
         </is>
       </c>
-      <c r="D269" s="17" t="inlineStr">
+      <c r="D269" s="5" t="inlineStr">
         <is>
           <t>042</t>
         </is>
@@ -47593,7 +47593,7 @@
           <t>549</t>
         </is>
       </c>
-      <c r="AD270" s="14" t="inlineStr">
+      <c r="AD270" s="17" t="inlineStr">
         <is>
           <t>072</t>
         </is>
@@ -47982,7 +47982,7 @@
           <t>080</t>
         </is>
       </c>
-      <c r="AG272" s="15" t="inlineStr">
+      <c r="AG272" s="17" t="inlineStr">
         <is>
           <t>702</t>
         </is>
@@ -48523,7 +48523,7 @@
           <t>315</t>
         </is>
       </c>
-      <c r="AC275" s="14" t="inlineStr">
+      <c r="AC275" s="17" t="inlineStr">
         <is>
           <t>243</t>
         </is>
@@ -48927,7 +48927,7 @@
           <t>000</t>
         </is>
       </c>
-      <c r="AI277" s="17" t="inlineStr">
+      <c r="AI277" s="16" t="inlineStr">
         <is>
           <t>042</t>
         </is>
@@ -49430,7 +49430,7 @@
           <t>221</t>
         </is>
       </c>
-      <c r="F283" s="17" t="inlineStr">
+      <c r="F283" s="6" t="inlineStr">
         <is>
           <t>204</t>
         </is>
@@ -49939,7 +49939,7 @@
           <t>621</t>
         </is>
       </c>
-      <c r="AG285" s="15" t="inlineStr">
+      <c r="AG285" s="17" t="inlineStr">
         <is>
           <t>324</t>
         </is>
@@ -50126,7 +50126,7 @@
           <t>971</t>
         </is>
       </c>
-      <c r="AG286" s="15" t="inlineStr">
+      <c r="AG286" s="17" t="inlineStr">
         <is>
           <t>027</t>
         </is>
@@ -50233,7 +50233,7 @@
           <t>325</t>
         </is>
       </c>
-      <c r="Q287" s="10" t="inlineStr">
+      <c r="Q287" s="17" t="inlineStr">
         <is>
           <t>720</t>
         </is>
@@ -50470,7 +50470,7 @@
           <t>642</t>
         </is>
       </c>
-      <c r="AA288" s="13" t="inlineStr">
+      <c r="AA288" s="17" t="inlineStr">
         <is>
           <t>342</t>
         </is>
@@ -50597,7 +50597,7 @@
           <t>807</t>
         </is>
       </c>
-      <c r="O289" s="17" t="inlineStr">
+      <c r="O289" s="9" t="inlineStr">
         <is>
           <t>420</t>
         </is>
@@ -51415,7 +51415,7 @@
           <t>320</t>
         </is>
       </c>
-      <c r="AC293" s="14" t="inlineStr">
+      <c r="AC293" s="17" t="inlineStr">
         <is>
           <t>072</t>
         </is>
@@ -52001,7 +52001,7 @@
           <t>905</t>
         </is>
       </c>
-      <c r="AH296" s="15" t="inlineStr">
+      <c r="AH296" s="17" t="inlineStr">
         <is>
           <t>720</t>
         </is>
@@ -52477,7 +52477,7 @@
           <t>477</t>
         </is>
       </c>
-      <c r="Q299" s="10" t="inlineStr">
+      <c r="Q299" s="17" t="inlineStr">
         <is>
           <t>432</t>
         </is>
@@ -52851,7 +52851,7 @@
           <t>130</t>
         </is>
       </c>
-      <c r="Q301" s="10" t="inlineStr">
+      <c r="Q301" s="17" t="inlineStr">
         <is>
           <t>207</t>
         </is>
@@ -53599,7 +53599,7 @@
           <t>607</t>
         </is>
       </c>
-      <c r="Q305" s="10" t="inlineStr">
+      <c r="Q305" s="17" t="inlineStr">
         <is>
           <t>270</t>
         </is>
@@ -53614,7 +53614,7 @@
           <t>623</t>
         </is>
       </c>
-      <c r="T305" s="17" t="inlineStr">
+      <c r="T305" s="11" t="inlineStr">
         <is>
           <t>420</t>
         </is>
@@ -54277,7 +54277,7 @@
           <t>138</t>
         </is>
       </c>
-      <c r="C309" s="17" t="inlineStr">
+      <c r="C309" s="5" t="inlineStr">
         <is>
           <t>204</t>
         </is>
@@ -54514,7 +54514,7 @@
           <t>428</t>
         </is>
       </c>
-      <c r="M310" s="8" t="inlineStr">
+      <c r="M310" s="17" t="inlineStr">
         <is>
           <t>720</t>
         </is>
@@ -54736,7 +54736,7 @@
           <t>743</t>
         </is>
       </c>
-      <c r="T311" s="11" t="inlineStr">
+      <c r="T311" s="17" t="inlineStr">
         <is>
           <t>324</t>
         </is>
@@ -54873,7 +54873,7 @@
           <t>845</t>
         </is>
       </c>
-      <c r="J312" s="7" t="inlineStr">
+      <c r="J312" s="17" t="inlineStr">
         <is>
           <t>324</t>
         </is>
@@ -56137,7 +56137,7 @@
           <t>816</t>
         </is>
       </c>
-      <c r="U321" s="11" t="inlineStr">
+      <c r="U321" s="17" t="inlineStr">
         <is>
           <t>270</t>
         </is>
@@ -56344,7 +56344,7 @@
           <t>372</t>
         </is>
       </c>
-      <c r="Y322" s="12" t="inlineStr">
+      <c r="Y322" s="17" t="inlineStr">
         <is>
           <t>720</t>
         </is>
@@ -56486,7 +56486,7 @@
           <t>362</t>
         </is>
       </c>
-      <c r="P323" s="9" t="inlineStr">
+      <c r="P323" s="17" t="inlineStr">
         <is>
           <t>342</t>
         </is>
@@ -56566,7 +56566,7 @@
           <t>949</t>
         </is>
       </c>
-      <c r="AF323" s="15" t="inlineStr">
+      <c r="AF323" s="17" t="inlineStr">
         <is>
           <t>234</t>
         </is>
@@ -56708,7 +56708,7 @@
           <t>847</t>
         </is>
       </c>
-      <c r="W324" s="12" t="inlineStr">
+      <c r="W324" s="17" t="inlineStr">
         <is>
           <t>702</t>
         </is>
@@ -56945,7 +56945,7 @@
           <t>698</t>
         </is>
       </c>
-      <c r="AG325" s="17" t="inlineStr">
+      <c r="AG325" s="15" t="inlineStr">
         <is>
           <t>204</t>
         </is>
@@ -57107,7 +57107,7 @@
           <t>631</t>
         </is>
       </c>
-      <c r="AB326" s="13" t="inlineStr">
+      <c r="AB326" s="17" t="inlineStr">
         <is>
           <t>207</t>
         </is>
@@ -57117,7 +57117,7 @@
           <t>840</t>
         </is>
       </c>
-      <c r="AD326" s="14" t="inlineStr">
+      <c r="AD326" s="17" t="inlineStr">
         <is>
           <t>324</t>
         </is>
@@ -57189,7 +57189,7 @@
           <t>138</t>
         </is>
       </c>
-      <c r="G327" s="6" t="inlineStr">
+      <c r="G327" s="17" t="inlineStr">
         <is>
           <t>342</t>
         </is>
@@ -57279,7 +57279,7 @@
           <t>855</t>
         </is>
       </c>
-      <c r="Y327" s="12" t="inlineStr">
+      <c r="Y327" s="17" t="inlineStr">
         <is>
           <t>270</t>
         </is>
@@ -57376,12 +57376,12 @@
           <t>325</t>
         </is>
       </c>
-      <c r="G328" s="6" t="inlineStr">
+      <c r="G328" s="17" t="inlineStr">
         <is>
           <t>243</t>
         </is>
       </c>
-      <c r="H328" s="7" t="inlineStr">
+      <c r="H328" s="17" t="inlineStr">
         <is>
           <t>270</t>
         </is>
@@ -57426,7 +57426,7 @@
           <t>015</t>
         </is>
       </c>
-      <c r="Q328" s="10" t="inlineStr">
+      <c r="Q328" s="17" t="inlineStr">
         <is>
           <t>207</t>
         </is>
@@ -58139,7 +58139,7 @@
           <t>452</t>
         </is>
       </c>
-      <c r="J332" s="7" t="inlineStr">
+      <c r="J332" s="17" t="inlineStr">
         <is>
           <t>270</t>
         </is>
@@ -58386,7 +58386,7 @@
           <t>737</t>
         </is>
       </c>
-      <c r="V333" s="17" t="inlineStr">
+      <c r="V333" s="11" t="inlineStr">
         <is>
           <t>240</t>
         </is>
@@ -58638,7 +58638,7 @@
           <t>165</t>
         </is>
       </c>
-      <c r="AI334" s="16" t="inlineStr">
+      <c r="AI334" s="17" t="inlineStr">
         <is>
           <t>072</t>
         </is>
@@ -59114,7 +59114,7 @@
           <t>972</t>
         </is>
       </c>
-      <c r="R337" s="10" t="inlineStr">
+      <c r="R337" s="17" t="inlineStr">
         <is>
           <t>243</t>
         </is>
@@ -59266,7 +59266,7 @@
           <t>419</t>
         </is>
       </c>
-      <c r="K338" s="8" t="inlineStr">
+      <c r="K338" s="17" t="inlineStr">
         <is>
           <t>702</t>
         </is>
@@ -59750,7 +59750,7 @@
           <t>827</t>
         </is>
       </c>
-      <c r="AG340" s="17" t="inlineStr">
+      <c r="AG340" s="15" t="inlineStr">
         <is>
           <t>240</t>
         </is>
@@ -60024,7 +60024,7 @@
           <t>590</t>
         </is>
       </c>
-      <c r="M342" s="8" t="inlineStr">
+      <c r="M342" s="17" t="inlineStr">
         <is>
           <t>270</t>
         </is>
@@ -60296,7 +60296,7 @@
           <t>120</t>
         </is>
       </c>
-      <c r="AD343" s="14" t="inlineStr">
+      <c r="AD343" s="17" t="inlineStr">
         <is>
           <t>270</t>
         </is>
@@ -61024,7 +61024,7 @@
           <t>339</t>
         </is>
       </c>
-      <c r="Z347" s="17" t="inlineStr">
+      <c r="Z347" s="13" t="inlineStr">
         <is>
           <t>204</t>
         </is>
@@ -61034,7 +61034,7 @@
           <t>392</t>
         </is>
       </c>
-      <c r="AB347" s="17" t="inlineStr">
+      <c r="AB347" s="13" t="inlineStr">
         <is>
           <t>204</t>
         </is>
@@ -61727,7 +61727,7 @@
           <t>375</t>
         </is>
       </c>
-      <c r="AK353" s="16" t="inlineStr">
+      <c r="AK353" s="17" t="inlineStr">
         <is>
           <t>324</t>
         </is>
@@ -61961,7 +61961,7 @@
           <t>377</t>
         </is>
       </c>
-      <c r="I355" s="17" t="inlineStr">
+      <c r="I355" s="7" t="inlineStr">
         <is>
           <t>204</t>
         </is>
@@ -62921,7 +62921,7 @@
           <t>909</t>
         </is>
       </c>
-      <c r="N360" s="9" t="inlineStr">
+      <c r="N360" s="17" t="inlineStr">
         <is>
           <t>207</t>
         </is>
@@ -63031,7 +63031,7 @@
           <t>785</t>
         </is>
       </c>
-      <c r="AJ360" s="16" t="inlineStr">
+      <c r="AJ360" s="17" t="inlineStr">
         <is>
           <t>072</t>
         </is>
@@ -63143,7 +63143,7 @@
           <t>089</t>
         </is>
       </c>
-      <c r="U361" s="11" t="inlineStr">
+      <c r="U361" s="17" t="inlineStr">
         <is>
           <t>243</t>
         </is>
@@ -64048,7 +64048,7 @@
           <t>851</t>
         </is>
       </c>
-      <c r="O366" s="9" t="inlineStr">
+      <c r="O366" s="17" t="inlineStr">
         <is>
           <t>423</t>
         </is>
@@ -64078,7 +64078,7 @@
           <t>329</t>
         </is>
       </c>
-      <c r="U366" s="17" t="inlineStr">
+      <c r="U366" s="11" t="inlineStr">
         <is>
           <t>240</t>
         </is>
@@ -64158,7 +64158,7 @@
           <t>047</t>
         </is>
       </c>
-      <c r="AK366" s="16" t="inlineStr">
+      <c r="AK366" s="17" t="inlineStr">
         <is>
           <t>423</t>
         </is>
@@ -64649,7 +64649,7 @@
           <t>644</t>
         </is>
       </c>
-      <c r="W369" s="17" t="inlineStr">
+      <c r="W369" s="12" t="inlineStr">
         <is>
           <t>240</t>
         </is>
@@ -64719,7 +64719,7 @@
           <t>009</t>
         </is>
       </c>
-      <c r="AK369" s="16" t="inlineStr">
+      <c r="AK369" s="17" t="inlineStr">
         <is>
           <t>423</t>
         </is>
@@ -64861,7 +64861,7 @@
           <t>582</t>
         </is>
       </c>
-      <c r="AB370" s="13" t="inlineStr">
+      <c r="AB370" s="17" t="inlineStr">
         <is>
           <t>432</t>
         </is>
@@ -64953,7 +64953,7 @@
           <t>617</t>
         </is>
       </c>
-      <c r="I371" s="7" t="inlineStr">
+      <c r="I371" s="17" t="inlineStr">
         <is>
           <t>207</t>
         </is>
@@ -65003,7 +65003,7 @@
           <t>872</t>
         </is>
       </c>
-      <c r="S371" s="10" t="inlineStr">
+      <c r="S371" s="17" t="inlineStr">
         <is>
           <t>702</t>
         </is>
@@ -65412,7 +65412,7 @@
           <t>035</t>
         </is>
       </c>
-      <c r="Z373" s="13" t="inlineStr">
+      <c r="Z373" s="17" t="inlineStr">
         <is>
           <t>342</t>
         </is>
@@ -65422,7 +65422,7 @@
           <t>678</t>
         </is>
       </c>
-      <c r="AB373" s="13" t="inlineStr">
+      <c r="AB373" s="17" t="inlineStr">
         <is>
           <t>072</t>
         </is>
@@ -66272,7 +66272,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="K378" s="8" t="inlineStr">
+      <c r="K378" s="17" t="inlineStr">
         <is>
           <t>027</t>
         </is>
@@ -66327,7 +66327,7 @@
           <t>206</t>
         </is>
       </c>
-      <c r="V378" s="11" t="inlineStr">
+      <c r="V378" s="17" t="inlineStr">
         <is>
           <t>720</t>
         </is>
@@ -66387,7 +66387,7 @@
           <t>871</t>
         </is>
       </c>
-      <c r="AH378" s="15" t="inlineStr">
+      <c r="AH378" s="17" t="inlineStr">
         <is>
           <t>423</t>
         </is>
@@ -66549,7 +66549,7 @@
           <t>339</t>
         </is>
       </c>
-      <c r="AC379" s="14" t="inlineStr">
+      <c r="AC379" s="17" t="inlineStr">
         <is>
           <t>072</t>
         </is>
@@ -66606,7 +66606,7 @@
           <t>157</t>
         </is>
       </c>
-      <c r="C380" s="17" t="inlineStr">
+      <c r="C380" s="5" t="inlineStr">
         <is>
           <t>420</t>
         </is>
@@ -66853,7 +66853,7 @@
           <t>380</t>
         </is>
       </c>
-      <c r="O381" s="9" t="inlineStr">
+      <c r="O381" s="17" t="inlineStr">
         <is>
           <t>423</t>
         </is>
@@ -67095,7 +67095,7 @@
           <t>626</t>
         </is>
       </c>
-      <c r="Z382" s="13" t="inlineStr">
+      <c r="Z382" s="17" t="inlineStr">
         <is>
           <t>243</t>
         </is>
@@ -67172,7 +67172,7 @@
           <t>297</t>
         </is>
       </c>
-      <c r="D383" s="17" t="inlineStr">
+      <c r="D383" s="5" t="inlineStr">
         <is>
           <t>402</t>
         </is>
@@ -67835,7 +67835,7 @@
           <t>351</t>
         </is>
       </c>
-      <c r="G389" s="6" t="inlineStr">
+      <c r="G389" s="17" t="inlineStr">
         <is>
           <t>720</t>
         </is>
@@ -68162,7 +68162,7 @@
           <t>465</t>
         </is>
       </c>
-      <c r="AI390" s="17" t="inlineStr">
+      <c r="AI390" s="16" t="inlineStr">
         <is>
           <t>042</t>
         </is>
@@ -69067,7 +69067,7 @@
           <t>168</t>
         </is>
       </c>
-      <c r="AC395" s="17" t="inlineStr">
+      <c r="AC395" s="14" t="inlineStr">
         <is>
           <t>204</t>
         </is>
@@ -69259,7 +69259,7 @@
           <t>858</t>
         </is>
       </c>
-      <c r="AD396" s="17" t="inlineStr">
+      <c r="AD396" s="14" t="inlineStr">
         <is>
           <t>420</t>
         </is>
@@ -69279,7 +69279,7 @@
           <t>845</t>
         </is>
       </c>
-      <c r="AH396" s="15" t="inlineStr">
+      <c r="AH396" s="17" t="inlineStr">
         <is>
           <t>720</t>
         </is>
@@ -69765,7 +69765,7 @@
           <t>183</t>
         </is>
       </c>
-      <c r="S399" s="17" t="inlineStr">
+      <c r="S399" s="10" t="inlineStr">
         <is>
           <t>402</t>
         </is>
@@ -69997,7 +69997,7 @@
           <t>183</t>
         </is>
       </c>
-      <c r="AB400" s="17" t="inlineStr">
+      <c r="AB400" s="13" t="inlineStr">
         <is>
           <t>420</t>
         </is>
@@ -70271,7 +70271,7 @@
           <t>088</t>
         </is>
       </c>
-      <c r="H402" s="7" t="inlineStr">
+      <c r="H402" s="17" t="inlineStr">
         <is>
           <t>072</t>
         </is>
@@ -70715,7 +70715,7 @@
           <t>210</t>
         </is>
       </c>
-      <c r="V404" s="11" t="inlineStr">
+      <c r="V404" s="17" t="inlineStr">
         <is>
           <t>027</t>
         </is>
@@ -70947,7 +70947,7 @@
           <t>687</t>
         </is>
       </c>
-      <c r="AE405" s="17" t="inlineStr">
+      <c r="AE405" s="14" t="inlineStr">
         <is>
           <t>420</t>
         </is>
@@ -70977,7 +70977,7 @@
           <t>666</t>
         </is>
       </c>
-      <c r="AK405" s="17" t="inlineStr">
+      <c r="AK405" s="16" t="inlineStr">
         <is>
           <t>402</t>
         </is>
@@ -72216,7 +72216,7 @@
           <t>836</t>
         </is>
       </c>
-      <c r="W412" s="12" t="inlineStr">
+      <c r="W412" s="17" t="inlineStr">
         <is>
           <t>243</t>
         </is>
@@ -72298,7 +72298,7 @@
           <t>26</t>
         </is>
       </c>
-      <c r="B413" s="5" t="inlineStr">
+      <c r="B413" s="17" t="inlineStr">
         <is>
           <t>207</t>
         </is>
@@ -72453,7 +72453,7 @@
           <t>842</t>
         </is>
       </c>
-      <c r="AG413" s="15" t="inlineStr">
+      <c r="AG413" s="17" t="inlineStr">
         <is>
           <t>270</t>
         </is>
@@ -73348,7 +73348,7 @@
           <t>053</t>
         </is>
       </c>
-      <c r="Y418" s="12" t="inlineStr">
+      <c r="Y418" s="17" t="inlineStr">
         <is>
           <t>423</t>
         </is>
@@ -73378,7 +73378,7 @@
           <t>317</t>
         </is>
       </c>
-      <c r="AE418" s="14" t="inlineStr">
+      <c r="AE418" s="17" t="inlineStr">
         <is>
           <t>072</t>
         </is>
@@ -73911,7 +73911,7 @@
           <t>855</t>
         </is>
       </c>
-      <c r="H424" s="7" t="inlineStr">
+      <c r="H424" s="17" t="inlineStr">
         <is>
           <t>207</t>
         </is>
@@ -74073,7 +74073,7 @@
           <t>750</t>
         </is>
       </c>
-      <c r="C425" s="5" t="inlineStr">
+      <c r="C425" s="17" t="inlineStr">
         <is>
           <t>324</t>
         </is>
@@ -74739,7 +74739,7 @@
           <t>586</t>
         </is>
       </c>
-      <c r="X428" s="12" t="inlineStr">
+      <c r="X428" s="17" t="inlineStr">
         <is>
           <t>702</t>
         </is>
@@ -74976,7 +74976,7 @@
           <t>921</t>
         </is>
       </c>
-      <c r="AH429" s="15" t="inlineStr">
+      <c r="AH429" s="17" t="inlineStr">
         <is>
           <t>423</t>
         </is>
@@ -75891,7 +75891,7 @@
           <t>094</t>
         </is>
       </c>
-      <c r="AD434" s="17" t="inlineStr">
+      <c r="AD434" s="14" t="inlineStr">
         <is>
           <t>240</t>
         </is>
@@ -76113,7 +76113,7 @@
           <t>384</t>
         </is>
       </c>
-      <c r="AK435" s="16" t="inlineStr">
+      <c r="AK435" s="17" t="inlineStr">
         <is>
           <t>432</t>
         </is>
@@ -76130,7 +76130,7 @@
           <t>836</t>
         </is>
       </c>
-      <c r="C436" s="17" t="inlineStr">
+      <c r="C436" s="5" t="inlineStr">
         <is>
           <t>042</t>
         </is>
@@ -76392,7 +76392,7 @@
           <t>151</t>
         </is>
       </c>
-      <c r="R437" s="10" t="inlineStr">
+      <c r="R437" s="17" t="inlineStr">
         <is>
           <t>702</t>
         </is>
@@ -76973,7 +76973,7 @@
           <t>685</t>
         </is>
       </c>
-      <c r="V440" s="11" t="inlineStr">
+      <c r="V440" s="17" t="inlineStr">
         <is>
           <t>207</t>
         </is>
@@ -77853,7 +77853,7 @@
           <t>948</t>
         </is>
       </c>
-      <c r="K445" s="17" t="inlineStr">
+      <c r="K445" s="8" t="inlineStr">
         <is>
           <t>024</t>
         </is>
@@ -77888,7 +77888,7 @@
           <t>553</t>
         </is>
       </c>
-      <c r="R445" s="10" t="inlineStr">
+      <c r="R445" s="17" t="inlineStr">
         <is>
           <t>270</t>
         </is>
@@ -77938,7 +77938,7 @@
           <t>258</t>
         </is>
       </c>
-      <c r="AB445" s="13" t="inlineStr">
+      <c r="AB445" s="17" t="inlineStr">
         <is>
           <t>027</t>
         </is>
@@ -78509,7 +78509,7 @@
           <t>706</t>
         </is>
       </c>
-      <c r="AD448" s="17" t="inlineStr">
+      <c r="AD448" s="14" t="inlineStr">
         <is>
           <t>240</t>
         </is>
@@ -79399,7 +79399,7 @@
           <t>677</t>
         </is>
       </c>
-      <c r="U453" s="11" t="inlineStr">
+      <c r="U453" s="17" t="inlineStr">
         <is>
           <t>243</t>
         </is>
@@ -79870,7 +79870,7 @@
           <t>310</t>
         </is>
       </c>
-      <c r="W458" s="12" t="inlineStr">
+      <c r="W458" s="17" t="inlineStr">
         <is>
           <t>234</t>
         </is>
@@ -80097,7 +80097,7 @@
           <t>545</t>
         </is>
       </c>
-      <c r="AE459" s="17" t="inlineStr">
+      <c r="AE459" s="14" t="inlineStr">
         <is>
           <t>024</t>
         </is>
@@ -80249,7 +80249,7 @@
           <t>682</t>
         </is>
       </c>
-      <c r="X460" s="12" t="inlineStr">
+      <c r="X460" s="17" t="inlineStr">
         <is>
           <t>720</t>
         </is>
@@ -80314,7 +80314,7 @@
           <t>976</t>
         </is>
       </c>
-      <c r="AK460" s="17" t="inlineStr">
+      <c r="AK460" s="16" t="inlineStr">
         <is>
           <t>420</t>
         </is>
@@ -80568,7 +80568,7 @@
           <t>100</t>
         </is>
       </c>
-      <c r="M462" s="8" t="inlineStr">
+      <c r="M462" s="17" t="inlineStr">
         <is>
           <t>702</t>
         </is>
@@ -80688,7 +80688,7 @@
           <t>542</t>
         </is>
       </c>
-      <c r="AK462" s="16" t="inlineStr">
+      <c r="AK462" s="17" t="inlineStr">
         <is>
           <t>243</t>
         </is>
@@ -81613,7 +81613,7 @@
           <t>248</t>
         </is>
       </c>
-      <c r="AI467" s="16" t="inlineStr">
+      <c r="AI467" s="17" t="inlineStr">
         <is>
           <t>243</t>
         </is>
@@ -81675,7 +81675,7 @@
           <t>638</t>
         </is>
       </c>
-      <c r="J468" s="7" t="inlineStr">
+      <c r="J468" s="17" t="inlineStr">
         <is>
           <t>270</t>
         </is>
@@ -81800,7 +81800,7 @@
           <t>044</t>
         </is>
       </c>
-      <c r="AI468" s="17" t="inlineStr">
+      <c r="AI468" s="16" t="inlineStr">
         <is>
           <t>042</t>
         </is>
@@ -82438,7 +82438,7 @@
           <t>570</t>
         </is>
       </c>
-      <c r="M472" s="17" t="inlineStr">
+      <c r="M472" s="8" t="inlineStr">
         <is>
           <t>240</t>
         </is>
@@ -83261,7 +83261,7 @@
           <t>705</t>
         </is>
       </c>
-      <c r="AB476" s="17" t="inlineStr">
+      <c r="AB476" s="13" t="inlineStr">
         <is>
           <t>420</t>
         </is>
@@ -83428,7 +83428,7 @@
           <t>475</t>
         </is>
       </c>
-      <c r="X477" s="12" t="inlineStr">
+      <c r="X477" s="17" t="inlineStr">
         <is>
           <t>423</t>
         </is>
@@ -83650,7 +83650,7 @@
           <t>741</t>
         </is>
       </c>
-      <c r="AE478" s="14" t="inlineStr">
+      <c r="AE478" s="17" t="inlineStr">
         <is>
           <t>027</t>
         </is>
@@ -83817,7 +83817,7 @@
           <t>479</t>
         </is>
       </c>
-      <c r="AA479" s="13" t="inlineStr">
+      <c r="AA479" s="17" t="inlineStr">
         <is>
           <t>720</t>
         </is>
@@ -83909,7 +83909,7 @@
           <t>551</t>
         </is>
       </c>
-      <c r="H480" s="7" t="inlineStr">
+      <c r="H480" s="17" t="inlineStr">
         <is>
           <t>234</t>
         </is>
@@ -84054,7 +84054,7 @@
           <t>033</t>
         </is>
       </c>
-      <c r="AK480" s="17" t="inlineStr">
+      <c r="AK480" s="16" t="inlineStr">
         <is>
           <t>204</t>
         </is>
@@ -84096,7 +84096,7 @@
           <t>186</t>
         </is>
       </c>
-      <c r="H481" s="7" t="inlineStr">
+      <c r="H481" s="17" t="inlineStr">
         <is>
           <t>702</t>
         </is>
@@ -84151,7 +84151,7 @@
           <t>707</t>
         </is>
       </c>
-      <c r="S481" s="10" t="inlineStr">
+      <c r="S481" s="17" t="inlineStr">
         <is>
           <t>720</t>
         </is>
@@ -85066,7 +85066,7 @@
           <t>369</t>
         </is>
       </c>
-      <c r="O486" s="9" t="inlineStr">
+      <c r="O486" s="17" t="inlineStr">
         <is>
           <t>702</t>
         </is>
@@ -85233,7 +85233,7 @@
           <t>436</t>
         </is>
       </c>
-      <c r="K487" s="8" t="inlineStr">
+      <c r="K487" s="17" t="inlineStr">
         <is>
           <t>243</t>
         </is>
@@ -87684,7 +87684,7 @@
           <t>191</t>
         </is>
       </c>
-      <c r="AI502" s="16" t="inlineStr">
+      <c r="AI502" s="17" t="inlineStr">
         <is>
           <t>324</t>
         </is>
@@ -88100,7 +88100,7 @@
           <t>037</t>
         </is>
       </c>
-      <c r="F505" s="6" t="inlineStr">
+      <c r="F505" s="17" t="inlineStr">
         <is>
           <t>027</t>
         </is>
@@ -88614,7 +88614,7 @@
           <t>583</t>
         </is>
       </c>
-      <c r="AH507" s="15" t="inlineStr">
+      <c r="AH507" s="17" t="inlineStr">
         <is>
           <t>027</t>
         </is>
@@ -89721,7 +89721,7 @@
           <t>039</t>
         </is>
       </c>
-      <c r="AE513" s="17" t="inlineStr">
+      <c r="AE513" s="14" t="inlineStr">
         <is>
           <t>204</t>
         </is>
@@ -89913,7 +89913,7 @@
           <t>445</t>
         </is>
       </c>
-      <c r="AF514" s="17" t="inlineStr">
+      <c r="AF514" s="15" t="inlineStr">
         <is>
           <t>024</t>
         </is>
@@ -90095,7 +90095,7 @@
           <t>939</t>
         </is>
       </c>
-      <c r="AE515" s="14" t="inlineStr">
+      <c r="AE515" s="17" t="inlineStr">
         <is>
           <t>270</t>
         </is>
@@ -90698,12 +90698,12 @@
           <t>27</t>
         </is>
       </c>
-      <c r="B519" s="5" t="inlineStr">
+      <c r="B519" s="17" t="inlineStr">
         <is>
           <t>324</t>
         </is>
       </c>
-      <c r="C519" s="5" t="inlineStr">
+      <c r="C519" s="17" t="inlineStr">
         <is>
           <t>720</t>
         </is>
@@ -90823,7 +90823,7 @@
           <t>448</t>
         </is>
       </c>
-      <c r="AA519" s="13" t="inlineStr">
+      <c r="AA519" s="17" t="inlineStr">
         <is>
           <t>423</t>
         </is>
@@ -91989,7 +91989,7 @@
           <t>975</t>
         </is>
       </c>
-      <c r="F533" s="6" t="inlineStr">
+      <c r="F533" s="17" t="inlineStr">
         <is>
           <t>027</t>
         </is>
@@ -92103,7 +92103,7 @@
           <t>601</t>
         </is>
       </c>
-      <c r="H535" s="7" t="inlineStr">
+      <c r="H535" s="17" t="inlineStr">
         <is>
           <t>342</t>
         </is>
@@ -92462,7 +92462,7 @@
           <t>166</t>
         </is>
       </c>
-      <c r="G542" s="6" t="inlineStr">
+      <c r="G542" s="17" t="inlineStr">
         <is>
           <t>324</t>
         </is>
@@ -92546,7 +92546,7 @@
           <t>622</t>
         </is>
       </c>
-      <c r="C544" s="5" t="inlineStr">
+      <c r="C544" s="17" t="inlineStr">
         <is>
           <t>027</t>
         </is>
@@ -92729,17 +92729,17 @@
       </c>
       <c r="H547" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>044</t>
         </is>
       </c>
       <c r="I547" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>377</t>
         </is>
       </c>
       <c r="J547" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>631</t>
         </is>
       </c>
     </row>
@@ -92781,17 +92781,17 @@
       </c>
       <c r="H548" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>438</t>
         </is>
       </c>
       <c r="I548" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>782</t>
         </is>
       </c>
       <c r="J548" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>790</t>
         </is>
       </c>
     </row>
@@ -92833,17 +92833,17 @@
       </c>
       <c r="H549" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>689</t>
         </is>
       </c>
       <c r="I549" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>561</t>
         </is>
       </c>
       <c r="J549" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>134</t>
         </is>
       </c>
     </row>
@@ -92885,17 +92885,17 @@
       </c>
       <c r="H550" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>340</t>
         </is>
       </c>
       <c r="I550" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>404</t>
         </is>
       </c>
       <c r="J550" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>560</t>
         </is>
       </c>
     </row>
@@ -92937,17 +92937,17 @@
       </c>
       <c r="H551" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>438</t>
         </is>
       </c>
       <c r="I551" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>453</t>
         </is>
       </c>
       <c r="J551" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>370</t>
         </is>
       </c>
     </row>
@@ -92989,17 +92989,17 @@
       </c>
       <c r="H552" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>968</t>
         </is>
       </c>
       <c r="I552" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>406</t>
         </is>
       </c>
       <c r="J552" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>461</t>
         </is>
       </c>
     </row>
@@ -93041,17 +93041,17 @@
       </c>
       <c r="H553" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>245</t>
         </is>
       </c>
       <c r="I553" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>200</t>
         </is>
       </c>
       <c r="J553" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>913</t>
         </is>
       </c>
     </row>
@@ -93093,17 +93093,17 @@
       </c>
       <c r="H554" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>321</t>
         </is>
       </c>
       <c r="I554" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>463</t>
         </is>
       </c>
       <c r="J554" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>788</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
update solid pattern info
</commit_message>
<xml_diff>
--- a/swertres/excel_results.xlsx
+++ b/swertres/excel_results.xlsx
@@ -48,17 +48,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="00FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="00ff6633"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="00ccff33"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FFFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -223,10 +223,10 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
@@ -253,7 +253,7 @@
     <xf numFmtId="0" fontId="1" fillId="14" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2176,7 +2176,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="G10" s="6" t="inlineStr">
+      <c r="G10" s="17" t="inlineStr">
         <is>
           <t>560</t>
         </is>
@@ -2206,7 +2206,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="M10" s="8" t="inlineStr">
+      <c r="M10" s="17" t="inlineStr">
         <is>
           <t>199</t>
         </is>
@@ -2782,7 +2782,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="P13" s="17" t="inlineStr">
+      <c r="P13" s="9" t="inlineStr">
         <is>
           <t>234</t>
         </is>
@@ -3605,7 +3605,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="AE17" s="14" t="inlineStr">
+      <c r="AE17" s="17" t="inlineStr">
         <is>
           <t>506</t>
         </is>
@@ -3807,7 +3807,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="AH18" s="17" t="inlineStr">
+      <c r="AH18" s="15" t="inlineStr">
         <is>
           <t>702</t>
         </is>
@@ -4368,7 +4368,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="AH21" s="17" t="inlineStr">
+      <c r="AH21" s="15" t="inlineStr">
         <is>
           <t>342</t>
         </is>
@@ -5198,7 +5198,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="M26" s="17" t="inlineStr">
+      <c r="M26" s="8" t="inlineStr">
         <is>
           <t>072</t>
         </is>
@@ -6928,7 +6928,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="E38" s="17" t="inlineStr">
+      <c r="E38" s="6" t="inlineStr">
         <is>
           <t>702</t>
         </is>
@@ -7170,7 +7170,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="P39" s="17" t="inlineStr">
+      <c r="P39" s="9" t="inlineStr">
         <is>
           <t>342</t>
         </is>
@@ -7848,7 +7848,7 @@
           <t>06</t>
         </is>
       </c>
-      <c r="B43" s="5" t="inlineStr">
+      <c r="B43" s="17" t="inlineStr">
         <is>
           <t>506</t>
         </is>
@@ -7953,7 +7953,7 @@
           <t>817</t>
         </is>
       </c>
-      <c r="W43" s="17" t="inlineStr">
+      <c r="W43" s="12" t="inlineStr">
         <is>
           <t>432</t>
         </is>
@@ -8357,7 +8357,7 @@
           <t>346</t>
         </is>
       </c>
-      <c r="AC45" s="17" t="inlineStr">
+      <c r="AC45" s="14" t="inlineStr">
         <is>
           <t>243</t>
         </is>
@@ -8636,7 +8636,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="J47" s="17" t="inlineStr">
+      <c r="J47" s="7" t="inlineStr">
         <is>
           <t>342</t>
         </is>
@@ -9262,7 +9262,7 @@
           <t>955</t>
         </is>
       </c>
-      <c r="W50" s="12" t="inlineStr">
+      <c r="W50" s="17" t="inlineStr">
         <is>
           <t>991</t>
         </is>
@@ -9504,7 +9504,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="AH51" s="17" t="inlineStr">
+      <c r="AH51" s="15" t="inlineStr">
         <is>
           <t>072</t>
         </is>
@@ -9743,7 +9743,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="G53" s="17" t="inlineStr">
+      <c r="G53" s="6" t="inlineStr">
         <is>
           <t>270</t>
         </is>
@@ -9758,7 +9758,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="J53" s="17" t="inlineStr">
+      <c r="J53" s="7" t="inlineStr">
         <is>
           <t>072</t>
         </is>
@@ -10092,7 +10092,7 @@
           <t>18</t>
         </is>
       </c>
-      <c r="B55" s="17" t="inlineStr">
+      <c r="B55" s="5" t="inlineStr">
         <is>
           <t>423</t>
         </is>
@@ -10177,7 +10177,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="S55" s="10" t="inlineStr">
+      <c r="S55" s="17" t="inlineStr">
         <is>
           <t>065</t>
         </is>
@@ -10414,7 +10414,7 @@
           <t>837</t>
         </is>
       </c>
-      <c r="AC56" s="14" t="inlineStr">
+      <c r="AC56" s="17" t="inlineStr">
         <is>
           <t>199</t>
         </is>
@@ -10586,7 +10586,7 @@
           <t>767</t>
         </is>
       </c>
-      <c r="Z57" s="13" t="inlineStr">
+      <c r="Z57" s="17" t="inlineStr">
         <is>
           <t>056</t>
         </is>
@@ -10813,7 +10813,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="AH58" s="15" t="inlineStr">
+      <c r="AH58" s="17" t="inlineStr">
         <is>
           <t>919</t>
         </is>
@@ -11015,7 +11015,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="AK59" s="17" t="inlineStr">
+      <c r="AK59" s="16" t="inlineStr">
         <is>
           <t>342</t>
         </is>
@@ -11132,7 +11132,7 @@
           <t>130</t>
         </is>
       </c>
-      <c r="W60" s="17" t="inlineStr">
+      <c r="W60" s="12" t="inlineStr">
         <is>
           <t>072</t>
         </is>
@@ -11319,7 +11319,7 @@
           <t>617</t>
         </is>
       </c>
-      <c r="W61" s="17" t="inlineStr">
+      <c r="W61" s="12" t="inlineStr">
         <is>
           <t>342</t>
         </is>
@@ -11940,7 +11940,7 @@
           <t>930</t>
         </is>
       </c>
-      <c r="AI64" s="17" t="inlineStr">
+      <c r="AI64" s="16" t="inlineStr">
         <is>
           <t>432</t>
         </is>
@@ -12314,7 +12314,7 @@
           <t>339</t>
         </is>
       </c>
-      <c r="AI66" s="16" t="inlineStr">
+      <c r="AI66" s="17" t="inlineStr">
         <is>
           <t>506</t>
         </is>
@@ -13211,7 +13211,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="J74" s="7" t="inlineStr">
+      <c r="J74" s="17" t="inlineStr">
         <is>
           <t>065</t>
         </is>
@@ -13635,7 +13635,7 @@
           <t>510</t>
         </is>
       </c>
-      <c r="T76" s="17" t="inlineStr">
+      <c r="T76" s="11" t="inlineStr">
         <is>
           <t>027</t>
         </is>
@@ -13882,7 +13882,7 @@
           <t>753</t>
         </is>
       </c>
-      <c r="AF77" s="15" t="inlineStr">
+      <c r="AF77" s="17" t="inlineStr">
         <is>
           <t>506</t>
         </is>
@@ -13984,7 +13984,7 @@
           <t>886</t>
         </is>
       </c>
-      <c r="O78" s="9" t="inlineStr">
+      <c r="O78" s="17" t="inlineStr">
         <is>
           <t>650</t>
         </is>
@@ -14383,7 +14383,7 @@
           <t>706</t>
         </is>
       </c>
-      <c r="T80" s="11" t="inlineStr">
+      <c r="T80" s="17" t="inlineStr">
         <is>
           <t>199</t>
         </is>
@@ -14560,7 +14560,7 @@
           <t>005</t>
         </is>
       </c>
-      <c r="R81" s="10" t="inlineStr">
+      <c r="R81" s="17" t="inlineStr">
         <is>
           <t>650</t>
         </is>
@@ -14827,7 +14827,7 @@
           <t>858</t>
         </is>
       </c>
-      <c r="AH82" s="17" t="inlineStr">
+      <c r="AH82" s="15" t="inlineStr">
         <is>
           <t>324</t>
         </is>
@@ -14869,7 +14869,7 @@
           <t>313</t>
         </is>
       </c>
-      <c r="E83" s="6" t="inlineStr">
+      <c r="E83" s="17" t="inlineStr">
         <is>
           <t>991</t>
         </is>
@@ -14984,12 +14984,12 @@
           <t>023</t>
         </is>
       </c>
-      <c r="AB83" s="13" t="inlineStr">
+      <c r="AB83" s="17" t="inlineStr">
         <is>
           <t>650</t>
         </is>
       </c>
-      <c r="AC83" s="14" t="inlineStr">
+      <c r="AC83" s="17" t="inlineStr">
         <is>
           <t>991</t>
         </is>
@@ -15348,7 +15348,7 @@
           <t>136</t>
         </is>
       </c>
-      <c r="Z85" s="13" t="inlineStr">
+      <c r="Z85" s="17" t="inlineStr">
         <is>
           <t>056</t>
         </is>
@@ -15363,7 +15363,7 @@
           <t>269</t>
         </is>
       </c>
-      <c r="AC85" s="14" t="inlineStr">
+      <c r="AC85" s="17" t="inlineStr">
         <is>
           <t>056</t>
         </is>
@@ -15667,7 +15667,7 @@
           <t>904</t>
         </is>
       </c>
-      <c r="O87" s="17" t="inlineStr">
+      <c r="O87" s="9" t="inlineStr">
         <is>
           <t>720</t>
         </is>
@@ -16263,7 +16263,7 @@
           <t>798</t>
         </is>
       </c>
-      <c r="V90" s="17" t="inlineStr">
+      <c r="V90" s="11" t="inlineStr">
         <is>
           <t>720</t>
         </is>
@@ -17036,7 +17036,7 @@
           <t>028</t>
         </is>
       </c>
-      <c r="AA94" s="13" t="inlineStr">
+      <c r="AA94" s="17" t="inlineStr">
         <is>
           <t>199</t>
         </is>
@@ -17749,7 +17749,7 @@
           <t>408</t>
         </is>
       </c>
-      <c r="T98" s="17" t="inlineStr">
+      <c r="T98" s="11" t="inlineStr">
         <is>
           <t>027</t>
         </is>
@@ -17931,7 +17931,7 @@
           <t>748</t>
         </is>
       </c>
-      <c r="S99" s="17" t="inlineStr">
+      <c r="S99" s="10" t="inlineStr">
         <is>
           <t>234</t>
         </is>
@@ -18048,7 +18048,7 @@
           <t>811</t>
         </is>
       </c>
-      <c r="E100" s="6" t="inlineStr">
+      <c r="E100" s="17" t="inlineStr">
         <is>
           <t>560</t>
         </is>
@@ -18128,7 +18128,7 @@
           <t>863</t>
         </is>
       </c>
-      <c r="U100" s="17" t="inlineStr">
+      <c r="U100" s="11" t="inlineStr">
         <is>
           <t>234</t>
         </is>
@@ -18335,7 +18335,7 @@
           <t>031</t>
         </is>
       </c>
-      <c r="Y101" s="17" t="inlineStr">
+      <c r="Y101" s="12" t="inlineStr">
         <is>
           <t>342</t>
         </is>
@@ -19085,7 +19085,7 @@
           <t>846</t>
         </is>
       </c>
-      <c r="H108" s="17" t="inlineStr">
+      <c r="H108" s="7" t="inlineStr">
         <is>
           <t>324</t>
         </is>
@@ -19519,7 +19519,7 @@
           <t>247</t>
         </is>
       </c>
-      <c r="T110" s="11" t="inlineStr">
+      <c r="T110" s="17" t="inlineStr">
         <is>
           <t>199</t>
         </is>
@@ -19781,7 +19781,7 @@
           <t>883</t>
         </is>
       </c>
-      <c r="AI111" s="17" t="inlineStr">
+      <c r="AI111" s="16" t="inlineStr">
         <is>
           <t>072</t>
         </is>
@@ -19918,7 +19918,7 @@
           <t>357</t>
         </is>
       </c>
-      <c r="Y112" s="17" t="inlineStr">
+      <c r="Y112" s="12" t="inlineStr">
         <is>
           <t>243</t>
         </is>
@@ -20287,7 +20287,7 @@
           <t>881</t>
         </is>
       </c>
-      <c r="X114" s="12" t="inlineStr">
+      <c r="X114" s="17" t="inlineStr">
         <is>
           <t>919</t>
         </is>
@@ -21865,7 +21865,7 @@
           <t>172</t>
         </is>
       </c>
-      <c r="C123" s="5" t="inlineStr">
+      <c r="C123" s="17" t="inlineStr">
         <is>
           <t>560</t>
         </is>
@@ -22192,7 +22192,7 @@
           <t>538</t>
         </is>
       </c>
-      <c r="AE124" s="14" t="inlineStr">
+      <c r="AE124" s="17" t="inlineStr">
         <is>
           <t>199</t>
         </is>
@@ -22436,7 +22436,7 @@
           <t>277</t>
         </is>
       </c>
-      <c r="E126" s="6" t="inlineStr">
+      <c r="E126" s="17" t="inlineStr">
         <is>
           <t>056</t>
         </is>
@@ -22638,7 +22638,7 @@
           <t>739</t>
         </is>
       </c>
-      <c r="H127" s="17" t="inlineStr">
+      <c r="H127" s="7" t="inlineStr">
         <is>
           <t>423</t>
         </is>
@@ -22663,7 +22663,7 @@
           <t>405</t>
         </is>
       </c>
-      <c r="M127" s="8" t="inlineStr">
+      <c r="M127" s="17" t="inlineStr">
         <is>
           <t>506</t>
         </is>
@@ -22773,7 +22773,7 @@
           <t>978</t>
         </is>
       </c>
-      <c r="AI127" s="16" t="inlineStr">
+      <c r="AI127" s="17" t="inlineStr">
         <is>
           <t>605</t>
         </is>
@@ -22850,7 +22850,7 @@
           <t>267</t>
         </is>
       </c>
-      <c r="M128" s="17" t="inlineStr">
+      <c r="M128" s="8" t="inlineStr">
         <is>
           <t>720</t>
         </is>
@@ -22895,7 +22895,7 @@
           <t>377</t>
         </is>
       </c>
-      <c r="V128" s="17" t="inlineStr">
+      <c r="V128" s="11" t="inlineStr">
         <is>
           <t>720</t>
         </is>
@@ -23087,7 +23087,7 @@
           <t>906</t>
         </is>
       </c>
-      <c r="W129" s="17" t="inlineStr">
+      <c r="W129" s="12" t="inlineStr">
         <is>
           <t>243</t>
         </is>
@@ -23122,7 +23122,7 @@
           <t>450</t>
         </is>
       </c>
-      <c r="AD129" s="17" t="inlineStr">
+      <c r="AD129" s="14" t="inlineStr">
         <is>
           <t>270</t>
         </is>
@@ -23451,7 +23451,7 @@
           <t>717</t>
         </is>
       </c>
-      <c r="U131" s="17" t="inlineStr">
+      <c r="U131" s="11" t="inlineStr">
         <is>
           <t>423</t>
         </is>
@@ -23461,7 +23461,7 @@
           <t>205</t>
         </is>
       </c>
-      <c r="W131" s="12" t="inlineStr">
+      <c r="W131" s="17" t="inlineStr">
         <is>
           <t>560</t>
         </is>
@@ -23501,7 +23501,7 @@
           <t>827</t>
         </is>
       </c>
-      <c r="AE131" s="14" t="inlineStr">
+      <c r="AE131" s="17" t="inlineStr">
         <is>
           <t>199</t>
         </is>
@@ -23543,7 +23543,7 @@
           <t>25</t>
         </is>
       </c>
-      <c r="B132" s="17" t="inlineStr">
+      <c r="B132" s="5" t="inlineStr">
         <is>
           <t>243</t>
         </is>
@@ -23563,7 +23563,7 @@
           <t>543</t>
         </is>
       </c>
-      <c r="F132" s="6" t="inlineStr">
+      <c r="F132" s="17" t="inlineStr">
         <is>
           <t>919</t>
         </is>
@@ -23900,7 +23900,7 @@
           <t>209</t>
         </is>
       </c>
-      <c r="AJ133" s="16" t="inlineStr">
+      <c r="AJ133" s="17" t="inlineStr">
         <is>
           <t>560</t>
         </is>
@@ -24239,7 +24239,7 @@
           <t>586</t>
         </is>
       </c>
-      <c r="AC135" s="17" t="inlineStr">
+      <c r="AC135" s="14" t="inlineStr">
         <is>
           <t>702</t>
         </is>
@@ -24588,7 +24588,7 @@
           <t>158</t>
         </is>
       </c>
-      <c r="X137" s="12" t="inlineStr">
+      <c r="X137" s="17" t="inlineStr">
         <is>
           <t>065</t>
         </is>
@@ -24628,7 +24628,7 @@
           <t>640</t>
         </is>
       </c>
-      <c r="AF137" s="15" t="inlineStr">
+      <c r="AF137" s="17" t="inlineStr">
         <is>
           <t>605</t>
         </is>
@@ -24775,7 +24775,7 @@
           <t>239</t>
         </is>
       </c>
-      <c r="X138" s="17" t="inlineStr">
+      <c r="X138" s="12" t="inlineStr">
         <is>
           <t>423</t>
         </is>
@@ -25151,7 +25151,7 @@
           <t>263</t>
         </is>
       </c>
-      <c r="G143" s="6" t="inlineStr">
+      <c r="G143" s="17" t="inlineStr">
         <is>
           <t>650</t>
         </is>
@@ -25423,7 +25423,7 @@
           <t>014</t>
         </is>
       </c>
-      <c r="X144" s="12" t="inlineStr">
+      <c r="X144" s="17" t="inlineStr">
         <is>
           <t>199</t>
         </is>
@@ -25510,7 +25510,7 @@
           <t>517</t>
         </is>
       </c>
-      <c r="D145" s="17" t="inlineStr">
+      <c r="D145" s="5" t="inlineStr">
         <is>
           <t>324</t>
         </is>
@@ -25949,7 +25949,7 @@
           <t>525</t>
         </is>
       </c>
-      <c r="Q147" s="10" t="inlineStr">
+      <c r="Q147" s="17" t="inlineStr">
         <is>
           <t>991</t>
         </is>
@@ -26226,7 +26226,7 @@
           <t>439</t>
         </is>
       </c>
-      <c r="AI148" s="17" t="inlineStr">
+      <c r="AI148" s="16" t="inlineStr">
         <is>
           <t>342</t>
         </is>
@@ -26540,7 +26540,7 @@
           <t>880</t>
         </is>
       </c>
-      <c r="W150" s="17" t="inlineStr">
+      <c r="W150" s="12" t="inlineStr">
         <is>
           <t>720</t>
         </is>
@@ -26929,7 +26929,7 @@
           <t>019</t>
         </is>
       </c>
-      <c r="Z152" s="13" t="inlineStr">
+      <c r="Z152" s="17" t="inlineStr">
         <is>
           <t>991</t>
         </is>
@@ -26939,7 +26939,7 @@
           <t>470</t>
         </is>
       </c>
-      <c r="AB152" s="17" t="inlineStr">
+      <c r="AB152" s="13" t="inlineStr">
         <is>
           <t>324</t>
         </is>
@@ -27076,12 +27076,12 @@
           <t>487</t>
         </is>
       </c>
-      <c r="R153" s="17" t="inlineStr">
+      <c r="R153" s="10" t="inlineStr">
         <is>
           <t>243</t>
         </is>
       </c>
-      <c r="S153" s="17" t="inlineStr">
+      <c r="S153" s="10" t="inlineStr">
         <is>
           <t>027</t>
         </is>
@@ -27218,7 +27218,7 @@
           <t>428</t>
         </is>
       </c>
-      <c r="I154" s="17" t="inlineStr">
+      <c r="I154" s="7" t="inlineStr">
         <is>
           <t>243</t>
         </is>
@@ -27662,7 +27662,7 @@
           <t>538</t>
         </is>
       </c>
-      <c r="W156" s="17" t="inlineStr">
+      <c r="W156" s="12" t="inlineStr">
         <is>
           <t>432</t>
         </is>
@@ -29203,7 +29203,7 @@
           <t>076</t>
         </is>
       </c>
-      <c r="AF164" s="17" t="inlineStr">
+      <c r="AF164" s="15" t="inlineStr">
         <is>
           <t>702</t>
         </is>
@@ -29335,7 +29335,7 @@
           <t>806</t>
         </is>
       </c>
-      <c r="U165" s="11" t="inlineStr">
+      <c r="U165" s="17" t="inlineStr">
         <is>
           <t>991</t>
         </is>
@@ -29502,7 +29502,7 @@
           <t>475</t>
         </is>
       </c>
-      <c r="Q166" s="10" t="inlineStr">
+      <c r="Q166" s="17" t="inlineStr">
         <is>
           <t>199</t>
         </is>
@@ -29614,7 +29614,7 @@
           <t>25</t>
         </is>
       </c>
-      <c r="B167" s="5" t="inlineStr">
+      <c r="B167" s="17" t="inlineStr">
         <is>
           <t>991</t>
         </is>
@@ -30649,7 +30649,7 @@
           <t>317</t>
         </is>
       </c>
-      <c r="V172" s="11" t="inlineStr">
+      <c r="V172" s="17" t="inlineStr">
         <is>
           <t>560</t>
         </is>
@@ -30679,7 +30679,7 @@
           <t>620</t>
         </is>
       </c>
-      <c r="AB172" s="13" t="inlineStr">
+      <c r="AB172" s="17" t="inlineStr">
         <is>
           <t>919</t>
         </is>
@@ -30689,7 +30689,7 @@
           <t>909</t>
         </is>
       </c>
-      <c r="AD172" s="17" t="inlineStr">
+      <c r="AD172" s="14" t="inlineStr">
         <is>
           <t>342</t>
         </is>
@@ -31763,7 +31763,7 @@
           <t>462</t>
         </is>
       </c>
-      <c r="C181" s="17" t="inlineStr">
+      <c r="C181" s="5" t="inlineStr">
         <is>
           <t>324</t>
         </is>
@@ -31858,7 +31858,7 @@
           <t>803</t>
         </is>
       </c>
-      <c r="V181" s="17" t="inlineStr">
+      <c r="V181" s="11" t="inlineStr">
         <is>
           <t>270</t>
         </is>
@@ -32000,7 +32000,7 @@
           <t>408</t>
         </is>
       </c>
-      <c r="M182" s="8" t="inlineStr">
+      <c r="M182" s="17" t="inlineStr">
         <is>
           <t>991</t>
         </is>
@@ -32025,7 +32025,7 @@
           <t>520</t>
         </is>
       </c>
-      <c r="R182" s="10" t="inlineStr">
+      <c r="R182" s="17" t="inlineStr">
         <is>
           <t>199</t>
         </is>
@@ -32561,7 +32561,7 @@
           <t>950</t>
         </is>
       </c>
-      <c r="M185" s="8" t="inlineStr">
+      <c r="M185" s="17" t="inlineStr">
         <is>
           <t>065</t>
         </is>
@@ -32601,7 +32601,7 @@
           <t>841</t>
         </is>
       </c>
-      <c r="U185" s="11" t="inlineStr">
+      <c r="U185" s="17" t="inlineStr">
         <is>
           <t>056</t>
         </is>
@@ -32880,7 +32880,7 @@
           <t>10</t>
         </is>
       </c>
-      <c r="B187" s="5" t="inlineStr">
+      <c r="B187" s="17" t="inlineStr">
         <is>
           <t>605</t>
         </is>
@@ -33010,7 +33010,7 @@
           <t>406</t>
         </is>
       </c>
-      <c r="AB187" s="13" t="inlineStr">
+      <c r="AB187" s="17" t="inlineStr">
         <is>
           <t>605</t>
         </is>
@@ -33217,7 +33217,7 @@
           <t>898</t>
         </is>
       </c>
-      <c r="AF188" s="17" t="inlineStr">
+      <c r="AF188" s="15" t="inlineStr">
         <is>
           <t>243</t>
         </is>
@@ -33409,7 +33409,7 @@
           <t>565</t>
         </is>
       </c>
-      <c r="AG189" s="17" t="inlineStr">
+      <c r="AG189" s="15" t="inlineStr">
         <is>
           <t>423</t>
         </is>
@@ -33536,7 +33536,7 @@
           <t>251</t>
         </is>
       </c>
-      <c r="U190" s="17" t="inlineStr">
+      <c r="U190" s="11" t="inlineStr">
         <is>
           <t>270</t>
         </is>
@@ -33728,7 +33728,7 @@
           <t>833</t>
         </is>
       </c>
-      <c r="V191" s="11" t="inlineStr">
+      <c r="V191" s="17" t="inlineStr">
         <is>
           <t>650</t>
         </is>
@@ -33738,7 +33738,7 @@
           <t>728</t>
         </is>
       </c>
-      <c r="X191" s="12" t="inlineStr">
+      <c r="X191" s="17" t="inlineStr">
         <is>
           <t>919</t>
         </is>
@@ -34022,7 +34022,7 @@
           <t>970</t>
         </is>
       </c>
-      <c r="F193" s="17" t="inlineStr">
+      <c r="F193" s="6" t="inlineStr">
         <is>
           <t>027</t>
         </is>
@@ -34107,7 +34107,7 @@
           <t>825</t>
         </is>
       </c>
-      <c r="W193" s="12" t="inlineStr">
+      <c r="W193" s="17" t="inlineStr">
         <is>
           <t>560</t>
         </is>
@@ -34152,7 +34152,7 @@
           <t>438</t>
         </is>
       </c>
-      <c r="AF193" s="15" t="inlineStr">
+      <c r="AF193" s="17" t="inlineStr">
         <is>
           <t>991</t>
         </is>
@@ -34618,7 +34618,7 @@
           <t>989</t>
         </is>
       </c>
-      <c r="M196" s="17" t="inlineStr">
+      <c r="M196" s="8" t="inlineStr">
         <is>
           <t>243</t>
         </is>
@@ -34713,7 +34713,7 @@
           <t>069</t>
         </is>
       </c>
-      <c r="AF196" s="17" t="inlineStr">
+      <c r="AF196" s="15" t="inlineStr">
         <is>
           <t>423</t>
         </is>
@@ -34738,7 +34738,7 @@
           <t>980</t>
         </is>
       </c>
-      <c r="AK196" s="16" t="inlineStr">
+      <c r="AK196" s="17" t="inlineStr">
         <is>
           <t>199</t>
         </is>
@@ -34925,7 +34925,7 @@
           <t>773</t>
         </is>
       </c>
-      <c r="AK197" s="16" t="inlineStr">
+      <c r="AK197" s="17" t="inlineStr">
         <is>
           <t>560</t>
         </is>
@@ -34942,7 +34942,7 @@
           <t>087</t>
         </is>
       </c>
-      <c r="C198" s="17" t="inlineStr">
+      <c r="C198" s="5" t="inlineStr">
         <is>
           <t>720</t>
         </is>
@@ -35007,7 +35007,7 @@
           <t>477</t>
         </is>
       </c>
-      <c r="P198" s="9" t="inlineStr">
+      <c r="P198" s="17" t="inlineStr">
         <is>
           <t>199</t>
         </is>
@@ -35092,7 +35092,7 @@
           <t>177</t>
         </is>
       </c>
-      <c r="AG198" s="15" t="inlineStr">
+      <c r="AG198" s="17" t="inlineStr">
         <is>
           <t>056</t>
         </is>
@@ -35259,7 +35259,7 @@
           <t>059</t>
         </is>
       </c>
-      <c r="AC199" s="17" t="inlineStr">
+      <c r="AC199" s="14" t="inlineStr">
         <is>
           <t>207</t>
         </is>
@@ -35346,7 +35346,7 @@
           <t>715</t>
         </is>
       </c>
-      <c r="I200" s="17" t="inlineStr">
+      <c r="I200" s="7" t="inlineStr">
         <is>
           <t>234</t>
         </is>
@@ -35987,7 +35987,7 @@
           <t>068</t>
         </is>
       </c>
-      <c r="Y203" s="17" t="inlineStr">
+      <c r="Y203" s="12" t="inlineStr">
         <is>
           <t>243</t>
         </is>
@@ -36528,7 +36528,7 @@
           <t>669</t>
         </is>
       </c>
-      <c r="U206" s="11" t="inlineStr">
+      <c r="U206" s="17" t="inlineStr">
         <is>
           <t>650</t>
         </is>
@@ -36750,7 +36750,7 @@
           <t>658</t>
         </is>
       </c>
-      <c r="AB207" s="13" t="inlineStr">
+      <c r="AB207" s="17" t="inlineStr">
         <is>
           <t>199</t>
         </is>
@@ -37368,7 +37368,7 @@
           <t>965</t>
         </is>
       </c>
-      <c r="V213" s="11" t="inlineStr">
+      <c r="V213" s="17" t="inlineStr">
         <is>
           <t>199</t>
         </is>
@@ -38116,7 +38116,7 @@
           <t>905</t>
         </is>
       </c>
-      <c r="V217" s="17" t="inlineStr">
+      <c r="V217" s="11" t="inlineStr">
         <is>
           <t>423</t>
         </is>
@@ -38318,7 +38318,7 @@
           <t>041</t>
         </is>
       </c>
-      <c r="Y218" s="12" t="inlineStr">
+      <c r="Y218" s="17" t="inlineStr">
         <is>
           <t>199</t>
         </is>
@@ -38395,7 +38395,7 @@
           <t>499</t>
         </is>
       </c>
-      <c r="C219" s="5" t="inlineStr">
+      <c r="C219" s="17" t="inlineStr">
         <is>
           <t>506</t>
         </is>
@@ -38410,7 +38410,7 @@
           <t>957</t>
         </is>
       </c>
-      <c r="F219" s="6" t="inlineStr">
+      <c r="F219" s="17" t="inlineStr">
         <is>
           <t>065</t>
         </is>
@@ -38637,7 +38637,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="N220" s="9" t="inlineStr">
+      <c r="N220" s="17" t="inlineStr">
         <is>
           <t>056</t>
         </is>
@@ -38879,7 +38879,7 @@
           <t>359</t>
         </is>
       </c>
-      <c r="Y221" s="12" t="inlineStr">
+      <c r="Y221" s="17" t="inlineStr">
         <is>
           <t>560</t>
         </is>
@@ -38939,7 +38939,7 @@
           <t>018</t>
         </is>
       </c>
-      <c r="AK221" s="17" t="inlineStr">
+      <c r="AK221" s="16" t="inlineStr">
         <is>
           <t>342</t>
         </is>
@@ -39298,7 +39298,7 @@
           <t>795</t>
         </is>
       </c>
-      <c r="AH223" s="15" t="inlineStr">
+      <c r="AH223" s="17" t="inlineStr">
         <is>
           <t>506</t>
         </is>
@@ -39734,7 +39734,7 @@
           <t>488</t>
         </is>
       </c>
-      <c r="I226" s="17" t="inlineStr">
+      <c r="I226" s="7" t="inlineStr">
         <is>
           <t>072</t>
         </is>
@@ -39869,7 +39869,7 @@
           <t>411</t>
         </is>
       </c>
-      <c r="AJ226" s="17" t="inlineStr">
+      <c r="AJ226" s="16" t="inlineStr">
         <is>
           <t>207</t>
         </is>
@@ -40183,7 +40183,7 @@
           <t>479</t>
         </is>
       </c>
-      <c r="X228" s="17" t="inlineStr">
+      <c r="X228" s="12" t="inlineStr">
         <is>
           <t>720</t>
         </is>
@@ -40634,7 +40634,7 @@
           <t>19</t>
         </is>
       </c>
-      <c r="B231" s="17" t="inlineStr">
+      <c r="B231" s="5" t="inlineStr">
         <is>
           <t>234</t>
         </is>
@@ -40759,7 +40759,7 @@
           <t>122</t>
         </is>
       </c>
-      <c r="AA231" s="17" t="inlineStr">
+      <c r="AA231" s="13" t="inlineStr">
         <is>
           <t>432</t>
         </is>
@@ -40981,7 +40981,7 @@
           <t>671</t>
         </is>
       </c>
-      <c r="AH232" s="17" t="inlineStr">
+      <c r="AH232" s="15" t="inlineStr">
         <is>
           <t>720</t>
         </is>
@@ -41088,7 +41088,7 @@
           <t>615</t>
         </is>
       </c>
-      <c r="R233" s="17" t="inlineStr">
+      <c r="R233" s="10" t="inlineStr">
         <is>
           <t>234</t>
         </is>
@@ -41629,7 +41629,7 @@
           <t>372</t>
         </is>
       </c>
-      <c r="N236" s="17" t="inlineStr">
+      <c r="N236" s="9" t="inlineStr">
         <is>
           <t>027</t>
         </is>
@@ -41821,7 +41821,7 @@
           <t>786</t>
         </is>
       </c>
-      <c r="O237" s="17" t="inlineStr">
+      <c r="O237" s="9" t="inlineStr">
         <is>
           <t>027</t>
         </is>
@@ -42068,7 +42068,7 @@
           <t>935</t>
         </is>
       </c>
-      <c r="AA238" s="17" t="inlineStr">
+      <c r="AA238" s="13" t="inlineStr">
         <is>
           <t>324</t>
         </is>
@@ -42230,7 +42230,7 @@
           <t>881</t>
         </is>
       </c>
-      <c r="V239" s="17" t="inlineStr">
+      <c r="V239" s="11" t="inlineStr">
         <is>
           <t>234</t>
         </is>
@@ -42270,7 +42270,7 @@
           <t>670</t>
         </is>
       </c>
-      <c r="AD239" s="14" t="inlineStr">
+      <c r="AD239" s="17" t="inlineStr">
         <is>
           <t>199</t>
         </is>
@@ -42337,7 +42337,7 @@
           <t>228</t>
         </is>
       </c>
-      <c r="F240" s="17" t="inlineStr">
+      <c r="F240" s="6" t="inlineStr">
         <is>
           <t>432</t>
         </is>
@@ -42664,7 +42664,7 @@
           <t>491</t>
         </is>
       </c>
-      <c r="AH241" s="15" t="inlineStr">
+      <c r="AH241" s="17" t="inlineStr">
         <is>
           <t>199</t>
         </is>
@@ -42674,7 +42674,7 @@
           <t>677</t>
         </is>
       </c>
-      <c r="AJ241" s="16" t="inlineStr">
+      <c r="AJ241" s="17" t="inlineStr">
         <is>
           <t>919</t>
         </is>
@@ -43606,7 +43606,7 @@
           <t>568</t>
         </is>
       </c>
-      <c r="R249" s="10" t="inlineStr">
+      <c r="R249" s="17" t="inlineStr">
         <is>
           <t>991</t>
         </is>
@@ -43621,7 +43621,7 @@
           <t>372</t>
         </is>
       </c>
-      <c r="U249" s="11" t="inlineStr">
+      <c r="U249" s="17" t="inlineStr">
         <is>
           <t>560</t>
         </is>
@@ -43813,7 +43813,7 @@
           <t>341</t>
         </is>
       </c>
-      <c r="V250" s="11" t="inlineStr">
+      <c r="V250" s="17" t="inlineStr">
         <is>
           <t>199</t>
         </is>
@@ -43920,7 +43920,7 @@
           <t>681</t>
         </is>
       </c>
-      <c r="F251" s="17" t="inlineStr">
+      <c r="F251" s="6" t="inlineStr">
         <is>
           <t>720</t>
         </is>
@@ -44092,7 +44092,7 @@
           <t>752</t>
         </is>
       </c>
-      <c r="C252" s="17" t="inlineStr">
+      <c r="C252" s="5" t="inlineStr">
         <is>
           <t>027</t>
         </is>
@@ -44182,7 +44182,7 @@
           <t>813</t>
         </is>
       </c>
-      <c r="U252" s="17" t="inlineStr">
+      <c r="U252" s="11" t="inlineStr">
         <is>
           <t>423</t>
         </is>
@@ -44439,7 +44439,7 @@
           <t>320</t>
         </is>
       </c>
-      <c r="AI253" s="17" t="inlineStr">
+      <c r="AI253" s="16" t="inlineStr">
         <is>
           <t>324</t>
         </is>
@@ -45314,7 +45314,7 @@
           <t>047</t>
         </is>
       </c>
-      <c r="W258" s="17" t="inlineStr">
+      <c r="W258" s="12" t="inlineStr">
         <is>
           <t>270</t>
         </is>
@@ -46017,7 +46017,7 @@
           <t>971</t>
         </is>
       </c>
-      <c r="N262" s="9" t="inlineStr">
+      <c r="N262" s="17" t="inlineStr">
         <is>
           <t>056</t>
         </is>
@@ -46304,7 +46304,7 @@
           <t>756</t>
         </is>
       </c>
-      <c r="AH263" s="17" t="inlineStr">
+      <c r="AH263" s="15" t="inlineStr">
         <is>
           <t>324</t>
         </is>
@@ -47593,7 +47593,7 @@
           <t>549</t>
         </is>
       </c>
-      <c r="AD270" s="17" t="inlineStr">
+      <c r="AD270" s="14" t="inlineStr">
         <is>
           <t>072</t>
         </is>
@@ -47982,7 +47982,7 @@
           <t>080</t>
         </is>
       </c>
-      <c r="AG272" s="17" t="inlineStr">
+      <c r="AG272" s="15" t="inlineStr">
         <is>
           <t>702</t>
         </is>
@@ -48393,7 +48393,7 @@
           <t>753</t>
         </is>
       </c>
-      <c r="C275" s="5" t="inlineStr">
+      <c r="C275" s="17" t="inlineStr">
         <is>
           <t>506</t>
         </is>
@@ -48523,7 +48523,7 @@
           <t>315</t>
         </is>
       </c>
-      <c r="AC275" s="17" t="inlineStr">
+      <c r="AC275" s="14" t="inlineStr">
         <is>
           <t>243</t>
         </is>
@@ -49834,7 +49834,7 @@
           <t>193</t>
         </is>
       </c>
-      <c r="L285" s="8" t="inlineStr">
+      <c r="L285" s="17" t="inlineStr">
         <is>
           <t>560</t>
         </is>
@@ -49939,7 +49939,7 @@
           <t>621</t>
         </is>
       </c>
-      <c r="AG285" s="17" t="inlineStr">
+      <c r="AG285" s="15" t="inlineStr">
         <is>
           <t>324</t>
         </is>
@@ -50126,7 +50126,7 @@
           <t>971</t>
         </is>
       </c>
-      <c r="AG286" s="17" t="inlineStr">
+      <c r="AG286" s="15" t="inlineStr">
         <is>
           <t>027</t>
         </is>
@@ -50233,7 +50233,7 @@
           <t>325</t>
         </is>
       </c>
-      <c r="Q287" s="17" t="inlineStr">
+      <c r="Q287" s="10" t="inlineStr">
         <is>
           <t>720</t>
         </is>
@@ -50470,7 +50470,7 @@
           <t>642</t>
         </is>
       </c>
-      <c r="AA288" s="17" t="inlineStr">
+      <c r="AA288" s="13" t="inlineStr">
         <is>
           <t>342</t>
         </is>
@@ -50769,7 +50769,7 @@
           <t>987</t>
         </is>
       </c>
-      <c r="L290" s="8" t="inlineStr">
+      <c r="L290" s="17" t="inlineStr">
         <is>
           <t>650</t>
         </is>
@@ -51415,7 +51415,7 @@
           <t>320</t>
         </is>
       </c>
-      <c r="AC293" s="17" t="inlineStr">
+      <c r="AC293" s="14" t="inlineStr">
         <is>
           <t>072</t>
         </is>
@@ -51956,7 +51956,7 @@
           <t>769</t>
         </is>
       </c>
-      <c r="Y296" s="12" t="inlineStr">
+      <c r="Y296" s="17" t="inlineStr">
         <is>
           <t>605</t>
         </is>
@@ -52001,7 +52001,7 @@
           <t>905</t>
         </is>
       </c>
-      <c r="AH296" s="17" t="inlineStr">
+      <c r="AH296" s="15" t="inlineStr">
         <is>
           <t>720</t>
         </is>
@@ -52477,7 +52477,7 @@
           <t>477</t>
         </is>
       </c>
-      <c r="Q299" s="17" t="inlineStr">
+      <c r="Q299" s="10" t="inlineStr">
         <is>
           <t>432</t>
         </is>
@@ -52851,7 +52851,7 @@
           <t>130</t>
         </is>
       </c>
-      <c r="Q301" s="17" t="inlineStr">
+      <c r="Q301" s="10" t="inlineStr">
         <is>
           <t>207</t>
         </is>
@@ -52968,7 +52968,7 @@
           <t>528</t>
         </is>
       </c>
-      <c r="C302" s="5" t="inlineStr">
+      <c r="C302" s="17" t="inlineStr">
         <is>
           <t>199</t>
         </is>
@@ -53599,7 +53599,7 @@
           <t>607</t>
         </is>
       </c>
-      <c r="Q305" s="17" t="inlineStr">
+      <c r="Q305" s="10" t="inlineStr">
         <is>
           <t>270</t>
         </is>
@@ -53993,7 +53993,7 @@
           <t>010</t>
         </is>
       </c>
-      <c r="U307" s="11" t="inlineStr">
+      <c r="U307" s="17" t="inlineStr">
         <is>
           <t>919</t>
         </is>
@@ -54028,7 +54028,7 @@
           <t>563</t>
         </is>
       </c>
-      <c r="AB307" s="13" t="inlineStr">
+      <c r="AB307" s="17" t="inlineStr">
         <is>
           <t>605</t>
         </is>
@@ -54514,7 +54514,7 @@
           <t>428</t>
         </is>
       </c>
-      <c r="M310" s="17" t="inlineStr">
+      <c r="M310" s="8" t="inlineStr">
         <is>
           <t>720</t>
         </is>
@@ -54736,7 +54736,7 @@
           <t>743</t>
         </is>
       </c>
-      <c r="T311" s="17" t="inlineStr">
+      <c r="T311" s="11" t="inlineStr">
         <is>
           <t>324</t>
         </is>
@@ -54873,7 +54873,7 @@
           <t>845</t>
         </is>
       </c>
-      <c r="J312" s="17" t="inlineStr">
+      <c r="J312" s="7" t="inlineStr">
         <is>
           <t>324</t>
         </is>
@@ -55085,7 +55085,7 @@
           <t>615</t>
         </is>
       </c>
-      <c r="O313" s="9" t="inlineStr">
+      <c r="O313" s="17" t="inlineStr">
         <is>
           <t>605</t>
         </is>
@@ -55120,7 +55120,7 @@
           <t>928</t>
         </is>
       </c>
-      <c r="V313" s="11" t="inlineStr">
+      <c r="V313" s="17" t="inlineStr">
         <is>
           <t>506</t>
         </is>
@@ -55556,7 +55556,7 @@
           <t>960</t>
         </is>
       </c>
-      <c r="Q318" s="10" t="inlineStr">
+      <c r="Q318" s="17" t="inlineStr">
         <is>
           <t>650</t>
         </is>
@@ -56137,7 +56137,7 @@
           <t>816</t>
         </is>
       </c>
-      <c r="U321" s="17" t="inlineStr">
+      <c r="U321" s="11" t="inlineStr">
         <is>
           <t>270</t>
         </is>
@@ -56344,7 +56344,7 @@
           <t>372</t>
         </is>
       </c>
-      <c r="Y322" s="17" t="inlineStr">
+      <c r="Y322" s="12" t="inlineStr">
         <is>
           <t>720</t>
         </is>
@@ -56486,7 +56486,7 @@
           <t>362</t>
         </is>
       </c>
-      <c r="P323" s="17" t="inlineStr">
+      <c r="P323" s="9" t="inlineStr">
         <is>
           <t>342</t>
         </is>
@@ -56566,7 +56566,7 @@
           <t>949</t>
         </is>
       </c>
-      <c r="AF323" s="17" t="inlineStr">
+      <c r="AF323" s="15" t="inlineStr">
         <is>
           <t>234</t>
         </is>
@@ -56708,7 +56708,7 @@
           <t>847</t>
         </is>
       </c>
-      <c r="W324" s="17" t="inlineStr">
+      <c r="W324" s="12" t="inlineStr">
         <is>
           <t>702</t>
         </is>
@@ -57107,7 +57107,7 @@
           <t>631</t>
         </is>
       </c>
-      <c r="AB326" s="17" t="inlineStr">
+      <c r="AB326" s="13" t="inlineStr">
         <is>
           <t>207</t>
         </is>
@@ -57117,7 +57117,7 @@
           <t>840</t>
         </is>
       </c>
-      <c r="AD326" s="17" t="inlineStr">
+      <c r="AD326" s="14" t="inlineStr">
         <is>
           <t>324</t>
         </is>
@@ -57189,7 +57189,7 @@
           <t>138</t>
         </is>
       </c>
-      <c r="G327" s="17" t="inlineStr">
+      <c r="G327" s="6" t="inlineStr">
         <is>
           <t>342</t>
         </is>
@@ -57279,7 +57279,7 @@
           <t>855</t>
         </is>
       </c>
-      <c r="Y327" s="17" t="inlineStr">
+      <c r="Y327" s="12" t="inlineStr">
         <is>
           <t>270</t>
         </is>
@@ -57376,12 +57376,12 @@
           <t>325</t>
         </is>
       </c>
-      <c r="G328" s="17" t="inlineStr">
+      <c r="G328" s="6" t="inlineStr">
         <is>
           <t>243</t>
         </is>
       </c>
-      <c r="H328" s="17" t="inlineStr">
+      <c r="H328" s="7" t="inlineStr">
         <is>
           <t>270</t>
         </is>
@@ -57426,7 +57426,7 @@
           <t>015</t>
         </is>
       </c>
-      <c r="Q328" s="17" t="inlineStr">
+      <c r="Q328" s="10" t="inlineStr">
         <is>
           <t>207</t>
         </is>
@@ -57688,7 +57688,7 @@
           <t>613</t>
         </is>
       </c>
-      <c r="AF329" s="15" t="inlineStr">
+      <c r="AF329" s="17" t="inlineStr">
         <is>
           <t>605</t>
         </is>
@@ -57790,7 +57790,7 @@
           <t>300</t>
         </is>
       </c>
-      <c r="O330" s="9" t="inlineStr">
+      <c r="O330" s="17" t="inlineStr">
         <is>
           <t>919</t>
         </is>
@@ -57942,7 +57942,7 @@
           <t>075</t>
         </is>
       </c>
-      <c r="H331" s="7" t="inlineStr">
+      <c r="H331" s="17" t="inlineStr">
         <is>
           <t>919</t>
         </is>
@@ -58139,7 +58139,7 @@
           <t>452</t>
         </is>
       </c>
-      <c r="J332" s="17" t="inlineStr">
+      <c r="J332" s="7" t="inlineStr">
         <is>
           <t>270</t>
         </is>
@@ -58229,7 +58229,7 @@
           <t>374</t>
         </is>
       </c>
-      <c r="AB332" s="13" t="inlineStr">
+      <c r="AB332" s="17" t="inlineStr">
         <is>
           <t>605</t>
         </is>
@@ -58638,7 +58638,7 @@
           <t>165</t>
         </is>
       </c>
-      <c r="AI334" s="17" t="inlineStr">
+      <c r="AI334" s="16" t="inlineStr">
         <is>
           <t>072</t>
         </is>
@@ -59114,7 +59114,7 @@
           <t>972</t>
         </is>
       </c>
-      <c r="R337" s="17" t="inlineStr">
+      <c r="R337" s="10" t="inlineStr">
         <is>
           <t>243</t>
         </is>
@@ -59226,7 +59226,7 @@
           <t>636</t>
         </is>
       </c>
-      <c r="C338" s="5" t="inlineStr">
+      <c r="C338" s="17" t="inlineStr">
         <is>
           <t>065</t>
         </is>
@@ -59266,7 +59266,7 @@
           <t>419</t>
         </is>
       </c>
-      <c r="K338" s="17" t="inlineStr">
+      <c r="K338" s="8" t="inlineStr">
         <is>
           <t>702</t>
         </is>
@@ -59685,7 +59685,7 @@
           <t>902</t>
         </is>
       </c>
-      <c r="T340" s="11" t="inlineStr">
+      <c r="T340" s="17" t="inlineStr">
         <is>
           <t>605</t>
         </is>
@@ -60024,7 +60024,7 @@
           <t>590</t>
         </is>
       </c>
-      <c r="M342" s="17" t="inlineStr">
+      <c r="M342" s="8" t="inlineStr">
         <is>
           <t>270</t>
         </is>
@@ -60296,7 +60296,7 @@
           <t>120</t>
         </is>
       </c>
-      <c r="AD343" s="17" t="inlineStr">
+      <c r="AD343" s="14" t="inlineStr">
         <is>
           <t>270</t>
         </is>
@@ -61727,7 +61727,7 @@
           <t>375</t>
         </is>
       </c>
-      <c r="AK353" s="17" t="inlineStr">
+      <c r="AK353" s="16" t="inlineStr">
         <is>
           <t>324</t>
         </is>
@@ -62410,7 +62410,7 @@
           <t>855</t>
         </is>
       </c>
-      <c r="X357" s="12" t="inlineStr">
+      <c r="X357" s="17" t="inlineStr">
         <is>
           <t>199</t>
         </is>
@@ -62921,7 +62921,7 @@
           <t>909</t>
         </is>
       </c>
-      <c r="N360" s="17" t="inlineStr">
+      <c r="N360" s="9" t="inlineStr">
         <is>
           <t>207</t>
         </is>
@@ -63031,7 +63031,7 @@
           <t>785</t>
         </is>
       </c>
-      <c r="AJ360" s="17" t="inlineStr">
+      <c r="AJ360" s="16" t="inlineStr">
         <is>
           <t>072</t>
         </is>
@@ -63143,7 +63143,7 @@
           <t>089</t>
         </is>
       </c>
-      <c r="U361" s="17" t="inlineStr">
+      <c r="U361" s="11" t="inlineStr">
         <is>
           <t>243</t>
         </is>
@@ -64048,7 +64048,7 @@
           <t>851</t>
         </is>
       </c>
-      <c r="O366" s="17" t="inlineStr">
+      <c r="O366" s="9" t="inlineStr">
         <is>
           <t>423</t>
         </is>
@@ -64158,7 +64158,7 @@
           <t>047</t>
         </is>
       </c>
-      <c r="AK366" s="17" t="inlineStr">
+      <c r="AK366" s="16" t="inlineStr">
         <is>
           <t>423</t>
         </is>
@@ -64392,7 +64392,7 @@
           <t>412</t>
         </is>
       </c>
-      <c r="I368" s="7" t="inlineStr">
+      <c r="I368" s="17" t="inlineStr">
         <is>
           <t>506</t>
         </is>
@@ -64447,7 +64447,7 @@
           <t>708</t>
         </is>
       </c>
-      <c r="T368" s="11" t="inlineStr">
+      <c r="T368" s="17" t="inlineStr">
         <is>
           <t>991</t>
         </is>
@@ -64719,7 +64719,7 @@
           <t>009</t>
         </is>
       </c>
-      <c r="AK369" s="17" t="inlineStr">
+      <c r="AK369" s="16" t="inlineStr">
         <is>
           <t>423</t>
         </is>
@@ -64861,7 +64861,7 @@
           <t>582</t>
         </is>
       </c>
-      <c r="AB370" s="17" t="inlineStr">
+      <c r="AB370" s="13" t="inlineStr">
         <is>
           <t>432</t>
         </is>
@@ -64953,7 +64953,7 @@
           <t>617</t>
         </is>
       </c>
-      <c r="I371" s="17" t="inlineStr">
+      <c r="I371" s="7" t="inlineStr">
         <is>
           <t>207</t>
         </is>
@@ -64963,7 +64963,7 @@
           <t>020</t>
         </is>
       </c>
-      <c r="K371" s="8" t="inlineStr">
+      <c r="K371" s="17" t="inlineStr">
         <is>
           <t>506</t>
         </is>
@@ -65003,7 +65003,7 @@
           <t>872</t>
         </is>
       </c>
-      <c r="S371" s="17" t="inlineStr">
+      <c r="S371" s="10" t="inlineStr">
         <is>
           <t>702</t>
         </is>
@@ -65412,7 +65412,7 @@
           <t>035</t>
         </is>
       </c>
-      <c r="Z373" s="17" t="inlineStr">
+      <c r="Z373" s="13" t="inlineStr">
         <is>
           <t>342</t>
         </is>
@@ -65422,7 +65422,7 @@
           <t>678</t>
         </is>
       </c>
-      <c r="AB373" s="17" t="inlineStr">
+      <c r="AB373" s="13" t="inlineStr">
         <is>
           <t>072</t>
         </is>
@@ -65786,7 +65786,7 @@
           <t>553</t>
         </is>
       </c>
-      <c r="Z375" s="13" t="inlineStr">
+      <c r="Z375" s="17" t="inlineStr">
         <is>
           <t>056</t>
         </is>
@@ -66145,7 +66145,7 @@
           <t>057</t>
         </is>
       </c>
-      <c r="W377" s="12" t="inlineStr">
+      <c r="W377" s="17" t="inlineStr">
         <is>
           <t>605</t>
         </is>
@@ -66272,7 +66272,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="K378" s="17" t="inlineStr">
+      <c r="K378" s="8" t="inlineStr">
         <is>
           <t>027</t>
         </is>
@@ -66327,7 +66327,7 @@
           <t>206</t>
         </is>
       </c>
-      <c r="V378" s="17" t="inlineStr">
+      <c r="V378" s="11" t="inlineStr">
         <is>
           <t>720</t>
         </is>
@@ -66387,7 +66387,7 @@
           <t>871</t>
         </is>
       </c>
-      <c r="AH378" s="17" t="inlineStr">
+      <c r="AH378" s="15" t="inlineStr">
         <is>
           <t>423</t>
         </is>
@@ -66549,7 +66549,7 @@
           <t>339</t>
         </is>
       </c>
-      <c r="AC379" s="17" t="inlineStr">
+      <c r="AC379" s="14" t="inlineStr">
         <is>
           <t>072</t>
         </is>
@@ -66706,7 +66706,7 @@
           <t>090</t>
         </is>
       </c>
-      <c r="W380" s="12" t="inlineStr">
+      <c r="W380" s="17" t="inlineStr">
         <is>
           <t>991</t>
         </is>
@@ -66731,7 +66731,7 @@
           <t>858</t>
         </is>
       </c>
-      <c r="AB380" s="13" t="inlineStr">
+      <c r="AB380" s="17" t="inlineStr">
         <is>
           <t>065</t>
         </is>
@@ -66853,7 +66853,7 @@
           <t>380</t>
         </is>
       </c>
-      <c r="O381" s="17" t="inlineStr">
+      <c r="O381" s="9" t="inlineStr">
         <is>
           <t>423</t>
         </is>
@@ -67060,7 +67060,7 @@
           <t>132</t>
         </is>
       </c>
-      <c r="S382" s="10" t="inlineStr">
+      <c r="S382" s="17" t="inlineStr">
         <is>
           <t>650</t>
         </is>
@@ -67095,7 +67095,7 @@
           <t>626</t>
         </is>
       </c>
-      <c r="Z382" s="17" t="inlineStr">
+      <c r="Z382" s="13" t="inlineStr">
         <is>
           <t>243</t>
         </is>
@@ -67758,7 +67758,7 @@
           <t>641</t>
         </is>
       </c>
-      <c r="AC388" s="14" t="inlineStr">
+      <c r="AC388" s="17" t="inlineStr">
         <is>
           <t>506</t>
         </is>
@@ -67835,7 +67835,7 @@
           <t>351</t>
         </is>
       </c>
-      <c r="G389" s="17" t="inlineStr">
+      <c r="G389" s="6" t="inlineStr">
         <is>
           <t>720</t>
         </is>
@@ -67865,7 +67865,7 @@
           <t>366</t>
         </is>
       </c>
-      <c r="M389" s="8" t="inlineStr">
+      <c r="M389" s="17" t="inlineStr">
         <is>
           <t>506</t>
         </is>
@@ -67915,7 +67915,7 @@
           <t>816</t>
         </is>
       </c>
-      <c r="W389" s="12" t="inlineStr">
+      <c r="W389" s="17" t="inlineStr">
         <is>
           <t>919</t>
         </is>
@@ -68476,7 +68476,7 @@
           <t>912</t>
         </is>
       </c>
-      <c r="W392" s="12" t="inlineStr">
+      <c r="W392" s="17" t="inlineStr">
         <is>
           <t>056</t>
         </is>
@@ -69279,7 +69279,7 @@
           <t>845</t>
         </is>
       </c>
-      <c r="AH396" s="17" t="inlineStr">
+      <c r="AH396" s="15" t="inlineStr">
         <is>
           <t>720</t>
         </is>
@@ -69907,7 +69907,7 @@
           <t>438</t>
         </is>
       </c>
-      <c r="J400" s="7" t="inlineStr">
+      <c r="J400" s="17" t="inlineStr">
         <is>
           <t>056</t>
         </is>
@@ -70271,7 +70271,7 @@
           <t>088</t>
         </is>
       </c>
-      <c r="H402" s="17" t="inlineStr">
+      <c r="H402" s="7" t="inlineStr">
         <is>
           <t>072</t>
         </is>
@@ -70316,7 +70316,7 @@
           <t>971</t>
         </is>
       </c>
-      <c r="Q402" s="10" t="inlineStr">
+      <c r="Q402" s="17" t="inlineStr">
         <is>
           <t>919</t>
         </is>
@@ -70351,7 +70351,7 @@
           <t>524</t>
         </is>
       </c>
-      <c r="X402" s="12" t="inlineStr">
+      <c r="X402" s="17" t="inlineStr">
         <is>
           <t>650</t>
         </is>
@@ -70715,7 +70715,7 @@
           <t>210</t>
         </is>
       </c>
-      <c r="V404" s="17" t="inlineStr">
+      <c r="V404" s="11" t="inlineStr">
         <is>
           <t>027</t>
         </is>
@@ -71630,7 +71630,7 @@
           <t>618</t>
         </is>
       </c>
-      <c r="R409" s="10" t="inlineStr">
+      <c r="R409" s="17" t="inlineStr">
         <is>
           <t>650</t>
         </is>
@@ -72216,7 +72216,7 @@
           <t>836</t>
         </is>
       </c>
-      <c r="W412" s="17" t="inlineStr">
+      <c r="W412" s="12" t="inlineStr">
         <is>
           <t>243</t>
         </is>
@@ -72298,7 +72298,7 @@
           <t>26</t>
         </is>
       </c>
-      <c r="B413" s="17" t="inlineStr">
+      <c r="B413" s="5" t="inlineStr">
         <is>
           <t>207</t>
         </is>
@@ -72453,7 +72453,7 @@
           <t>842</t>
         </is>
       </c>
-      <c r="AG413" s="17" t="inlineStr">
+      <c r="AG413" s="15" t="inlineStr">
         <is>
           <t>270</t>
         </is>
@@ -72832,7 +72832,7 @@
           <t>974</t>
         </is>
       </c>
-      <c r="AH415" s="15" t="inlineStr">
+      <c r="AH415" s="17" t="inlineStr">
         <is>
           <t>919</t>
         </is>
@@ -72979,7 +72979,7 @@
           <t>078</t>
         </is>
       </c>
-      <c r="Z416" s="13" t="inlineStr">
+      <c r="Z416" s="17" t="inlineStr">
         <is>
           <t>560</t>
         </is>
@@ -73019,7 +73019,7 @@
           <t>327</t>
         </is>
       </c>
-      <c r="AH416" s="15" t="inlineStr">
+      <c r="AH416" s="17" t="inlineStr">
         <is>
           <t>919</t>
         </is>
@@ -73196,7 +73196,7 @@
           <t>515</t>
         </is>
       </c>
-      <c r="AF417" s="15" t="inlineStr">
+      <c r="AF417" s="17" t="inlineStr">
         <is>
           <t>056</t>
         </is>
@@ -73348,7 +73348,7 @@
           <t>053</t>
         </is>
       </c>
-      <c r="Y418" s="17" t="inlineStr">
+      <c r="Y418" s="12" t="inlineStr">
         <is>
           <t>423</t>
         </is>
@@ -73378,7 +73378,7 @@
           <t>317</t>
         </is>
       </c>
-      <c r="AE418" s="17" t="inlineStr">
+      <c r="AE418" s="14" t="inlineStr">
         <is>
           <t>072</t>
         </is>
@@ -73714,7 +73714,7 @@
           <t>380</t>
         </is>
       </c>
-      <c r="F423" s="6" t="inlineStr">
+      <c r="F423" s="17" t="inlineStr">
         <is>
           <t>065</t>
         </is>
@@ -73839,7 +73839,7 @@
           <t>968</t>
         </is>
       </c>
-      <c r="AE423" s="14" t="inlineStr">
+      <c r="AE423" s="17" t="inlineStr">
         <is>
           <t>056</t>
         </is>
@@ -73911,7 +73911,7 @@
           <t>855</t>
         </is>
       </c>
-      <c r="H424" s="17" t="inlineStr">
+      <c r="H424" s="7" t="inlineStr">
         <is>
           <t>207</t>
         </is>
@@ -74073,7 +74073,7 @@
           <t>750</t>
         </is>
       </c>
-      <c r="C425" s="17" t="inlineStr">
+      <c r="C425" s="5" t="inlineStr">
         <is>
           <t>324</t>
         </is>
@@ -74739,7 +74739,7 @@
           <t>586</t>
         </is>
       </c>
-      <c r="X428" s="17" t="inlineStr">
+      <c r="X428" s="12" t="inlineStr">
         <is>
           <t>702</t>
         </is>
@@ -74976,7 +74976,7 @@
           <t>921</t>
         </is>
       </c>
-      <c r="AH429" s="17" t="inlineStr">
+      <c r="AH429" s="15" t="inlineStr">
         <is>
           <t>423</t>
         </is>
@@ -75068,7 +75068,7 @@
           <t>725</t>
         </is>
       </c>
-      <c r="O430" s="9" t="inlineStr">
+      <c r="O430" s="17" t="inlineStr">
         <is>
           <t>605</t>
         </is>
@@ -75427,7 +75427,7 @@
           <t>884</t>
         </is>
       </c>
-      <c r="L432" s="8" t="inlineStr">
+      <c r="L432" s="17" t="inlineStr">
         <is>
           <t>056</t>
         </is>
@@ -75776,7 +75776,7 @@
           <t>323</t>
         </is>
       </c>
-      <c r="G434" s="6" t="inlineStr">
+      <c r="G434" s="17" t="inlineStr">
         <is>
           <t>919</t>
         </is>
@@ -76113,7 +76113,7 @@
           <t>384</t>
         </is>
       </c>
-      <c r="AK435" s="17" t="inlineStr">
+      <c r="AK435" s="16" t="inlineStr">
         <is>
           <t>432</t>
         </is>
@@ -76392,7 +76392,7 @@
           <t>151</t>
         </is>
       </c>
-      <c r="R437" s="17" t="inlineStr">
+      <c r="R437" s="10" t="inlineStr">
         <is>
           <t>702</t>
         </is>
@@ -76711,7 +76711,7 @@
           <t>135</t>
         </is>
       </c>
-      <c r="G439" s="6" t="inlineStr">
+      <c r="G439" s="17" t="inlineStr">
         <is>
           <t>991</t>
         </is>
@@ -76888,7 +76888,7 @@
           <t>805</t>
         </is>
       </c>
-      <c r="E440" s="6" t="inlineStr">
+      <c r="E440" s="17" t="inlineStr">
         <is>
           <t>506</t>
         </is>
@@ -76973,7 +76973,7 @@
           <t>685</t>
         </is>
       </c>
-      <c r="V440" s="17" t="inlineStr">
+      <c r="V440" s="11" t="inlineStr">
         <is>
           <t>207</t>
         </is>
@@ -77210,7 +77210,7 @@
           <t>457</t>
         </is>
       </c>
-      <c r="AF441" s="15" t="inlineStr">
+      <c r="AF441" s="17" t="inlineStr">
         <is>
           <t>605</t>
         </is>
@@ -77347,7 +77347,7 @@
           <t>998</t>
         </is>
       </c>
-      <c r="V442" s="11" t="inlineStr">
+      <c r="V442" s="17" t="inlineStr">
         <is>
           <t>506</t>
         </is>
@@ -77559,7 +77559,7 @@
           <t>138</t>
         </is>
       </c>
-      <c r="AA443" s="13" t="inlineStr">
+      <c r="AA443" s="17" t="inlineStr">
         <is>
           <t>056</t>
         </is>
@@ -77609,7 +77609,7 @@
           <t>672</t>
         </is>
       </c>
-      <c r="AK443" s="16" t="inlineStr">
+      <c r="AK443" s="17" t="inlineStr">
         <is>
           <t>506</t>
         </is>
@@ -77888,7 +77888,7 @@
           <t>553</t>
         </is>
       </c>
-      <c r="R445" s="17" t="inlineStr">
+      <c r="R445" s="10" t="inlineStr">
         <is>
           <t>270</t>
         </is>
@@ -77928,7 +77928,7 @@
           <t>541</t>
         </is>
       </c>
-      <c r="Z445" s="13" t="inlineStr">
+      <c r="Z445" s="17" t="inlineStr">
         <is>
           <t>991</t>
         </is>
@@ -77938,7 +77938,7 @@
           <t>258</t>
         </is>
       </c>
-      <c r="AB445" s="17" t="inlineStr">
+      <c r="AB445" s="13" t="inlineStr">
         <is>
           <t>027</t>
         </is>
@@ -79035,7 +79035,7 @@
           <t>932</t>
         </is>
       </c>
-      <c r="W451" s="12" t="inlineStr">
+      <c r="W451" s="17" t="inlineStr">
         <is>
           <t>506</t>
         </is>
@@ -79399,7 +79399,7 @@
           <t>677</t>
         </is>
       </c>
-      <c r="U453" s="17" t="inlineStr">
+      <c r="U453" s="11" t="inlineStr">
         <is>
           <t>243</t>
         </is>
@@ -79835,7 +79835,7 @@
           <t>110</t>
         </is>
       </c>
-      <c r="P458" s="9" t="inlineStr">
+      <c r="P458" s="17" t="inlineStr">
         <is>
           <t>065</t>
         </is>
@@ -79870,7 +79870,7 @@
           <t>310</t>
         </is>
       </c>
-      <c r="W458" s="17" t="inlineStr">
+      <c r="W458" s="12" t="inlineStr">
         <is>
           <t>234</t>
         </is>
@@ -80072,7 +80072,7 @@
           <t>261</t>
         </is>
       </c>
-      <c r="Z459" s="13" t="inlineStr">
+      <c r="Z459" s="17" t="inlineStr">
         <is>
           <t>650</t>
         </is>
@@ -80249,7 +80249,7 @@
           <t>682</t>
         </is>
       </c>
-      <c r="X460" s="17" t="inlineStr">
+      <c r="X460" s="12" t="inlineStr">
         <is>
           <t>720</t>
         </is>
@@ -80381,7 +80381,7 @@
           <t>189</t>
         </is>
       </c>
-      <c r="M461" s="8" t="inlineStr">
+      <c r="M461" s="17" t="inlineStr">
         <is>
           <t>560</t>
         </is>
@@ -80568,7 +80568,7 @@
           <t>100</t>
         </is>
       </c>
-      <c r="M462" s="17" t="inlineStr">
+      <c r="M462" s="8" t="inlineStr">
         <is>
           <t>702</t>
         </is>
@@ -80688,7 +80688,7 @@
           <t>542</t>
         </is>
       </c>
-      <c r="AK462" s="17" t="inlineStr">
+      <c r="AK462" s="16" t="inlineStr">
         <is>
           <t>243</t>
         </is>
@@ -81234,7 +81234,7 @@
           <t>689</t>
         </is>
       </c>
-      <c r="AH465" s="15" t="inlineStr">
+      <c r="AH465" s="17" t="inlineStr">
         <is>
           <t>991</t>
         </is>
@@ -81458,7 +81458,7 @@
           <t>294</t>
         </is>
       </c>
-      <c r="D467" s="5" t="inlineStr">
+      <c r="D467" s="17" t="inlineStr">
         <is>
           <t>650</t>
         </is>
@@ -81613,7 +81613,7 @@
           <t>248</t>
         </is>
       </c>
-      <c r="AI467" s="17" t="inlineStr">
+      <c r="AI467" s="16" t="inlineStr">
         <is>
           <t>243</t>
         </is>
@@ -81675,7 +81675,7 @@
           <t>638</t>
         </is>
       </c>
-      <c r="J468" s="17" t="inlineStr">
+      <c r="J468" s="7" t="inlineStr">
         <is>
           <t>270</t>
         </is>
@@ -83428,7 +83428,7 @@
           <t>475</t>
         </is>
       </c>
-      <c r="X477" s="17" t="inlineStr">
+      <c r="X477" s="12" t="inlineStr">
         <is>
           <t>423</t>
         </is>
@@ -83650,7 +83650,7 @@
           <t>741</t>
         </is>
       </c>
-      <c r="AE478" s="17" t="inlineStr">
+      <c r="AE478" s="14" t="inlineStr">
         <is>
           <t>027</t>
         </is>
@@ -83817,7 +83817,7 @@
           <t>479</t>
         </is>
       </c>
-      <c r="AA479" s="17" t="inlineStr">
+      <c r="AA479" s="13" t="inlineStr">
         <is>
           <t>720</t>
         </is>
@@ -83909,7 +83909,7 @@
           <t>551</t>
         </is>
       </c>
-      <c r="H480" s="17" t="inlineStr">
+      <c r="H480" s="7" t="inlineStr">
         <is>
           <t>234</t>
         </is>
@@ -84096,7 +84096,7 @@
           <t>186</t>
         </is>
       </c>
-      <c r="H481" s="17" t="inlineStr">
+      <c r="H481" s="7" t="inlineStr">
         <is>
           <t>702</t>
         </is>
@@ -84141,7 +84141,7 @@
           <t>233</t>
         </is>
       </c>
-      <c r="Q481" s="10" t="inlineStr">
+      <c r="Q481" s="17" t="inlineStr">
         <is>
           <t>199</t>
         </is>
@@ -84151,7 +84151,7 @@
           <t>707</t>
         </is>
       </c>
-      <c r="S481" s="17" t="inlineStr">
+      <c r="S481" s="10" t="inlineStr">
         <is>
           <t>720</t>
         </is>
@@ -85066,7 +85066,7 @@
           <t>369</t>
         </is>
       </c>
-      <c r="O486" s="17" t="inlineStr">
+      <c r="O486" s="9" t="inlineStr">
         <is>
           <t>702</t>
         </is>
@@ -85233,7 +85233,7 @@
           <t>436</t>
         </is>
       </c>
-      <c r="K487" s="17" t="inlineStr">
+      <c r="K487" s="8" t="inlineStr">
         <is>
           <t>243</t>
         </is>
@@ -86001,7 +86001,7 @@
           <t>712</t>
         </is>
       </c>
-      <c r="AI493" s="16" t="inlineStr">
+      <c r="AI493" s="17" t="inlineStr">
         <is>
           <t>991</t>
         </is>
@@ -86048,7 +86048,7 @@
           <t>797</t>
         </is>
       </c>
-      <c r="G494" s="6" t="inlineStr">
+      <c r="G494" s="17" t="inlineStr">
         <is>
           <t>605</t>
         </is>
@@ -86791,7 +86791,7 @@
           <t>410</t>
         </is>
       </c>
-      <c r="F498" s="6" t="inlineStr">
+      <c r="F498" s="17" t="inlineStr">
         <is>
           <t>506</t>
         </is>
@@ -87123,7 +87123,7 @@
           <t>911</t>
         </is>
       </c>
-      <c r="AI499" s="16" t="inlineStr">
+      <c r="AI499" s="17" t="inlineStr">
         <is>
           <t>991</t>
         </is>
@@ -87133,7 +87133,7 @@
           <t>355</t>
         </is>
       </c>
-      <c r="AK499" s="16" t="inlineStr">
+      <c r="AK499" s="17" t="inlineStr">
         <is>
           <t>919</t>
         </is>
@@ -87290,7 +87290,7 @@
           <t>964</t>
         </is>
       </c>
-      <c r="AE500" s="14" t="inlineStr">
+      <c r="AE500" s="17" t="inlineStr">
         <is>
           <t>650</t>
         </is>
@@ -87684,7 +87684,7 @@
           <t>191</t>
         </is>
       </c>
-      <c r="AI502" s="17" t="inlineStr">
+      <c r="AI502" s="16" t="inlineStr">
         <is>
           <t>324</t>
         </is>
@@ -87706,7 +87706,7 @@
           <t>11</t>
         </is>
       </c>
-      <c r="B503" s="5" t="inlineStr">
+      <c r="B503" s="17" t="inlineStr">
         <is>
           <t>991</t>
         </is>
@@ -88100,7 +88100,7 @@
           <t>037</t>
         </is>
       </c>
-      <c r="F505" s="17" t="inlineStr">
+      <c r="F505" s="6" t="inlineStr">
         <is>
           <t>027</t>
         </is>
@@ -88614,7 +88614,7 @@
           <t>583</t>
         </is>
       </c>
-      <c r="AH507" s="17" t="inlineStr">
+      <c r="AH507" s="15" t="inlineStr">
         <is>
           <t>027</t>
         </is>
@@ -89357,7 +89357,7 @@
           <t>558</t>
         </is>
       </c>
-      <c r="AG511" s="15" t="inlineStr">
+      <c r="AG511" s="17" t="inlineStr">
         <is>
           <t>056</t>
         </is>
@@ -90095,7 +90095,7 @@
           <t>939</t>
         </is>
       </c>
-      <c r="AE515" s="17" t="inlineStr">
+      <c r="AE515" s="14" t="inlineStr">
         <is>
           <t>270</t>
         </is>
@@ -90521,7 +90521,7 @@
           <t>043</t>
         </is>
       </c>
-      <c r="D518" s="5" t="inlineStr">
+      <c r="D518" s="17" t="inlineStr">
         <is>
           <t>605</t>
         </is>
@@ -90698,12 +90698,12 @@
           <t>27</t>
         </is>
       </c>
-      <c r="B519" s="17" t="inlineStr">
+      <c r="B519" s="5" t="inlineStr">
         <is>
           <t>324</t>
         </is>
       </c>
-      <c r="C519" s="17" t="inlineStr">
+      <c r="C519" s="5" t="inlineStr">
         <is>
           <t>720</t>
         </is>
@@ -90823,7 +90823,7 @@
           <t>448</t>
         </is>
       </c>
-      <c r="AA519" s="17" t="inlineStr">
+      <c r="AA519" s="13" t="inlineStr">
         <is>
           <t>423</t>
         </is>
@@ -91259,12 +91259,12 @@
           <t>30</t>
         </is>
       </c>
-      <c r="B522" s="5" t="inlineStr">
+      <c r="B522" s="17" t="inlineStr">
         <is>
           <t>199</t>
         </is>
       </c>
-      <c r="C522" s="5" t="inlineStr">
+      <c r="C522" s="17" t="inlineStr">
         <is>
           <t>056</t>
         </is>
@@ -91989,7 +91989,7 @@
           <t>975</t>
         </is>
       </c>
-      <c r="F533" s="17" t="inlineStr">
+      <c r="F533" s="6" t="inlineStr">
         <is>
           <t>027</t>
         </is>
@@ -92103,7 +92103,7 @@
           <t>601</t>
         </is>
       </c>
-      <c r="H535" s="17" t="inlineStr">
+      <c r="H535" s="7" t="inlineStr">
         <is>
           <t>342</t>
         </is>
@@ -92254,7 +92254,7 @@
           <t>198</t>
         </is>
       </c>
-      <c r="G538" s="6" t="inlineStr">
+      <c r="G538" s="17" t="inlineStr">
         <is>
           <t>605</t>
         </is>
@@ -92462,7 +92462,7 @@
           <t>166</t>
         </is>
       </c>
-      <c r="G542" s="17" t="inlineStr">
+      <c r="G542" s="6" t="inlineStr">
         <is>
           <t>324</t>
         </is>
@@ -92546,7 +92546,7 @@
           <t>622</t>
         </is>
       </c>
-      <c r="C544" s="17" t="inlineStr">
+      <c r="C544" s="5" t="inlineStr">
         <is>
           <t>027</t>
         </is>
@@ -92893,7 +92893,7 @@
           <t>404</t>
         </is>
       </c>
-      <c r="J550" s="7" t="inlineStr">
+      <c r="J550" s="17" t="inlineStr">
         <is>
           <t>560</t>
         </is>

</xml_diff>

<commit_message>
updated results and added solid pattern findings
</commit_message>
<xml_diff>
--- a/swertres/excel_results.xlsx
+++ b/swertres/excel_results.xlsx
@@ -43,12 +43,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00ff6666"/>
+        <fgColor rgb="00FFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FFFFFF"/>
+        <fgColor rgb="00ff6666"/>
       </patternFill>
     </fill>
     <fill>
@@ -220,7 +220,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
@@ -253,7 +253,7 @@
     <xf numFmtId="0" fontId="1" fillId="14" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1376,7 +1376,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="AH5" s="15" t="inlineStr">
+      <c r="AH5" s="17" t="inlineStr">
         <is>
           <t>836</t>
         </is>
@@ -2176,7 +2176,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="G10" s="17" t="inlineStr">
+      <c r="G10" s="6" t="inlineStr">
         <is>
           <t>560</t>
         </is>
@@ -2206,7 +2206,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="M10" s="17" t="inlineStr">
+      <c r="M10" s="8" t="inlineStr">
         <is>
           <t>199</t>
         </is>
@@ -2722,7 +2722,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="D13" s="5" t="inlineStr">
+      <c r="D13" s="17" t="inlineStr">
         <is>
           <t>606</t>
         </is>
@@ -3605,7 +3605,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="AE17" s="17" t="inlineStr">
+      <c r="AE17" s="14" t="inlineStr">
         <is>
           <t>506</t>
         </is>
@@ -5086,7 +5086,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="AB25" s="13" t="inlineStr">
+      <c r="AB25" s="17" t="inlineStr">
         <is>
           <t>606</t>
         </is>
@@ -7205,7 +7205,7 @@
           <t>225</t>
         </is>
       </c>
-      <c r="W39" s="12" t="inlineStr">
+      <c r="W39" s="17" t="inlineStr">
         <is>
           <t>386</t>
         </is>
@@ -7848,7 +7848,7 @@
           <t>06</t>
         </is>
       </c>
-      <c r="B43" s="17" t="inlineStr">
+      <c r="B43" s="5" t="inlineStr">
         <is>
           <t>506</t>
         </is>
@@ -8439,7 +8439,7 @@
           <t>928</t>
         </is>
       </c>
-      <c r="H46" s="7" t="inlineStr">
+      <c r="H46" s="17" t="inlineStr">
         <is>
           <t>066</t>
         </is>
@@ -9262,7 +9262,7 @@
           <t>955</t>
         </is>
       </c>
-      <c r="W50" s="17" t="inlineStr">
+      <c r="W50" s="12" t="inlineStr">
         <is>
           <t>991</t>
         </is>
@@ -10177,7 +10177,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="S55" s="17" t="inlineStr">
+      <c r="S55" s="10" t="inlineStr">
         <is>
           <t>065</t>
         </is>
@@ -10339,7 +10339,7 @@
           <t>015</t>
         </is>
       </c>
-      <c r="N56" s="9" t="inlineStr">
+      <c r="N56" s="17" t="inlineStr">
         <is>
           <t>660</t>
         </is>
@@ -10414,7 +10414,7 @@
           <t>837</t>
         </is>
       </c>
-      <c r="AC56" s="17" t="inlineStr">
+      <c r="AC56" s="14" t="inlineStr">
         <is>
           <t>199</t>
         </is>
@@ -10586,7 +10586,7 @@
           <t>767</t>
         </is>
       </c>
-      <c r="Z57" s="17" t="inlineStr">
+      <c r="Z57" s="13" t="inlineStr">
         <is>
           <t>056</t>
         </is>
@@ -10798,7 +10798,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="AE58" s="14" t="inlineStr">
+      <c r="AE58" s="17" t="inlineStr">
         <is>
           <t>386</t>
         </is>
@@ -10813,7 +10813,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="AH58" s="17" t="inlineStr">
+      <c r="AH58" s="15" t="inlineStr">
         <is>
           <t>919</t>
         </is>
@@ -10975,7 +10975,7 @@
           <t>327</t>
         </is>
       </c>
-      <c r="AC59" s="14" t="inlineStr">
+      <c r="AC59" s="17" t="inlineStr">
         <is>
           <t>368</t>
         </is>
@@ -12314,7 +12314,7 @@
           <t>339</t>
         </is>
       </c>
-      <c r="AI66" s="17" t="inlineStr">
+      <c r="AI66" s="16" t="inlineStr">
         <is>
           <t>506</t>
         </is>
@@ -13211,7 +13211,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="J74" s="17" t="inlineStr">
+      <c r="J74" s="7" t="inlineStr">
         <is>
           <t>065</t>
         </is>
@@ -13316,7 +13316,7 @@
           <t>857</t>
         </is>
       </c>
-      <c r="AE74" s="14" t="inlineStr">
+      <c r="AE74" s="17" t="inlineStr">
         <is>
           <t>606</t>
         </is>
@@ -13882,7 +13882,7 @@
           <t>753</t>
         </is>
       </c>
-      <c r="AF77" s="17" t="inlineStr">
+      <c r="AF77" s="15" t="inlineStr">
         <is>
           <t>506</t>
         </is>
@@ -13959,7 +13959,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="J78" s="7" t="inlineStr">
+      <c r="J78" s="17" t="inlineStr">
         <is>
           <t>683</t>
         </is>
@@ -13984,7 +13984,7 @@
           <t>886</t>
         </is>
       </c>
-      <c r="O78" s="17" t="inlineStr">
+      <c r="O78" s="9" t="inlineStr">
         <is>
           <t>650</t>
         </is>
@@ -14216,7 +14216,7 @@
           <t>598</t>
         </is>
       </c>
-      <c r="X79" s="12" t="inlineStr">
+      <c r="X79" s="17" t="inlineStr">
         <is>
           <t>660</t>
         </is>
@@ -14383,7 +14383,7 @@
           <t>706</t>
         </is>
       </c>
-      <c r="T80" s="17" t="inlineStr">
+      <c r="T80" s="11" t="inlineStr">
         <is>
           <t>199</t>
         </is>
@@ -14560,7 +14560,7 @@
           <t>005</t>
         </is>
       </c>
-      <c r="R81" s="17" t="inlineStr">
+      <c r="R81" s="10" t="inlineStr">
         <is>
           <t>650</t>
         </is>
@@ -14787,7 +14787,7 @@
           <t>946</t>
         </is>
       </c>
-      <c r="Z82" s="13" t="inlineStr">
+      <c r="Z82" s="17" t="inlineStr">
         <is>
           <t>863</t>
         </is>
@@ -14869,7 +14869,7 @@
           <t>313</t>
         </is>
       </c>
-      <c r="E83" s="17" t="inlineStr">
+      <c r="E83" s="6" t="inlineStr">
         <is>
           <t>991</t>
         </is>
@@ -14984,12 +14984,12 @@
           <t>023</t>
         </is>
       </c>
-      <c r="AB83" s="17" t="inlineStr">
+      <c r="AB83" s="13" t="inlineStr">
         <is>
           <t>650</t>
         </is>
       </c>
-      <c r="AC83" s="17" t="inlineStr">
+      <c r="AC83" s="14" t="inlineStr">
         <is>
           <t>991</t>
         </is>
@@ -15009,7 +15009,7 @@
           <t>211</t>
         </is>
       </c>
-      <c r="AG83" s="15" t="inlineStr">
+      <c r="AG83" s="17" t="inlineStr">
         <is>
           <t>066</t>
         </is>
@@ -15121,7 +15121,7 @@
           <t>900</t>
         </is>
       </c>
-      <c r="R84" s="10" t="inlineStr">
+      <c r="R84" s="17" t="inlineStr">
         <is>
           <t>066</t>
         </is>
@@ -15348,7 +15348,7 @@
           <t>136</t>
         </is>
       </c>
-      <c r="Z85" s="17" t="inlineStr">
+      <c r="Z85" s="13" t="inlineStr">
         <is>
           <t>056</t>
         </is>
@@ -15363,7 +15363,7 @@
           <t>269</t>
         </is>
       </c>
-      <c r="AC85" s="17" t="inlineStr">
+      <c r="AC85" s="14" t="inlineStr">
         <is>
           <t>056</t>
         </is>
@@ -15657,7 +15657,7 @@
           <t>191</t>
         </is>
       </c>
-      <c r="M87" s="8" t="inlineStr">
+      <c r="M87" s="17" t="inlineStr">
         <is>
           <t>368</t>
         </is>
@@ -16662,7 +16662,7 @@
           <t>283</t>
         </is>
       </c>
-      <c r="AA92" s="13" t="inlineStr">
+      <c r="AA92" s="17" t="inlineStr">
         <is>
           <t>836</t>
         </is>
@@ -16839,7 +16839,7 @@
           <t>558</t>
         </is>
       </c>
-      <c r="Y93" s="12" t="inlineStr">
+      <c r="Y93" s="17" t="inlineStr">
         <is>
           <t>368</t>
         </is>
@@ -16859,7 +16859,7 @@
           <t>501</t>
         </is>
       </c>
-      <c r="AC93" s="14" t="inlineStr">
+      <c r="AC93" s="17" t="inlineStr">
         <is>
           <t>638</t>
         </is>
@@ -17036,7 +17036,7 @@
           <t>028</t>
         </is>
       </c>
-      <c r="AA94" s="17" t="inlineStr">
+      <c r="AA94" s="13" t="inlineStr">
         <is>
           <t>199</t>
         </is>
@@ -17203,7 +17203,7 @@
           <t>680</t>
         </is>
       </c>
-      <c r="W95" s="12" t="inlineStr">
+      <c r="W95" s="17" t="inlineStr">
         <is>
           <t>638</t>
         </is>
@@ -17607,7 +17607,7 @@
           <t>318</t>
         </is>
       </c>
-      <c r="AC97" s="14" t="inlineStr">
+      <c r="AC97" s="17" t="inlineStr">
         <is>
           <t>066</t>
         </is>
@@ -18048,7 +18048,7 @@
           <t>811</t>
         </is>
       </c>
-      <c r="E100" s="17" t="inlineStr">
+      <c r="E100" s="6" t="inlineStr">
         <is>
           <t>560</t>
         </is>
@@ -18123,7 +18123,7 @@
           <t>547</t>
         </is>
       </c>
-      <c r="T100" s="11" t="inlineStr">
+      <c r="T100" s="17" t="inlineStr">
         <is>
           <t>863</t>
         </is>
@@ -19519,7 +19519,7 @@
           <t>247</t>
         </is>
       </c>
-      <c r="T110" s="17" t="inlineStr">
+      <c r="T110" s="11" t="inlineStr">
         <is>
           <t>199</t>
         </is>
@@ -20287,7 +20287,7 @@
           <t>881</t>
         </is>
       </c>
-      <c r="X114" s="17" t="inlineStr">
+      <c r="X114" s="12" t="inlineStr">
         <is>
           <t>919</t>
         </is>
@@ -21030,7 +21030,7 @@
           <t>972</t>
         </is>
       </c>
-      <c r="W118" s="12" t="inlineStr">
+      <c r="W118" s="17" t="inlineStr">
         <is>
           <t>683</t>
         </is>
@@ -21848,7 +21848,7 @@
           <t>297</t>
         </is>
       </c>
-      <c r="AK122" s="16" t="inlineStr">
+      <c r="AK122" s="17" t="inlineStr">
         <is>
           <t>066</t>
         </is>
@@ -21865,7 +21865,7 @@
           <t>172</t>
         </is>
       </c>
-      <c r="C123" s="17" t="inlineStr">
+      <c r="C123" s="5" t="inlineStr">
         <is>
           <t>560</t>
         </is>
@@ -21940,7 +21940,7 @@
           <t>037</t>
         </is>
       </c>
-      <c r="R123" s="10" t="inlineStr">
+      <c r="R123" s="17" t="inlineStr">
         <is>
           <t>863</t>
         </is>
@@ -21975,7 +21975,7 @@
           <t>597</t>
         </is>
       </c>
-      <c r="Y123" s="12" t="inlineStr">
+      <c r="Y123" s="17" t="inlineStr">
         <is>
           <t>368</t>
         </is>
@@ -22192,7 +22192,7 @@
           <t>538</t>
         </is>
       </c>
-      <c r="AE124" s="17" t="inlineStr">
+      <c r="AE124" s="14" t="inlineStr">
         <is>
           <t>199</t>
         </is>
@@ -22436,7 +22436,7 @@
           <t>277</t>
         </is>
       </c>
-      <c r="E126" s="17" t="inlineStr">
+      <c r="E126" s="6" t="inlineStr">
         <is>
           <t>056</t>
         </is>
@@ -22653,7 +22653,7 @@
           <t>889</t>
         </is>
       </c>
-      <c r="K127" s="8" t="inlineStr">
+      <c r="K127" s="17" t="inlineStr">
         <is>
           <t>638</t>
         </is>
@@ -22663,7 +22663,7 @@
           <t>405</t>
         </is>
       </c>
-      <c r="M127" s="17" t="inlineStr">
+      <c r="M127" s="8" t="inlineStr">
         <is>
           <t>506</t>
         </is>
@@ -22773,7 +22773,7 @@
           <t>978</t>
         </is>
       </c>
-      <c r="AI127" s="17" t="inlineStr">
+      <c r="AI127" s="16" t="inlineStr">
         <is>
           <t>605</t>
         </is>
@@ -23461,7 +23461,7 @@
           <t>205</t>
         </is>
       </c>
-      <c r="W131" s="17" t="inlineStr">
+      <c r="W131" s="12" t="inlineStr">
         <is>
           <t>560</t>
         </is>
@@ -23501,7 +23501,7 @@
           <t>827</t>
         </is>
       </c>
-      <c r="AE131" s="17" t="inlineStr">
+      <c r="AE131" s="14" t="inlineStr">
         <is>
           <t>199</t>
         </is>
@@ -23563,7 +23563,7 @@
           <t>543</t>
         </is>
       </c>
-      <c r="F132" s="17" t="inlineStr">
+      <c r="F132" s="6" t="inlineStr">
         <is>
           <t>919</t>
         </is>
@@ -23900,7 +23900,7 @@
           <t>209</t>
         </is>
       </c>
-      <c r="AJ133" s="17" t="inlineStr">
+      <c r="AJ133" s="16" t="inlineStr">
         <is>
           <t>560</t>
         </is>
@@ -24588,12 +24588,12 @@
           <t>158</t>
         </is>
       </c>
-      <c r="X137" s="17" t="inlineStr">
+      <c r="X137" s="12" t="inlineStr">
         <is>
           <t>065</t>
         </is>
       </c>
-      <c r="Y137" s="12" t="inlineStr">
+      <c r="Y137" s="17" t="inlineStr">
         <is>
           <t>836</t>
         </is>
@@ -24628,7 +24628,7 @@
           <t>640</t>
         </is>
       </c>
-      <c r="AF137" s="17" t="inlineStr">
+      <c r="AF137" s="15" t="inlineStr">
         <is>
           <t>605</t>
         </is>
@@ -24735,7 +24735,7 @@
           <t>080</t>
         </is>
       </c>
-      <c r="P138" s="9" t="inlineStr">
+      <c r="P138" s="17" t="inlineStr">
         <is>
           <t>836</t>
         </is>
@@ -25151,7 +25151,7 @@
           <t>263</t>
         </is>
       </c>
-      <c r="G143" s="17" t="inlineStr">
+      <c r="G143" s="6" t="inlineStr">
         <is>
           <t>650</t>
         </is>
@@ -25423,7 +25423,7 @@
           <t>014</t>
         </is>
       </c>
-      <c r="X144" s="17" t="inlineStr">
+      <c r="X144" s="12" t="inlineStr">
         <is>
           <t>199</t>
         </is>
@@ -25934,7 +25934,7 @@
           <t>750</t>
         </is>
       </c>
-      <c r="N147" s="9" t="inlineStr">
+      <c r="N147" s="17" t="inlineStr">
         <is>
           <t>638</t>
         </is>
@@ -25949,7 +25949,7 @@
           <t>525</t>
         </is>
       </c>
-      <c r="Q147" s="17" t="inlineStr">
+      <c r="Q147" s="10" t="inlineStr">
         <is>
           <t>991</t>
         </is>
@@ -26403,7 +26403,7 @@
           <t>905</t>
         </is>
       </c>
-      <c r="AG149" s="15" t="inlineStr">
+      <c r="AG149" s="17" t="inlineStr">
         <is>
           <t>066</t>
         </is>
@@ -26545,7 +26545,7 @@
           <t>720</t>
         </is>
       </c>
-      <c r="X150" s="12" t="inlineStr">
+      <c r="X150" s="17" t="inlineStr">
         <is>
           <t>386</t>
         </is>
@@ -26929,7 +26929,7 @@
           <t>019</t>
         </is>
       </c>
-      <c r="Z152" s="17" t="inlineStr">
+      <c r="Z152" s="13" t="inlineStr">
         <is>
           <t>991</t>
         </is>
@@ -27001,7 +27001,7 @@
           <t>232</t>
         </is>
       </c>
-      <c r="C153" s="5" t="inlineStr">
+      <c r="C153" s="17" t="inlineStr">
         <is>
           <t>638</t>
         </is>
@@ -27136,7 +27136,7 @@
           <t>078</t>
         </is>
       </c>
-      <c r="AD153" s="14" t="inlineStr">
+      <c r="AD153" s="17" t="inlineStr">
         <is>
           <t>863</t>
         </is>
@@ -27183,7 +27183,7 @@
           <t>12</t>
         </is>
       </c>
-      <c r="B154" s="5" t="inlineStr">
+      <c r="B154" s="17" t="inlineStr">
         <is>
           <t>683</t>
         </is>
@@ -28238,7 +28238,7 @@
           <t>710</t>
         </is>
       </c>
-      <c r="Z159" s="13" t="inlineStr">
+      <c r="Z159" s="17" t="inlineStr">
         <is>
           <t>368</t>
         </is>
@@ -28956,7 +28956,7 @@
           <t>624</t>
         </is>
       </c>
-      <c r="T163" s="11" t="inlineStr">
+      <c r="T163" s="17" t="inlineStr">
         <is>
           <t>683</t>
         </is>
@@ -29335,7 +29335,7 @@
           <t>806</t>
         </is>
       </c>
-      <c r="U165" s="17" t="inlineStr">
+      <c r="U165" s="11" t="inlineStr">
         <is>
           <t>991</t>
         </is>
@@ -29502,7 +29502,7 @@
           <t>475</t>
         </is>
       </c>
-      <c r="Q166" s="17" t="inlineStr">
+      <c r="Q166" s="10" t="inlineStr">
         <is>
           <t>199</t>
         </is>
@@ -29614,7 +29614,7 @@
           <t>25</t>
         </is>
       </c>
-      <c r="B167" s="17" t="inlineStr">
+      <c r="B167" s="5" t="inlineStr">
         <is>
           <t>991</t>
         </is>
@@ -30148,7 +30148,7 @@
           <t>046</t>
         </is>
       </c>
-      <c r="AH169" s="15" t="inlineStr">
+      <c r="AH169" s="17" t="inlineStr">
         <is>
           <t>606</t>
         </is>
@@ -30215,7 +30215,7 @@
           <t>085</t>
         </is>
       </c>
-      <c r="J170" s="7" t="inlineStr">
+      <c r="J170" s="17" t="inlineStr">
         <is>
           <t>863</t>
         </is>
@@ -30649,7 +30649,7 @@
           <t>317</t>
         </is>
       </c>
-      <c r="V172" s="17" t="inlineStr">
+      <c r="V172" s="11" t="inlineStr">
         <is>
           <t>560</t>
         </is>
@@ -30664,7 +30664,7 @@
           <t>541</t>
         </is>
       </c>
-      <c r="Y172" s="12" t="inlineStr">
+      <c r="Y172" s="17" t="inlineStr">
         <is>
           <t>386</t>
         </is>
@@ -30679,7 +30679,7 @@
           <t>620</t>
         </is>
       </c>
-      <c r="AB172" s="17" t="inlineStr">
+      <c r="AB172" s="13" t="inlineStr">
         <is>
           <t>919</t>
         </is>
@@ -31474,7 +31474,7 @@
           <t>482</t>
         </is>
       </c>
-      <c r="T179" s="11" t="inlineStr">
+      <c r="T179" s="17" t="inlineStr">
         <is>
           <t>836</t>
         </is>
@@ -32000,7 +32000,7 @@
           <t>408</t>
         </is>
       </c>
-      <c r="M182" s="17" t="inlineStr">
+      <c r="M182" s="8" t="inlineStr">
         <is>
           <t>991</t>
         </is>
@@ -32025,7 +32025,7 @@
           <t>520</t>
         </is>
       </c>
-      <c r="R182" s="17" t="inlineStr">
+      <c r="R182" s="10" t="inlineStr">
         <is>
           <t>199</t>
         </is>
@@ -32040,7 +32040,7 @@
           <t>542</t>
         </is>
       </c>
-      <c r="U182" s="11" t="inlineStr">
+      <c r="U182" s="17" t="inlineStr">
         <is>
           <t>660</t>
         </is>
@@ -32267,7 +32267,7 @@
           <t>125</t>
         </is>
       </c>
-      <c r="AC183" s="14" t="inlineStr">
+      <c r="AC183" s="17" t="inlineStr">
         <is>
           <t>836</t>
         </is>
@@ -32561,7 +32561,7 @@
           <t>950</t>
         </is>
       </c>
-      <c r="M185" s="17" t="inlineStr">
+      <c r="M185" s="8" t="inlineStr">
         <is>
           <t>065</t>
         </is>
@@ -32601,7 +32601,7 @@
           <t>841</t>
         </is>
       </c>
-      <c r="U185" s="17" t="inlineStr">
+      <c r="U185" s="11" t="inlineStr">
         <is>
           <t>056</t>
         </is>
@@ -32880,7 +32880,7 @@
           <t>10</t>
         </is>
       </c>
-      <c r="B187" s="17" t="inlineStr">
+      <c r="B187" s="5" t="inlineStr">
         <is>
           <t>605</t>
         </is>
@@ -33010,7 +33010,7 @@
           <t>406</t>
         </is>
       </c>
-      <c r="AB187" s="17" t="inlineStr">
+      <c r="AB187" s="13" t="inlineStr">
         <is>
           <t>605</t>
         </is>
@@ -33142,7 +33142,7 @@
           <t>761</t>
         </is>
       </c>
-      <c r="Q188" s="10" t="inlineStr">
+      <c r="Q188" s="17" t="inlineStr">
         <is>
           <t>660</t>
         </is>
@@ -33728,7 +33728,7 @@
           <t>833</t>
         </is>
       </c>
-      <c r="V191" s="17" t="inlineStr">
+      <c r="V191" s="11" t="inlineStr">
         <is>
           <t>650</t>
         </is>
@@ -33738,7 +33738,7 @@
           <t>728</t>
         </is>
       </c>
-      <c r="X191" s="17" t="inlineStr">
+      <c r="X191" s="12" t="inlineStr">
         <is>
           <t>919</t>
         </is>
@@ -34107,7 +34107,7 @@
           <t>825</t>
         </is>
       </c>
-      <c r="W193" s="17" t="inlineStr">
+      <c r="W193" s="12" t="inlineStr">
         <is>
           <t>560</t>
         </is>
@@ -34152,7 +34152,7 @@
           <t>438</t>
         </is>
       </c>
-      <c r="AF193" s="17" t="inlineStr">
+      <c r="AF193" s="15" t="inlineStr">
         <is>
           <t>991</t>
         </is>
@@ -34738,7 +34738,7 @@
           <t>980</t>
         </is>
       </c>
-      <c r="AK196" s="17" t="inlineStr">
+      <c r="AK196" s="16" t="inlineStr">
         <is>
           <t>199</t>
         </is>
@@ -34925,7 +34925,7 @@
           <t>773</t>
         </is>
       </c>
-      <c r="AK197" s="17" t="inlineStr">
+      <c r="AK197" s="16" t="inlineStr">
         <is>
           <t>560</t>
         </is>
@@ -34957,7 +34957,7 @@
           <t>689</t>
         </is>
       </c>
-      <c r="F198" s="6" t="inlineStr">
+      <c r="F198" s="17" t="inlineStr">
         <is>
           <t>638</t>
         </is>
@@ -35007,7 +35007,7 @@
           <t>477</t>
         </is>
       </c>
-      <c r="P198" s="17" t="inlineStr">
+      <c r="P198" s="9" t="inlineStr">
         <is>
           <t>199</t>
         </is>
@@ -35092,7 +35092,7 @@
           <t>177</t>
         </is>
       </c>
-      <c r="AG198" s="17" t="inlineStr">
+      <c r="AG198" s="15" t="inlineStr">
         <is>
           <t>056</t>
         </is>
@@ -35690,7 +35690,7 @@
           <t>045</t>
         </is>
       </c>
-      <c r="C202" s="5" t="inlineStr">
+      <c r="C202" s="17" t="inlineStr">
         <is>
           <t>863</t>
         </is>
@@ -36301,12 +36301,12 @@
           <t>131</t>
         </is>
       </c>
-      <c r="M205" s="8" t="inlineStr">
+      <c r="M205" s="17" t="inlineStr">
         <is>
           <t>386</t>
         </is>
       </c>
-      <c r="N205" s="9" t="inlineStr">
+      <c r="N205" s="17" t="inlineStr">
         <is>
           <t>863</t>
         </is>
@@ -36528,7 +36528,7 @@
           <t>669</t>
         </is>
       </c>
-      <c r="U206" s="17" t="inlineStr">
+      <c r="U206" s="11" t="inlineStr">
         <is>
           <t>650</t>
         </is>
@@ -36750,7 +36750,7 @@
           <t>658</t>
         </is>
       </c>
-      <c r="AB207" s="17" t="inlineStr">
+      <c r="AB207" s="13" t="inlineStr">
         <is>
           <t>199</t>
         </is>
@@ -37368,7 +37368,7 @@
           <t>965</t>
         </is>
       </c>
-      <c r="V213" s="17" t="inlineStr">
+      <c r="V213" s="11" t="inlineStr">
         <is>
           <t>199</t>
         </is>
@@ -37515,7 +37515,7 @@
           <t>585</t>
         </is>
       </c>
-      <c r="N214" s="9" t="inlineStr">
+      <c r="N214" s="17" t="inlineStr">
         <is>
           <t>683</t>
         </is>
@@ -38176,7 +38176,7 @@
           <t>970</t>
         </is>
       </c>
-      <c r="AH217" s="15" t="inlineStr">
+      <c r="AH217" s="17" t="inlineStr">
         <is>
           <t>368</t>
         </is>
@@ -38318,7 +38318,7 @@
           <t>041</t>
         </is>
       </c>
-      <c r="Y218" s="17" t="inlineStr">
+      <c r="Y218" s="12" t="inlineStr">
         <is>
           <t>199</t>
         </is>
@@ -38395,7 +38395,7 @@
           <t>499</t>
         </is>
       </c>
-      <c r="C219" s="17" t="inlineStr">
+      <c r="C219" s="5" t="inlineStr">
         <is>
           <t>506</t>
         </is>
@@ -38410,7 +38410,7 @@
           <t>957</t>
         </is>
       </c>
-      <c r="F219" s="17" t="inlineStr">
+      <c r="F219" s="6" t="inlineStr">
         <is>
           <t>065</t>
         </is>
@@ -38637,7 +38637,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="N220" s="17" t="inlineStr">
+      <c r="N220" s="9" t="inlineStr">
         <is>
           <t>056</t>
         </is>
@@ -38879,7 +38879,7 @@
           <t>359</t>
         </is>
       </c>
-      <c r="Y221" s="17" t="inlineStr">
+      <c r="Y221" s="12" t="inlineStr">
         <is>
           <t>560</t>
         </is>
@@ -39298,7 +39298,7 @@
           <t>795</t>
         </is>
       </c>
-      <c r="AH223" s="17" t="inlineStr">
+      <c r="AH223" s="15" t="inlineStr">
         <is>
           <t>506</t>
         </is>
@@ -40866,7 +40866,7 @@
           <t>954</t>
         </is>
       </c>
-      <c r="K232" s="8" t="inlineStr">
+      <c r="K232" s="17" t="inlineStr">
         <is>
           <t>386</t>
         </is>
@@ -41270,7 +41270,7 @@
           <t>669</t>
         </is>
       </c>
-      <c r="Q234" s="10" t="inlineStr">
+      <c r="Q234" s="17" t="inlineStr">
         <is>
           <t>368</t>
         </is>
@@ -41906,7 +41906,7 @@
           <t>637</t>
         </is>
       </c>
-      <c r="AF237" s="15" t="inlineStr">
+      <c r="AF237" s="17" t="inlineStr">
         <is>
           <t>368</t>
         </is>
@@ -42043,7 +42043,7 @@
           <t>095</t>
         </is>
       </c>
-      <c r="V238" s="11" t="inlineStr">
+      <c r="V238" s="17" t="inlineStr">
         <is>
           <t>638</t>
         </is>
@@ -42270,7 +42270,7 @@
           <t>670</t>
         </is>
       </c>
-      <c r="AD239" s="17" t="inlineStr">
+      <c r="AD239" s="14" t="inlineStr">
         <is>
           <t>199</t>
         </is>
@@ -42487,7 +42487,7 @@
           <t>845</t>
         </is>
       </c>
-      <c r="AJ240" s="16" t="inlineStr">
+      <c r="AJ240" s="17" t="inlineStr">
         <is>
           <t>386</t>
         </is>
@@ -42589,7 +42589,7 @@
           <t>543</t>
         </is>
       </c>
-      <c r="S241" s="10" t="inlineStr">
+      <c r="S241" s="17" t="inlineStr">
         <is>
           <t>386</t>
         </is>
@@ -42664,7 +42664,7 @@
           <t>491</t>
         </is>
       </c>
-      <c r="AH241" s="17" t="inlineStr">
+      <c r="AH241" s="15" t="inlineStr">
         <is>
           <t>199</t>
         </is>
@@ -42674,12 +42674,12 @@
           <t>677</t>
         </is>
       </c>
-      <c r="AJ241" s="17" t="inlineStr">
+      <c r="AJ241" s="16" t="inlineStr">
         <is>
           <t>919</t>
         </is>
       </c>
-      <c r="AK241" s="16" t="inlineStr">
+      <c r="AK241" s="17" t="inlineStr">
         <is>
           <t>836</t>
         </is>
@@ -43566,7 +43566,7 @@
           <t>800</t>
         </is>
       </c>
-      <c r="J249" s="7" t="inlineStr">
+      <c r="J249" s="17" t="inlineStr">
         <is>
           <t>606</t>
         </is>
@@ -43606,7 +43606,7 @@
           <t>568</t>
         </is>
       </c>
-      <c r="R249" s="17" t="inlineStr">
+      <c r="R249" s="10" t="inlineStr">
         <is>
           <t>991</t>
         </is>
@@ -43621,7 +43621,7 @@
           <t>372</t>
         </is>
       </c>
-      <c r="U249" s="17" t="inlineStr">
+      <c r="U249" s="11" t="inlineStr">
         <is>
           <t>560</t>
         </is>
@@ -43813,7 +43813,7 @@
           <t>341</t>
         </is>
       </c>
-      <c r="V250" s="17" t="inlineStr">
+      <c r="V250" s="11" t="inlineStr">
         <is>
           <t>199</t>
         </is>
@@ -44242,7 +44242,7 @@
           <t>439</t>
         </is>
       </c>
-      <c r="AG252" s="15" t="inlineStr">
+      <c r="AG252" s="17" t="inlineStr">
         <is>
           <t>606</t>
         </is>
@@ -44658,7 +44658,7 @@
           <t>818</t>
         </is>
       </c>
-      <c r="D255" s="5" t="inlineStr">
+      <c r="D255" s="17" t="inlineStr">
         <is>
           <t>386</t>
         </is>
@@ -44728,7 +44728,7 @@
           <t>249</t>
         </is>
       </c>
-      <c r="R255" s="10" t="inlineStr">
+      <c r="R255" s="17" t="inlineStr">
         <is>
           <t>660</t>
         </is>
@@ -45057,7 +45057,7 @@
           <t>623</t>
         </is>
       </c>
-      <c r="I257" s="7" t="inlineStr">
+      <c r="I257" s="17" t="inlineStr">
         <is>
           <t>638</t>
         </is>
@@ -45289,7 +45289,7 @@
           <t>654</t>
         </is>
       </c>
-      <c r="R258" s="10" t="inlineStr">
+      <c r="R258" s="17" t="inlineStr">
         <is>
           <t>660</t>
         </is>
@@ -45785,7 +45785,7 @@
           <t>601</t>
         </is>
       </c>
-      <c r="E261" s="6" t="inlineStr">
+      <c r="E261" s="17" t="inlineStr">
         <is>
           <t>066</t>
         </is>
@@ -45962,7 +45962,7 @@
           <t>513</t>
         </is>
       </c>
-      <c r="C262" s="5" t="inlineStr">
+      <c r="C262" s="17" t="inlineStr">
         <is>
           <t>368</t>
         </is>
@@ -46017,7 +46017,7 @@
           <t>971</t>
         </is>
       </c>
-      <c r="N262" s="17" t="inlineStr">
+      <c r="N262" s="9" t="inlineStr">
         <is>
           <t>056</t>
         </is>
@@ -46214,7 +46214,7 @@
           <t>838</t>
         </is>
       </c>
-      <c r="P263" s="9" t="inlineStr">
+      <c r="P263" s="17" t="inlineStr">
         <is>
           <t>386</t>
         </is>
@@ -46269,7 +46269,7 @@
           <t>878</t>
         </is>
       </c>
-      <c r="AA263" s="13" t="inlineStr">
+      <c r="AA263" s="17" t="inlineStr">
         <is>
           <t>066</t>
         </is>
@@ -47079,7 +47079,7 @@
           <t>21</t>
         </is>
       </c>
-      <c r="B268" s="5" t="inlineStr">
+      <c r="B268" s="17" t="inlineStr">
         <is>
           <t>368</t>
         </is>
@@ -47114,7 +47114,7 @@
           <t>546</t>
         </is>
       </c>
-      <c r="I268" s="7" t="inlineStr">
+      <c r="I268" s="17" t="inlineStr">
         <is>
           <t>660</t>
         </is>
@@ -48393,7 +48393,7 @@
           <t>753</t>
         </is>
       </c>
-      <c r="C275" s="17" t="inlineStr">
+      <c r="C275" s="5" t="inlineStr">
         <is>
           <t>506</t>
         </is>
@@ -49834,7 +49834,7 @@
           <t>193</t>
         </is>
       </c>
-      <c r="L285" s="17" t="inlineStr">
+      <c r="L285" s="8" t="inlineStr">
         <is>
           <t>560</t>
         </is>
@@ -49844,7 +49844,7 @@
           <t>562</t>
         </is>
       </c>
-      <c r="N285" s="9" t="inlineStr">
+      <c r="N285" s="17" t="inlineStr">
         <is>
           <t>368</t>
         </is>
@@ -50515,7 +50515,7 @@
           <t>657</t>
         </is>
       </c>
-      <c r="AJ288" s="16" t="inlineStr">
+      <c r="AJ288" s="17" t="inlineStr">
         <is>
           <t>606</t>
         </is>
@@ -50769,7 +50769,7 @@
           <t>987</t>
         </is>
       </c>
-      <c r="L290" s="17" t="inlineStr">
+      <c r="L290" s="8" t="inlineStr">
         <is>
           <t>650</t>
         </is>
@@ -51178,7 +51178,7 @@
           <t>433</t>
         </is>
       </c>
-      <c r="S292" s="10" t="inlineStr">
+      <c r="S292" s="17" t="inlineStr">
         <is>
           <t>638</t>
         </is>
@@ -51223,7 +51223,7 @@
           <t>703</t>
         </is>
       </c>
-      <c r="AB292" s="13" t="inlineStr">
+      <c r="AB292" s="17" t="inlineStr">
         <is>
           <t>863</t>
         </is>
@@ -51669,7 +51669,7 @@
           <t>980</t>
         </is>
       </c>
-      <c r="E295" s="6" t="inlineStr">
+      <c r="E295" s="17" t="inlineStr">
         <is>
           <t>386</t>
         </is>
@@ -51956,7 +51956,7 @@
           <t>769</t>
         </is>
       </c>
-      <c r="Y296" s="17" t="inlineStr">
+      <c r="Y296" s="12" t="inlineStr">
         <is>
           <t>605</t>
         </is>
@@ -52043,7 +52043,7 @@
           <t>867</t>
         </is>
       </c>
-      <c r="E297" s="6" t="inlineStr">
+      <c r="E297" s="17" t="inlineStr">
         <is>
           <t>638</t>
         </is>
@@ -52088,7 +52088,7 @@
           <t>714</t>
         </is>
       </c>
-      <c r="N297" s="9" t="inlineStr">
+      <c r="N297" s="17" t="inlineStr">
         <is>
           <t>863</t>
         </is>
@@ -52946,7 +52946,7 @@
           <t>918</t>
         </is>
       </c>
-      <c r="AJ301" s="16" t="inlineStr">
+      <c r="AJ301" s="17" t="inlineStr">
         <is>
           <t>836</t>
         </is>
@@ -52968,7 +52968,7 @@
           <t>528</t>
         </is>
       </c>
-      <c r="C302" s="17" t="inlineStr">
+      <c r="C302" s="5" t="inlineStr">
         <is>
           <t>199</t>
         </is>
@@ -53240,7 +53240,7 @@
           <t>232</t>
         </is>
       </c>
-      <c r="T303" s="11" t="inlineStr">
+      <c r="T303" s="17" t="inlineStr">
         <is>
           <t>606</t>
         </is>
@@ -53933,7 +53933,7 @@
           <t>288</t>
         </is>
       </c>
-      <c r="I307" s="7" t="inlineStr">
+      <c r="I307" s="17" t="inlineStr">
         <is>
           <t>066</t>
         </is>
@@ -53993,7 +53993,7 @@
           <t>010</t>
         </is>
       </c>
-      <c r="U307" s="17" t="inlineStr">
+      <c r="U307" s="11" t="inlineStr">
         <is>
           <t>919</t>
         </is>
@@ -54028,7 +54028,7 @@
           <t>563</t>
         </is>
       </c>
-      <c r="AB307" s="17" t="inlineStr">
+      <c r="AB307" s="13" t="inlineStr">
         <is>
           <t>605</t>
         </is>
@@ -54125,7 +54125,7 @@
           <t>662</t>
         </is>
       </c>
-      <c r="J308" s="7" t="inlineStr">
+      <c r="J308" s="17" t="inlineStr">
         <is>
           <t>066</t>
         </is>
@@ -54170,7 +54170,7 @@
           <t>703</t>
         </is>
       </c>
-      <c r="S308" s="10" t="inlineStr">
+      <c r="S308" s="17" t="inlineStr">
         <is>
           <t>368</t>
         </is>
@@ -54357,7 +54357,7 @@
           <t>482</t>
         </is>
       </c>
-      <c r="S309" s="10" t="inlineStr">
+      <c r="S309" s="17" t="inlineStr">
         <is>
           <t>386</t>
         </is>
@@ -54913,7 +54913,7 @@
           <t>623</t>
         </is>
       </c>
-      <c r="R312" s="10" t="inlineStr">
+      <c r="R312" s="17" t="inlineStr">
         <is>
           <t>606</t>
         </is>
@@ -55085,7 +55085,7 @@
           <t>615</t>
         </is>
       </c>
-      <c r="O313" s="17" t="inlineStr">
+      <c r="O313" s="9" t="inlineStr">
         <is>
           <t>605</t>
         </is>
@@ -55120,7 +55120,7 @@
           <t>928</t>
         </is>
       </c>
-      <c r="V313" s="17" t="inlineStr">
+      <c r="V313" s="11" t="inlineStr">
         <is>
           <t>506</t>
         </is>
@@ -55556,12 +55556,12 @@
           <t>960</t>
         </is>
       </c>
-      <c r="Q318" s="17" t="inlineStr">
+      <c r="Q318" s="10" t="inlineStr">
         <is>
           <t>650</t>
         </is>
       </c>
-      <c r="R318" s="10" t="inlineStr">
+      <c r="R318" s="17" t="inlineStr">
         <is>
           <t>368</t>
         </is>
@@ -55880,7 +55880,7 @@
           <t>636</t>
         </is>
       </c>
-      <c r="G320" s="6" t="inlineStr">
+      <c r="G320" s="17" t="inlineStr">
         <is>
           <t>683</t>
         </is>
@@ -56466,7 +56466,7 @@
           <t>304</t>
         </is>
       </c>
-      <c r="L323" s="8" t="inlineStr">
+      <c r="L323" s="17" t="inlineStr">
         <is>
           <t>368</t>
         </is>
@@ -57067,7 +57067,7 @@
           <t>161</t>
         </is>
       </c>
-      <c r="T326" s="11" t="inlineStr">
+      <c r="T326" s="17" t="inlineStr">
         <is>
           <t>638</t>
         </is>
@@ -57239,7 +57239,7 @@
           <t>603</t>
         </is>
       </c>
-      <c r="Q327" s="10" t="inlineStr">
+      <c r="Q327" s="17" t="inlineStr">
         <is>
           <t>683</t>
         </is>
@@ -57688,7 +57688,7 @@
           <t>613</t>
         </is>
       </c>
-      <c r="AF329" s="17" t="inlineStr">
+      <c r="AF329" s="15" t="inlineStr">
         <is>
           <t>605</t>
         </is>
@@ -57713,7 +57713,7 @@
           <t>103</t>
         </is>
       </c>
-      <c r="AK329" s="16" t="inlineStr">
+      <c r="AK329" s="17" t="inlineStr">
         <is>
           <t>386</t>
         </is>
@@ -57790,7 +57790,7 @@
           <t>300</t>
         </is>
       </c>
-      <c r="O330" s="17" t="inlineStr">
+      <c r="O330" s="9" t="inlineStr">
         <is>
           <t>919</t>
         </is>
@@ -57865,7 +57865,7 @@
           <t>774</t>
         </is>
       </c>
-      <c r="AD330" s="14" t="inlineStr">
+      <c r="AD330" s="17" t="inlineStr">
         <is>
           <t>606</t>
         </is>
@@ -57942,7 +57942,7 @@
           <t>075</t>
         </is>
       </c>
-      <c r="H331" s="17" t="inlineStr">
+      <c r="H331" s="7" t="inlineStr">
         <is>
           <t>919</t>
         </is>
@@ -58229,7 +58229,7 @@
           <t>374</t>
         </is>
       </c>
-      <c r="AB332" s="17" t="inlineStr">
+      <c r="AB332" s="13" t="inlineStr">
         <is>
           <t>605</t>
         </is>
@@ -58628,7 +58628,7 @@
           <t>633</t>
         </is>
       </c>
-      <c r="AG334" s="15" t="inlineStr">
+      <c r="AG334" s="17" t="inlineStr">
         <is>
           <t>606</t>
         </is>
@@ -58882,7 +58882,7 @@
           <t>878</t>
         </is>
       </c>
-      <c r="I336" s="7" t="inlineStr">
+      <c r="I336" s="17" t="inlineStr">
         <is>
           <t>863</t>
         </is>
@@ -59226,7 +59226,7 @@
           <t>636</t>
         </is>
       </c>
-      <c r="C338" s="17" t="inlineStr">
+      <c r="C338" s="5" t="inlineStr">
         <is>
           <t>065</t>
         </is>
@@ -59630,7 +59630,7 @@
           <t>575</t>
         </is>
       </c>
-      <c r="I340" s="7" t="inlineStr">
+      <c r="I340" s="17" t="inlineStr">
         <is>
           <t>863</t>
         </is>
@@ -59685,7 +59685,7 @@
           <t>902</t>
         </is>
       </c>
-      <c r="T340" s="17" t="inlineStr">
+      <c r="T340" s="11" t="inlineStr">
         <is>
           <t>605</t>
         </is>
@@ -60236,7 +60236,7 @@
           <t>328</t>
         </is>
       </c>
-      <c r="R343" s="10" t="inlineStr">
+      <c r="R343" s="17" t="inlineStr">
         <is>
           <t>066</t>
         </is>
@@ -60363,7 +60363,7 @@
           <t>983</t>
         </is>
       </c>
-      <c r="F344" s="6" t="inlineStr">
+      <c r="F344" s="17" t="inlineStr">
         <is>
           <t>638</t>
         </is>
@@ -62410,7 +62410,7 @@
           <t>855</t>
         </is>
       </c>
-      <c r="X357" s="17" t="inlineStr">
+      <c r="X357" s="12" t="inlineStr">
         <is>
           <t>199</t>
         </is>
@@ -63557,7 +63557,7 @@
           <t>632</t>
         </is>
       </c>
-      <c r="AC363" s="14" t="inlineStr">
+      <c r="AC363" s="17" t="inlineStr">
         <is>
           <t>683</t>
         </is>
@@ -63592,7 +63592,7 @@
           <t>449</t>
         </is>
       </c>
-      <c r="AJ363" s="16" t="inlineStr">
+      <c r="AJ363" s="17" t="inlineStr">
         <is>
           <t>683</t>
         </is>
@@ -63946,7 +63946,7 @@
           <t>211</t>
         </is>
       </c>
-      <c r="AF365" s="15" t="inlineStr">
+      <c r="AF365" s="17" t="inlineStr">
         <is>
           <t>606</t>
         </is>
@@ -64392,7 +64392,7 @@
           <t>412</t>
         </is>
       </c>
-      <c r="I368" s="17" t="inlineStr">
+      <c r="I368" s="7" t="inlineStr">
         <is>
           <t>506</t>
         </is>
@@ -64447,7 +64447,7 @@
           <t>708</t>
         </is>
       </c>
-      <c r="T368" s="17" t="inlineStr">
+      <c r="T368" s="11" t="inlineStr">
         <is>
           <t>991</t>
         </is>
@@ -64614,7 +64614,7 @@
           <t>972</t>
         </is>
       </c>
-      <c r="P369" s="9" t="inlineStr">
+      <c r="P369" s="17" t="inlineStr">
         <is>
           <t>660</t>
         </is>
@@ -64963,7 +64963,7 @@
           <t>020</t>
         </is>
       </c>
-      <c r="K371" s="17" t="inlineStr">
+      <c r="K371" s="8" t="inlineStr">
         <is>
           <t>506</t>
         </is>
@@ -65063,7 +65063,7 @@
           <t>452</t>
         </is>
       </c>
-      <c r="AE371" s="14" t="inlineStr">
+      <c r="AE371" s="17" t="inlineStr">
         <is>
           <t>368</t>
         </is>
@@ -65489,7 +65489,7 @@
           <t>696</t>
         </is>
       </c>
-      <c r="D374" s="5" t="inlineStr">
+      <c r="D374" s="17" t="inlineStr">
         <is>
           <t>386</t>
         </is>
@@ -65786,7 +65786,7 @@
           <t>553</t>
         </is>
       </c>
-      <c r="Z375" s="17" t="inlineStr">
+      <c r="Z375" s="13" t="inlineStr">
         <is>
           <t>056</t>
         </is>
@@ -66145,7 +66145,7 @@
           <t>057</t>
         </is>
       </c>
-      <c r="W377" s="17" t="inlineStr">
+      <c r="W377" s="12" t="inlineStr">
         <is>
           <t>605</t>
         </is>
@@ -66434,7 +66434,7 @@
           <t>163</t>
         </is>
       </c>
-      <c r="F379" s="6" t="inlineStr">
+      <c r="F379" s="17" t="inlineStr">
         <is>
           <t>863</t>
         </is>
@@ -66706,7 +66706,7 @@
           <t>090</t>
         </is>
       </c>
-      <c r="W380" s="17" t="inlineStr">
+      <c r="W380" s="12" t="inlineStr">
         <is>
           <t>991</t>
         </is>
@@ -66731,7 +66731,7 @@
           <t>858</t>
         </is>
       </c>
-      <c r="AB380" s="17" t="inlineStr">
+      <c r="AB380" s="13" t="inlineStr">
         <is>
           <t>065</t>
         </is>
@@ -66913,7 +66913,7 @@
           <t>886</t>
         </is>
       </c>
-      <c r="AA381" s="13" t="inlineStr">
+      <c r="AA381" s="17" t="inlineStr">
         <is>
           <t>386</t>
         </is>
@@ -67060,7 +67060,7 @@
           <t>132</t>
         </is>
       </c>
-      <c r="S382" s="17" t="inlineStr">
+      <c r="S382" s="10" t="inlineStr">
         <is>
           <t>650</t>
         </is>
@@ -67758,7 +67758,7 @@
           <t>641</t>
         </is>
       </c>
-      <c r="AC388" s="17" t="inlineStr">
+      <c r="AC388" s="14" t="inlineStr">
         <is>
           <t>506</t>
         </is>
@@ -67865,7 +67865,7 @@
           <t>366</t>
         </is>
       </c>
-      <c r="M389" s="17" t="inlineStr">
+      <c r="M389" s="8" t="inlineStr">
         <is>
           <t>506</t>
         </is>
@@ -67915,7 +67915,7 @@
           <t>816</t>
         </is>
       </c>
-      <c r="W389" s="17" t="inlineStr">
+      <c r="W389" s="12" t="inlineStr">
         <is>
           <t>919</t>
         </is>
@@ -68229,7 +68229,7 @@
           <t>099</t>
         </is>
       </c>
-      <c r="K391" s="8" t="inlineStr">
+      <c r="K391" s="17" t="inlineStr">
         <is>
           <t>863</t>
         </is>
@@ -68476,7 +68476,7 @@
           <t>912</t>
         </is>
       </c>
-      <c r="W392" s="17" t="inlineStr">
+      <c r="W392" s="12" t="inlineStr">
         <is>
           <t>056</t>
         </is>
@@ -68708,7 +68708,7 @@
           <t>707</t>
         </is>
       </c>
-      <c r="AF393" s="15" t="inlineStr">
+      <c r="AF393" s="17" t="inlineStr">
         <is>
           <t>606</t>
         </is>
@@ -69668,7 +69668,7 @@
           <t>275</t>
         </is>
       </c>
-      <c r="AK398" s="16" t="inlineStr">
+      <c r="AK398" s="17" t="inlineStr">
         <is>
           <t>863</t>
         </is>
@@ -69907,7 +69907,7 @@
           <t>438</t>
         </is>
       </c>
-      <c r="J400" s="17" t="inlineStr">
+      <c r="J400" s="7" t="inlineStr">
         <is>
           <t>056</t>
         </is>
@@ -70189,7 +70189,7 @@
           <t>295</t>
         </is>
       </c>
-      <c r="AC401" s="14" t="inlineStr">
+      <c r="AC401" s="17" t="inlineStr">
         <is>
           <t>368</t>
         </is>
@@ -70316,7 +70316,7 @@
           <t>971</t>
         </is>
       </c>
-      <c r="Q402" s="17" t="inlineStr">
+      <c r="Q402" s="10" t="inlineStr">
         <is>
           <t>919</t>
         </is>
@@ -70351,7 +70351,7 @@
           <t>524</t>
         </is>
       </c>
-      <c r="X402" s="17" t="inlineStr">
+      <c r="X402" s="12" t="inlineStr">
         <is>
           <t>650</t>
         </is>
@@ -71149,7 +71149,7 @@
           <t>763</t>
         </is>
       </c>
-      <c r="AH406" s="15" t="inlineStr">
+      <c r="AH406" s="17" t="inlineStr">
         <is>
           <t>863</t>
         </is>
@@ -71186,7 +71186,7 @@
           <t>755</t>
         </is>
       </c>
-      <c r="D407" s="5" t="inlineStr">
+      <c r="D407" s="17" t="inlineStr">
         <is>
           <t>863</t>
         </is>
@@ -71286,7 +71286,7 @@
           <t>594</t>
         </is>
       </c>
-      <c r="X407" s="12" t="inlineStr">
+      <c r="X407" s="17" t="inlineStr">
         <is>
           <t>660</t>
         </is>
@@ -71326,7 +71326,7 @@
           <t>621</t>
         </is>
       </c>
-      <c r="AF407" s="15" t="inlineStr">
+      <c r="AF407" s="17" t="inlineStr">
         <is>
           <t>660</t>
         </is>
@@ -71630,7 +71630,7 @@
           <t>618</t>
         </is>
       </c>
-      <c r="R409" s="17" t="inlineStr">
+      <c r="R409" s="10" t="inlineStr">
         <is>
           <t>650</t>
         </is>
@@ -72211,7 +72211,7 @@
           <t>339</t>
         </is>
       </c>
-      <c r="V412" s="11" t="inlineStr">
+      <c r="V412" s="17" t="inlineStr">
         <is>
           <t>836</t>
         </is>
@@ -72832,7 +72832,7 @@
           <t>974</t>
         </is>
       </c>
-      <c r="AH415" s="17" t="inlineStr">
+      <c r="AH415" s="15" t="inlineStr">
         <is>
           <t>919</t>
         </is>
@@ -72944,7 +72944,7 @@
           <t>619</t>
         </is>
       </c>
-      <c r="S416" s="10" t="inlineStr">
+      <c r="S416" s="17" t="inlineStr">
         <is>
           <t>683</t>
         </is>
@@ -72979,7 +72979,7 @@
           <t>078</t>
         </is>
       </c>
-      <c r="Z416" s="17" t="inlineStr">
+      <c r="Z416" s="13" t="inlineStr">
         <is>
           <t>560</t>
         </is>
@@ -73019,7 +73019,7 @@
           <t>327</t>
         </is>
       </c>
-      <c r="AH416" s="17" t="inlineStr">
+      <c r="AH416" s="15" t="inlineStr">
         <is>
           <t>919</t>
         </is>
@@ -73196,7 +73196,7 @@
           <t>515</t>
         </is>
       </c>
-      <c r="AF417" s="17" t="inlineStr">
+      <c r="AF417" s="15" t="inlineStr">
         <is>
           <t>056</t>
         </is>
@@ -73714,7 +73714,7 @@
           <t>380</t>
         </is>
       </c>
-      <c r="F423" s="17" t="inlineStr">
+      <c r="F423" s="6" t="inlineStr">
         <is>
           <t>065</t>
         </is>
@@ -73809,7 +73809,7 @@
           <t>801</t>
         </is>
       </c>
-      <c r="Y423" s="12" t="inlineStr">
+      <c r="Y423" s="17" t="inlineStr">
         <is>
           <t>386</t>
         </is>
@@ -73839,7 +73839,7 @@
           <t>968</t>
         </is>
       </c>
-      <c r="AE423" s="17" t="inlineStr">
+      <c r="AE423" s="14" t="inlineStr">
         <is>
           <t>056</t>
         </is>
@@ -75068,7 +75068,7 @@
           <t>725</t>
         </is>
       </c>
-      <c r="O430" s="17" t="inlineStr">
+      <c r="O430" s="9" t="inlineStr">
         <is>
           <t>605</t>
         </is>
@@ -75270,7 +75270,7 @@
           <t>724</t>
         </is>
       </c>
-      <c r="R431" s="10" t="inlineStr">
+      <c r="R431" s="17" t="inlineStr">
         <is>
           <t>066</t>
         </is>
@@ -75427,7 +75427,7 @@
           <t>884</t>
         </is>
       </c>
-      <c r="L432" s="17" t="inlineStr">
+      <c r="L432" s="8" t="inlineStr">
         <is>
           <t>056</t>
         </is>
@@ -75776,7 +75776,7 @@
           <t>323</t>
         </is>
       </c>
-      <c r="G434" s="17" t="inlineStr">
+      <c r="G434" s="6" t="inlineStr">
         <is>
           <t>919</t>
         </is>
@@ -76125,7 +76125,7 @@
           <t>14</t>
         </is>
       </c>
-      <c r="B436" s="5" t="inlineStr">
+      <c r="B436" s="17" t="inlineStr">
         <is>
           <t>836</t>
         </is>
@@ -76529,7 +76529,7 @@
           <t>008</t>
         </is>
       </c>
-      <c r="H438" s="7" t="inlineStr">
+      <c r="H438" s="17" t="inlineStr">
         <is>
           <t>683</t>
         </is>
@@ -76544,7 +76544,7 @@
           <t>057</t>
         </is>
       </c>
-      <c r="K438" s="8" t="inlineStr">
+      <c r="K438" s="17" t="inlineStr">
         <is>
           <t>836</t>
         </is>
@@ -76711,7 +76711,7 @@
           <t>135</t>
         </is>
       </c>
-      <c r="G439" s="17" t="inlineStr">
+      <c r="G439" s="6" t="inlineStr">
         <is>
           <t>991</t>
         </is>
@@ -76888,7 +76888,7 @@
           <t>805</t>
         </is>
       </c>
-      <c r="E440" s="17" t="inlineStr">
+      <c r="E440" s="6" t="inlineStr">
         <is>
           <t>506</t>
         </is>
@@ -77110,7 +77110,7 @@
           <t>879</t>
         </is>
       </c>
-      <c r="L441" s="8" t="inlineStr">
+      <c r="L441" s="17" t="inlineStr">
         <is>
           <t>606</t>
         </is>
@@ -77210,7 +77210,7 @@
           <t>457</t>
         </is>
       </c>
-      <c r="AF441" s="17" t="inlineStr">
+      <c r="AF441" s="15" t="inlineStr">
         <is>
           <t>605</t>
         </is>
@@ -77262,7 +77262,7 @@
           <t>475</t>
         </is>
       </c>
-      <c r="E442" s="6" t="inlineStr">
+      <c r="E442" s="17" t="inlineStr">
         <is>
           <t>606</t>
         </is>
@@ -77347,7 +77347,7 @@
           <t>998</t>
         </is>
       </c>
-      <c r="V442" s="17" t="inlineStr">
+      <c r="V442" s="11" t="inlineStr">
         <is>
           <t>506</t>
         </is>
@@ -77559,7 +77559,7 @@
           <t>138</t>
         </is>
       </c>
-      <c r="AA443" s="17" t="inlineStr">
+      <c r="AA443" s="13" t="inlineStr">
         <is>
           <t>056</t>
         </is>
@@ -77609,7 +77609,7 @@
           <t>672</t>
         </is>
       </c>
-      <c r="AK443" s="17" t="inlineStr">
+      <c r="AK443" s="16" t="inlineStr">
         <is>
           <t>506</t>
         </is>
@@ -77928,7 +77928,7 @@
           <t>541</t>
         </is>
       </c>
-      <c r="Z445" s="17" t="inlineStr">
+      <c r="Z445" s="13" t="inlineStr">
         <is>
           <t>991</t>
         </is>
@@ -78182,7 +78182,7 @@
           <t>25</t>
         </is>
       </c>
-      <c r="B447" s="5" t="inlineStr">
+      <c r="B447" s="17" t="inlineStr">
         <is>
           <t>386</t>
         </is>
@@ -79035,7 +79035,7 @@
           <t>932</t>
         </is>
       </c>
-      <c r="W451" s="17" t="inlineStr">
+      <c r="W451" s="12" t="inlineStr">
         <is>
           <t>506</t>
         </is>
@@ -79162,7 +79162,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="K452" s="8" t="inlineStr">
+      <c r="K452" s="17" t="inlineStr">
         <is>
           <t>638</t>
         </is>
@@ -79835,7 +79835,7 @@
           <t>110</t>
         </is>
       </c>
-      <c r="P458" s="17" t="inlineStr">
+      <c r="P458" s="9" t="inlineStr">
         <is>
           <t>065</t>
         </is>
@@ -79987,7 +79987,7 @@
           <t>911</t>
         </is>
       </c>
-      <c r="I459" s="7" t="inlineStr">
+      <c r="I459" s="17" t="inlineStr">
         <is>
           <t>368</t>
         </is>
@@ -80072,7 +80072,7 @@
           <t>261</t>
         </is>
       </c>
-      <c r="Z459" s="17" t="inlineStr">
+      <c r="Z459" s="13" t="inlineStr">
         <is>
           <t>650</t>
         </is>
@@ -80381,7 +80381,7 @@
           <t>189</t>
         </is>
       </c>
-      <c r="M461" s="17" t="inlineStr">
+      <c r="M461" s="8" t="inlineStr">
         <is>
           <t>560</t>
         </is>
@@ -81234,7 +81234,7 @@
           <t>689</t>
         </is>
       </c>
-      <c r="AH465" s="17" t="inlineStr">
+      <c r="AH465" s="15" t="inlineStr">
         <is>
           <t>991</t>
         </is>
@@ -81361,7 +81361,7 @@
           <t>079</t>
         </is>
       </c>
-      <c r="V466" s="11" t="inlineStr">
+      <c r="V466" s="17" t="inlineStr">
         <is>
           <t>660</t>
         </is>
@@ -81421,7 +81421,7 @@
           <t>944</t>
         </is>
       </c>
-      <c r="AH466" s="15" t="inlineStr">
+      <c r="AH466" s="17" t="inlineStr">
         <is>
           <t>660</t>
         </is>
@@ -81458,7 +81458,7 @@
           <t>294</t>
         </is>
       </c>
-      <c r="D467" s="17" t="inlineStr">
+      <c r="D467" s="5" t="inlineStr">
         <is>
           <t>650</t>
         </is>
@@ -81583,7 +81583,7 @@
           <t>835</t>
         </is>
       </c>
-      <c r="AC467" s="14" t="inlineStr">
+      <c r="AC467" s="17" t="inlineStr">
         <is>
           <t>386</t>
         </is>
@@ -81670,7 +81670,7 @@
           <t>624</t>
         </is>
       </c>
-      <c r="I468" s="7" t="inlineStr">
+      <c r="I468" s="17" t="inlineStr">
         <is>
           <t>638</t>
         </is>
@@ -81962,7 +81962,7 @@
           <t>346</t>
         </is>
       </c>
-      <c r="AD469" s="14" t="inlineStr">
+      <c r="AD469" s="17" t="inlineStr">
         <is>
           <t>386</t>
         </is>
@@ -82024,7 +82024,7 @@
           <t>385</t>
         </is>
       </c>
-      <c r="E470" s="6" t="inlineStr">
+      <c r="E470" s="17" t="inlineStr">
         <is>
           <t>683</t>
         </is>
@@ -82039,7 +82039,7 @@
           <t>145</t>
         </is>
       </c>
-      <c r="H470" s="7" t="inlineStr">
+      <c r="H470" s="17" t="inlineStr">
         <is>
           <t>683</t>
         </is>
@@ -82802,7 +82802,7 @@
           <t>215</t>
         </is>
       </c>
-      <c r="K474" s="8" t="inlineStr">
+      <c r="K474" s="17" t="inlineStr">
         <is>
           <t>863</t>
         </is>
@@ -83635,7 +83635,7 @@
           <t>685</t>
         </is>
       </c>
-      <c r="AB478" s="13" t="inlineStr">
+      <c r="AB478" s="17" t="inlineStr">
         <is>
           <t>066</t>
         </is>
@@ -84141,7 +84141,7 @@
           <t>233</t>
         </is>
       </c>
-      <c r="Q481" s="17" t="inlineStr">
+      <c r="Q481" s="10" t="inlineStr">
         <is>
           <t>199</t>
         </is>
@@ -84844,7 +84844,7 @@
           <t>677</t>
         </is>
       </c>
-      <c r="H485" s="7" t="inlineStr">
+      <c r="H485" s="17" t="inlineStr">
         <is>
           <t>606</t>
         </is>
@@ -86001,7 +86001,7 @@
           <t>712</t>
         </is>
       </c>
-      <c r="AI493" s="17" t="inlineStr">
+      <c r="AI493" s="16" t="inlineStr">
         <is>
           <t>991</t>
         </is>
@@ -86048,7 +86048,7 @@
           <t>797</t>
         </is>
       </c>
-      <c r="G494" s="17" t="inlineStr">
+      <c r="G494" s="6" t="inlineStr">
         <is>
           <t>605</t>
         </is>
@@ -86791,12 +86791,12 @@
           <t>410</t>
         </is>
       </c>
-      <c r="F498" s="17" t="inlineStr">
+      <c r="F498" s="6" t="inlineStr">
         <is>
           <t>506</t>
         </is>
       </c>
-      <c r="G498" s="6" t="inlineStr">
+      <c r="G498" s="17" t="inlineStr">
         <is>
           <t>368</t>
         </is>
@@ -87123,7 +87123,7 @@
           <t>911</t>
         </is>
       </c>
-      <c r="AI499" s="17" t="inlineStr">
+      <c r="AI499" s="16" t="inlineStr">
         <is>
           <t>991</t>
         </is>
@@ -87133,7 +87133,7 @@
           <t>355</t>
         </is>
       </c>
-      <c r="AK499" s="17" t="inlineStr">
+      <c r="AK499" s="16" t="inlineStr">
         <is>
           <t>919</t>
         </is>
@@ -87290,7 +87290,7 @@
           <t>964</t>
         </is>
       </c>
-      <c r="AE500" s="17" t="inlineStr">
+      <c r="AE500" s="14" t="inlineStr">
         <is>
           <t>650</t>
         </is>
@@ -87689,7 +87689,7 @@
           <t>324</t>
         </is>
       </c>
-      <c r="AJ502" s="16" t="inlineStr">
+      <c r="AJ502" s="17" t="inlineStr">
         <is>
           <t>066</t>
         </is>
@@ -87706,7 +87706,7 @@
           <t>11</t>
         </is>
       </c>
-      <c r="B503" s="17" t="inlineStr">
+      <c r="B503" s="5" t="inlineStr">
         <is>
           <t>991</t>
         </is>
@@ -88302,7 +88302,7 @@
           <t>527</t>
         </is>
       </c>
-      <c r="I506" s="7" t="inlineStr">
+      <c r="I506" s="17" t="inlineStr">
         <is>
           <t>066</t>
         </is>
@@ -88397,7 +88397,7 @@
           <t>241</t>
         </is>
       </c>
-      <c r="AB506" s="13" t="inlineStr">
+      <c r="AB506" s="17" t="inlineStr">
         <is>
           <t>638</t>
         </is>
@@ -88599,7 +88599,7 @@
           <t>399</t>
         </is>
       </c>
-      <c r="AE507" s="14" t="inlineStr">
+      <c r="AE507" s="17" t="inlineStr">
         <is>
           <t>863</t>
         </is>
@@ -89207,7 +89207,7 @@
           <t>533</t>
         </is>
       </c>
-      <c r="C511" s="5" t="inlineStr">
+      <c r="C511" s="17" t="inlineStr">
         <is>
           <t>863</t>
         </is>
@@ -89357,7 +89357,7 @@
           <t>558</t>
         </is>
       </c>
-      <c r="AG511" s="17" t="inlineStr">
+      <c r="AG511" s="15" t="inlineStr">
         <is>
           <t>056</t>
         </is>
@@ -90521,7 +90521,7 @@
           <t>043</t>
         </is>
       </c>
-      <c r="D518" s="17" t="inlineStr">
+      <c r="D518" s="5" t="inlineStr">
         <is>
           <t>605</t>
         </is>
@@ -91187,7 +91187,7 @@
           <t>363</t>
         </is>
       </c>
-      <c r="Y521" s="12" t="inlineStr">
+      <c r="Y521" s="17" t="inlineStr">
         <is>
           <t>683</t>
         </is>
@@ -91259,12 +91259,12 @@
           <t>30</t>
         </is>
       </c>
-      <c r="B522" s="17" t="inlineStr">
+      <c r="B522" s="5" t="inlineStr">
         <is>
           <t>199</t>
         </is>
       </c>
-      <c r="C522" s="17" t="inlineStr">
+      <c r="C522" s="5" t="inlineStr">
         <is>
           <t>056</t>
         </is>
@@ -91654,6 +91654,13 @@
       </c>
       <c r="I526" s="2" t="n"/>
       <c r="J526" s="3" t="n"/>
+      <c r="K526" s="1" t="inlineStr">
+        <is>
+          <t>April 2021</t>
+        </is>
+      </c>
+      <c r="L526" s="2" t="n"/>
+      <c r="M526" s="3" t="n"/>
     </row>
     <row r="527">
       <c r="A527" s="4" t="n"/>
@@ -91702,6 +91709,21 @@
           <t>9PM</t>
         </is>
       </c>
+      <c r="K527" s="1" t="inlineStr">
+        <is>
+          <t>11AM</t>
+        </is>
+      </c>
+      <c r="L527" s="1" t="inlineStr">
+        <is>
+          <t>4PM</t>
+        </is>
+      </c>
+      <c r="M527" s="1" t="inlineStr">
+        <is>
+          <t>9PM</t>
+        </is>
+      </c>
     </row>
     <row r="528">
       <c r="A528" s="1" t="inlineStr">
@@ -91754,6 +91776,21 @@
           <t>107</t>
         </is>
       </c>
+      <c r="K528" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L528" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M528" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="529">
       <c r="A529" s="1" t="inlineStr">
@@ -91806,6 +91843,21 @@
           <t>113</t>
         </is>
       </c>
+      <c r="K529" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L529" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M529" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="530">
       <c r="A530" s="1" t="inlineStr">
@@ -91858,6 +91910,21 @@
           <t>310</t>
         </is>
       </c>
+      <c r="K530" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L530" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M530" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="531">
       <c r="A531" s="1" t="inlineStr">
@@ -91910,6 +91977,21 @@
           <t>813</t>
         </is>
       </c>
+      <c r="K531" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L531" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M531" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="532">
       <c r="A532" s="1" t="inlineStr">
@@ -91962,6 +92044,21 @@
           <t>089</t>
         </is>
       </c>
+      <c r="K532" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L532" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M532" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="533">
       <c r="A533" s="1" t="inlineStr">
@@ -92014,6 +92111,21 @@
           <t>079</t>
         </is>
       </c>
+      <c r="K533" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L533" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M533" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="534">
       <c r="A534" s="1" t="inlineStr">
@@ -92066,6 +92178,21 @@
           <t>197</t>
         </is>
       </c>
+      <c r="K534" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L534" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M534" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="535">
       <c r="A535" s="1" t="inlineStr">
@@ -92118,6 +92245,21 @@
           <t>681</t>
         </is>
       </c>
+      <c r="K535" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L535" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M535" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="536">
       <c r="A536" s="1" t="inlineStr">
@@ -92170,6 +92312,21 @@
           <t>363</t>
         </is>
       </c>
+      <c r="K536" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L536" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M536" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="537">
       <c r="A537" s="1" t="inlineStr">
@@ -92222,6 +92379,21 @@
           <t>607</t>
         </is>
       </c>
+      <c r="K537" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L537" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M537" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="538">
       <c r="A538" s="1" t="inlineStr">
@@ -92254,7 +92426,7 @@
           <t>198</t>
         </is>
       </c>
-      <c r="G538" s="17" t="inlineStr">
+      <c r="G538" s="6" t="inlineStr">
         <is>
           <t>605</t>
         </is>
@@ -92272,6 +92444,21 @@
       <c r="J538" s="7" t="inlineStr">
         <is>
           <t>811</t>
+        </is>
+      </c>
+      <c r="K538" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L538" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M538" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
     </row>
@@ -92326,6 +92513,21 @@
           <t>996</t>
         </is>
       </c>
+      <c r="K539" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L539" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M539" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="540">
       <c r="A540" s="1" t="inlineStr">
@@ -92378,6 +92580,21 @@
           <t>442</t>
         </is>
       </c>
+      <c r="K540" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L540" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M540" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="541">
       <c r="A541" s="1" t="inlineStr">
@@ -92430,6 +92647,21 @@
           <t>126</t>
         </is>
       </c>
+      <c r="K541" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L541" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M541" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="542">
       <c r="A542" s="1" t="inlineStr">
@@ -92482,6 +92714,21 @@
           <t>950</t>
         </is>
       </c>
+      <c r="K542" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L542" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M542" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="543">
       <c r="A543" s="1" t="inlineStr">
@@ -92534,6 +92781,21 @@
           <t>274</t>
         </is>
       </c>
+      <c r="K543" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L543" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M543" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="544">
       <c r="A544" s="1" t="inlineStr">
@@ -92586,6 +92848,21 @@
           <t>584</t>
         </is>
       </c>
+      <c r="K544" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L544" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M544" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="545">
       <c r="A545" s="1" t="inlineStr">
@@ -92638,6 +92915,21 @@
           <t>952</t>
         </is>
       </c>
+      <c r="K545" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L545" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M545" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="546">
       <c r="A546" s="1" t="inlineStr">
@@ -92675,12 +92967,12 @@
           <t>446</t>
         </is>
       </c>
-      <c r="H546" s="7" t="inlineStr">
+      <c r="H546" s="17" t="inlineStr">
         <is>
           <t>683</t>
         </is>
       </c>
-      <c r="I546" s="7" t="inlineStr">
+      <c r="I546" s="17" t="inlineStr">
         <is>
           <t>606</t>
         </is>
@@ -92688,6 +92980,21 @@
       <c r="J546" s="7" t="inlineStr">
         <is>
           <t>530</t>
+        </is>
+      </c>
+      <c r="K546" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L546" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M546" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
     </row>
@@ -92742,6 +93049,21 @@
           <t>631</t>
         </is>
       </c>
+      <c r="K547" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L547" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M547" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="548">
       <c r="A548" s="1" t="inlineStr">
@@ -92769,7 +93091,7 @@
           <t>323</t>
         </is>
       </c>
-      <c r="F548" s="6" t="inlineStr">
+      <c r="F548" s="17" t="inlineStr">
         <is>
           <t>660</t>
         </is>
@@ -92792,6 +93114,21 @@
       <c r="J548" s="7" t="inlineStr">
         <is>
           <t>790</t>
+        </is>
+      </c>
+      <c r="K548" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L548" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M548" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
     </row>
@@ -92846,6 +93183,21 @@
           <t>134</t>
         </is>
       </c>
+      <c r="K549" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L549" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M549" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="550">
       <c r="A550" s="1" t="inlineStr">
@@ -92873,7 +93225,7 @@
           <t>414</t>
         </is>
       </c>
-      <c r="F550" s="6" t="inlineStr">
+      <c r="F550" s="17" t="inlineStr">
         <is>
           <t>863</t>
         </is>
@@ -92893,9 +93245,24 @@
           <t>404</t>
         </is>
       </c>
-      <c r="J550" s="17" t="inlineStr">
+      <c r="J550" s="7" t="inlineStr">
         <is>
           <t>560</t>
+        </is>
+      </c>
+      <c r="K550" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L550" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M550" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
     </row>
@@ -92950,6 +93317,21 @@
           <t>370</t>
         </is>
       </c>
+      <c r="K551" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L551" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M551" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="552">
       <c r="A552" s="1" t="inlineStr">
@@ -93002,6 +93384,21 @@
           <t>461</t>
         </is>
       </c>
+      <c r="K552" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L552" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M552" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="553">
       <c r="A553" s="1" t="inlineStr">
@@ -93054,6 +93451,21 @@
           <t>913</t>
         </is>
       </c>
+      <c r="K553" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L553" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M553" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="554">
       <c r="A554" s="1" t="inlineStr">
@@ -93106,6 +93518,21 @@
           <t>788</t>
         </is>
       </c>
+      <c r="K554" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L554" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M554" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="555">
       <c r="A555" s="1" t="inlineStr">
@@ -93145,15 +93572,30 @@
       </c>
       <c r="H555" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>338</t>
         </is>
       </c>
       <c r="I555" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>727</t>
         </is>
       </c>
       <c r="J555" s="7" t="inlineStr">
+        <is>
+          <t>094</t>
+        </is>
+      </c>
+      <c r="K555" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L555" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M555" s="8" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -93197,15 +93639,30 @@
       </c>
       <c r="H556" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>915</t>
         </is>
       </c>
       <c r="I556" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>934</t>
         </is>
       </c>
       <c r="J556" s="7" t="inlineStr">
+        <is>
+          <t>994</t>
+        </is>
+      </c>
+      <c r="K556" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L556" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M556" s="8" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -93217,7 +93674,7 @@
           <t>30</t>
         </is>
       </c>
-      <c r="B557" s="5" t="inlineStr">
+      <c r="B557" s="17" t="inlineStr">
         <is>
           <t>066</t>
         </is>
@@ -93249,15 +93706,30 @@
       </c>
       <c r="H557" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>797</t>
         </is>
       </c>
       <c r="I557" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>412</t>
         </is>
       </c>
       <c r="J557" s="7" t="inlineStr">
+        <is>
+          <t>939</t>
+        </is>
+      </c>
+      <c r="K557" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L557" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M557" s="8" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -93301,22 +93773,37 @@
       </c>
       <c r="H558" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>998</t>
         </is>
       </c>
       <c r="I558" s="7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>231</t>
         </is>
       </c>
       <c r="J558" s="7" t="inlineStr">
+        <is>
+          <t>886</t>
+        </is>
+      </c>
+      <c r="K558" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L558" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M558" s="8" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="199">
+  <mergeCells count="200">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
@@ -93516,6 +94003,7 @@
     <mergeCell ref="B526:D526"/>
     <mergeCell ref="E526:G526"/>
     <mergeCell ref="H526:J526"/>
+    <mergeCell ref="K526:M526"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
update results with new solid pattern proof
</commit_message>
<xml_diff>
--- a/swertres/excel_results.xlsx
+++ b/swertres/excel_results.xlsx
@@ -92105,17 +92105,17 @@
       </c>
       <c r="K533" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>335</t>
         </is>
       </c>
       <c r="L533" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>772</t>
         </is>
       </c>
       <c r="M533" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>650</t>
         </is>
       </c>
     </row>
@@ -92172,17 +92172,17 @@
       </c>
       <c r="K534" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>405</t>
         </is>
       </c>
       <c r="L534" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>197</t>
         </is>
       </c>
       <c r="M534" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>155</t>
         </is>
       </c>
     </row>
@@ -92239,17 +92239,17 @@
       </c>
       <c r="K535" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>693</t>
         </is>
       </c>
       <c r="L535" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>787</t>
         </is>
       </c>
       <c r="M535" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>816</t>
         </is>
       </c>
     </row>
@@ -92306,17 +92306,17 @@
       </c>
       <c r="K536" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>407</t>
         </is>
       </c>
       <c r="L536" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>498</t>
         </is>
       </c>
       <c r="M536" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>198</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
optimize filtering results for script_excel_results.py
</commit_message>
<xml_diff>
--- a/swertres/excel_results.xlsx
+++ b/swertres/excel_results.xlsx
@@ -92373,17 +92373,17 @@
       </c>
       <c r="K537" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>768</t>
         </is>
       </c>
       <c r="L537" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>550</t>
         </is>
       </c>
       <c r="M537" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>168</t>
         </is>
       </c>
     </row>
@@ -92440,17 +92440,17 @@
       </c>
       <c r="K538" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>065</t>
         </is>
       </c>
       <c r="L538" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>555</t>
         </is>
       </c>
       <c r="M538" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>340</t>
         </is>
       </c>
     </row>
@@ -92507,12 +92507,12 @@
       </c>
       <c r="K539" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>959</t>
         </is>
       </c>
       <c r="L539" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>729</t>
         </is>
       </c>
       <c r="M539" s="8" t="inlineStr">

</xml_diff>

<commit_message>
position of prev results does not matter
</commit_message>
<xml_diff>
--- a/swertres/excel_results.xlsx
+++ b/swertres/excel_results.xlsx
@@ -29,7 +29,7 @@
       <sz val="15"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill/>
     </fill>
@@ -54,6 +54,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="00ccff33"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -204,7 +209,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
@@ -222,9 +227,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
@@ -246,6 +248,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1652,7 +1660,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="P7" s="9" t="inlineStr">
+      <c r="P7" s="17" t="inlineStr">
         <is>
           <t>877</t>
         </is>
@@ -1742,7 +1750,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="AH7" s="15" t="inlineStr">
+      <c r="AH7" s="17" t="inlineStr">
         <is>
           <t>778</t>
         </is>
@@ -2273,7 +2281,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="AB10" s="13" t="inlineStr">
+      <c r="AB10" s="17" t="inlineStr">
         <is>
           <t>487</t>
         </is>
@@ -4442,7 +4450,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="M22" s="8" t="inlineStr">
+      <c r="M22" s="17" t="inlineStr">
         <is>
           <t>784</t>
         </is>
@@ -8688,7 +8696,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="V47" s="11" t="inlineStr">
+      <c r="V47" s="17" t="inlineStr">
         <is>
           <t>874</t>
         </is>
@@ -9159,7 +9167,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="D50" s="5" t="inlineStr">
+      <c r="D50" s="17" t="inlineStr">
         <is>
           <t>877</t>
         </is>
@@ -9441,7 +9449,7 @@
           <t>271</t>
         </is>
       </c>
-      <c r="W51" s="12" t="inlineStr">
+      <c r="W51" s="17" t="inlineStr">
         <is>
           <t>778</t>
         </is>
@@ -11655,7 +11663,7 @@
           <t>798</t>
         </is>
       </c>
-      <c r="Q63" s="10" t="inlineStr">
+      <c r="Q63" s="17" t="inlineStr">
         <is>
           <t>787</t>
         </is>
@@ -12129,7 +12137,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="AK65" s="16" t="inlineStr">
+      <c r="AK65" s="17" t="inlineStr">
         <is>
           <t>877</t>
         </is>
@@ -16432,7 +16440,7 @@
           <t>083</t>
         </is>
       </c>
-      <c r="T91" s="11" t="inlineStr">
+      <c r="T91" s="17" t="inlineStr">
         <is>
           <t>487</t>
         </is>
@@ -16594,7 +16602,7 @@
           <t>266</t>
         </is>
       </c>
-      <c r="O92" s="9" t="inlineStr">
+      <c r="O92" s="17" t="inlineStr">
         <is>
           <t>778</t>
         </is>
@@ -17200,7 +17208,7 @@
           <t>638</t>
         </is>
       </c>
-      <c r="X95" s="12" t="inlineStr">
+      <c r="X95" s="17" t="inlineStr">
         <is>
           <t>487</t>
         </is>
@@ -17539,7 +17547,7 @@
           <t>921</t>
         </is>
       </c>
-      <c r="Q97" s="10" t="inlineStr">
+      <c r="Q97" s="17" t="inlineStr">
         <is>
           <t>748</t>
         </is>
@@ -17918,7 +17926,7 @@
           <t>151</t>
         </is>
       </c>
-      <c r="R99" s="10" t="inlineStr">
+      <c r="R99" s="17" t="inlineStr">
         <is>
           <t>748</t>
         </is>
@@ -18050,7 +18058,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="G100" s="6" t="inlineStr">
+      <c r="G100" s="17" t="inlineStr">
         <is>
           <t>487</t>
         </is>
@@ -19409,7 +19417,7 @@
           <t>832</t>
         </is>
       </c>
-      <c r="AK109" s="16" t="inlineStr">
+      <c r="AK109" s="17" t="inlineStr">
         <is>
           <t>778</t>
         </is>
@@ -19738,7 +19746,7 @@
           <t>989</t>
         </is>
       </c>
-      <c r="AB111" s="13" t="inlineStr">
+      <c r="AB111" s="17" t="inlineStr">
         <is>
           <t>784</t>
         </is>
@@ -19835,7 +19843,7 @@
           <t>381</t>
         </is>
       </c>
-      <c r="J112" s="7" t="inlineStr">
+      <c r="J112" s="17" t="inlineStr">
         <is>
           <t>784</t>
         </is>
@@ -20381,7 +20389,7 @@
           <t>562</t>
         </is>
       </c>
-      <c r="G115" s="6" t="inlineStr">
+      <c r="G115" s="17" t="inlineStr">
         <is>
           <t>478</t>
         </is>
@@ -20471,7 +20479,7 @@
           <t>613</t>
         </is>
       </c>
-      <c r="Y115" s="12" t="inlineStr">
+      <c r="Y115" s="17" t="inlineStr">
         <is>
           <t>847</t>
         </is>
@@ -22478,7 +22486,7 @@
           <t>375</t>
         </is>
       </c>
-      <c r="O126" s="9" t="inlineStr">
+      <c r="O126" s="17" t="inlineStr">
         <is>
           <t>478</t>
         </is>
@@ -26208,7 +26216,7 @@
           <t>929</t>
         </is>
       </c>
-      <c r="AG148" s="15" t="inlineStr">
+      <c r="AG148" s="17" t="inlineStr">
         <is>
           <t>787</t>
         </is>
@@ -27063,7 +27071,7 @@
           <t>936</t>
         </is>
       </c>
-      <c r="Q153" s="10" t="inlineStr">
+      <c r="Q153" s="17" t="inlineStr">
         <is>
           <t>487</t>
         </is>
@@ -28377,7 +28385,7 @@
           <t>652</t>
         </is>
       </c>
-      <c r="R160" s="10" t="inlineStr">
+      <c r="R160" s="17" t="inlineStr">
         <is>
           <t>478</t>
         </is>
@@ -28796,7 +28804,7 @@
           <t>956</t>
         </is>
       </c>
-      <c r="AA162" s="13" t="inlineStr">
+      <c r="AA162" s="17" t="inlineStr">
         <is>
           <t>874</t>
         </is>
@@ -28928,7 +28936,7 @@
           <t>294</t>
         </is>
       </c>
-      <c r="P163" s="9" t="inlineStr">
+      <c r="P163" s="17" t="inlineStr">
         <is>
           <t>478</t>
         </is>
@@ -29499,7 +29507,7 @@
           <t>199</t>
         </is>
       </c>
-      <c r="R166" s="10" t="inlineStr">
+      <c r="R166" s="17" t="inlineStr">
         <is>
           <t>478</t>
         </is>
@@ -29534,7 +29542,7 @@
           <t>340</t>
         </is>
       </c>
-      <c r="Y166" s="12" t="inlineStr">
+      <c r="Y166" s="17" t="inlineStr">
         <is>
           <t>877</t>
         </is>
@@ -29746,7 +29754,7 @@
           <t>799</t>
         </is>
       </c>
-      <c r="AD167" s="14" t="inlineStr">
+      <c r="AD167" s="17" t="inlineStr">
         <is>
           <t>847</t>
         </is>
@@ -30257,7 +30265,7 @@
           <t>908</t>
         </is>
       </c>
-      <c r="T170" s="11" t="inlineStr">
+      <c r="T170" s="17" t="inlineStr">
         <is>
           <t>877</t>
         </is>
@@ -31294,7 +31302,7 @@
           <t>021</t>
         </is>
       </c>
-      <c r="W178" s="12" t="inlineStr">
+      <c r="W178" s="17" t="inlineStr">
         <is>
           <t>787</t>
         </is>
@@ -31962,7 +31970,7 @@
           <t>279</t>
         </is>
       </c>
-      <c r="G182" s="6" t="inlineStr">
+      <c r="G182" s="17" t="inlineStr">
         <is>
           <t>784</t>
         </is>
@@ -32740,7 +32748,7 @@
           <t>455</t>
         </is>
       </c>
-      <c r="M186" s="8" t="inlineStr">
+      <c r="M186" s="17" t="inlineStr">
         <is>
           <t>787</t>
         </is>
@@ -32750,7 +32758,7 @@
           <t>126</t>
         </is>
       </c>
-      <c r="O186" s="9" t="inlineStr">
+      <c r="O186" s="17" t="inlineStr">
         <is>
           <t>874</t>
         </is>
@@ -34802,7 +34810,7 @@
           <t>756</t>
         </is>
       </c>
-      <c r="N197" s="9" t="inlineStr">
+      <c r="N197" s="17" t="inlineStr">
         <is>
           <t>784</t>
         </is>
@@ -35655,7 +35663,7 @@
           <t>327</t>
         </is>
       </c>
-      <c r="AI201" s="16" t="inlineStr">
+      <c r="AI201" s="17" t="inlineStr">
         <is>
           <t>478</t>
         </is>
@@ -35772,7 +35780,7 @@
           <t>841</t>
         </is>
       </c>
-      <c r="U202" s="11" t="inlineStr">
+      <c r="U202" s="17" t="inlineStr">
         <is>
           <t>487</t>
         </is>
@@ -35879,7 +35887,7 @@
           <t>097</t>
         </is>
       </c>
-      <c r="E203" s="6" t="inlineStr">
+      <c r="E203" s="17" t="inlineStr">
         <is>
           <t>778</t>
         </is>
@@ -38128,7 +38136,7 @@
           <t>275</t>
         </is>
       </c>
-      <c r="Z217" s="13" t="inlineStr">
+      <c r="Z217" s="17" t="inlineStr">
         <is>
           <t>877</t>
         </is>
@@ -38148,7 +38156,7 @@
           <t>740</t>
         </is>
       </c>
-      <c r="AD217" s="14" t="inlineStr">
+      <c r="AD217" s="17" t="inlineStr">
         <is>
           <t>847</t>
         </is>
@@ -38230,7 +38238,7 @@
           <t>033</t>
         </is>
       </c>
-      <c r="I218" s="7" t="inlineStr">
+      <c r="I218" s="17" t="inlineStr">
         <is>
           <t>778</t>
         </is>
@@ -38517,7 +38525,7 @@
           <t>532</t>
         </is>
       </c>
-      <c r="AC219" s="14" t="inlineStr">
+      <c r="AC219" s="17" t="inlineStr">
         <is>
           <t>847</t>
         </is>
@@ -40584,7 +40592,7 @@
           <t>192</t>
         </is>
       </c>
-      <c r="AE230" s="14" t="inlineStr">
+      <c r="AE230" s="17" t="inlineStr">
         <is>
           <t>847</t>
         </is>
@@ -41529,7 +41537,7 @@
           <t>403</t>
         </is>
       </c>
-      <c r="AG235" s="15" t="inlineStr">
+      <c r="AG235" s="17" t="inlineStr">
         <is>
           <t>787</t>
         </is>
@@ -42596,7 +42604,7 @@
           <t>860</t>
         </is>
       </c>
-      <c r="V241" s="11" t="inlineStr">
+      <c r="V241" s="17" t="inlineStr">
         <is>
           <t>787</t>
         </is>
@@ -43386,7 +43394,7 @@
           <t>825</t>
         </is>
       </c>
-      <c r="M248" s="8" t="inlineStr">
+      <c r="M248" s="17" t="inlineStr">
         <is>
           <t>787</t>
         </is>
@@ -44346,7 +44354,7 @@
           <t>269</t>
         </is>
       </c>
-      <c r="R253" s="10" t="inlineStr">
+      <c r="R253" s="17" t="inlineStr">
         <is>
           <t>877</t>
         </is>
@@ -44750,7 +44758,7 @@
           <t>411</t>
         </is>
       </c>
-      <c r="X255" s="12" t="inlineStr">
+      <c r="X255" s="17" t="inlineStr">
         <is>
           <t>877</t>
         </is>
@@ -45366,7 +45374,7 @@
           <t>465</t>
         </is>
       </c>
-      <c r="AI258" s="16" t="inlineStr">
+      <c r="AI258" s="17" t="inlineStr">
         <is>
           <t>478</t>
         </is>
@@ -45533,7 +45541,7 @@
           <t>519</t>
         </is>
       </c>
-      <c r="AE259" s="14" t="inlineStr">
+      <c r="AE259" s="17" t="inlineStr">
         <is>
           <t>478</t>
         </is>
@@ -45862,7 +45870,7 @@
           <t>691</t>
         </is>
       </c>
-      <c r="V261" s="11" t="inlineStr">
+      <c r="V261" s="17" t="inlineStr">
         <is>
           <t>778</t>
         </is>
@@ -46186,7 +46194,7 @@
           <t>371</t>
         </is>
       </c>
-      <c r="L263" s="8" t="inlineStr">
+      <c r="L263" s="17" t="inlineStr">
         <is>
           <t>748</t>
         </is>
@@ -46413,7 +46421,7 @@
           <t>959</t>
         </is>
       </c>
-      <c r="T264" s="11" t="inlineStr">
+      <c r="T264" s="17" t="inlineStr">
         <is>
           <t>847</t>
         </is>
@@ -46525,7 +46533,7 @@
           <t>835</t>
         </is>
       </c>
-      <c r="E265" s="6" t="inlineStr">
+      <c r="E265" s="17" t="inlineStr">
         <is>
           <t>478</t>
         </is>
@@ -47054,7 +47062,7 @@
           <t>495</t>
         </is>
       </c>
-      <c r="AJ267" s="16" t="inlineStr">
+      <c r="AJ267" s="17" t="inlineStr">
         <is>
           <t>748</t>
         </is>
@@ -47368,7 +47376,7 @@
           <t>618</t>
         </is>
       </c>
-      <c r="X269" s="12" t="inlineStr">
+      <c r="X269" s="17" t="inlineStr">
         <is>
           <t>787</t>
         </is>
@@ -47418,7 +47426,7 @@
           <t>588</t>
         </is>
       </c>
-      <c r="AH269" s="15" t="inlineStr">
+      <c r="AH269" s="17" t="inlineStr">
         <is>
           <t>877</t>
         </is>
@@ -47530,7 +47538,7 @@
           <t>217</t>
         </is>
       </c>
-      <c r="S270" s="10" t="inlineStr">
+      <c r="S270" s="17" t="inlineStr">
         <is>
           <t>784</t>
         </is>
@@ -47914,7 +47922,7 @@
           <t>856</t>
         </is>
       </c>
-      <c r="U272" s="11" t="inlineStr">
+      <c r="U272" s="17" t="inlineStr">
         <is>
           <t>778</t>
         </is>
@@ -47959,7 +47967,7 @@
           <t>643</t>
         </is>
       </c>
-      <c r="AD272" s="14" t="inlineStr">
+      <c r="AD272" s="17" t="inlineStr">
         <is>
           <t>877</t>
         </is>
@@ -48849,7 +48857,7 @@
           <t>227</t>
         </is>
       </c>
-      <c r="U277" s="11" t="inlineStr">
+      <c r="U277" s="17" t="inlineStr">
         <is>
           <t>784</t>
         </is>
@@ -49659,7 +49667,7 @@
           <t>763</t>
         </is>
       </c>
-      <c r="P284" s="9" t="inlineStr">
+      <c r="P284" s="17" t="inlineStr">
         <is>
           <t>847</t>
         </is>
@@ -50185,7 +50193,7 @@
           <t>584</t>
         </is>
       </c>
-      <c r="I287" s="7" t="inlineStr">
+      <c r="I287" s="17" t="inlineStr">
         <is>
           <t>487</t>
         </is>
@@ -51327,7 +51335,7 @@
           <t>964</t>
         </is>
       </c>
-      <c r="M293" s="8" t="inlineStr">
+      <c r="M293" s="17" t="inlineStr">
         <is>
           <t>847</t>
         </is>
@@ -51539,7 +51547,7 @@
           <t>858</t>
         </is>
       </c>
-      <c r="R294" s="10" t="inlineStr">
+      <c r="R294" s="17" t="inlineStr">
         <is>
           <t>778</t>
         </is>
@@ -51838,7 +51846,7 @@
           <t>046</t>
         </is>
       </c>
-      <c r="C296" s="5" t="inlineStr">
+      <c r="C296" s="17" t="inlineStr">
         <is>
           <t>847</t>
         </is>
@@ -52008,7 +52016,7 @@
           <t>148</t>
         </is>
       </c>
-      <c r="AK296" s="16" t="inlineStr">
+      <c r="AK296" s="17" t="inlineStr">
         <is>
           <t>847</t>
         </is>
@@ -52217,7 +52225,7 @@
           <t>160</t>
         </is>
       </c>
-      <c r="D298" s="5" t="inlineStr">
+      <c r="D298" s="17" t="inlineStr">
         <is>
           <t>874</t>
         </is>
@@ -52706,7 +52714,7 @@
           <t>046</t>
         </is>
       </c>
-      <c r="AA300" s="13" t="inlineStr">
+      <c r="AA300" s="17" t="inlineStr">
         <is>
           <t>478</t>
         </is>
@@ -53317,7 +53325,7 @@
           <t>063</t>
         </is>
       </c>
-      <c r="AK303" s="16" t="inlineStr">
+      <c r="AK303" s="17" t="inlineStr">
         <is>
           <t>784</t>
         </is>
@@ -54369,7 +54377,7 @@
           <t>244</t>
         </is>
       </c>
-      <c r="W309" s="12" t="inlineStr">
+      <c r="W309" s="17" t="inlineStr">
         <is>
           <t>748</t>
         </is>
@@ -54379,7 +54387,7 @@
           <t>524</t>
         </is>
       </c>
-      <c r="Y309" s="12" t="inlineStr">
+      <c r="Y309" s="17" t="inlineStr">
         <is>
           <t>778</t>
         </is>
@@ -54429,7 +54437,7 @@
           <t>688</t>
         </is>
       </c>
-      <c r="AI309" s="16" t="inlineStr">
+      <c r="AI309" s="17" t="inlineStr">
         <is>
           <t>787</t>
         </is>
@@ -55047,7 +55055,7 @@
           <t>547</t>
         </is>
       </c>
-      <c r="I313" s="7" t="inlineStr">
+      <c r="I313" s="17" t="inlineStr">
         <is>
           <t>847</t>
         </is>
@@ -56074,7 +56082,7 @@
           <t>205</t>
         </is>
       </c>
-      <c r="J321" s="7" t="inlineStr">
+      <c r="J321" s="17" t="inlineStr">
         <is>
           <t>778</t>
         </is>
@@ -56610,7 +56618,7 @@
           <t>653</t>
         </is>
       </c>
-      <c r="E324" s="6" t="inlineStr">
+      <c r="E324" s="17" t="inlineStr">
         <is>
           <t>487</t>
         </is>
@@ -56695,7 +56703,7 @@
           <t>217</t>
         </is>
       </c>
-      <c r="V324" s="11" t="inlineStr">
+      <c r="V324" s="17" t="inlineStr">
         <is>
           <t>847</t>
         </is>
@@ -56872,7 +56880,7 @@
           <t>242</t>
         </is>
       </c>
-      <c r="T325" s="11" t="inlineStr">
+      <c r="T325" s="17" t="inlineStr">
         <is>
           <t>874</t>
         </is>
@@ -57161,7 +57169,7 @@
           <t>726</t>
         </is>
       </c>
-      <c r="C327" s="5" t="inlineStr">
+      <c r="C327" s="17" t="inlineStr">
         <is>
           <t>748</t>
         </is>
@@ -58054,7 +58062,7 @@
           <t>201</t>
         </is>
       </c>
-      <c r="AF331" s="15" t="inlineStr">
+      <c r="AF331" s="17" t="inlineStr">
         <is>
           <t>847</t>
         </is>
@@ -58767,7 +58775,7 @@
           <t>279</t>
         </is>
       </c>
-      <c r="Y335" s="12" t="inlineStr">
+      <c r="Y335" s="17" t="inlineStr">
         <is>
           <t>847</t>
         </is>
@@ -60415,7 +60423,7 @@
           <t>184</t>
         </is>
       </c>
-      <c r="R344" s="10" t="inlineStr">
+      <c r="R344" s="17" t="inlineStr">
         <is>
           <t>787</t>
         </is>
@@ -60956,7 +60964,7 @@
           <t>231</t>
         </is>
       </c>
-      <c r="N347" s="9" t="inlineStr">
+      <c r="N347" s="17" t="inlineStr">
         <is>
           <t>847</t>
         </is>
@@ -61801,7 +61809,7 @@
           <t>517</t>
         </is>
       </c>
-      <c r="P354" s="9" t="inlineStr">
+      <c r="P354" s="17" t="inlineStr">
         <is>
           <t>784</t>
         </is>
@@ -63449,7 +63457,7 @@
           <t>016</t>
         </is>
       </c>
-      <c r="I363" s="7" t="inlineStr">
+      <c r="I363" s="17" t="inlineStr">
         <is>
           <t>487</t>
         </is>
@@ -63943,7 +63951,7 @@
           <t>606</t>
         </is>
       </c>
-      <c r="AG365" s="15" t="inlineStr">
+      <c r="AG365" s="17" t="inlineStr">
         <is>
           <t>874</t>
         </is>
@@ -64459,7 +64467,7 @@
           <t>938</t>
         </is>
       </c>
-      <c r="X368" s="12" t="inlineStr">
+      <c r="X368" s="17" t="inlineStr">
         <is>
           <t>784</t>
         </is>
@@ -65516,7 +65524,7 @@
           <t>040</t>
         </is>
       </c>
-      <c r="K374" s="8" t="inlineStr">
+      <c r="K374" s="17" t="inlineStr">
         <is>
           <t>778</t>
         </is>
@@ -65683,7 +65691,7 @@
           <t>958</t>
         </is>
       </c>
-      <c r="G375" s="6" t="inlineStr">
+      <c r="G375" s="17" t="inlineStr">
         <is>
           <t>487</t>
         </is>
@@ -65713,7 +65721,7 @@
           <t>822</t>
         </is>
       </c>
-      <c r="M375" s="8" t="inlineStr">
+      <c r="M375" s="17" t="inlineStr">
         <is>
           <t>877</t>
         </is>
@@ -65975,7 +65983,7 @@
           <t>307</t>
         </is>
       </c>
-      <c r="AB376" s="13" t="inlineStr">
+      <c r="AB376" s="17" t="inlineStr">
         <is>
           <t>778</t>
         </is>
@@ -66005,7 +66013,7 @@
           <t>003</t>
         </is>
       </c>
-      <c r="AH376" s="15" t="inlineStr">
+      <c r="AH376" s="17" t="inlineStr">
         <is>
           <t>478</t>
         </is>
@@ -66102,7 +66110,7 @@
           <t>624</t>
         </is>
       </c>
-      <c r="P377" s="9" t="inlineStr">
+      <c r="P377" s="17" t="inlineStr">
         <is>
           <t>778</t>
         </is>
@@ -66618,7 +66626,7 @@
           <t>913</t>
         </is>
       </c>
-      <c r="G380" s="6" t="inlineStr">
+      <c r="G380" s="17" t="inlineStr">
         <is>
           <t>847</t>
         </is>
@@ -66673,7 +66681,7 @@
           <t>711</t>
         </is>
       </c>
-      <c r="R380" s="10" t="inlineStr">
+      <c r="R380" s="17" t="inlineStr">
         <is>
           <t>487</t>
         </is>
@@ -66967,7 +66975,7 @@
           <t>30</t>
         </is>
       </c>
-      <c r="B382" s="5" t="inlineStr">
+      <c r="B382" s="17" t="inlineStr">
         <is>
           <t>487</t>
         </is>
@@ -67785,7 +67793,7 @@
           <t>935</t>
         </is>
       </c>
-      <c r="AJ388" s="16" t="inlineStr">
+      <c r="AJ388" s="17" t="inlineStr">
         <is>
           <t>874</t>
         </is>
@@ -68346,7 +68354,7 @@
           <t>585</t>
         </is>
       </c>
-      <c r="AJ391" s="16" t="inlineStr">
+      <c r="AJ391" s="17" t="inlineStr">
         <is>
           <t>847</t>
         </is>
@@ -69373,7 +69381,7 @@
           <t>747</t>
         </is>
       </c>
-      <c r="Q397" s="10" t="inlineStr">
+      <c r="Q397" s="17" t="inlineStr">
         <is>
           <t>847</t>
         </is>
@@ -69495,7 +69503,7 @@
           <t>364</t>
         </is>
       </c>
-      <c r="D398" s="5" t="inlineStr">
+      <c r="D398" s="17" t="inlineStr">
         <is>
           <t>748</t>
         </is>
@@ -69640,7 +69648,7 @@
           <t>759</t>
         </is>
       </c>
-      <c r="AG398" s="15" t="inlineStr">
+      <c r="AG398" s="17" t="inlineStr">
         <is>
           <t>778</t>
         </is>
@@ -71303,7 +71311,7 @@
           <t>698</t>
         </is>
       </c>
-      <c r="AC407" s="14" t="inlineStr">
+      <c r="AC407" s="17" t="inlineStr">
         <is>
           <t>787</t>
         </is>
@@ -71854,7 +71862,7 @@
           <t>813</t>
         </is>
       </c>
-      <c r="AA410" s="13" t="inlineStr">
+      <c r="AA410" s="17" t="inlineStr">
         <is>
           <t>748</t>
         </is>
@@ -74125,7 +74133,7 @@
           <t>398</t>
         </is>
       </c>
-      <c r="O425" s="9" t="inlineStr">
+      <c r="O425" s="17" t="inlineStr">
         <is>
           <t>874</t>
         </is>
@@ -75758,7 +75766,7 @@
           <t>306</t>
         </is>
       </c>
-      <c r="E434" s="6" t="inlineStr">
+      <c r="E434" s="17" t="inlineStr">
         <is>
           <t>778</t>
         </is>
@@ -76818,7 +76826,7 @@
           <t>102</t>
         </is>
       </c>
-      <c r="AD439" s="14" t="inlineStr">
+      <c r="AD439" s="17" t="inlineStr">
         <is>
           <t>487</t>
         </is>
@@ -76905,12 +76913,12 @@
           <t>279</t>
         </is>
       </c>
-      <c r="J440" s="7" t="inlineStr">
+      <c r="J440" s="17" t="inlineStr">
         <is>
           <t>874</t>
         </is>
       </c>
-      <c r="K440" s="8" t="inlineStr">
+      <c r="K440" s="17" t="inlineStr">
         <is>
           <t>748</t>
         </is>
@@ -77501,7 +77509,7 @@
           <t>239</t>
         </is>
       </c>
-      <c r="Q443" s="10" t="inlineStr">
+      <c r="Q443" s="17" t="inlineStr">
         <is>
           <t>877</t>
         </is>
@@ -77521,7 +77529,7 @@
           <t>502</t>
         </is>
       </c>
-      <c r="U443" s="11" t="inlineStr">
+      <c r="U443" s="17" t="inlineStr">
         <is>
           <t>778</t>
         </is>
@@ -78264,7 +78272,7 @@
           <t>882</t>
         </is>
       </c>
-      <c r="T447" s="11" t="inlineStr">
+      <c r="T447" s="17" t="inlineStr">
         <is>
           <t>487</t>
         </is>
@@ -78673,7 +78681,7 @@
           <t>520</t>
         </is>
       </c>
-      <c r="AA449" s="13" t="inlineStr">
+      <c r="AA449" s="17" t="inlineStr">
         <is>
           <t>874</t>
         </is>
@@ -78693,7 +78701,7 @@
           <t>758</t>
         </is>
       </c>
-      <c r="AE449" s="14" t="inlineStr">
+      <c r="AE449" s="17" t="inlineStr">
         <is>
           <t>487</t>
         </is>
@@ -80054,7 +80062,7 @@
           <t>841</t>
         </is>
       </c>
-      <c r="X459" s="12" t="inlineStr">
+      <c r="X459" s="17" t="inlineStr">
         <is>
           <t>787</t>
         </is>
@@ -80797,7 +80805,7 @@
           <t>217</t>
         </is>
       </c>
-      <c r="W463" s="12" t="inlineStr">
+      <c r="W463" s="17" t="inlineStr">
         <is>
           <t>487</t>
         </is>
@@ -81066,7 +81074,7 @@
           <t>08</t>
         </is>
       </c>
-      <c r="B465" s="5" t="inlineStr">
+      <c r="B465" s="17" t="inlineStr">
         <is>
           <t>874</t>
         </is>
@@ -81869,7 +81877,7 @@
           <t>310</t>
         </is>
       </c>
-      <c r="M469" s="8" t="inlineStr">
+      <c r="M469" s="17" t="inlineStr">
         <is>
           <t>847</t>
         </is>
@@ -83128,7 +83136,7 @@
           <t>375</t>
         </is>
       </c>
-      <c r="C476" s="5" t="inlineStr">
+      <c r="C476" s="17" t="inlineStr">
         <is>
           <t>874</t>
         </is>
@@ -83739,7 +83747,7 @@
           <t>897</t>
         </is>
       </c>
-      <c r="M479" s="8" t="inlineStr">
+      <c r="M479" s="17" t="inlineStr">
         <is>
           <t>487</t>
         </is>
@@ -84118,7 +84126,7 @@
           <t>383</t>
         </is>
       </c>
-      <c r="N481" s="9" t="inlineStr">
+      <c r="N481" s="17" t="inlineStr">
         <is>
           <t>877</t>
         </is>
@@ -84365,7 +84373,7 @@
           <t>952</t>
         </is>
       </c>
-      <c r="Z482" s="13" t="inlineStr">
+      <c r="Z482" s="17" t="inlineStr">
         <is>
           <t>478</t>
         </is>
@@ -84896,7 +84904,7 @@
           <t>518</t>
         </is>
       </c>
-      <c r="T485" s="11" t="inlineStr">
+      <c r="T485" s="17" t="inlineStr">
         <is>
           <t>748</t>
         </is>
@@ -85397,7 +85405,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="H488" s="7" t="inlineStr">
+      <c r="H488" s="17" t="inlineStr">
         <is>
           <t>487</t>
         </is>
@@ -86893,7 +86901,7 @@
           <t>839</t>
         </is>
       </c>
-      <c r="AB498" s="13" t="inlineStr">
+      <c r="AB498" s="17" t="inlineStr">
         <is>
           <t>784</t>
         </is>
@@ -90279,7 +90287,7 @@
           <t>343</t>
         </is>
       </c>
-      <c r="AF516" s="15" t="inlineStr">
+      <c r="AF516" s="17" t="inlineStr">
         <is>
           <t>877</t>
         </is>
@@ -90471,7 +90479,7 @@
           <t>039</t>
         </is>
       </c>
-      <c r="AG517" s="15" t="inlineStr">
+      <c r="AG517" s="17" t="inlineStr">
         <is>
           <t>748</t>
         </is>
@@ -90623,7 +90631,7 @@
           <t>304</t>
         </is>
       </c>
-      <c r="Z518" s="13" t="inlineStr">
+      <c r="Z518" s="17" t="inlineStr">
         <is>
           <t>478</t>
         </is>
@@ -90850,7 +90858,7 @@
           <t>376</t>
         </is>
       </c>
-      <c r="AH519" s="15" t="inlineStr">
+      <c r="AH519" s="17" t="inlineStr">
         <is>
           <t>877</t>
         </is>
@@ -92006,7 +92014,7 @@
           <t>852</t>
         </is>
       </c>
-      <c r="E532" s="6" t="inlineStr">
+      <c r="E532" s="17" t="inlineStr">
         <is>
           <t>778</t>
         </is>
@@ -92036,12 +92044,12 @@
           <t>089</t>
         </is>
       </c>
-      <c r="K532" s="8" t="inlineStr">
+      <c r="K532" s="17" t="inlineStr">
         <is>
           <t>778</t>
         </is>
       </c>
-      <c r="L532" s="8" t="inlineStr">
+      <c r="L532" s="17" t="inlineStr">
         <is>
           <t>847</t>
         </is>
@@ -92242,7 +92250,7 @@
           <t>693</t>
         </is>
       </c>
-      <c r="L535" s="8" t="inlineStr">
+      <c r="L535" s="17" t="inlineStr">
         <is>
           <t>787</t>
         </is>
@@ -92517,7 +92525,7 @@
       </c>
       <c r="M539" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>368</t>
         </is>
       </c>
     </row>
@@ -92624,7 +92632,7 @@
           <t>597</t>
         </is>
       </c>
-      <c r="H541" s="7" t="inlineStr">
+      <c r="H541" s="17" t="inlineStr">
         <is>
           <t>487</t>
         </is>

</xml_diff>

<commit_message>
update results, new pattern added
</commit_message>
<xml_diff>
--- a/swertres/excel_results.xlsx
+++ b/swertres/excel_results.xlsx
@@ -29,7 +29,7 @@
       <sz val="15"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="14">
     <fill>
       <patternFill/>
     </fill>
@@ -54,11 +54,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="00ccff33"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FFFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -209,7 +204,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
@@ -227,6 +222,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
@@ -248,12 +246,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1660,7 +1652,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="P7" s="17" t="inlineStr">
+      <c r="P7" s="9" t="inlineStr">
         <is>
           <t>877</t>
         </is>
@@ -1750,7 +1742,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="AH7" s="17" t="inlineStr">
+      <c r="AH7" s="15" t="inlineStr">
         <is>
           <t>778</t>
         </is>
@@ -2281,7 +2273,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="AB10" s="17" t="inlineStr">
+      <c r="AB10" s="13" t="inlineStr">
         <is>
           <t>487</t>
         </is>
@@ -4450,7 +4442,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="M22" s="17" t="inlineStr">
+      <c r="M22" s="8" t="inlineStr">
         <is>
           <t>784</t>
         </is>
@@ -8696,7 +8688,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="V47" s="17" t="inlineStr">
+      <c r="V47" s="11" t="inlineStr">
         <is>
           <t>874</t>
         </is>
@@ -9167,7 +9159,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="D50" s="17" t="inlineStr">
+      <c r="D50" s="5" t="inlineStr">
         <is>
           <t>877</t>
         </is>
@@ -9449,7 +9441,7 @@
           <t>271</t>
         </is>
       </c>
-      <c r="W51" s="17" t="inlineStr">
+      <c r="W51" s="12" t="inlineStr">
         <is>
           <t>778</t>
         </is>
@@ -11663,7 +11655,7 @@
           <t>798</t>
         </is>
       </c>
-      <c r="Q63" s="17" t="inlineStr">
+      <c r="Q63" s="10" t="inlineStr">
         <is>
           <t>787</t>
         </is>
@@ -12137,7 +12129,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="AK65" s="17" t="inlineStr">
+      <c r="AK65" s="16" t="inlineStr">
         <is>
           <t>877</t>
         </is>
@@ -16440,7 +16432,7 @@
           <t>083</t>
         </is>
       </c>
-      <c r="T91" s="17" t="inlineStr">
+      <c r="T91" s="11" t="inlineStr">
         <is>
           <t>487</t>
         </is>
@@ -16602,7 +16594,7 @@
           <t>266</t>
         </is>
       </c>
-      <c r="O92" s="17" t="inlineStr">
+      <c r="O92" s="9" t="inlineStr">
         <is>
           <t>778</t>
         </is>
@@ -17208,7 +17200,7 @@
           <t>638</t>
         </is>
       </c>
-      <c r="X95" s="17" t="inlineStr">
+      <c r="X95" s="12" t="inlineStr">
         <is>
           <t>487</t>
         </is>
@@ -17547,7 +17539,7 @@
           <t>921</t>
         </is>
       </c>
-      <c r="Q97" s="17" t="inlineStr">
+      <c r="Q97" s="10" t="inlineStr">
         <is>
           <t>748</t>
         </is>
@@ -17926,7 +17918,7 @@
           <t>151</t>
         </is>
       </c>
-      <c r="R99" s="17" t="inlineStr">
+      <c r="R99" s="10" t="inlineStr">
         <is>
           <t>748</t>
         </is>
@@ -18058,7 +18050,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="G100" s="17" t="inlineStr">
+      <c r="G100" s="6" t="inlineStr">
         <is>
           <t>487</t>
         </is>
@@ -19417,7 +19409,7 @@
           <t>832</t>
         </is>
       </c>
-      <c r="AK109" s="17" t="inlineStr">
+      <c r="AK109" s="16" t="inlineStr">
         <is>
           <t>778</t>
         </is>
@@ -19746,7 +19738,7 @@
           <t>989</t>
         </is>
       </c>
-      <c r="AB111" s="17" t="inlineStr">
+      <c r="AB111" s="13" t="inlineStr">
         <is>
           <t>784</t>
         </is>
@@ -19843,7 +19835,7 @@
           <t>381</t>
         </is>
       </c>
-      <c r="J112" s="17" t="inlineStr">
+      <c r="J112" s="7" t="inlineStr">
         <is>
           <t>784</t>
         </is>
@@ -20389,7 +20381,7 @@
           <t>562</t>
         </is>
       </c>
-      <c r="G115" s="17" t="inlineStr">
+      <c r="G115" s="6" t="inlineStr">
         <is>
           <t>478</t>
         </is>
@@ -20479,7 +20471,7 @@
           <t>613</t>
         </is>
       </c>
-      <c r="Y115" s="17" t="inlineStr">
+      <c r="Y115" s="12" t="inlineStr">
         <is>
           <t>847</t>
         </is>
@@ -22486,7 +22478,7 @@
           <t>375</t>
         </is>
       </c>
-      <c r="O126" s="17" t="inlineStr">
+      <c r="O126" s="9" t="inlineStr">
         <is>
           <t>478</t>
         </is>
@@ -26216,7 +26208,7 @@
           <t>929</t>
         </is>
       </c>
-      <c r="AG148" s="17" t="inlineStr">
+      <c r="AG148" s="15" t="inlineStr">
         <is>
           <t>787</t>
         </is>
@@ -27071,7 +27063,7 @@
           <t>936</t>
         </is>
       </c>
-      <c r="Q153" s="17" t="inlineStr">
+      <c r="Q153" s="10" t="inlineStr">
         <is>
           <t>487</t>
         </is>
@@ -28385,7 +28377,7 @@
           <t>652</t>
         </is>
       </c>
-      <c r="R160" s="17" t="inlineStr">
+      <c r="R160" s="10" t="inlineStr">
         <is>
           <t>478</t>
         </is>
@@ -28804,7 +28796,7 @@
           <t>956</t>
         </is>
       </c>
-      <c r="AA162" s="17" t="inlineStr">
+      <c r="AA162" s="13" t="inlineStr">
         <is>
           <t>874</t>
         </is>
@@ -28936,7 +28928,7 @@
           <t>294</t>
         </is>
       </c>
-      <c r="P163" s="17" t="inlineStr">
+      <c r="P163" s="9" t="inlineStr">
         <is>
           <t>478</t>
         </is>
@@ -29507,7 +29499,7 @@
           <t>199</t>
         </is>
       </c>
-      <c r="R166" s="17" t="inlineStr">
+      <c r="R166" s="10" t="inlineStr">
         <is>
           <t>478</t>
         </is>
@@ -29542,7 +29534,7 @@
           <t>340</t>
         </is>
       </c>
-      <c r="Y166" s="17" t="inlineStr">
+      <c r="Y166" s="12" t="inlineStr">
         <is>
           <t>877</t>
         </is>
@@ -29754,7 +29746,7 @@
           <t>799</t>
         </is>
       </c>
-      <c r="AD167" s="17" t="inlineStr">
+      <c r="AD167" s="14" t="inlineStr">
         <is>
           <t>847</t>
         </is>
@@ -30265,7 +30257,7 @@
           <t>908</t>
         </is>
       </c>
-      <c r="T170" s="17" t="inlineStr">
+      <c r="T170" s="11" t="inlineStr">
         <is>
           <t>877</t>
         </is>
@@ -31302,7 +31294,7 @@
           <t>021</t>
         </is>
       </c>
-      <c r="W178" s="17" t="inlineStr">
+      <c r="W178" s="12" t="inlineStr">
         <is>
           <t>787</t>
         </is>
@@ -31970,7 +31962,7 @@
           <t>279</t>
         </is>
       </c>
-      <c r="G182" s="17" t="inlineStr">
+      <c r="G182" s="6" t="inlineStr">
         <is>
           <t>784</t>
         </is>
@@ -32748,7 +32740,7 @@
           <t>455</t>
         </is>
       </c>
-      <c r="M186" s="17" t="inlineStr">
+      <c r="M186" s="8" t="inlineStr">
         <is>
           <t>787</t>
         </is>
@@ -32758,7 +32750,7 @@
           <t>126</t>
         </is>
       </c>
-      <c r="O186" s="17" t="inlineStr">
+      <c r="O186" s="9" t="inlineStr">
         <is>
           <t>874</t>
         </is>
@@ -34810,7 +34802,7 @@
           <t>756</t>
         </is>
       </c>
-      <c r="N197" s="17" t="inlineStr">
+      <c r="N197" s="9" t="inlineStr">
         <is>
           <t>784</t>
         </is>
@@ -35663,7 +35655,7 @@
           <t>327</t>
         </is>
       </c>
-      <c r="AI201" s="17" t="inlineStr">
+      <c r="AI201" s="16" t="inlineStr">
         <is>
           <t>478</t>
         </is>
@@ -35780,7 +35772,7 @@
           <t>841</t>
         </is>
       </c>
-      <c r="U202" s="17" t="inlineStr">
+      <c r="U202" s="11" t="inlineStr">
         <is>
           <t>487</t>
         </is>
@@ -35887,7 +35879,7 @@
           <t>097</t>
         </is>
       </c>
-      <c r="E203" s="17" t="inlineStr">
+      <c r="E203" s="6" t="inlineStr">
         <is>
           <t>778</t>
         </is>
@@ -38136,7 +38128,7 @@
           <t>275</t>
         </is>
       </c>
-      <c r="Z217" s="17" t="inlineStr">
+      <c r="Z217" s="13" t="inlineStr">
         <is>
           <t>877</t>
         </is>
@@ -38156,7 +38148,7 @@
           <t>740</t>
         </is>
       </c>
-      <c r="AD217" s="17" t="inlineStr">
+      <c r="AD217" s="14" t="inlineStr">
         <is>
           <t>847</t>
         </is>
@@ -38238,7 +38230,7 @@
           <t>033</t>
         </is>
       </c>
-      <c r="I218" s="17" t="inlineStr">
+      <c r="I218" s="7" t="inlineStr">
         <is>
           <t>778</t>
         </is>
@@ -38525,7 +38517,7 @@
           <t>532</t>
         </is>
       </c>
-      <c r="AC219" s="17" t="inlineStr">
+      <c r="AC219" s="14" t="inlineStr">
         <is>
           <t>847</t>
         </is>
@@ -40592,7 +40584,7 @@
           <t>192</t>
         </is>
       </c>
-      <c r="AE230" s="17" t="inlineStr">
+      <c r="AE230" s="14" t="inlineStr">
         <is>
           <t>847</t>
         </is>
@@ -41537,7 +41529,7 @@
           <t>403</t>
         </is>
       </c>
-      <c r="AG235" s="17" t="inlineStr">
+      <c r="AG235" s="15" t="inlineStr">
         <is>
           <t>787</t>
         </is>
@@ -42604,7 +42596,7 @@
           <t>860</t>
         </is>
       </c>
-      <c r="V241" s="17" t="inlineStr">
+      <c r="V241" s="11" t="inlineStr">
         <is>
           <t>787</t>
         </is>
@@ -43394,7 +43386,7 @@
           <t>825</t>
         </is>
       </c>
-      <c r="M248" s="17" t="inlineStr">
+      <c r="M248" s="8" t="inlineStr">
         <is>
           <t>787</t>
         </is>
@@ -44354,7 +44346,7 @@
           <t>269</t>
         </is>
       </c>
-      <c r="R253" s="17" t="inlineStr">
+      <c r="R253" s="10" t="inlineStr">
         <is>
           <t>877</t>
         </is>
@@ -44758,7 +44750,7 @@
           <t>411</t>
         </is>
       </c>
-      <c r="X255" s="17" t="inlineStr">
+      <c r="X255" s="12" t="inlineStr">
         <is>
           <t>877</t>
         </is>
@@ -45374,7 +45366,7 @@
           <t>465</t>
         </is>
       </c>
-      <c r="AI258" s="17" t="inlineStr">
+      <c r="AI258" s="16" t="inlineStr">
         <is>
           <t>478</t>
         </is>
@@ -45541,7 +45533,7 @@
           <t>519</t>
         </is>
       </c>
-      <c r="AE259" s="17" t="inlineStr">
+      <c r="AE259" s="14" t="inlineStr">
         <is>
           <t>478</t>
         </is>
@@ -45870,7 +45862,7 @@
           <t>691</t>
         </is>
       </c>
-      <c r="V261" s="17" t="inlineStr">
+      <c r="V261" s="11" t="inlineStr">
         <is>
           <t>778</t>
         </is>
@@ -46194,7 +46186,7 @@
           <t>371</t>
         </is>
       </c>
-      <c r="L263" s="17" t="inlineStr">
+      <c r="L263" s="8" t="inlineStr">
         <is>
           <t>748</t>
         </is>
@@ -46421,7 +46413,7 @@
           <t>959</t>
         </is>
       </c>
-      <c r="T264" s="17" t="inlineStr">
+      <c r="T264" s="11" t="inlineStr">
         <is>
           <t>847</t>
         </is>
@@ -46533,7 +46525,7 @@
           <t>835</t>
         </is>
       </c>
-      <c r="E265" s="17" t="inlineStr">
+      <c r="E265" s="6" t="inlineStr">
         <is>
           <t>478</t>
         </is>
@@ -47062,7 +47054,7 @@
           <t>495</t>
         </is>
       </c>
-      <c r="AJ267" s="17" t="inlineStr">
+      <c r="AJ267" s="16" t="inlineStr">
         <is>
           <t>748</t>
         </is>
@@ -47376,7 +47368,7 @@
           <t>618</t>
         </is>
       </c>
-      <c r="X269" s="17" t="inlineStr">
+      <c r="X269" s="12" t="inlineStr">
         <is>
           <t>787</t>
         </is>
@@ -47426,7 +47418,7 @@
           <t>588</t>
         </is>
       </c>
-      <c r="AH269" s="17" t="inlineStr">
+      <c r="AH269" s="15" t="inlineStr">
         <is>
           <t>877</t>
         </is>
@@ -47538,7 +47530,7 @@
           <t>217</t>
         </is>
       </c>
-      <c r="S270" s="17" t="inlineStr">
+      <c r="S270" s="10" t="inlineStr">
         <is>
           <t>784</t>
         </is>
@@ -47922,7 +47914,7 @@
           <t>856</t>
         </is>
       </c>
-      <c r="U272" s="17" t="inlineStr">
+      <c r="U272" s="11" t="inlineStr">
         <is>
           <t>778</t>
         </is>
@@ -47967,7 +47959,7 @@
           <t>643</t>
         </is>
       </c>
-      <c r="AD272" s="17" t="inlineStr">
+      <c r="AD272" s="14" t="inlineStr">
         <is>
           <t>877</t>
         </is>
@@ -48857,7 +48849,7 @@
           <t>227</t>
         </is>
       </c>
-      <c r="U277" s="17" t="inlineStr">
+      <c r="U277" s="11" t="inlineStr">
         <is>
           <t>784</t>
         </is>
@@ -49667,7 +49659,7 @@
           <t>763</t>
         </is>
       </c>
-      <c r="P284" s="17" t="inlineStr">
+      <c r="P284" s="9" t="inlineStr">
         <is>
           <t>847</t>
         </is>
@@ -50193,7 +50185,7 @@
           <t>584</t>
         </is>
       </c>
-      <c r="I287" s="17" t="inlineStr">
+      <c r="I287" s="7" t="inlineStr">
         <is>
           <t>487</t>
         </is>
@@ -51335,7 +51327,7 @@
           <t>964</t>
         </is>
       </c>
-      <c r="M293" s="17" t="inlineStr">
+      <c r="M293" s="8" t="inlineStr">
         <is>
           <t>847</t>
         </is>
@@ -51547,7 +51539,7 @@
           <t>858</t>
         </is>
       </c>
-      <c r="R294" s="17" t="inlineStr">
+      <c r="R294" s="10" t="inlineStr">
         <is>
           <t>778</t>
         </is>
@@ -51846,7 +51838,7 @@
           <t>046</t>
         </is>
       </c>
-      <c r="C296" s="17" t="inlineStr">
+      <c r="C296" s="5" t="inlineStr">
         <is>
           <t>847</t>
         </is>
@@ -52016,7 +52008,7 @@
           <t>148</t>
         </is>
       </c>
-      <c r="AK296" s="17" t="inlineStr">
+      <c r="AK296" s="16" t="inlineStr">
         <is>
           <t>847</t>
         </is>
@@ -52225,7 +52217,7 @@
           <t>160</t>
         </is>
       </c>
-      <c r="D298" s="17" t="inlineStr">
+      <c r="D298" s="5" t="inlineStr">
         <is>
           <t>874</t>
         </is>
@@ -52714,7 +52706,7 @@
           <t>046</t>
         </is>
       </c>
-      <c r="AA300" s="17" t="inlineStr">
+      <c r="AA300" s="13" t="inlineStr">
         <is>
           <t>478</t>
         </is>
@@ -53325,7 +53317,7 @@
           <t>063</t>
         </is>
       </c>
-      <c r="AK303" s="17" t="inlineStr">
+      <c r="AK303" s="16" t="inlineStr">
         <is>
           <t>784</t>
         </is>
@@ -54377,7 +54369,7 @@
           <t>244</t>
         </is>
       </c>
-      <c r="W309" s="17" t="inlineStr">
+      <c r="W309" s="12" t="inlineStr">
         <is>
           <t>748</t>
         </is>
@@ -54387,7 +54379,7 @@
           <t>524</t>
         </is>
       </c>
-      <c r="Y309" s="17" t="inlineStr">
+      <c r="Y309" s="12" t="inlineStr">
         <is>
           <t>778</t>
         </is>
@@ -54437,7 +54429,7 @@
           <t>688</t>
         </is>
       </c>
-      <c r="AI309" s="17" t="inlineStr">
+      <c r="AI309" s="16" t="inlineStr">
         <is>
           <t>787</t>
         </is>
@@ -55055,7 +55047,7 @@
           <t>547</t>
         </is>
       </c>
-      <c r="I313" s="17" t="inlineStr">
+      <c r="I313" s="7" t="inlineStr">
         <is>
           <t>847</t>
         </is>
@@ -56082,7 +56074,7 @@
           <t>205</t>
         </is>
       </c>
-      <c r="J321" s="17" t="inlineStr">
+      <c r="J321" s="7" t="inlineStr">
         <is>
           <t>778</t>
         </is>
@@ -56618,7 +56610,7 @@
           <t>653</t>
         </is>
       </c>
-      <c r="E324" s="17" t="inlineStr">
+      <c r="E324" s="6" t="inlineStr">
         <is>
           <t>487</t>
         </is>
@@ -56703,7 +56695,7 @@
           <t>217</t>
         </is>
       </c>
-      <c r="V324" s="17" t="inlineStr">
+      <c r="V324" s="11" t="inlineStr">
         <is>
           <t>847</t>
         </is>
@@ -56880,7 +56872,7 @@
           <t>242</t>
         </is>
       </c>
-      <c r="T325" s="17" t="inlineStr">
+      <c r="T325" s="11" t="inlineStr">
         <is>
           <t>874</t>
         </is>
@@ -57169,7 +57161,7 @@
           <t>726</t>
         </is>
       </c>
-      <c r="C327" s="17" t="inlineStr">
+      <c r="C327" s="5" t="inlineStr">
         <is>
           <t>748</t>
         </is>
@@ -58062,7 +58054,7 @@
           <t>201</t>
         </is>
       </c>
-      <c r="AF331" s="17" t="inlineStr">
+      <c r="AF331" s="15" t="inlineStr">
         <is>
           <t>847</t>
         </is>
@@ -58775,7 +58767,7 @@
           <t>279</t>
         </is>
       </c>
-      <c r="Y335" s="17" t="inlineStr">
+      <c r="Y335" s="12" t="inlineStr">
         <is>
           <t>847</t>
         </is>
@@ -60423,7 +60415,7 @@
           <t>184</t>
         </is>
       </c>
-      <c r="R344" s="17" t="inlineStr">
+      <c r="R344" s="10" t="inlineStr">
         <is>
           <t>787</t>
         </is>
@@ -60964,7 +60956,7 @@
           <t>231</t>
         </is>
       </c>
-      <c r="N347" s="17" t="inlineStr">
+      <c r="N347" s="9" t="inlineStr">
         <is>
           <t>847</t>
         </is>
@@ -61809,7 +61801,7 @@
           <t>517</t>
         </is>
       </c>
-      <c r="P354" s="17" t="inlineStr">
+      <c r="P354" s="9" t="inlineStr">
         <is>
           <t>784</t>
         </is>
@@ -63457,7 +63449,7 @@
           <t>016</t>
         </is>
       </c>
-      <c r="I363" s="17" t="inlineStr">
+      <c r="I363" s="7" t="inlineStr">
         <is>
           <t>487</t>
         </is>
@@ -63951,7 +63943,7 @@
           <t>606</t>
         </is>
       </c>
-      <c r="AG365" s="17" t="inlineStr">
+      <c r="AG365" s="15" t="inlineStr">
         <is>
           <t>874</t>
         </is>
@@ -64467,7 +64459,7 @@
           <t>938</t>
         </is>
       </c>
-      <c r="X368" s="17" t="inlineStr">
+      <c r="X368" s="12" t="inlineStr">
         <is>
           <t>784</t>
         </is>
@@ -65524,7 +65516,7 @@
           <t>040</t>
         </is>
       </c>
-      <c r="K374" s="17" t="inlineStr">
+      <c r="K374" s="8" t="inlineStr">
         <is>
           <t>778</t>
         </is>
@@ -65691,7 +65683,7 @@
           <t>958</t>
         </is>
       </c>
-      <c r="G375" s="17" t="inlineStr">
+      <c r="G375" s="6" t="inlineStr">
         <is>
           <t>487</t>
         </is>
@@ -65721,7 +65713,7 @@
           <t>822</t>
         </is>
       </c>
-      <c r="M375" s="17" t="inlineStr">
+      <c r="M375" s="8" t="inlineStr">
         <is>
           <t>877</t>
         </is>
@@ -65983,7 +65975,7 @@
           <t>307</t>
         </is>
       </c>
-      <c r="AB376" s="17" t="inlineStr">
+      <c r="AB376" s="13" t="inlineStr">
         <is>
           <t>778</t>
         </is>
@@ -66013,7 +66005,7 @@
           <t>003</t>
         </is>
       </c>
-      <c r="AH376" s="17" t="inlineStr">
+      <c r="AH376" s="15" t="inlineStr">
         <is>
           <t>478</t>
         </is>
@@ -66110,7 +66102,7 @@
           <t>624</t>
         </is>
       </c>
-      <c r="P377" s="17" t="inlineStr">
+      <c r="P377" s="9" t="inlineStr">
         <is>
           <t>778</t>
         </is>
@@ -66626,7 +66618,7 @@
           <t>913</t>
         </is>
       </c>
-      <c r="G380" s="17" t="inlineStr">
+      <c r="G380" s="6" t="inlineStr">
         <is>
           <t>847</t>
         </is>
@@ -66681,7 +66673,7 @@
           <t>711</t>
         </is>
       </c>
-      <c r="R380" s="17" t="inlineStr">
+      <c r="R380" s="10" t="inlineStr">
         <is>
           <t>487</t>
         </is>
@@ -66975,7 +66967,7 @@
           <t>30</t>
         </is>
       </c>
-      <c r="B382" s="17" t="inlineStr">
+      <c r="B382" s="5" t="inlineStr">
         <is>
           <t>487</t>
         </is>
@@ -67793,7 +67785,7 @@
           <t>935</t>
         </is>
       </c>
-      <c r="AJ388" s="17" t="inlineStr">
+      <c r="AJ388" s="16" t="inlineStr">
         <is>
           <t>874</t>
         </is>
@@ -68354,7 +68346,7 @@
           <t>585</t>
         </is>
       </c>
-      <c r="AJ391" s="17" t="inlineStr">
+      <c r="AJ391" s="16" t="inlineStr">
         <is>
           <t>847</t>
         </is>
@@ -69381,7 +69373,7 @@
           <t>747</t>
         </is>
       </c>
-      <c r="Q397" s="17" t="inlineStr">
+      <c r="Q397" s="10" t="inlineStr">
         <is>
           <t>847</t>
         </is>
@@ -69503,7 +69495,7 @@
           <t>364</t>
         </is>
       </c>
-      <c r="D398" s="17" t="inlineStr">
+      <c r="D398" s="5" t="inlineStr">
         <is>
           <t>748</t>
         </is>
@@ -69648,7 +69640,7 @@
           <t>759</t>
         </is>
       </c>
-      <c r="AG398" s="17" t="inlineStr">
+      <c r="AG398" s="15" t="inlineStr">
         <is>
           <t>778</t>
         </is>
@@ -71311,7 +71303,7 @@
           <t>698</t>
         </is>
       </c>
-      <c r="AC407" s="17" t="inlineStr">
+      <c r="AC407" s="14" t="inlineStr">
         <is>
           <t>787</t>
         </is>
@@ -71862,7 +71854,7 @@
           <t>813</t>
         </is>
       </c>
-      <c r="AA410" s="17" t="inlineStr">
+      <c r="AA410" s="13" t="inlineStr">
         <is>
           <t>748</t>
         </is>
@@ -74133,7 +74125,7 @@
           <t>398</t>
         </is>
       </c>
-      <c r="O425" s="17" t="inlineStr">
+      <c r="O425" s="9" t="inlineStr">
         <is>
           <t>874</t>
         </is>
@@ -75766,7 +75758,7 @@
           <t>306</t>
         </is>
       </c>
-      <c r="E434" s="17" t="inlineStr">
+      <c r="E434" s="6" t="inlineStr">
         <is>
           <t>778</t>
         </is>
@@ -76826,7 +76818,7 @@
           <t>102</t>
         </is>
       </c>
-      <c r="AD439" s="17" t="inlineStr">
+      <c r="AD439" s="14" t="inlineStr">
         <is>
           <t>487</t>
         </is>
@@ -76913,12 +76905,12 @@
           <t>279</t>
         </is>
       </c>
-      <c r="J440" s="17" t="inlineStr">
+      <c r="J440" s="7" t="inlineStr">
         <is>
           <t>874</t>
         </is>
       </c>
-      <c r="K440" s="17" t="inlineStr">
+      <c r="K440" s="8" t="inlineStr">
         <is>
           <t>748</t>
         </is>
@@ -77509,7 +77501,7 @@
           <t>239</t>
         </is>
       </c>
-      <c r="Q443" s="17" t="inlineStr">
+      <c r="Q443" s="10" t="inlineStr">
         <is>
           <t>877</t>
         </is>
@@ -77529,7 +77521,7 @@
           <t>502</t>
         </is>
       </c>
-      <c r="U443" s="17" t="inlineStr">
+      <c r="U443" s="11" t="inlineStr">
         <is>
           <t>778</t>
         </is>
@@ -78272,7 +78264,7 @@
           <t>882</t>
         </is>
       </c>
-      <c r="T447" s="17" t="inlineStr">
+      <c r="T447" s="11" t="inlineStr">
         <is>
           <t>487</t>
         </is>
@@ -78681,7 +78673,7 @@
           <t>520</t>
         </is>
       </c>
-      <c r="AA449" s="17" t="inlineStr">
+      <c r="AA449" s="13" t="inlineStr">
         <is>
           <t>874</t>
         </is>
@@ -78701,7 +78693,7 @@
           <t>758</t>
         </is>
       </c>
-      <c r="AE449" s="17" t="inlineStr">
+      <c r="AE449" s="14" t="inlineStr">
         <is>
           <t>487</t>
         </is>
@@ -80062,7 +80054,7 @@
           <t>841</t>
         </is>
       </c>
-      <c r="X459" s="17" t="inlineStr">
+      <c r="X459" s="12" t="inlineStr">
         <is>
           <t>787</t>
         </is>
@@ -80805,7 +80797,7 @@
           <t>217</t>
         </is>
       </c>
-      <c r="W463" s="17" t="inlineStr">
+      <c r="W463" s="12" t="inlineStr">
         <is>
           <t>487</t>
         </is>
@@ -81074,7 +81066,7 @@
           <t>08</t>
         </is>
       </c>
-      <c r="B465" s="17" t="inlineStr">
+      <c r="B465" s="5" t="inlineStr">
         <is>
           <t>874</t>
         </is>
@@ -81877,7 +81869,7 @@
           <t>310</t>
         </is>
       </c>
-      <c r="M469" s="17" t="inlineStr">
+      <c r="M469" s="8" t="inlineStr">
         <is>
           <t>847</t>
         </is>
@@ -83136,7 +83128,7 @@
           <t>375</t>
         </is>
       </c>
-      <c r="C476" s="17" t="inlineStr">
+      <c r="C476" s="5" t="inlineStr">
         <is>
           <t>874</t>
         </is>
@@ -83747,7 +83739,7 @@
           <t>897</t>
         </is>
       </c>
-      <c r="M479" s="17" t="inlineStr">
+      <c r="M479" s="8" t="inlineStr">
         <is>
           <t>487</t>
         </is>
@@ -84126,7 +84118,7 @@
           <t>383</t>
         </is>
       </c>
-      <c r="N481" s="17" t="inlineStr">
+      <c r="N481" s="9" t="inlineStr">
         <is>
           <t>877</t>
         </is>
@@ -84373,7 +84365,7 @@
           <t>952</t>
         </is>
       </c>
-      <c r="Z482" s="17" t="inlineStr">
+      <c r="Z482" s="13" t="inlineStr">
         <is>
           <t>478</t>
         </is>
@@ -84904,7 +84896,7 @@
           <t>518</t>
         </is>
       </c>
-      <c r="T485" s="17" t="inlineStr">
+      <c r="T485" s="11" t="inlineStr">
         <is>
           <t>748</t>
         </is>
@@ -85405,7 +85397,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="H488" s="17" t="inlineStr">
+      <c r="H488" s="7" t="inlineStr">
         <is>
           <t>487</t>
         </is>
@@ -86901,7 +86893,7 @@
           <t>839</t>
         </is>
       </c>
-      <c r="AB498" s="17" t="inlineStr">
+      <c r="AB498" s="13" t="inlineStr">
         <is>
           <t>784</t>
         </is>
@@ -90287,7 +90279,7 @@
           <t>343</t>
         </is>
       </c>
-      <c r="AF516" s="17" t="inlineStr">
+      <c r="AF516" s="15" t="inlineStr">
         <is>
           <t>877</t>
         </is>
@@ -90479,7 +90471,7 @@
           <t>039</t>
         </is>
       </c>
-      <c r="AG517" s="17" t="inlineStr">
+      <c r="AG517" s="15" t="inlineStr">
         <is>
           <t>748</t>
         </is>
@@ -90631,7 +90623,7 @@
           <t>304</t>
         </is>
       </c>
-      <c r="Z518" s="17" t="inlineStr">
+      <c r="Z518" s="13" t="inlineStr">
         <is>
           <t>478</t>
         </is>
@@ -90858,7 +90850,7 @@
           <t>376</t>
         </is>
       </c>
-      <c r="AH519" s="17" t="inlineStr">
+      <c r="AH519" s="15" t="inlineStr">
         <is>
           <t>877</t>
         </is>
@@ -92014,7 +92006,7 @@
           <t>852</t>
         </is>
       </c>
-      <c r="E532" s="17" t="inlineStr">
+      <c r="E532" s="6" t="inlineStr">
         <is>
           <t>778</t>
         </is>
@@ -92044,12 +92036,12 @@
           <t>089</t>
         </is>
       </c>
-      <c r="K532" s="17" t="inlineStr">
+      <c r="K532" s="8" t="inlineStr">
         <is>
           <t>778</t>
         </is>
       </c>
-      <c r="L532" s="17" t="inlineStr">
+      <c r="L532" s="8" t="inlineStr">
         <is>
           <t>847</t>
         </is>
@@ -92250,7 +92242,7 @@
           <t>693</t>
         </is>
       </c>
-      <c r="L535" s="17" t="inlineStr">
+      <c r="L535" s="8" t="inlineStr">
         <is>
           <t>787</t>
         </is>
@@ -92582,17 +92574,17 @@
       </c>
       <c r="K540" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>248</t>
         </is>
       </c>
       <c r="L540" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>764</t>
         </is>
       </c>
       <c r="M540" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>471</t>
         </is>
       </c>
     </row>
@@ -92632,7 +92624,7 @@
           <t>597</t>
         </is>
       </c>
-      <c r="H541" s="17" t="inlineStr">
+      <c r="H541" s="7" t="inlineStr">
         <is>
           <t>487</t>
         </is>
@@ -92649,17 +92641,17 @@
       </c>
       <c r="K541" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>727</t>
         </is>
       </c>
       <c r="L541" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>081</t>
         </is>
       </c>
       <c r="M541" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>392</t>
         </is>
       </c>
     </row>
@@ -92716,17 +92708,17 @@
       </c>
       <c r="K542" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>389</t>
         </is>
       </c>
       <c r="L542" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>818</t>
         </is>
       </c>
       <c r="M542" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>546</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
new pattern found, duplicate pairs with syndicate mirror pairs
</commit_message>
<xml_diff>
--- a/swertres/excel_results.xlsx
+++ b/swertres/excel_results.xlsx
@@ -92545,17 +92545,17 @@
       </c>
       <c r="N537" s="9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>809</t>
         </is>
       </c>
       <c r="O537" s="9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>925</t>
         </is>
       </c>
       <c r="P537" s="9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>373</t>
         </is>
       </c>
     </row>
@@ -92627,17 +92627,17 @@
       </c>
       <c r="N538" s="9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>377</t>
         </is>
       </c>
       <c r="O538" s="9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>563</t>
         </is>
       </c>
       <c r="P538" s="9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>536</t>
         </is>
       </c>
     </row>
@@ -92709,17 +92709,17 @@
       </c>
       <c r="N539" s="9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>264</t>
         </is>
       </c>
       <c r="O539" s="9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>282</t>
         </is>
       </c>
       <c r="P539" s="9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>881</t>
         </is>
       </c>
     </row>
@@ -92791,17 +92791,17 @@
       </c>
       <c r="N540" s="9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>703</t>
         </is>
       </c>
       <c r="O540" s="9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>293</t>
         </is>
       </c>
       <c r="P540" s="9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>236</t>
         </is>
       </c>
     </row>
@@ -92873,17 +92873,17 @@
       </c>
       <c r="N541" s="9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>235</t>
         </is>
       </c>
       <c r="O541" s="9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>048</t>
         </is>
       </c>
       <c r="P541" s="9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>066</t>
         </is>
       </c>
     </row>
@@ -92955,12 +92955,12 @@
       </c>
       <c r="N542" s="9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>901</t>
         </is>
       </c>
       <c r="O542" s="9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>733</t>
         </is>
       </c>
       <c r="P542" s="9" t="inlineStr">

</xml_diff>

<commit_message>
improve output for skip_pattern script
</commit_message>
<xml_diff>
--- a/swertres/excel_results.xlsx
+++ b/swertres/excel_results.xlsx
@@ -92965,7 +92965,7 @@
       </c>
       <c r="P542" s="9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>637</t>
         </is>
       </c>
     </row>
@@ -93037,17 +93037,17 @@
       </c>
       <c r="N543" s="9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>266</t>
         </is>
       </c>
       <c r="O543" s="9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>434</t>
         </is>
       </c>
       <c r="P543" s="9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>116</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
add sfo patterns; created excel_results_3
</commit_message>
<xml_diff>
--- a/swertres/excel_results.xlsx
+++ b/swertres/excel_results.xlsx
@@ -93119,17 +93119,17 @@
       </c>
       <c r="N544" s="9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>380</t>
         </is>
       </c>
       <c r="O544" s="9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>820</t>
         </is>
       </c>
       <c r="P544" s="9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>244</t>
         </is>
       </c>
     </row>
@@ -93201,17 +93201,17 @@
       </c>
       <c r="N545" s="9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>786</t>
         </is>
       </c>
       <c r="O545" s="9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>404</t>
         </is>
       </c>
       <c r="P545" s="9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>374</t>
         </is>
       </c>
     </row>
@@ -93283,17 +93283,17 @@
       </c>
       <c r="N546" s="9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>197</t>
         </is>
       </c>
       <c r="O546" s="9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>385</t>
         </is>
       </c>
       <c r="P546" s="9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>592</t>
         </is>
       </c>
     </row>
@@ -93365,17 +93365,17 @@
       </c>
       <c r="N547" s="9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>696</t>
         </is>
       </c>
       <c r="O547" s="9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>728</t>
         </is>
       </c>
       <c r="P547" s="9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>564</t>
         </is>
       </c>
     </row>

</xml_diff>